<commit_message>
"field updates and corrections"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -13,15 +13,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="229">
   <si>
     <t>Document</t>
   </si>
@@ -1669,56 +1669,6 @@
     <t>New RPN Request</t>
   </si>
   <si>
-    <r>
-      <t>add ‘</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>employment start date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>’ as an optional request field.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>New PRSI exemption option '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' added</t>
-    </r>
-  </si>
-  <si>
     <t>Submission Request Line Items</t>
   </si>
   <si>
@@ -1943,6 +1893,496 @@
         <scheme val="minor"/>
       </rPr>
       <t>format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>New PRSI exemption option '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">' added                                                                                     Payslip requirement removed                                                                                               </t>
+    </r>
+  </si>
+  <si>
+    <t>Example 4.2</t>
+  </si>
+  <si>
+    <t>Example 5.2</t>
+  </si>
+  <si>
+    <t>Example 5.3</t>
+  </si>
+  <si>
+    <t>Example 5.9</t>
+  </si>
+  <si>
+    <t>Example 5.10</t>
+  </si>
+  <si>
+    <t>Example 9.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ppsn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' corrected</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employeePpsn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDToDelete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' corrected to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDsToDelete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>newEmployeeDetails</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> element added</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>taxYear'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>totalRPNCount'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> removed from NewRPNResponse example</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDToDelete'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> corrected to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDsToDelete'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pensionTracingNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' corrected to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pensionTracingNumbers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">incomeTacCalculationBasis' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>corrected to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incomeTaxCalculationBasis'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pensionTracingNumber' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>corrected format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uscPaidToDate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> correct to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USCDeductedToDate'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">yearlyUSCRateCutOff </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in taxRate property corrected to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yearlyRateCutOff</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Added ‘</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employment start date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>’ as an optional request field.</t>
+    </r>
+  </si>
+  <si>
+    <t>REST Integration Guide</t>
+  </si>
+  <si>
+    <t>HTTP-Method-Override</t>
+  </si>
+  <si>
+    <t>Example clarified</t>
+  </si>
+  <si>
+    <t>Property description clarified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employeeIDs </t>
+  </si>
+  <si>
+    <r>
+      <t>add ‘</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employmentStartDate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>’ as an optional request field.</t>
     </r>
   </si>
 </sst>
@@ -2528,7 +2968,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2709,13 +3149,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2735,6 +3169,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2782,22 +3231,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2808,32 +3266,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2849,9 +3325,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2874,47 +3347,55 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3283,12 +3764,12 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3313,12 +3794,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3361,10 +3842,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="87">
+      <c r="B7" s="90">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3379,8 +3860,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="85"/>
-      <c r="B8" s="88"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="91"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3393,8 +3874,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="85"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3407,8 +3888,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="85"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3421,8 +3902,8 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="85"/>
-      <c r="B11" s="88"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -3435,8 +3916,8 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="89"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -3449,10 +3930,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="87">
+      <c r="B13" s="90">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3467,8 +3948,8 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="93"/>
-      <c r="B14" s="89"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -3517,12 +3998,12 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="83"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="86"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3565,22 +4046,22 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="83"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="86"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="91">
+      <c r="B21" s="94">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -3595,8 +4076,8 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="95"/>
-      <c r="B22" s="89"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="92"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -3619,18 +4100,18 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="83"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="86"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="91">
+      <c r="B25" s="94">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -3645,8 +4126,8 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="85"/>
-      <c r="B26" s="88"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="91"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -3659,8 +4140,8 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="85"/>
-      <c r="B27" s="88"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="91"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -3673,8 +4154,8 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="85"/>
-      <c r="B28" s="88"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="91"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -3687,8 +4168,8 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="85"/>
-      <c r="B29" s="88"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="91"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -3701,8 +4182,8 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
-      <c r="B30" s="88"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="91"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -3715,8 +4196,8 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="85"/>
-      <c r="B31" s="88"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="91"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -3729,8 +4210,8 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
-      <c r="B32" s="89"/>
+      <c r="A32" s="89"/>
+      <c r="B32" s="92"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -3855,12 +4336,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="82"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="83"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="86"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -3920,7 +4401,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3930,7 +4411,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4040,10 +4521,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4054,8 +4535,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="106"/>
-      <c r="B8" s="105"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4064,8 +4545,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="106"/>
-      <c r="B9" s="105"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4074,8 +4555,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="106"/>
-      <c r="B10" s="105"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4084,8 +4565,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="106"/>
-      <c r="B11" s="105"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4094,8 +4575,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="106"/>
-      <c r="B12" s="105"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4104,10 +4585,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4118,8 +4599,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108"/>
-      <c r="B14" s="105"/>
+      <c r="A14" s="112"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4128,8 +4609,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108"/>
-      <c r="B15" s="105"/>
+      <c r="A15" s="112"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4138,10 +4619,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="111" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4152,8 +4633,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4162,8 +4643,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
-      <c r="B18" s="100"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4172,8 +4653,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
-      <c r="B19" s="100"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4182,8 +4663,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109"/>
-      <c r="B20" s="100"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4192,8 +4673,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
-      <c r="B21" s="100"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4202,8 +4683,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="109"/>
-      <c r="B22" s="100"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4212,8 +4693,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="109"/>
-      <c r="B23" s="100"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="111"/>
       <c r="C23" s="68" t="s">
         <v>159</v>
       </c>
@@ -4222,26 +4703,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="109" t="s">
+      <c r="A24" s="99"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="100" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="109"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="110"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="100"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="106" t="s">
+      <c r="A26" s="101" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="105" t="s">
+      <c r="B26" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4252,8 +4733,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="106"/>
-      <c r="B27" s="105"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="102"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -4280,28 +4761,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="107" t="s">
+      <c r="A30" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="105" t="s">
+      <c r="B30" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="99" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="107" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="107"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="109"/>
-      <c r="D31" s="98"/>
+      <c r="A31" s="103"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="107"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="107"/>
-      <c r="B32" s="105"/>
+      <c r="A32" s="103"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4310,8 +4791,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="107"/>
-      <c r="B33" s="105"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4320,8 +4801,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="107"/>
-      <c r="B34" s="105"/>
+      <c r="A34" s="103"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="69" t="s">
         <v>170</v>
       </c>
@@ -4330,8 +4811,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="107"/>
-      <c r="B35" s="105"/>
+      <c r="A35" s="103"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4340,8 +4821,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="107"/>
-      <c r="B36" s="105"/>
+      <c r="A36" s="103"/>
+      <c r="B36" s="102"/>
       <c r="C36" s="69" t="s">
         <v>159</v>
       </c>
@@ -4350,26 +4831,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="107"/>
-      <c r="B37" s="105"/>
-      <c r="C37" s="111" t="s">
+      <c r="A37" s="103"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="104" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="113" t="s">
+      <c r="D37" s="106" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="107"/>
-      <c r="B38" s="105"/>
-      <c r="C38" s="112"/>
-      <c r="D38" s="113"/>
+      <c r="A38" s="103"/>
+      <c r="B38" s="102"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="106"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="106" t="s">
+      <c r="A39" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4380,8 +4861,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="106"/>
-      <c r="B40" s="105"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="102"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -4408,10 +4889,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="107" t="s">
+      <c r="A43" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4420,8 +4901,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="107"/>
-      <c r="B44" s="105"/>
+      <c r="A44" s="103"/>
+      <c r="B44" s="102"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -4430,10 +4911,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="102" t="s">
+      <c r="A45" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="105" t="s">
+      <c r="B45" s="102" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -4442,8 +4923,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="103"/>
-      <c r="B46" s="105"/>
+      <c r="A46" s="109"/>
+      <c r="B46" s="102"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -4452,8 +4933,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="103"/>
-      <c r="B47" s="105"/>
+      <c r="A47" s="109"/>
+      <c r="B47" s="102"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -4462,8 +4943,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="104"/>
-      <c r="B48" s="105"/>
+      <c r="A48" s="110"/>
+      <c r="B48" s="102"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -4472,10 +4953,10 @@
       </c>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="100" t="s">
+      <c r="A49" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="100" t="s">
+      <c r="B49" s="111" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -8579,8 +9060,8 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="100"/>
-      <c r="B50" s="100"/>
+      <c r="A50" s="111"/>
+      <c r="B50" s="111"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -12684,8 +13165,8 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="100"/>
-      <c r="B51" s="100"/>
+      <c r="A51" s="111"/>
+      <c r="B51" s="111"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -16789,8 +17270,8 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="100"/>
-      <c r="B52" s="100"/>
+      <c r="A52" s="111"/>
+      <c r="B52" s="111"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -20894,12 +21375,12 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="100"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="97" t="s">
+      <c r="A53" s="111"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="98" t="s">
+      <c r="D53" s="107" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -24999,10 +25480,10 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="100"/>
-      <c r="B54" s="100"/>
-      <c r="C54" s="97"/>
-      <c r="D54" s="98"/>
+      <c r="A54" s="111"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="114"/>
+      <c r="D54" s="107"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29120,10 +29601,10 @@
       </c>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="99" t="s">
+      <c r="A57" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="100" t="s">
+      <c r="B57" s="111" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29134,8 +29615,8 @@
       </c>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="99"/>
-      <c r="B58" s="100"/>
+      <c r="A58" s="115"/>
+      <c r="B58" s="111"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29144,8 +29625,8 @@
       </c>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="100"/>
+      <c r="A59" s="115"/>
+      <c r="B59" s="111"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29154,8 +29635,8 @@
       </c>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="99"/>
-      <c r="B60" s="100"/>
+      <c r="A60" s="115"/>
+      <c r="B60" s="111"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29164,8 +29645,8 @@
       </c>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="99"/>
-      <c r="B61" s="100"/>
+      <c r="A61" s="115"/>
+      <c r="B61" s="111"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29174,8 +29655,8 @@
       </c>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="99"/>
-      <c r="B62" s="100"/>
+      <c r="A62" s="115"/>
+      <c r="B62" s="111"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29184,8 +29665,8 @@
       </c>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="99"/>
-      <c r="B63" s="100"/>
+      <c r="A63" s="115"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29194,16 +29675,16 @@
       </c>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="99"/>
-      <c r="B64" s="100"/>
+      <c r="A64" s="115"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="99"/>
-      <c r="B65" s="100"/>
+      <c r="A65" s="115"/>
+      <c r="B65" s="111"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29212,16 +29693,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="99"/>
-      <c r="B66" s="100"/>
+      <c r="A66" s="115"/>
+      <c r="B66" s="111"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="99"/>
-      <c r="B67" s="100"/>
+      <c r="A67" s="115"/>
+      <c r="B67" s="111"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29230,8 +29711,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="99"/>
-      <c r="B68" s="100"/>
+      <c r="A68" s="115"/>
+      <c r="B68" s="111"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29240,8 +29721,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="99"/>
-      <c r="B69" s="100"/>
+      <c r="A69" s="115"/>
+      <c r="B69" s="111"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29250,8 +29731,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
-      <c r="B70" s="100"/>
+      <c r="A70" s="115"/>
+      <c r="B70" s="111"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29260,8 +29741,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="99"/>
-      <c r="B71" s="100"/>
+      <c r="A71" s="115"/>
+      <c r="B71" s="111"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29270,8 +29751,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="99"/>
-      <c r="B72" s="100"/>
+      <c r="A72" s="115"/>
+      <c r="B72" s="111"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29280,16 +29761,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="99"/>
-      <c r="B73" s="100"/>
+      <c r="A73" s="115"/>
+      <c r="B73" s="111"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="99"/>
-      <c r="B74" s="100"/>
+      <c r="A74" s="115"/>
+      <c r="B74" s="111"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29298,18 +29779,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="99"/>
-      <c r="B75" s="100"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="101" t="s">
+      <c r="A75" s="115"/>
+      <c r="B75" s="111"/>
+      <c r="C75" s="113"/>
+      <c r="D75" s="116" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="99"/>
-      <c r="B76" s="100"/>
-      <c r="C76" s="96"/>
-      <c r="D76" s="101"/>
+      <c r="A76" s="115"/>
+      <c r="B76" s="111"/>
+      <c r="C76" s="113"/>
+      <c r="D76" s="116"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -29333,8 +29814,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -29343,13 +29824,31 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="B16:B25"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="A39:A40"/>
@@ -29362,24 +29861,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29391,7 +29872,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D14"/>
+      <selection activeCell="B38" sqref="B38:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29425,175 +29906,171 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="75" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="71" t="s">
-        <v>198</v>
+      <c r="C4" s="82" t="s">
+        <v>196</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="136"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="119" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="142" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="118" t="s">
-        <v>205</v>
+      <c r="D5" s="144" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="136"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="118"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="145"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="140"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="136"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="49"/>
+      <c r="A8" s="109"/>
+      <c r="B8" s="140"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="136"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="80"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="137" t="s">
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="146" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="118" t="s">
+      <c r="C10" s="126"/>
+      <c r="D10" s="144" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="137"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="118"/>
+      <c r="A11" s="147"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="149"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="137"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="129"/>
-      <c r="D12" s="118"/>
+      <c r="A12" s="148"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="145"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="122"/>
-      <c r="D13" s="118" t="s">
-        <v>206</v>
+      <c r="C13" s="133"/>
+      <c r="D13" s="130" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="139"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="118"/>
+      <c r="A14" s="118"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="130"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="139"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="123"/>
+      <c r="A15" s="118"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="134"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="139"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="123"/>
+      <c r="A16" s="118"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="139"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="123"/>
+      <c r="A17" s="118"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="134"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="139"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="123"/>
+      <c r="A18" s="118"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="139"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="123"/>
+      <c r="A19" s="118"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="139"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="123"/>
+      <c r="A20" s="118"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="139"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="123"/>
+      <c r="A21" s="118"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="139"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="123"/>
+      <c r="A22" s="118"/>
+      <c r="B22" s="111"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="140"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="124"/>
+      <c r="A23" s="119"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="135"/>
       <c r="D23" s="58" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="76" t="s">
         <v>187</v>
       </c>
       <c r="B24" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="71" t="s">
         <v>190</v>
       </c>
       <c r="D24" s="54" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="79" t="s">
+    <row r="25" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="77" t="s">
         <v>165</v>
       </c>
       <c r="B25" s="63" t="s">
@@ -29613,80 +30090,92 @@
       <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="133" t="s">
+      <c r="A27" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="105" t="s">
+      <c r="B27" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="83" t="s">
         <v>191</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="134"/>
-      <c r="B28" s="105"/>
-      <c r="C28" s="74" t="s">
+    <row r="28" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="121"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="72" t="s">
         <v>189</v>
       </c>
       <c r="D28" s="70" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="134"/>
-      <c r="B29" s="105"/>
-      <c r="C29" s="125" t="s">
+      <c r="A29" s="121"/>
+      <c r="B29" s="140"/>
+      <c r="C29" s="83" t="s">
         <v>190</v>
       </c>
-      <c r="D29" s="126" t="s">
-        <v>204</v>
+      <c r="D29" s="79" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="134"/>
-      <c r="B30" s="105"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="127"/>
+      <c r="A30" s="121"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="155" t="s">
+        <v>227</v>
+      </c>
+      <c r="D30" s="137" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="134"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="127"/>
+      <c r="A31" s="122"/>
+      <c r="B31" s="141"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="138"/>
     </row>
     <row r="32" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="134"/>
-      <c r="B32" s="105"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="127"/>
+      <c r="A32" s="81"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="79"/>
     </row>
     <row r="33" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="134"/>
-      <c r="B33" s="105"/>
-      <c r="C33" s="125"/>
-      <c r="D33" s="127"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="79"/>
     </row>
     <row r="34" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="134"/>
-      <c r="B34" s="105"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="127"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="79"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="135"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="128"/>
+    <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="81" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" s="79" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="80" t="s">
         <v>185</v>
       </c>
       <c r="C36" s="38"/>
@@ -29702,24 +30191,24 @@
       <c r="C37" s="39"/>
       <c r="D37" s="44"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="107" t="s">
+    <row r="38" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="105" t="s">
+      <c r="B38" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="D38" s="75" t="s">
-        <v>195</v>
+      <c r="C38" s="74" t="s">
+        <v>192</v>
+      </c>
+      <c r="D38" s="73" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="107"/>
-      <c r="B39" s="105"/>
-      <c r="C39" s="72" t="s">
+    <row r="39" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="103"/>
+      <c r="B39" s="102"/>
+      <c r="C39" s="71" t="s">
         <v>190</v>
       </c>
       <c r="D39" s="52" t="s">
@@ -29727,84 +30216,84 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="102" t="s">
+      <c r="A40" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="105" t="s">
+      <c r="B40" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="C40" s="114" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="116" t="s">
-        <v>196</v>
+      <c r="C40" s="126" t="s">
+        <v>195</v>
+      </c>
+      <c r="D40" s="128" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="103"/>
-      <c r="B41" s="105"/>
-      <c r="C41" s="115"/>
-      <c r="D41" s="117"/>
+      <c r="A41" s="109"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="127"/>
+      <c r="D41" s="129"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="103"/>
-      <c r="B42" s="105"/>
-      <c r="C42" s="114" t="s">
+      <c r="A42" s="109"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="126" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="120" t="s">
+      <c r="D42" s="131" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="104"/>
-      <c r="B43" s="105"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="121"/>
+      <c r="A43" s="110"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="132"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="130" t="s">
+      <c r="A44" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="100" t="s">
+      <c r="B44" s="111" t="s">
         <v>185</v>
       </c>
       <c r="C44" s="58"/>
       <c r="D44" s="47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="131"/>
-      <c r="B45" s="100"/>
+      <c r="A45" s="124"/>
+      <c r="B45" s="111"/>
       <c r="C45" s="59"/>
       <c r="D45" s="60" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="131"/>
-      <c r="B46" s="100"/>
+      <c r="A46" s="124"/>
+      <c r="B46" s="111"/>
       <c r="C46" s="38"/>
       <c r="D46" s="47"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="131"/>
-      <c r="B47" s="100"/>
+      <c r="A47" s="124"/>
+      <c r="B47" s="111"/>
       <c r="C47" s="58"/>
       <c r="D47" s="47"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="131"/>
-      <c r="B48" s="100"/>
-      <c r="C48" s="97"/>
-      <c r="D48" s="98"/>
+      <c r="A48" s="124"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="114"/>
+      <c r="D48" s="107"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="132"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="97"/>
-      <c r="D49" s="98"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="114"/>
+      <c r="D49" s="107"/>
     </row>
     <row r="50" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="39" t="s">
@@ -29827,165 +30316,169 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="115" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="100" t="s">
+      <c r="B52" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="58" t="s">
-        <v>200</v>
+      <c r="C52" s="83" t="s">
+        <v>198</v>
       </c>
       <c r="D52" s="47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="99"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="58" t="s">
+      <c r="A53" s="115"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="83" t="s">
         <v>190</v>
       </c>
       <c r="D53" s="47" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="99"/>
-      <c r="B54" s="100"/>
-      <c r="C54" s="58"/>
+    <row r="54" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="115"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="152" t="s">
+        <v>213</v>
+      </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="99"/>
-      <c r="B55" s="100"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="62"/>
+    <row r="55" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="115"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="136" t="s">
+        <v>209</v>
+      </c>
+      <c r="D55" s="151" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="99"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="47"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="136"/>
+      <c r="D56" s="47" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="99"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="47"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="83" t="s">
+        <v>210</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="99"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="47"/>
+      <c r="A58" s="115"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="D58" s="151" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="47"/>
+      <c r="A59" s="115"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="136" t="s">
+        <v>208</v>
+      </c>
+      <c r="D59" s="46" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="99"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="47"/>
+      <c r="A60" s="115"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="136"/>
+      <c r="D60" s="46" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="99"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="46"/>
+    <row r="61" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="115"/>
+      <c r="B61" s="111"/>
+      <c r="C61" s="136"/>
+      <c r="D61" s="151" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="99"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="62"/>
+    <row r="62" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="115"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="126" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" s="45" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="99"/>
-      <c r="B63" s="100"/>
-      <c r="C63" s="61"/>
-      <c r="D63" s="62"/>
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="115"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="150"/>
+      <c r="D63" s="131" t="s">
+        <v>221</v>
+      </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="99"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="61"/>
-      <c r="D64" s="47"/>
+    <row r="64" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="115"/>
+      <c r="B64" s="111"/>
+      <c r="C64" s="150"/>
+      <c r="D64" s="153"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="99"/>
-      <c r="B65" s="100"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="47"/>
+    <row r="65" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="115"/>
+      <c r="B65" s="111"/>
+      <c r="C65" s="150"/>
+      <c r="D65" s="153"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="99"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="47"/>
+    <row r="66" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="115"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="127"/>
+      <c r="D66" s="132"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="99"/>
-      <c r="B67" s="100"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="47"/>
+    <row r="67" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="115"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="44"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="99"/>
-      <c r="B68" s="100"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="49"/>
+      <c r="A68" s="115"/>
+      <c r="B68" s="111"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="99"/>
-      <c r="B69" s="100"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="47"/>
+      <c r="A69" s="115"/>
+      <c r="B69" s="111"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
-      <c r="B70" s="100"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="101"/>
+      <c r="A70" s="115"/>
+      <c r="B70" s="111"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="99"/>
-      <c r="B71" s="100"/>
-      <c r="D71" s="101"/>
+      <c r="A71" s="115"/>
+      <c r="B71" s="111"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A27:A35"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="A52:A71"/>
-    <mergeCell ref="B52:B71"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D70:D71"/>
+  <mergeCells count="34">
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D40:D41"/>
@@ -29993,11 +30486,33 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="D29:D35"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A52:A71"/>
+    <mergeCell ref="B52:B71"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"SOAP and REST Guide Updates"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="234">
   <si>
     <t>Document</t>
   </si>
@@ -2385,12 +2385,28 @@
       <t>’ as an optional request field of NewEmployeeDetails property</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Additional information added in relation to digest algorithms used for ‘Digest’ HTTP header.
+</t>
+  </si>
+  <si>
+    <t>Section 4.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOAP Web Service Integration Guide </t>
+  </si>
+  <si>
+    <t>4.2.2 Timestamp</t>
+  </si>
+  <si>
+    <t>Added "maximum time" line</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2485,6 +2501,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3D3C40"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2926,7 +2949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3118,9 +3141,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3140,6 +3160,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3241,25 +3291,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3274,11 +3330,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3647,12 +3712,12 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3677,12 +3742,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="87"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3725,10 +3790,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="100">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3743,8 +3808,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3757,8 +3822,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="92"/>
+      <c r="A9" s="98"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3771,8 +3836,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
-      <c r="B10" s="92"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3785,8 +3850,8 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
-      <c r="B11" s="92"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -3799,8 +3864,8 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="90"/>
-      <c r="B12" s="93"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -3813,10 +3878,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="91">
+      <c r="B13" s="100">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3831,8 +3896,8 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="97"/>
-      <c r="B14" s="93"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -3881,12 +3946,12 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="87"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3929,22 +3994,22 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
+      <c r="A20" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="87"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="96"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="98" t="s">
+      <c r="A21" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="95">
+      <c r="B21" s="104">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -3959,8 +4024,8 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
-      <c r="B22" s="93"/>
+      <c r="A22" s="108"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -3983,18 +4048,18 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="85" t="s">
+      <c r="A24" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="87"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="96"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="95">
+      <c r="B25" s="104">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4009,8 +4074,8 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="89"/>
-      <c r="B26" s="92"/>
+      <c r="A26" s="98"/>
+      <c r="B26" s="101"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4023,8 +4088,8 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="92"/>
+      <c r="A27" s="98"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4037,8 +4102,8 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="92"/>
+      <c r="A28" s="98"/>
+      <c r="B28" s="101"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4051,8 +4116,8 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="92"/>
+      <c r="A29" s="98"/>
+      <c r="B29" s="101"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4065,8 +4130,8 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="89"/>
-      <c r="B30" s="92"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4079,8 +4144,8 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="89"/>
-      <c r="B31" s="92"/>
+      <c r="A31" s="98"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4093,8 +4158,8 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="90"/>
-      <c r="B32" s="93"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4219,12 +4284,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="87"/>
+      <c r="B41" s="95"/>
+      <c r="C41" s="95"/>
+      <c r="D41" s="96"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4404,10 +4469,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4418,8 +4483,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="102"/>
-      <c r="B8" s="103"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4428,8 +4493,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="102"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4438,8 +4503,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="102"/>
-      <c r="B10" s="103"/>
+      <c r="A10" s="111"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4448,8 +4513,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
-      <c r="B11" s="103"/>
+      <c r="A11" s="111"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4458,8 +4523,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
-      <c r="B12" s="103"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4468,10 +4533,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4482,8 +4547,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113"/>
-      <c r="B14" s="103"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="112"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4492,8 +4557,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="113"/>
-      <c r="B15" s="103"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4502,10 +4567,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="112" t="s">
+      <c r="B16" s="121" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4516,8 +4581,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
-      <c r="B17" s="112"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4526,8 +4591,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
-      <c r="B18" s="112"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4536,8 +4601,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="112"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="121"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4546,8 +4611,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
-      <c r="B20" s="112"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4556,8 +4621,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="112"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4566,8 +4631,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="112"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4576,8 +4641,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="112"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="121"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -4586,26 +4651,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100"/>
-      <c r="B24" s="112"/>
-      <c r="C24" s="100" t="s">
+      <c r="A24" s="109"/>
+      <c r="B24" s="121"/>
+      <c r="C24" s="109" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="110" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="100"/>
-      <c r="B25" s="112"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="101"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="110"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="102" t="s">
+      <c r="A26" s="111" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4616,8 +4681,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="102"/>
-      <c r="B27" s="103"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -4644,28 +4709,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="103" t="s">
+      <c r="B30" s="112" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="108" t="s">
+      <c r="D30" s="117" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="104"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="108"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="117"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="104"/>
-      <c r="B32" s="103"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="112"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4674,8 +4739,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="104"/>
-      <c r="B33" s="103"/>
+      <c r="A33" s="113"/>
+      <c r="B33" s="112"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4684,8 +4749,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="104"/>
-      <c r="B34" s="103"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -4694,8 +4759,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="104"/>
-      <c r="B35" s="103"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4704,8 +4769,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="104"/>
-      <c r="B36" s="103"/>
+      <c r="A36" s="113"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -4714,26 +4779,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="104"/>
-      <c r="B37" s="103"/>
-      <c r="C37" s="105" t="s">
+      <c r="A37" s="113"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="114" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="116" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="104"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="107"/>
+      <c r="A38" s="113"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="116"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="102" t="s">
+      <c r="A39" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4744,8 +4809,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="102"/>
-      <c r="B40" s="103"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -4772,10 +4837,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="104" t="s">
+      <c r="A43" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="103" t="s">
+      <c r="B43" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4784,8 +4849,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="104"/>
-      <c r="B44" s="103"/>
+      <c r="A44" s="113"/>
+      <c r="B44" s="112"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -4794,10 +4859,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="109" t="s">
+      <c r="A45" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="103" t="s">
+      <c r="B45" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -4806,8 +4871,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="110"/>
-      <c r="B46" s="103"/>
+      <c r="A46" s="119"/>
+      <c r="B46" s="112"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -4816,8 +4881,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="110"/>
-      <c r="B47" s="103"/>
+      <c r="A47" s="119"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -4826,8 +4891,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="111"/>
-      <c r="B48" s="103"/>
+      <c r="A48" s="120"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -4836,10 +4901,10 @@
       </c>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="112" t="s">
+      <c r="A49" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="121" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -8943,8 +9008,8 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="112"/>
-      <c r="B50" s="112"/>
+      <c r="A50" s="121"/>
+      <c r="B50" s="121"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13048,8 +13113,8 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="112"/>
-      <c r="B51" s="112"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="121"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17153,8 +17218,8 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="112"/>
-      <c r="B52" s="112"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21258,12 +21323,12 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="112"/>
-      <c r="B53" s="112"/>
-      <c r="C53" s="115" t="s">
+      <c r="A53" s="121"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="124" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="108" t="s">
+      <c r="D53" s="117" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -25363,10 +25428,10 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="112"/>
-      <c r="B54" s="112"/>
-      <c r="C54" s="115"/>
-      <c r="D54" s="108"/>
+      <c r="A54" s="121"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="124"/>
+      <c r="D54" s="117"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29484,10 +29549,10 @@
       </c>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="116" t="s">
+      <c r="A57" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="112" t="s">
+      <c r="B57" s="121" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29498,8 +29563,8 @@
       </c>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="116"/>
-      <c r="B58" s="112"/>
+      <c r="A58" s="125"/>
+      <c r="B58" s="121"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29508,8 +29573,8 @@
       </c>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="116"/>
-      <c r="B59" s="112"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="121"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29518,8 +29583,8 @@
       </c>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="116"/>
-      <c r="B60" s="112"/>
+      <c r="A60" s="125"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29528,8 +29593,8 @@
       </c>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="116"/>
-      <c r="B61" s="112"/>
+      <c r="A61" s="125"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29538,8 +29603,8 @@
       </c>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="116"/>
-      <c r="B62" s="112"/>
+      <c r="A62" s="125"/>
+      <c r="B62" s="121"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29548,8 +29613,8 @@
       </c>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="116"/>
-      <c r="B63" s="112"/>
+      <c r="A63" s="125"/>
+      <c r="B63" s="121"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29558,16 +29623,16 @@
       </c>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="116"/>
-      <c r="B64" s="112"/>
+      <c r="A64" s="125"/>
+      <c r="B64" s="121"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="116"/>
-      <c r="B65" s="112"/>
+      <c r="A65" s="125"/>
+      <c r="B65" s="121"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29576,16 +29641,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="116"/>
-      <c r="B66" s="112"/>
+      <c r="A66" s="125"/>
+      <c r="B66" s="121"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="116"/>
-      <c r="B67" s="112"/>
+      <c r="A67" s="125"/>
+      <c r="B67" s="121"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29594,8 +29659,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="116"/>
-      <c r="B68" s="112"/>
+      <c r="A68" s="125"/>
+      <c r="B68" s="121"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29604,8 +29669,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="116"/>
-      <c r="B69" s="112"/>
+      <c r="A69" s="125"/>
+      <c r="B69" s="121"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29614,8 +29679,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="116"/>
-      <c r="B70" s="112"/>
+      <c r="A70" s="125"/>
+      <c r="B70" s="121"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29624,8 +29689,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="116"/>
-      <c r="B71" s="112"/>
+      <c r="A71" s="125"/>
+      <c r="B71" s="121"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29634,8 +29699,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="116"/>
-      <c r="B72" s="112"/>
+      <c r="A72" s="125"/>
+      <c r="B72" s="121"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29644,16 +29709,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="116"/>
-      <c r="B73" s="112"/>
+      <c r="A73" s="125"/>
+      <c r="B73" s="121"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="116"/>
-      <c r="B74" s="112"/>
+      <c r="A74" s="125"/>
+      <c r="B74" s="121"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29662,18 +29727,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="116"/>
-      <c r="B75" s="112"/>
-      <c r="C75" s="114"/>
-      <c r="D75" s="117" t="s">
+      <c r="A75" s="125"/>
+      <c r="B75" s="121"/>
+      <c r="C75" s="123"/>
+      <c r="D75" s="126" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="116"/>
-      <c r="B76" s="112"/>
-      <c r="C76" s="114"/>
-      <c r="D76" s="117"/>
+      <c r="A76" s="125"/>
+      <c r="B76" s="121"/>
+      <c r="C76" s="123"/>
+      <c r="D76" s="126"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -29752,10 +29817,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:D41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29797,10 +29862,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="112" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -29811,133 +29876,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="121" t="s">
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="142" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="141" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="120"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="141"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="102"/>
-      <c r="B8" s="103"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="102"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="119"/>
-      <c r="D10" s="120" t="s">
+      <c r="C10" s="133"/>
+      <c r="D10" s="141" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="113"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="120"/>
+      <c r="A11" s="122"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="141"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="120"/>
+      <c r="A12" s="122"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="141"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="122"/>
-      <c r="D13" s="120" t="s">
+      <c r="C13" s="143"/>
+      <c r="D13" s="141" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="122"/>
-      <c r="D14" s="120"/>
+      <c r="A14" s="109"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="143"/>
+      <c r="D14" s="141"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="122"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="143"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="122"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="143"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
-      <c r="B17" s="112"/>
-      <c r="C17" s="122"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="143"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="122"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="143"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="122"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="143"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
-      <c r="B20" s="112"/>
-      <c r="C20" s="122"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="121"/>
+      <c r="C20" s="143"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="112"/>
-      <c r="C21" s="122"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="121"/>
+      <c r="C21" s="143"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="112"/>
-      <c r="C22" s="122"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="143"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="112"/>
-      <c r="C23" s="122"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="143"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -29952,423 +30017,435 @@
       <c r="C24" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="D24" s="78" t="s">
+      <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="48" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="144" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B26" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="73" t="s">
+      <c r="C26" s="38"/>
+      <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="104" t="s">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="103" t="s">
+      <c r="B28" s="84" t="s">
         <v>185</v>
       </c>
-      <c r="C27" s="79" t="s">
+      <c r="C28" s="88" t="s">
         <v>191</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="104"/>
-      <c r="B28" s="103"/>
-      <c r="C28" s="70" t="s">
+    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="85"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D29" s="68" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="104"/>
-      <c r="B29" s="103"/>
-      <c r="C29" s="79" t="s">
-        <v>190</v>
-      </c>
-      <c r="D29" s="76" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="104"/>
-      <c r="B30" s="103"/>
-      <c r="C30" s="123" t="s">
+      <c r="A30" s="85"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="88" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="85"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="89" t="s">
         <v>226</v>
       </c>
-      <c r="D30" s="108" t="s">
+      <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="104"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="108"/>
+    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="127" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="130" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="32" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="76"/>
+    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="128"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="75"/>
     </row>
-    <row r="33" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="75"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="76"/>
+    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="128"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="75"/>
     </row>
-    <row r="34" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="75"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="76"/>
+    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="128"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="75" t="s">
-        <v>222</v>
-      </c>
-      <c r="B35" s="74" t="s">
+    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="129"/>
+      <c r="B36" s="132"/>
+      <c r="C36" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="75" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="79" t="s">
-        <v>223</v>
-      </c>
-      <c r="D35" s="76" t="s">
-        <v>224</v>
+      <c r="C37" s="38"/>
+      <c r="D37" s="50" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="74" t="s">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="44"/>
+    </row>
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="113" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="50" t="s">
-        <v>79</v>
+      <c r="C39" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="44"/>
-    </row>
-    <row r="38" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="104" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="C38" s="77" t="s">
-        <v>192</v>
-      </c>
-      <c r="D38" s="82" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="104"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="69" t="s">
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="113"/>
+      <c r="B40" s="112"/>
+      <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="D39" s="52" t="s">
+      <c r="D40" s="52" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="119" t="s">
-        <v>194</v>
-      </c>
-      <c r="D40" s="100" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="102"/>
-      <c r="B41" s="103"/>
-      <c r="C41" s="119"/>
-      <c r="D41" s="100"/>
+      <c r="A41" s="111" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="112" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="133" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="109" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="102"/>
-      <c r="B42" s="103"/>
-      <c r="C42" s="119" t="s">
-        <v>190</v>
-      </c>
-      <c r="D42" s="117" t="s">
-        <v>188</v>
-      </c>
+      <c r="A42" s="111"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="133"/>
+      <c r="D42" s="109"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="102"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="117"/>
+      <c r="A43" s="111"/>
+      <c r="B43" s="112"/>
+      <c r="C43" s="133" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="126" t="s">
+        <v>188</v>
+      </c>
     </row>
-    <row r="44" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="116" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="111"/>
+      <c r="B44" s="112"/>
+      <c r="C44" s="133"/>
+      <c r="D44" s="126"/>
+    </row>
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="112" t="s">
+      <c r="B45" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="126"/>
-      <c r="D44" s="130" t="s">
+      <c r="C45" s="137"/>
+      <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="116"/>
-      <c r="B45" s="112"/>
-      <c r="C45" s="127"/>
-      <c r="D45" s="124" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="125"/>
+      <c r="B46" s="121"/>
+      <c r="C46" s="138"/>
+      <c r="D46" s="134" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="116"/>
-      <c r="B46" s="112"/>
-      <c r="C46" s="127"/>
-      <c r="D46" s="129"/>
+    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="125"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="135"/>
     </row>
-    <row r="47" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="116"/>
-      <c r="B47" s="112"/>
-      <c r="C47" s="128"/>
-      <c r="D47" s="129"/>
-    </row>
-    <row r="48" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="116"/>
-      <c r="B48" s="112"/>
-      <c r="C48" s="115"/>
-      <c r="D48" s="129"/>
+    <row r="48" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="125"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="139"/>
+      <c r="D48" s="135"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="116"/>
-      <c r="B49" s="112"/>
-      <c r="C49" s="115"/>
-      <c r="D49" s="125"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="124"/>
+      <c r="D49" s="135"/>
     </row>
-    <row r="50" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39" t="s">
+    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="125"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="124"/>
+      <c r="D50" s="136"/>
+    </row>
+    <row r="51" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="44"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="44"/>
     </row>
-    <row r="51" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="48" t="s">
+    <row r="52" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B52" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="49" t="s">
+      <c r="C52" s="38"/>
+      <c r="D52" s="49" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="112" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="112" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="D52" s="47" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="112"/>
-      <c r="B53" s="112"/>
-      <c r="C53" s="79" t="s">
+      <c r="A53" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="121" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="78" t="s">
+        <v>197</v>
+      </c>
+      <c r="D53" s="47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="121"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="D53" s="47" t="s">
+      <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="112"/>
-      <c r="B54" s="112"/>
-      <c r="C54" s="79" t="s">
+    <row r="55" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="121"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
-      <c r="D54" s="81" t="s">
+      <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="112"/>
-      <c r="B55" s="112"/>
-      <c r="C55" s="118" t="s">
+    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="121"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="140" t="s">
         <v>208</v>
       </c>
-      <c r="D55" s="80" t="s">
+      <c r="D56" s="79" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="112"/>
-      <c r="B56" s="112"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="47" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="112"/>
-      <c r="B57" s="112"/>
-      <c r="C57" s="79" t="s">
-        <v>209</v>
-      </c>
-      <c r="D57" s="46" t="s">
-        <v>214</v>
+      <c r="A57" s="121"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="140"/>
+      <c r="D57" s="47" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="112"/>
-      <c r="B58" s="112"/>
-      <c r="C58" s="79" t="s">
-        <v>210</v>
-      </c>
-      <c r="D58" s="80" t="s">
-        <v>215</v>
+      <c r="A58" s="121"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="78" t="s">
+        <v>209</v>
+      </c>
+      <c r="D58" s="46" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="112"/>
-      <c r="B59" s="112"/>
-      <c r="C59" s="118" t="s">
-        <v>207</v>
-      </c>
-      <c r="D59" s="46" t="s">
-        <v>216</v>
+      <c r="A59" s="121"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="78" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" s="79" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="112"/>
-      <c r="B60" s="112"/>
-      <c r="C60" s="118"/>
+      <c r="A60" s="121"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="140" t="s">
+        <v>207</v>
+      </c>
       <c r="D60" s="46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="121"/>
+      <c r="B61" s="121"/>
+      <c r="C61" s="140"/>
+      <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="112"/>
-      <c r="B61" s="112"/>
-      <c r="C61" s="118"/>
-      <c r="D61" s="80" t="s">
+    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="121"/>
+      <c r="B62" s="121"/>
+      <c r="C62" s="140"/>
+      <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="112"/>
-      <c r="B62" s="112"/>
-      <c r="C62" s="119" t="s">
+    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="121"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="133" t="s">
         <v>206</v>
       </c>
-      <c r="D62" s="45" t="s">
+      <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="112"/>
-      <c r="B63" s="112"/>
-      <c r="C63" s="119"/>
-      <c r="D63" s="117" t="s">
+    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="121"/>
+      <c r="B64" s="121"/>
+      <c r="C64" s="133"/>
+      <c r="D64" s="126" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="112"/>
-      <c r="B64" s="112"/>
-      <c r="C64" s="119"/>
-      <c r="D64" s="117"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="121"/>
+      <c r="B65" s="121"/>
+      <c r="C65" s="133"/>
+      <c r="D65" s="126"/>
     </row>
-    <row r="65" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="112"/>
-      <c r="B65" s="112"/>
-      <c r="C65" s="119"/>
-      <c r="D65" s="117"/>
+    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="121"/>
+      <c r="B66" s="121"/>
+      <c r="C66" s="133"/>
+      <c r="D66" s="126"/>
     </row>
-    <row r="66" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="112"/>
-      <c r="B66" s="112"/>
-      <c r="C66" s="119"/>
-      <c r="D66" s="117"/>
+    <row r="67" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="121"/>
+      <c r="B67" s="121"/>
+      <c r="C67" s="133"/>
+      <c r="D67" s="126"/>
     </row>
-    <row r="67" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="39"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="44"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="83"/>
-      <c r="B68" s="84"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="39"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="44"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="83"/>
-      <c r="B69" s="84"/>
+      <c r="A69" s="82"/>
+      <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="83"/>
-      <c r="B70" s="84"/>
+      <c r="A70" s="82"/>
+      <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="83"/>
-      <c r="B71" s="84"/>
+      <c r="A71" s="82"/>
+      <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
+      <c r="A72" s="82"/>
+      <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
@@ -30382,43 +30459,47 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="33">
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D43:D44"/>
     <mergeCell ref="C13:C23"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A52:A66"/>
-    <mergeCell ref="B52:B66"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D45:D49"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="A10:A12"/>

</xml_diff>

<commit_message>
"Example fix and Doc updates"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -13,9 +13,9 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -3183,14 +3183,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3238,19 +3241,49 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3261,53 +3294,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3333,17 +3327,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3712,12 +3712,12 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3742,12 +3742,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="96"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3790,10 +3790,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="100">
+      <c r="B7" s="101">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3808,8 +3808,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="98"/>
-      <c r="B8" s="101"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3822,8 +3822,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="98"/>
-      <c r="B9" s="101"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3836,8 +3836,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="98"/>
-      <c r="B10" s="101"/>
+      <c r="A10" s="99"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3850,8 +3850,8 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="98"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -3864,8 +3864,8 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="99"/>
-      <c r="B12" s="102"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -3878,10 +3878,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="100">
+      <c r="B13" s="101">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3896,8 +3896,8 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="106"/>
-      <c r="B14" s="102"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -3946,12 +3946,12 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="95"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="96"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="97"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3994,22 +3994,22 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="95"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="96"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="97"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="107" t="s">
+      <c r="A21" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="104">
+      <c r="B21" s="105">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4024,8 +4024,8 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="108"/>
-      <c r="B22" s="102"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4048,18 +4048,18 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="96"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="97"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="104">
+      <c r="B25" s="105">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4074,8 +4074,8 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="98"/>
-      <c r="B26" s="101"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4088,8 +4088,8 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="98"/>
-      <c r="B27" s="101"/>
+      <c r="A27" s="99"/>
+      <c r="B27" s="102"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4102,8 +4102,8 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="98"/>
-      <c r="B28" s="101"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4116,8 +4116,8 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="98"/>
-      <c r="B29" s="101"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4130,8 +4130,8 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4144,8 +4144,8 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="98"/>
-      <c r="B31" s="101"/>
+      <c r="A31" s="99"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4158,8 +4158,8 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="99"/>
-      <c r="B32" s="102"/>
+      <c r="A32" s="100"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4284,12 +4284,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="94" t="s">
+      <c r="A41" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="95"/>
-      <c r="C41" s="95"/>
-      <c r="D41" s="96"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="97"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4349,7 +4349,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4359,7 +4359,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4469,10 +4469,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4483,8 +4483,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="111"/>
-      <c r="B8" s="112"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4493,8 +4493,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="111"/>
-      <c r="B9" s="112"/>
+      <c r="A9" s="120"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4503,8 +4503,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="111"/>
-      <c r="B10" s="112"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4513,8 +4513,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="111"/>
-      <c r="B11" s="112"/>
+      <c r="A11" s="120"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4523,8 +4523,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="111"/>
-      <c r="B12" s="112"/>
+      <c r="A12" s="120"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4536,7 +4536,7 @@
       <c r="A13" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4548,7 +4548,7 @@
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="122"/>
-      <c r="B14" s="112"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4558,7 +4558,7 @@
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="122"/>
-      <c r="B15" s="112"/>
+      <c r="B15" s="119"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4567,10 +4567,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="114" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4581,8 +4581,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109"/>
-      <c r="B17" s="121"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="114"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4591,8 +4591,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
-      <c r="B18" s="121"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4601,8 +4601,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
-      <c r="B19" s="121"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="114"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4611,8 +4611,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109"/>
-      <c r="B20" s="121"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="114"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4621,8 +4621,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
-      <c r="B21" s="121"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="114"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4631,8 +4631,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="109"/>
-      <c r="B22" s="121"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4641,8 +4641,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="109"/>
-      <c r="B23" s="121"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="114"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -4651,26 +4651,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109"/>
-      <c r="B24" s="121"/>
-      <c r="C24" s="109" t="s">
+      <c r="A24" s="123"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="123" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="124" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="109"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="110"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="124"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="120" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="112" t="s">
+      <c r="B26" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4681,8 +4681,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="111"/>
-      <c r="B27" s="112"/>
+      <c r="A27" s="120"/>
+      <c r="B27" s="119"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -4709,28 +4709,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="113" t="s">
+      <c r="A30" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="112" t="s">
+      <c r="B30" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="117" t="s">
+      <c r="D30" s="112" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="113"/>
-      <c r="B31" s="112"/>
-      <c r="C31" s="109"/>
-      <c r="D31" s="117"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="123"/>
+      <c r="D31" s="112"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="113"/>
-      <c r="B32" s="112"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4739,8 +4739,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="113"/>
-      <c r="B33" s="112"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="119"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4749,8 +4749,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="113"/>
-      <c r="B34" s="112"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -4759,8 +4759,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="113"/>
-      <c r="B35" s="112"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="119"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4769,8 +4769,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="113"/>
-      <c r="B36" s="112"/>
+      <c r="A36" s="121"/>
+      <c r="B36" s="119"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -4779,26 +4779,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="113"/>
-      <c r="B37" s="112"/>
-      <c r="C37" s="114" t="s">
+      <c r="A37" s="121"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="125" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="116" t="s">
+      <c r="D37" s="127" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="113"/>
-      <c r="B38" s="112"/>
-      <c r="C38" s="115"/>
-      <c r="D38" s="116"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="126"/>
+      <c r="D38" s="127"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="111" t="s">
+      <c r="A39" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="112" t="s">
+      <c r="B39" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4809,8 +4809,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="111"/>
-      <c r="B40" s="112"/>
+      <c r="A40" s="120"/>
+      <c r="B40" s="119"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -4837,10 +4837,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="113" t="s">
+      <c r="A43" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="112" t="s">
+      <c r="B43" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4849,8 +4849,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="113"/>
-      <c r="B44" s="112"/>
+      <c r="A44" s="121"/>
+      <c r="B44" s="119"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -4859,10 +4859,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="118" t="s">
+      <c r="A45" s="116" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="112" t="s">
+      <c r="B45" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -4871,8 +4871,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="119"/>
-      <c r="B46" s="112"/>
+      <c r="A46" s="117"/>
+      <c r="B46" s="119"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -4881,8 +4881,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="119"/>
-      <c r="B47" s="112"/>
+      <c r="A47" s="117"/>
+      <c r="B47" s="119"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -4891,8 +4891,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="120"/>
-      <c r="B48" s="112"/>
+      <c r="A48" s="118"/>
+      <c r="B48" s="119"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -4901,10 +4901,10 @@
       </c>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="121" t="s">
+      <c r="A49" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="121" t="s">
+      <c r="B49" s="114" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9008,8 +9008,8 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="121"/>
-      <c r="B50" s="121"/>
+      <c r="A50" s="114"/>
+      <c r="B50" s="114"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13113,8 +13113,8 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="121"/>
-      <c r="B51" s="121"/>
+      <c r="A51" s="114"/>
+      <c r="B51" s="114"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17218,8 +17218,8 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="121"/>
-      <c r="B52" s="121"/>
+      <c r="A52" s="114"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21323,12 +21323,12 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="121"/>
-      <c r="B53" s="121"/>
-      <c r="C53" s="124" t="s">
+      <c r="A53" s="114"/>
+      <c r="B53" s="114"/>
+      <c r="C53" s="111" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="117" t="s">
+      <c r="D53" s="112" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -25428,10 +25428,10 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="121"/>
-      <c r="B54" s="121"/>
-      <c r="C54" s="124"/>
-      <c r="D54" s="117"/>
+      <c r="A54" s="114"/>
+      <c r="B54" s="114"/>
+      <c r="C54" s="111"/>
+      <c r="D54" s="112"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29549,10 +29549,10 @@
       </c>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="125" t="s">
+      <c r="A57" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="121" t="s">
+      <c r="B57" s="114" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29563,8 +29563,8 @@
       </c>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="125"/>
-      <c r="B58" s="121"/>
+      <c r="A58" s="113"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29573,8 +29573,8 @@
       </c>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="125"/>
-      <c r="B59" s="121"/>
+      <c r="A59" s="113"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29583,8 +29583,8 @@
       </c>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="125"/>
-      <c r="B60" s="121"/>
+      <c r="A60" s="113"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29593,8 +29593,8 @@
       </c>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="125"/>
-      <c r="B61" s="121"/>
+      <c r="A61" s="113"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29603,8 +29603,8 @@
       </c>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="125"/>
-      <c r="B62" s="121"/>
+      <c r="A62" s="113"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29613,8 +29613,8 @@
       </c>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="125"/>
-      <c r="B63" s="121"/>
+      <c r="A63" s="113"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29623,16 +29623,16 @@
       </c>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="125"/>
-      <c r="B64" s="121"/>
+      <c r="A64" s="113"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="125"/>
-      <c r="B65" s="121"/>
+      <c r="A65" s="113"/>
+      <c r="B65" s="114"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29641,16 +29641,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="125"/>
-      <c r="B66" s="121"/>
+      <c r="A66" s="113"/>
+      <c r="B66" s="114"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="125"/>
-      <c r="B67" s="121"/>
+      <c r="A67" s="113"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29659,8 +29659,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="125"/>
-      <c r="B68" s="121"/>
+      <c r="A68" s="113"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29669,8 +29669,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="125"/>
-      <c r="B69" s="121"/>
+      <c r="A69" s="113"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29679,8 +29679,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="125"/>
-      <c r="B70" s="121"/>
+      <c r="A70" s="113"/>
+      <c r="B70" s="114"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29689,8 +29689,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="125"/>
-      <c r="B71" s="121"/>
+      <c r="A71" s="113"/>
+      <c r="B71" s="114"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29699,8 +29699,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="125"/>
-      <c r="B72" s="121"/>
+      <c r="A72" s="113"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29709,16 +29709,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="125"/>
-      <c r="B73" s="121"/>
+      <c r="A73" s="113"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="125"/>
-      <c r="B74" s="121"/>
+      <c r="A74" s="113"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29727,18 +29727,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="125"/>
-      <c r="B75" s="121"/>
-      <c r="C75" s="123"/>
-      <c r="D75" s="126" t="s">
+      <c r="A75" s="113"/>
+      <c r="B75" s="114"/>
+      <c r="C75" s="110"/>
+      <c r="D75" s="115" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="125"/>
-      <c r="B76" s="121"/>
-      <c r="C76" s="123"/>
-      <c r="D76" s="126"/>
+      <c r="A76" s="113"/>
+      <c r="B76" s="114"/>
+      <c r="C76" s="110"/>
+      <c r="D76" s="115"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -29762,8 +29762,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -29772,19 +29772,25 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="A49:A54"/>
@@ -29797,18 +29803,12 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A25"/>
     <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29820,7 +29820,7 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29862,10 +29862,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="119" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -29876,36 +29876,36 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="142" t="s">
+      <c r="A5" s="120"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="129" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="141" t="s">
+      <c r="D5" s="128" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="111"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="141"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="128"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="111"/>
-      <c r="B7" s="112"/>
+      <c r="A7" s="120"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="111"/>
-      <c r="B8" s="112"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111"/>
-      <c r="B9" s="112"/>
+      <c r="A9" s="120"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
@@ -29913,96 +29913,96 @@
       <c r="A10" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="119" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="133"/>
-      <c r="D10" s="141" t="s">
+      <c r="C10" s="131"/>
+      <c r="D10" s="128" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="122"/>
-      <c r="B11" s="112"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="141"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="128"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="122"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="141"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="128"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="141" t="s">
+      <c r="C13" s="130"/>
+      <c r="D13" s="128" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="109"/>
-      <c r="B14" s="121"/>
-      <c r="C14" s="143"/>
-      <c r="D14" s="141"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="128"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="109"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="143"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="109"/>
-      <c r="B16" s="121"/>
-      <c r="C16" s="143"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109"/>
-      <c r="B17" s="121"/>
-      <c r="C17" s="143"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
-      <c r="B18" s="121"/>
-      <c r="C18" s="143"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="143"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109"/>
-      <c r="B20" s="121"/>
-      <c r="C20" s="143"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
-      <c r="B21" s="121"/>
-      <c r="C21" s="143"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="109"/>
-      <c r="B22" s="121"/>
-      <c r="C22" s="143"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="109"/>
-      <c r="B23" s="121"/>
-      <c r="C23" s="143"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30021,17 +30021,17 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="93" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="94" t="s">
         <v>232</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
     </row>
@@ -30100,13 +30100,13 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="127" t="s">
+      <c r="A32" s="139" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="130" t="s">
+      <c r="B32" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="C32" s="93" t="s">
+      <c r="C32" s="91" t="s">
         <v>230</v>
       </c>
       <c r="D32" s="87" t="s">
@@ -30114,26 +30114,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="128"/>
-      <c r="B33" s="131"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="143"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="128"/>
-      <c r="B34" s="131"/>
+      <c r="A34" s="140"/>
+      <c r="B34" s="143"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="128"/>
-      <c r="B35" s="131"/>
+      <c r="A35" s="140"/>
+      <c r="B35" s="143"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="129"/>
-      <c r="B36" s="132"/>
+      <c r="A36" s="141"/>
+      <c r="B36" s="144"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30162,10 +30162,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="113" t="s">
+      <c r="A39" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="112" t="s">
+      <c r="B39" s="119" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30176,8 +30176,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="113"/>
-      <c r="B40" s="112"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="119"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30186,84 +30186,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="111" t="s">
+      <c r="A41" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="112" t="s">
+      <c r="B41" s="119" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="133" t="s">
+      <c r="C41" s="131" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="109" t="s">
+      <c r="D41" s="123" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="111"/>
-      <c r="B42" s="112"/>
-      <c r="C42" s="133"/>
-      <c r="D42" s="109"/>
+      <c r="A42" s="120"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="123"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="111"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="133" t="s">
+      <c r="A43" s="120"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="131" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="126" t="s">
+      <c r="D43" s="115" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="111"/>
-      <c r="B44" s="112"/>
-      <c r="C44" s="133"/>
-      <c r="D44" s="126"/>
+      <c r="A44" s="120"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="115"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="125" t="s">
+      <c r="A45" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="121" t="s">
+      <c r="B45" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="137"/>
+      <c r="C45" s="135"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="125"/>
-      <c r="B46" s="121"/>
-      <c r="C46" s="138"/>
-      <c r="D46" s="134" t="s">
+      <c r="A46" s="113"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="136"/>
+      <c r="D46" s="132" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="125"/>
-      <c r="B47" s="121"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="135"/>
+      <c r="A47" s="113"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="136"/>
+      <c r="D47" s="133"/>
     </row>
     <row r="48" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="125"/>
-      <c r="B48" s="121"/>
-      <c r="C48" s="139"/>
-      <c r="D48" s="135"/>
+      <c r="A48" s="113"/>
+      <c r="B48" s="114"/>
+      <c r="C48" s="137"/>
+      <c r="D48" s="133"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="125"/>
-      <c r="B49" s="121"/>
-      <c r="C49" s="124"/>
-      <c r="D49" s="135"/>
+      <c r="A49" s="113"/>
+      <c r="B49" s="114"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="133"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="125"/>
-      <c r="B50" s="121"/>
-      <c r="C50" s="124"/>
-      <c r="D50" s="136"/>
+      <c r="A50" s="113"/>
+      <c r="B50" s="114"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="134"/>
     </row>
     <row r="51" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30286,10 +30286,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="121" t="s">
+      <c r="A53" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="121" t="s">
+      <c r="B53" s="114" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30300,8 +30300,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="121"/>
-      <c r="B54" s="121"/>
+      <c r="A54" s="114"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30310,8 +30310,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="121"/>
-      <c r="B55" s="121"/>
+      <c r="A55" s="114"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30320,9 +30320,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="121"/>
-      <c r="B56" s="121"/>
-      <c r="C56" s="140" t="s">
+      <c r="A56" s="114"/>
+      <c r="B56" s="114"/>
+      <c r="C56" s="138" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30330,16 +30330,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="121"/>
-      <c r="B57" s="121"/>
-      <c r="C57" s="140"/>
+      <c r="A57" s="114"/>
+      <c r="B57" s="114"/>
+      <c r="C57" s="138"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="121"/>
-      <c r="B58" s="121"/>
+      <c r="A58" s="114"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30348,8 +30348,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="121"/>
-      <c r="B59" s="121"/>
+      <c r="A59" s="114"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30358,9 +30358,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="121"/>
-      <c r="B60" s="121"/>
-      <c r="C60" s="140" t="s">
+      <c r="A60" s="114"/>
+      <c r="B60" s="114"/>
+      <c r="C60" s="138" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30368,25 +30368,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="121"/>
-      <c r="B61" s="121"/>
-      <c r="C61" s="140"/>
+      <c r="A61" s="114"/>
+      <c r="B61" s="114"/>
+      <c r="C61" s="138"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="121"/>
-      <c r="B62" s="121"/>
-      <c r="C62" s="140"/>
+      <c r="A62" s="114"/>
+      <c r="B62" s="114"/>
+      <c r="C62" s="138"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="121"/>
-      <c r="B63" s="121"/>
-      <c r="C63" s="133" t="s">
+      <c r="A63" s="114"/>
+      <c r="B63" s="114"/>
+      <c r="C63" s="131" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30394,30 +30394,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="121"/>
-      <c r="B64" s="121"/>
-      <c r="C64" s="133"/>
-      <c r="D64" s="126" t="s">
+      <c r="A64" s="114"/>
+      <c r="B64" s="114"/>
+      <c r="C64" s="131"/>
+      <c r="D64" s="115" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="121"/>
-      <c r="B65" s="121"/>
-      <c r="C65" s="133"/>
-      <c r="D65" s="126"/>
+      <c r="A65" s="114"/>
+      <c r="B65" s="114"/>
+      <c r="C65" s="131"/>
+      <c r="D65" s="115"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="121"/>
-      <c r="B66" s="121"/>
-      <c r="C66" s="133"/>
-      <c r="D66" s="126"/>
+      <c r="A66" s="114"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="131"/>
+      <c r="D66" s="115"/>
     </row>
     <row r="67" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="121"/>
-      <c r="B67" s="121"/>
-      <c r="C67" s="133"/>
-      <c r="D67" s="126"/>
+      <c r="A67" s="114"/>
+      <c r="B67" s="114"/>
+      <c r="C67" s="131"/>
+      <c r="D67" s="115"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -30473,13 +30473,19 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C63:C67"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B53:B67"/>
@@ -30493,19 +30499,13 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C63:C67"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Updated release date to 24/5/2018, corrected references in changelog"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15384" windowHeight="10008" activeTab="3"/>
+    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2412,16 +2412,7 @@
     <t>All Enums capitalised to match REST API</t>
   </si>
   <si>
-    <t>Returns Schema</t>
-  </si>
-  <si>
-    <t>Reflect addition of returns to schema</t>
-  </si>
-  <si>
     <t>REST API</t>
-  </si>
-  <si>
-    <t>Updated with Return and Reconciliation</t>
   </si>
   <si>
     <t>Reflects changes to the REST API</t>
@@ -2449,9 +2440,6 @@
   </si>
   <si>
     <t>Section 10 added</t>
-  </si>
-  <si>
-    <t>New section addded for Returns and Reconciliation examples</t>
   </si>
   <si>
     <t xml:space="preserve">PAYE Web Service Examples </t>
@@ -2495,6 +2483,18 @@
       </rPr>
       <t>to be a date and not a datetime</t>
     </r>
+  </si>
+  <si>
+    <t>New section addded for Returns Reconciliation examples</t>
+  </si>
+  <si>
+    <t>Reflect addition of Returns Reconciliation to schema</t>
+  </si>
+  <si>
+    <t>Updated with Returns Reconciliation</t>
+  </si>
+  <si>
+    <t>Returns Reconciliation Schema</t>
   </si>
 </sst>
 </file>
@@ -3312,6 +3312,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3358,19 +3370,49 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3381,53 +3423,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3453,14 +3456,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3471,18 +3483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3829,15 +3829,15 @@
       <selection activeCell="A25" sqref="A25:A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3855,13 +3855,13 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="102"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3885,19 +3885,19 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="108"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -3915,7 +3915,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -3933,11 +3933,11 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="103" t="s">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="106">
+      <c r="B7" s="112">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3951,9 +3951,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="104"/>
-      <c r="B8" s="107"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="110"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3965,9 +3965,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
-      <c r="B9" s="107"/>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="110"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3979,9 +3979,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="104"/>
-      <c r="B10" s="107"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="110"/>
+      <c r="B10" s="113"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3993,9 +3993,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="104"/>
-      <c r="B11" s="107"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="110"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4007,9 +4007,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="105"/>
-      <c r="B12" s="108"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="111"/>
+      <c r="B12" s="114"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4021,11 +4021,11 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="111" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="106">
+      <c r="B13" s="112">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4039,9 +4039,9 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="112"/>
-      <c r="B14" s="108"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="118"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4053,7 +4053,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4071,7 +4071,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4089,19 +4089,19 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="100" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="102"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="108"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4119,7 +4119,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4137,23 +4137,23 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="100" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="101"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="108"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="113" t="s">
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="110">
+      <c r="B21" s="116">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4167,9 +4167,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="114"/>
-      <c r="B22" s="108"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="120"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4191,19 +4191,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="100" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="102"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="108"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="109" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="110">
+      <c r="B25" s="116">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4217,9 +4217,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="104"/>
-      <c r="B26" s="107"/>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="110"/>
+      <c r="B26" s="113"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4231,9 +4231,9 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="104"/>
-      <c r="B27" s="107"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="110"/>
+      <c r="B27" s="113"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4245,9 +4245,9 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="104"/>
-      <c r="B28" s="107"/>
+    <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="110"/>
+      <c r="B28" s="113"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4259,9 +4259,9 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="104"/>
-      <c r="B29" s="107"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="110"/>
+      <c r="B29" s="113"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4273,9 +4273,9 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="104"/>
-      <c r="B30" s="107"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="110"/>
+      <c r="B30" s="113"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4287,9 +4287,9 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="104"/>
-      <c r="B31" s="107"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="110"/>
+      <c r="B31" s="113"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4301,9 +4301,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="105"/>
-      <c r="B32" s="108"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="111"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4315,7 +4315,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4427,15 +4427,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="100" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="102"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="107"/>
+      <c r="D41" s="108"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4493,7 +4493,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4503,7 +4503,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4538,15 +4538,15 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -4568,7 +4568,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -4612,11 +4612,11 @@
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="117" t="s">
+    <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4626,9 +4626,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="117"/>
-      <c r="B8" s="118"/>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="131"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4636,9 +4636,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="117"/>
-      <c r="B9" s="118"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="131"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4646,9 +4646,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="117"/>
-      <c r="B10" s="118"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="131"/>
+      <c r="B10" s="130"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4656,9 +4656,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="117"/>
-      <c r="B11" s="118"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="131"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4666,9 +4666,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="117"/>
-      <c r="B12" s="118"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="131"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4676,11 +4676,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="128" t="s">
+    <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="133" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4690,9 +4690,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="118"/>
+    <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="133"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4700,9 +4700,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="128"/>
-      <c r="B15" s="118"/>
+    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="133"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4710,11 +4710,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="115" t="s">
+    <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="127" t="s">
+      <c r="B16" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4724,9 +4724,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="115"/>
-      <c r="B17" s="127"/>
+    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="134"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4734,9 +4734,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="115"/>
-      <c r="B18" s="127"/>
+    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="134"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4744,9 +4744,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="115"/>
-      <c r="B19" s="127"/>
+    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4754,9 +4754,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="115"/>
-      <c r="B20" s="127"/>
+    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="134"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4764,9 +4764,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="115"/>
-      <c r="B21" s="127"/>
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="134"/>
+      <c r="B21" s="125"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4774,9 +4774,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="115"/>
-      <c r="B22" s="127"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="134"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4784,9 +4784,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="115"/>
-      <c r="B23" s="127"/>
+    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="134"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -4794,27 +4794,27 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="115"/>
-      <c r="B24" s="127"/>
-      <c r="C24" s="115" t="s">
+    <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="134"/>
+      <c r="B24" s="125"/>
+      <c r="C24" s="134" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="116" t="s">
+      <c r="D24" s="135" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="115"/>
-      <c r="B25" s="127"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="116"/>
+    <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="134"/>
+      <c r="B25" s="125"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="135"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="117" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="131" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="118" t="s">
+      <c r="B26" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4824,15 +4824,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="117"/>
-      <c r="B27" s="118"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="131"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -4852,29 +4852,29 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="119" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="118" t="s">
+      <c r="B30" s="130" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="115" t="s">
+      <c r="C30" s="134" t="s">
         <v>169</v>
       </c>
       <c r="D30" s="123" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="119"/>
-      <c r="B31" s="118"/>
-      <c r="C31" s="115"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="132"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="134"/>
       <c r="D31" s="123"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="119"/>
-      <c r="B32" s="118"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="132"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4882,9 +4882,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="119"/>
-      <c r="B33" s="118"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="132"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4892,9 +4892,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="119"/>
-      <c r="B34" s="118"/>
+    <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="132"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -4902,9 +4902,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="119"/>
-      <c r="B35" s="118"/>
+    <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="132"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4912,9 +4912,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="119"/>
-      <c r="B36" s="118"/>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="132"/>
+      <c r="B36" s="130"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -4922,27 +4922,27 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="119"/>
-      <c r="B37" s="118"/>
-      <c r="C37" s="120" t="s">
+    <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="132"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="136" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="122" t="s">
+      <c r="D37" s="138" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="119"/>
-      <c r="B38" s="118"/>
-      <c r="C38" s="121"/>
-      <c r="D38" s="122"/>
+    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="132"/>
+      <c r="B38" s="130"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="138"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="117" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="131" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4952,15 +4952,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="117"/>
-      <c r="B40" s="118"/>
+    <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="131"/>
+      <c r="B40" s="130"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
@@ -4980,11 +4980,11 @@
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="119" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="118" t="s">
+      <c r="B43" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4992,9 +4992,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="119"/>
-      <c r="B44" s="118"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="132"/>
+      <c r="B44" s="130"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5002,11 +5002,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="124" t="s">
+    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="118" t="s">
+      <c r="B45" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5014,9 +5014,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="125"/>
-      <c r="B46" s="118"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="128"/>
+      <c r="B46" s="130"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5024,9 +5024,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="125"/>
-      <c r="B47" s="118"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="128"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5034,9 +5034,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="126"/>
-      <c r="B48" s="118"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="129"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5044,11 +5044,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="127" t="s">
+    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A49" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="127" t="s">
+      <c r="B49" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9151,9 +9151,9 @@
       <c r="XEZ49" s="42"/>
       <c r="XFD49" s="42"/>
     </row>
-    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="127"/>
-      <c r="B50" s="127"/>
+    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="125"/>
+      <c r="B50" s="125"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13256,9 +13256,9 @@
       <c r="XEZ50" s="42"/>
       <c r="XFD50" s="42"/>
     </row>
-    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="127"/>
-      <c r="B51" s="127"/>
+    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A51" s="125"/>
+      <c r="B51" s="125"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17361,9 +17361,9 @@
       <c r="XEZ51" s="42"/>
       <c r="XFD51" s="42"/>
     </row>
-    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="127"/>
-      <c r="B52" s="127"/>
+    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A52" s="125"/>
+      <c r="B52" s="125"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21466,10 +21466,10 @@
       <c r="XEZ52" s="42"/>
       <c r="XFD52" s="42"/>
     </row>
-    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="127"/>
-      <c r="B53" s="127"/>
-      <c r="C53" s="130" t="s">
+    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A53" s="125"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="122" t="s">
         <v>109</v>
       </c>
       <c r="D53" s="123" t="s">
@@ -25571,10 +25571,10 @@
       <c r="XEZ53" s="42"/>
       <c r="XFD53" s="42"/>
     </row>
-    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="127"/>
-      <c r="B54" s="127"/>
-      <c r="C54" s="130"/>
+    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="125"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="122"/>
       <c r="D54" s="123"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
@@ -29672,7 +29672,7 @@
       <c r="XEZ54" s="42"/>
       <c r="XFD54" s="42"/>
     </row>
-    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
@@ -29680,7 +29680,7 @@
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
     </row>
-    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -29692,11 +29692,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="131" t="s">
+    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A57" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="127" t="s">
+      <c r="B57" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29706,9 +29706,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="131"/>
-      <c r="B58" s="127"/>
+    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="124"/>
+      <c r="B58" s="125"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29716,9 +29716,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="131"/>
-      <c r="B59" s="127"/>
+    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A59" s="124"/>
+      <c r="B59" s="125"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29726,9 +29726,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="131"/>
-      <c r="B60" s="127"/>
+    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="124"/>
+      <c r="B60" s="125"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29736,9 +29736,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="131"/>
-      <c r="B61" s="127"/>
+    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A61" s="124"/>
+      <c r="B61" s="125"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29746,9 +29746,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="131"/>
-      <c r="B62" s="127"/>
+    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A62" s="124"/>
+      <c r="B62" s="125"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29756,9 +29756,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="131"/>
-      <c r="B63" s="127"/>
+    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A63" s="124"/>
+      <c r="B63" s="125"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29766,17 +29766,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="131"/>
-      <c r="B64" s="127"/>
+    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A64" s="124"/>
+      <c r="B64" s="125"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="131"/>
-      <c r="B65" s="127"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="124"/>
+      <c r="B65" s="125"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29784,17 +29784,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="131"/>
-      <c r="B66" s="127"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="124"/>
+      <c r="B66" s="125"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="131"/>
-      <c r="B67" s="127"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="124"/>
+      <c r="B67" s="125"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29802,9 +29802,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="131"/>
-      <c r="B68" s="127"/>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="124"/>
+      <c r="B68" s="125"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29812,9 +29812,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="131"/>
-      <c r="B69" s="127"/>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="124"/>
+      <c r="B69" s="125"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29822,9 +29822,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="131"/>
-      <c r="B70" s="127"/>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="124"/>
+      <c r="B70" s="125"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29832,9 +29832,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="131"/>
-      <c r="B71" s="127"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="124"/>
+      <c r="B71" s="125"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29842,9 +29842,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="131"/>
-      <c r="B72" s="127"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="124"/>
+      <c r="B72" s="125"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29852,17 +29852,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="131"/>
-      <c r="B73" s="127"/>
+    <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="124"/>
+      <c r="B73" s="125"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="131"/>
-      <c r="B74" s="127"/>
+    <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="124"/>
+      <c r="B74" s="125"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29870,21 +29870,21 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="131"/>
-      <c r="B75" s="127"/>
-      <c r="C75" s="129"/>
-      <c r="D75" s="132" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="124"/>
+      <c r="B75" s="125"/>
+      <c r="C75" s="121"/>
+      <c r="D75" s="126" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="131"/>
-      <c r="B76" s="127"/>
-      <c r="C76" s="129"/>
-      <c r="D76" s="132"/>
+    <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="124"/>
+      <c r="B76" s="125"/>
+      <c r="C76" s="121"/>
+      <c r="D76" s="126"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
@@ -29892,13 +29892,13 @@
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -29906,8 +29906,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -29916,19 +29916,25 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="A49:A54"/>
@@ -29941,18 +29947,12 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A25"/>
     <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29967,15 +29967,15 @@
       <selection activeCell="A53" sqref="A53:A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.21875" customWidth="1"/>
-    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -29989,7 +29989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -30005,11 +30005,11 @@
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="130" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30019,134 +30019,134 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="117"/>
-      <c r="B5" s="118"/>
-      <c r="C5" s="148" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="131"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="147" t="s">
+      <c r="D5" s="139" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="117"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="147"/>
+    <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="131"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="139"/>
     </row>
-    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="117"/>
-      <c r="B7" s="118"/>
+    <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="131"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="117"/>
-      <c r="B8" s="118"/>
+    <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="131"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="117"/>
-      <c r="B9" s="118"/>
+    <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="131"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="128" t="s">
+    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="118" t="s">
+      <c r="B10" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="139"/>
-      <c r="D10" s="147" t="s">
+      <c r="C10" s="142"/>
+      <c r="D10" s="139" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="128"/>
-      <c r="B11" s="118"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="147"/>
+    <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="139"/>
     </row>
-    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="128"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="147"/>
+    <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="133"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="139"/>
     </row>
-    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="115" t="s">
+    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="125" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="149"/>
-      <c r="D13" s="147" t="s">
+      <c r="C13" s="141"/>
+      <c r="D13" s="139" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="115"/>
-      <c r="B14" s="127"/>
-      <c r="C14" s="149"/>
-      <c r="D14" s="147"/>
+    <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="134"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="139"/>
     </row>
-    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="115"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="149"/>
+    <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="134"/>
+      <c r="B15" s="125"/>
+      <c r="C15" s="141"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="115"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="149"/>
+      <c r="A16" s="134"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="115"/>
-      <c r="B17" s="127"/>
-      <c r="C17" s="149"/>
+    <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="134"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="49"/>
     </row>
-    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="115"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="149"/>
+    <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="134"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="141"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="115"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="149"/>
+    <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="134"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="141"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="115"/>
-      <c r="B20" s="127"/>
-      <c r="C20" s="149"/>
+    <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="134"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="141"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="115"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="149"/>
+    <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="134"/>
+      <c r="B21" s="125"/>
+      <c r="C21" s="141"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="115"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="149"/>
+    <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="134"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="141"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="115"/>
-      <c r="B23" s="127"/>
-      <c r="C23" s="149"/>
+    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="134"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30165,7 +30165,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30179,7 +30179,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30199,7 +30199,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30223,7 +30223,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30233,7 +30233,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30243,11 +30243,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="133" t="s">
+    <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="150" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="136" t="s">
+      <c r="B32" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30257,27 +30257,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="134"/>
-      <c r="B33" s="137"/>
+    <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="151"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="134"/>
-      <c r="B34" s="137"/>
+      <c r="A34" s="151"/>
+      <c r="B34" s="154"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="134"/>
-      <c r="B35" s="137"/>
+    <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="151"/>
+      <c r="B35" s="154"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
-    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="135"/>
-      <c r="B36" s="138"/>
+    <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="152"/>
+      <c r="B36" s="155"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30305,11 +30305,11 @@
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="119" t="s">
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="130" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30319,9 +30319,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="119"/>
-      <c r="B40" s="118"/>
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="132"/>
+      <c r="B40" s="130"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30329,87 +30329,87 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="117" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="118" t="s">
+      <c r="B41" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="139" t="s">
+      <c r="C41" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="115" t="s">
+      <c r="D41" s="134" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="117"/>
-      <c r="B42" s="118"/>
-      <c r="C42" s="139"/>
-      <c r="D42" s="115"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="131"/>
+      <c r="B42" s="130"/>
+      <c r="C42" s="142"/>
+      <c r="D42" s="134"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="117"/>
-      <c r="B43" s="118"/>
-      <c r="C43" s="139" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="131"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="142" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="132" t="s">
+      <c r="D43" s="126" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="117"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="139"/>
-      <c r="D44" s="132"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="131"/>
+      <c r="B44" s="130"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="126"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="131" t="s">
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="127" t="s">
+      <c r="B45" s="125" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="143"/>
+      <c r="C45" s="146"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="131"/>
-      <c r="B46" s="127"/>
-      <c r="C46" s="144"/>
-      <c r="D46" s="140" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="124"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="147"/>
+      <c r="D46" s="143" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="131"/>
-      <c r="B47" s="127"/>
-      <c r="C47" s="144"/>
-      <c r="D47" s="141"/>
+    <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="124"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="147"/>
+      <c r="D47" s="144"/>
     </row>
-    <row r="48" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="131"/>
-      <c r="B48" s="127"/>
-      <c r="C48" s="145"/>
-      <c r="D48" s="141"/>
+    <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="124"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="148"/>
+      <c r="D48" s="144"/>
     </row>
-    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="131"/>
-      <c r="B49" s="127"/>
-      <c r="C49" s="130"/>
-      <c r="D49" s="141"/>
+    <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="124"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="144"/>
     </row>
-    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="131"/>
-      <c r="B50" s="127"/>
-      <c r="C50" s="130"/>
-      <c r="D50" s="142"/>
+    <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="124"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="145"/>
     </row>
-    <row r="51" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
@@ -30429,11 +30429,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="127" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="127" t="s">
+      <c r="B53" s="125" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30443,9 +30443,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="127"/>
-      <c r="B54" s="127"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="125"/>
+      <c r="B54" s="125"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30453,9 +30453,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="127"/>
-      <c r="B55" s="127"/>
+    <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="125"/>
+      <c r="B55" s="125"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30463,27 +30463,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="127"/>
-      <c r="B56" s="127"/>
-      <c r="C56" s="146" t="s">
+    <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="125"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="149" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="127"/>
-      <c r="B57" s="127"/>
-      <c r="C57" s="146"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="125"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="149"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="127"/>
-      <c r="B58" s="127"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="125"/>
+      <c r="B58" s="125"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30491,9 +30491,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="127"/>
-      <c r="B59" s="127"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="125"/>
+      <c r="B59" s="125"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30501,129 +30501,135 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="127"/>
-      <c r="B60" s="127"/>
-      <c r="C60" s="146" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="125"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="149" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="127"/>
-      <c r="B61" s="127"/>
-      <c r="C61" s="146"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="125"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="149"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="127"/>
-      <c r="B62" s="127"/>
-      <c r="C62" s="146"/>
+    <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="125"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="149"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="127"/>
-      <c r="B63" s="127"/>
-      <c r="C63" s="139" t="s">
+    <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="125"/>
+      <c r="B63" s="125"/>
+      <c r="C63" s="142" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="127"/>
-      <c r="B64" s="127"/>
-      <c r="C64" s="139"/>
-      <c r="D64" s="132" t="s">
+    <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="125"/>
+      <c r="B64" s="125"/>
+      <c r="C64" s="142"/>
+      <c r="D64" s="126" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="127"/>
-      <c r="B65" s="127"/>
-      <c r="C65" s="139"/>
-      <c r="D65" s="132"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="125"/>
+      <c r="B65" s="125"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="126"/>
     </row>
-    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="127"/>
-      <c r="B66" s="127"/>
-      <c r="C66" s="139"/>
-      <c r="D66" s="132"/>
+    <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="125"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="142"/>
+      <c r="D66" s="126"/>
     </row>
-    <row r="67" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="127"/>
-      <c r="B67" s="127"/>
-      <c r="C67" s="139"/>
-      <c r="D67" s="132"/>
+    <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="125"/>
+      <c r="B67" s="125"/>
+      <c r="C67" s="142"/>
+      <c r="D67" s="126"/>
     </row>
-    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C63:C67"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B53:B67"/>
@@ -30637,19 +30643,13 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C63:C67"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30661,18 +30661,18 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30694,33 +30694,33 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="149" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="136" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="151"/>
-      <c r="C4" s="146"/>
-      <c r="D4" s="121"/>
+      <c r="B4" s="157"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="137"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>237</v>
-      </c>
-      <c r="B5" s="151"/>
+        <v>256</v>
+      </c>
+      <c r="B5" s="157"/>
       <c r="C5" s="99" t="s">
         <v>22</v>
       </c>
@@ -30728,14 +30728,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="152"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="58"/>
       <c r="D6" s="98" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -30746,26 +30746,26 @@
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="159" t="s">
-        <v>239</v>
-      </c>
-      <c r="B8" s="146" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="149" t="s">
         <v>234</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="160"/>
-      <c r="B9" s="146"/>
-      <c r="C9" s="158"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="105"/>
       <c r="D9" s="58" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="97" t="s">
         <v>27</v>
       </c>
@@ -30774,31 +30774,31 @@
       </c>
       <c r="C10" s="58"/>
       <c r="D10" s="58" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="149" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="102" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="100" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="146" t="s">
-        <v>222</v>
-      </c>
-      <c r="B11" s="146" t="s">
-        <v>234</v>
-      </c>
-      <c r="C11" s="155" t="s">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="149"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="102" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="61" t="s">
         <v>242</v>
-      </c>
-      <c r="D11" s="153" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="146"/>
-      <c r="B12" s="146"/>
-      <c r="C12" s="155" t="s">
-        <v>243</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -30809,9 +30809,9 @@
       <c r="C13" s="39"/>
       <c r="D13" s="44"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="95" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B14" s="95" t="s">
         <v>234</v>
@@ -30823,21 +30823,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="96" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="99" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="154" t="s">
-        <v>247</v>
+      <c r="C15" s="101" t="s">
+        <v>244</v>
       </c>
       <c r="D15" s="98" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39" t="s">
         <v>40</v>
       </c>
@@ -30845,7 +30845,7 @@
       <c r="C16" s="39"/>
       <c r="D16" s="44"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
         <v>84</v>
       </c>
@@ -30853,17 +30853,17 @@
         <v>234</v>
       </c>
       <c r="C17" s="99" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="115" t="s">
-        <v>251</v>
-      </c>
-      <c r="B18" s="146" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="134" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="149" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="99">
@@ -30873,9 +30873,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="115"/>
-      <c r="B19" s="146"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
+      <c r="B19" s="149"/>
       <c r="C19" s="99">
         <v>10.199999999999999</v>
       </c>
@@ -30884,38 +30884,38 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="156" t="s">
-        <v>252</v>
+      <c r="A20" s="103" t="s">
+        <v>248</v>
       </c>
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="44"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="58" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B21" s="99" t="s">
         <v>234</v>
       </c>
       <c r="C21" s="99" t="s">
-        <v>254</v>
-      </c>
-      <c r="D21" s="157" t="s">
-        <v>255</v>
+        <v>250</v>
+      </c>
+      <c r="D21" s="104" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Added updates to TDM manual, updated change log and validation rules spreadsheet"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMOD_Documentation\paye-employers-documentation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\userdatadubc11\homedir\pbarre02\Desktop_vdi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
+    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="290">
   <si>
     <t>Document</t>
   </si>
@@ -2663,6 +2663,24 @@
   <si>
     <t>Date Updated</t>
   </si>
+  <si>
+    <t>code 3007</t>
+  </si>
+  <si>
+    <t>code 1011</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>PIT Self Service Application Guide</t>
+  </si>
+  <si>
+    <t>Section 7 added (Agent functionality)</t>
+  </si>
+  <si>
+    <t>New section</t>
+  </si>
 </sst>
 </file>
 
@@ -3256,7 +3274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3559,6 +3577,44 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3604,11 +3660,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3619,32 +3684,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3657,6 +3707,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3736,12 +3795,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3754,49 +3807,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4175,16 +4199,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4204,21 +4228,21 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="116" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="197">
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="131">
         <v>43056</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -4231,24 +4255,24 @@
       <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="197"/>
+      <c r="E3" s="131"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="116" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="197"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="131"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -4261,12 +4285,12 @@
       <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="197"/>
+      <c r="E5" s="131"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -4279,16 +4303,16 @@
       <c r="D6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="197"/>
+      <c r="E6" s="131"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="119" t="s">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="122">
+      <c r="B7" s="138">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4297,86 +4321,86 @@
       <c r="D7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="197"/>
+      <c r="E7" s="131"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="123"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="136"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="197"/>
+      <c r="E8" s="131"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="123"/>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="136"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="197"/>
+      <c r="E9" s="131"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="123"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="136"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="197"/>
+      <c r="E10" s="131"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
-      <c r="B11" s="123"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="136"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="197"/>
+      <c r="E11" s="131"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="121"/>
-      <c r="B12" s="124"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="137"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="197"/>
+      <c r="E12" s="131"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="127" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="122">
+      <c r="B13" s="138">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4385,26 +4409,26 @@
       <c r="D13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="197"/>
+      <c r="E13" s="131"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="124"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="144"/>
+      <c r="B14" s="140"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="197"/>
+      <c r="E14" s="131"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4417,12 +4441,12 @@
       <c r="D15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="197"/>
+      <c r="E15" s="131"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4435,24 +4459,24 @@
       <c r="D16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="197"/>
+      <c r="E16" s="131"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="116" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="197"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="131"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4465,12 +4489,12 @@
       <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="197"/>
+      <c r="E18" s="131"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4483,28 +4507,28 @@
       <c r="D19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="197"/>
+      <c r="E19" s="131"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="116" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="117"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="197"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="131"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="129" t="s">
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="126">
+      <c r="B21" s="142">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4513,23 +4537,23 @@
       <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="197"/>
+      <c r="E21" s="131"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="130"/>
-      <c r="B22" s="124"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="146"/>
+      <c r="B22" s="140"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="197"/>
+      <c r="E22" s="131"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4542,22 +4566,22 @@
       <c r="D23" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="197"/>
+      <c r="E23" s="131"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="116" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="132" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="117"/>
-      <c r="C24" s="117"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="197"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="131"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="125" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="126">
+      <c r="B25" s="142">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4566,110 +4590,110 @@
       <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="197"/>
+      <c r="E25" s="131"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="120"/>
-      <c r="B26" s="123"/>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="136"/>
+      <c r="B26" s="139"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="197"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="120"/>
-      <c r="B27" s="123"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="136"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="197"/>
+      <c r="E27" s="131"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="120"/>
-      <c r="B28" s="123"/>
+    <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="136"/>
+      <c r="B28" s="139"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="197"/>
+      <c r="E28" s="131"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="120"/>
-      <c r="B29" s="123"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="136"/>
+      <c r="B29" s="139"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="197"/>
+      <c r="E29" s="131"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="120"/>
-      <c r="B30" s="123"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="136"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="197"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="120"/>
-      <c r="B31" s="123"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="136"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="197"/>
+      <c r="E31" s="131"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="121"/>
-      <c r="B32" s="124"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="137"/>
+      <c r="B32" s="140"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="197"/>
+      <c r="E32" s="131"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4682,9 +4706,9 @@
       <c r="D33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="197"/>
+      <c r="E33" s="131"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4697,9 +4721,9 @@
       <c r="D34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="197"/>
+      <c r="E34" s="131"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4712,9 +4736,9 @@
       <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="197"/>
+      <c r="E35" s="131"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4727,9 +4751,9 @@
       <c r="D36" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="197"/>
+      <c r="E36" s="131"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4742,9 +4766,9 @@
       <c r="D37" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="197"/>
+      <c r="E37" s="131"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4757,9 +4781,9 @@
       <c r="D38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="197"/>
+      <c r="E38" s="131"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4772,9 +4796,9 @@
       <c r="D39" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="197"/>
+      <c r="E39" s="131"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4787,18 +4811,18 @@
       <c r="D40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="197"/>
+      <c r="E40" s="131"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="116" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="117"/>
-      <c r="C41" s="117"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="197"/>
+      <c r="B41" s="133"/>
+      <c r="C41" s="133"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="131"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4811,9 +4835,9 @@
       <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="197"/>
+      <c r="E42" s="131"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4826,9 +4850,9 @@
       <c r="D43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="197"/>
+      <c r="E43" s="131"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4841,9 +4865,9 @@
       <c r="D44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="197"/>
+      <c r="E44" s="131"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4856,7 +4880,7 @@
       <c r="D45" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="197"/>
+      <c r="E45" s="131"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -4906,16 +4930,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4932,18 +4956,18 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="198">
+      <c r="E2" s="158">
         <v>43140</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -4954,9 +4978,9 @@
       <c r="D3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="198"/>
+      <c r="E3" s="158"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -4967,9 +4991,9 @@
       <c r="D4" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="198"/>
+      <c r="E4" s="158"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -4980,22 +5004,22 @@
       <c r="D5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="198"/>
+      <c r="E5" s="158"/>
     </row>
-    <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="198"/>
+      <c r="E6" s="158"/>
     </row>
-    <row r="7" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5004,68 +5028,68 @@
       <c r="D7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="198"/>
+      <c r="E7" s="158"/>
     </row>
-    <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="152"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="198"/>
+      <c r="E8" s="158"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="133"/>
-      <c r="B9" s="134"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="152"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="198"/>
+      <c r="E9" s="158"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
-      <c r="B10" s="134"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="152"/>
+      <c r="B10" s="153"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="198"/>
+      <c r="E10" s="158"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="133"/>
-      <c r="B11" s="134"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="152"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="198"/>
+      <c r="E11" s="158"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="152"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="198"/>
+      <c r="E12" s="158"/>
     </row>
-    <row r="13" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="144" t="s">
+    <row r="13" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5074,35 +5098,35 @@
       <c r="D13" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="198"/>
+      <c r="E13" s="158"/>
     </row>
-    <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="144"/>
-      <c r="B14" s="134"/>
+    <row r="14" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="155"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="198"/>
+      <c r="E14" s="158"/>
     </row>
-    <row r="15" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="144"/>
-      <c r="B15" s="134"/>
+    <row r="15" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="155"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="198"/>
+      <c r="E15" s="158"/>
     </row>
-    <row r="16" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="131" t="s">
+    <row r="16" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5111,108 +5135,108 @@
       <c r="D16" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="198"/>
+      <c r="E16" s="158"/>
     </row>
-    <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="131"/>
-      <c r="B17" s="143"/>
+    <row r="17" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="150"/>
+      <c r="B17" s="156"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="198"/>
+      <c r="E17" s="158"/>
     </row>
-    <row r="18" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="131"/>
-      <c r="B18" s="143"/>
+    <row r="18" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="150"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="198"/>
+      <c r="E18" s="158"/>
     </row>
-    <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="131"/>
-      <c r="B19" s="143"/>
+    <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="150"/>
+      <c r="B19" s="156"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="198"/>
+      <c r="E19" s="158"/>
     </row>
-    <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="131"/>
-      <c r="B20" s="143"/>
+    <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="150"/>
+      <c r="B20" s="156"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="198"/>
+      <c r="E20" s="158"/>
     </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="131"/>
-      <c r="B21" s="143"/>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="150"/>
+      <c r="B21" s="156"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="198"/>
+      <c r="E21" s="158"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="131"/>
-      <c r="B22" s="143"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="150"/>
+      <c r="B22" s="156"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="198"/>
+      <c r="E22" s="158"/>
     </row>
-    <row r="23" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="131"/>
-      <c r="B23" s="143"/>
+    <row r="23" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="150"/>
+      <c r="B23" s="156"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="E23" s="198"/>
+      <c r="E23" s="158"/>
     </row>
-    <row r="24" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="131"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="131" t="s">
+    <row r="24" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="150"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="150" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="132" t="s">
+      <c r="D24" s="157" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="198"/>
+      <c r="E24" s="158"/>
     </row>
-    <row r="25" spans="1:5" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="131"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="131"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="198"/>
+    <row r="25" spans="1:5" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="150"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="158"/>
     </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="133" t="s">
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="152" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="134" t="s">
+      <c r="B26" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5221,18 +5245,18 @@
       <c r="D26" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="198"/>
+      <c r="E26" s="158"/>
     </row>
-    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="133"/>
-      <c r="B27" s="134"/>
+    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="152"/>
+      <c r="B27" s="153"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="198"/>
+      <c r="E27" s="158"/>
     </row>
-    <row r="28" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -5243,117 +5267,117 @@
       <c r="D28" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="198"/>
+      <c r="E28" s="158"/>
     </row>
-    <row r="29" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="198"/>
+      <c r="E29" s="158"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="135" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="134" t="s">
+      <c r="B30" s="153" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="131" t="s">
+      <c r="C30" s="150" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="139" t="s">
+      <c r="D30" s="151" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="198"/>
+      <c r="E30" s="158"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="135"/>
-      <c r="B31" s="134"/>
-      <c r="C31" s="131"/>
-      <c r="D31" s="139"/>
-      <c r="E31" s="198"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="154"/>
+      <c r="B31" s="153"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="158"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="135"/>
-      <c r="B32" s="134"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="154"/>
+      <c r="B32" s="153"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="198"/>
+      <c r="E32" s="158"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="135"/>
-      <c r="B33" s="134"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="154"/>
+      <c r="B33" s="153"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="198"/>
+      <c r="E33" s="158"/>
     </row>
-    <row r="34" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="135"/>
-      <c r="B34" s="134"/>
+    <row r="34" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="154"/>
+      <c r="B34" s="153"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="198"/>
+      <c r="E34" s="158"/>
     </row>
-    <row r="35" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="135"/>
-      <c r="B35" s="134"/>
+    <row r="35" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="154"/>
+      <c r="B35" s="153"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="198"/>
+      <c r="E35" s="158"/>
     </row>
-    <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="135"/>
-      <c r="B36" s="134"/>
+    <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="154"/>
+      <c r="B36" s="153"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
       <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="198"/>
+      <c r="E36" s="158"/>
     </row>
-    <row r="37" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="135"/>
-      <c r="B37" s="134"/>
-      <c r="C37" s="136" t="s">
+    <row r="37" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="154"/>
+      <c r="B37" s="153"/>
+      <c r="C37" s="147" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="138" t="s">
+      <c r="D37" s="149" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="198"/>
+      <c r="E37" s="158"/>
     </row>
-    <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="135"/>
-      <c r="B38" s="134"/>
-      <c r="C38" s="137"/>
-      <c r="D38" s="138"/>
-      <c r="E38" s="198"/>
+    <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="154"/>
+      <c r="B38" s="153"/>
+      <c r="C38" s="148"/>
+      <c r="D38" s="149"/>
+      <c r="E38" s="158"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="133" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5362,18 +5386,18 @@
       <c r="D39" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="198"/>
+      <c r="E39" s="158"/>
     </row>
-    <row r="40" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="133"/>
-      <c r="B40" s="134"/>
+    <row r="40" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="152"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="198"/>
+      <c r="E40" s="158"/>
     </row>
-    <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -5384,99 +5408,99 @@
       <c r="D41" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="198"/>
+      <c r="E41" s="158"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="198"/>
+      <c r="E42" s="158"/>
     </row>
-    <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="135" t="s">
+    <row r="43" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="134" t="s">
+      <c r="B43" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="198"/>
+      <c r="E43" s="158"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="135"/>
-      <c r="B44" s="134"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="154"/>
+      <c r="B44" s="153"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D44" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="198"/>
+      <c r="E44" s="158"/>
     </row>
-    <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="140" t="s">
+    <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="163" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="134" t="s">
+      <c r="B45" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="198"/>
+      <c r="E45" s="158"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="141"/>
-      <c r="B46" s="134"/>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="164"/>
+      <c r="B46" s="153"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="198"/>
+      <c r="E46" s="158"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="141"/>
-      <c r="B47" s="134"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="164"/>
+      <c r="B47" s="153"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="198"/>
+      <c r="E47" s="158"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="142"/>
-      <c r="B48" s="134"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="165"/>
+      <c r="B48" s="153"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="198"/>
+      <c r="E48" s="158"/>
     </row>
-    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="143" t="s">
+    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A49" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="143" t="s">
+      <c r="B49" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="198"/>
+      <c r="E49" s="158"/>
       <c r="H49" s="42"/>
       <c r="L49" s="42"/>
       <c r="P49" s="42"/>
@@ -9573,16 +9597,16 @@
       <c r="XEZ49" s="42"/>
       <c r="XFD49" s="42"/>
     </row>
-    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="143"/>
-      <c r="B50" s="143"/>
+    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="156"/>
+      <c r="B50" s="156"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="198"/>
+      <c r="E50" s="158"/>
       <c r="H50" s="42"/>
       <c r="L50" s="42"/>
       <c r="P50" s="42"/>
@@ -13679,16 +13703,16 @@
       <c r="XEZ50" s="42"/>
       <c r="XFD50" s="42"/>
     </row>
-    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="143"/>
-      <c r="B51" s="143"/>
+    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A51" s="156"/>
+      <c r="B51" s="156"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="E51" s="198"/>
+      <c r="E51" s="158"/>
       <c r="H51" s="42"/>
       <c r="L51" s="42"/>
       <c r="P51" s="42"/>
@@ -17785,16 +17809,16 @@
       <c r="XEZ51" s="42"/>
       <c r="XFD51" s="42"/>
     </row>
-    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="143"/>
-      <c r="B52" s="143"/>
+    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A52" s="156"/>
+      <c r="B52" s="156"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="198"/>
+      <c r="E52" s="158"/>
       <c r="H52" s="42"/>
       <c r="L52" s="42"/>
       <c r="P52" s="42"/>
@@ -21891,16 +21915,16 @@
       <c r="XEZ52" s="42"/>
       <c r="XFD52" s="42"/>
     </row>
-    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="143"/>
-      <c r="B53" s="143"/>
-      <c r="C53" s="146" t="s">
+    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A53" s="156"/>
+      <c r="B53" s="156"/>
+      <c r="C53" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="139" t="s">
+      <c r="D53" s="151" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="198"/>
+      <c r="E53" s="158"/>
       <c r="H53" s="42"/>
       <c r="L53" s="42"/>
       <c r="P53" s="42"/>
@@ -25997,12 +26021,12 @@
       <c r="XEZ53" s="42"/>
       <c r="XFD53" s="42"/>
     </row>
-    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="146"/>
-      <c r="D54" s="139"/>
-      <c r="E54" s="198"/>
+    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="156"/>
+      <c r="B54" s="156"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="151"/>
+      <c r="E54" s="158"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -30099,16 +30123,16 @@
       <c r="XEZ54" s="42"/>
       <c r="XFD54" s="42"/>
     </row>
-    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
-      <c r="E55" s="198"/>
+      <c r="E55" s="158"/>
     </row>
-    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -30119,13 +30143,13 @@
       <c r="D56" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="198"/>
+      <c r="E56" s="158"/>
     </row>
-    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="147" t="s">
+    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A57" s="161" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="143" t="s">
+      <c r="B57" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30134,221 +30158,221 @@
       <c r="D57" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="198"/>
+      <c r="E57" s="158"/>
     </row>
-    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="147"/>
-      <c r="B58" s="143"/>
+    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="161"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="E58" s="198"/>
+      <c r="E58" s="158"/>
     </row>
-    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="147"/>
-      <c r="B59" s="143"/>
+    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A59" s="161"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D59" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="198"/>
+      <c r="E59" s="158"/>
     </row>
-    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="147"/>
-      <c r="B60" s="143"/>
+    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="161"/>
+      <c r="B60" s="156"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D60" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="198"/>
+      <c r="E60" s="158"/>
     </row>
-    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="147"/>
-      <c r="B61" s="143"/>
+    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A61" s="161"/>
+      <c r="B61" s="156"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="198"/>
+      <c r="E61" s="158"/>
     </row>
-    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="147"/>
-      <c r="B62" s="143"/>
+    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A62" s="161"/>
+      <c r="B62" s="156"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="198"/>
+      <c r="E62" s="158"/>
     </row>
-    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="147"/>
-      <c r="B63" s="143"/>
+    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A63" s="161"/>
+      <c r="B63" s="156"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D63" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="198"/>
+      <c r="E63" s="158"/>
     </row>
-    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="147"/>
-      <c r="B64" s="143"/>
+    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A64" s="161"/>
+      <c r="B64" s="156"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="198"/>
+      <c r="E64" s="158"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="147"/>
-      <c r="B65" s="143"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="161"/>
+      <c r="B65" s="156"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="198"/>
+      <c r="E65" s="158"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="147"/>
-      <c r="B66" s="143"/>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="161"/>
+      <c r="B66" s="156"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="198"/>
+      <c r="E66" s="158"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="147"/>
-      <c r="B67" s="143"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="161"/>
+      <c r="B67" s="156"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E67" s="198"/>
+      <c r="E67" s="158"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="147"/>
-      <c r="B68" s="143"/>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="161"/>
+      <c r="B68" s="156"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="198"/>
+      <c r="E68" s="158"/>
     </row>
-    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="147"/>
-      <c r="B69" s="143"/>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="161"/>
+      <c r="B69" s="156"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E69" s="198"/>
+      <c r="E69" s="158"/>
     </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="147"/>
-      <c r="B70" s="143"/>
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="161"/>
+      <c r="B70" s="156"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="198"/>
+      <c r="E70" s="158"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="147"/>
-      <c r="B71" s="143"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="161"/>
+      <c r="B71" s="156"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="198"/>
+      <c r="E71" s="158"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="147"/>
-      <c r="B72" s="143"/>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="161"/>
+      <c r="B72" s="156"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="198"/>
+      <c r="E72" s="158"/>
     </row>
-    <row r="73" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="147"/>
-      <c r="B73" s="143"/>
+    <row r="73" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="161"/>
+      <c r="B73" s="156"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="198"/>
+      <c r="E73" s="158"/>
     </row>
-    <row r="74" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="147"/>
-      <c r="B74" s="143"/>
+    <row r="74" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="161"/>
+      <c r="B74" s="156"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="E74" s="198"/>
+      <c r="E74" s="158"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="147"/>
-      <c r="B75" s="143"/>
-      <c r="C75" s="145"/>
-      <c r="D75" s="148" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="161"/>
+      <c r="B75" s="156"/>
+      <c r="C75" s="159"/>
+      <c r="D75" s="162" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="198"/>
+      <c r="E75" s="158"/>
     </row>
-    <row r="76" spans="1:5" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="147"/>
-      <c r="B76" s="143"/>
-      <c r="C76" s="145"/>
-      <c r="D76" s="148"/>
-      <c r="E76" s="198"/>
+    <row r="76" spans="1:5" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="161"/>
+      <c r="B76" s="156"/>
+      <c r="C76" s="159"/>
+      <c r="D76" s="162"/>
+      <c r="E76" s="158"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
-      <c r="E77" s="198"/>
+      <c r="E77" s="158"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -30373,10 +30397,11 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="31">
-    <mergeCell ref="E2:E77"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="A57:A76"/>
     <mergeCell ref="B57:B76"/>
     <mergeCell ref="D75:D76"/>
@@ -30384,26 +30409,25 @@
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="B49:B54"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B16:B25"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E2:E77"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A30:A38"/>
     <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="B16:B25"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30418,16 +30442,16 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" customWidth="1"/>
-    <col min="4" max="4" width="80.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30444,31 +30468,31 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="197">
+      <c r="E2" s="131">
         <v>43179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="197"/>
+      <c r="E3" s="131"/>
     </row>
-    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="133" t="s">
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30477,160 +30501,160 @@
       <c r="D4" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="197"/>
+      <c r="E4" s="131"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="133"/>
-      <c r="B5" s="134"/>
-      <c r="C5" s="164" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="152"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="181" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="163" t="s">
+      <c r="D5" s="180" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="197"/>
+      <c r="E5" s="131"/>
     </row>
-    <row r="6" spans="1:5" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="133"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="164"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="197"/>
+    <row r="6" spans="1:5" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="152"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="131"/>
     </row>
-    <row r="7" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="133"/>
-      <c r="B7" s="134"/>
+    <row r="7" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="152"/>
+      <c r="B7" s="153"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
-      <c r="E7" s="197"/>
+      <c r="E7" s="131"/>
     </row>
-    <row r="8" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
+    <row r="8" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="152"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
-      <c r="E8" s="197"/>
+      <c r="E8" s="131"/>
     </row>
-    <row r="9" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="133"/>
-      <c r="B9" s="134"/>
+    <row r="9" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="152"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
-      <c r="E9" s="197"/>
+      <c r="E9" s="131"/>
     </row>
-    <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="144" t="s">
+    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="134" t="s">
+      <c r="B10" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="155"/>
-      <c r="D10" s="163" t="s">
+      <c r="C10" s="172"/>
+      <c r="D10" s="180" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="197"/>
+      <c r="E10" s="131"/>
     </row>
-    <row r="11" spans="1:5" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="144"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="163"/>
-      <c r="E11" s="197"/>
+    <row r="11" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="155"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="180"/>
+      <c r="E11" s="131"/>
     </row>
-    <row r="12" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="144"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="155"/>
-      <c r="D12" s="163"/>
-      <c r="E12" s="197"/>
+    <row r="12" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="155"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="131"/>
     </row>
-    <row r="13" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="131" t="s">
+    <row r="13" spans="1:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="143" t="s">
+      <c r="B13" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="163" t="s">
+      <c r="C13" s="182"/>
+      <c r="D13" s="180" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="197"/>
+      <c r="E13" s="131"/>
     </row>
-    <row r="14" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="131"/>
-      <c r="B14" s="143"/>
-      <c r="C14" s="165"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="197"/>
+    <row r="14" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="150"/>
+      <c r="B14" s="156"/>
+      <c r="C14" s="182"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="131"/>
     </row>
-    <row r="15" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="131"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="165"/>
+    <row r="15" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="150"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="182"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="197"/>
+      <c r="E15" s="131"/>
     </row>
-    <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="131"/>
-      <c r="B16" s="143"/>
-      <c r="C16" s="165"/>
+    <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="150"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="182"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="197"/>
+      <c r="E16" s="131"/>
     </row>
-    <row r="17" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="131"/>
-      <c r="B17" s="143"/>
-      <c r="C17" s="165"/>
+    <row r="17" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="150"/>
+      <c r="B17" s="156"/>
+      <c r="C17" s="182"/>
       <c r="D17" s="49"/>
-      <c r="E17" s="197"/>
+      <c r="E17" s="131"/>
     </row>
-    <row r="18" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="131"/>
-      <c r="B18" s="143"/>
-      <c r="C18" s="165"/>
+    <row r="18" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="150"/>
+      <c r="B18" s="156"/>
+      <c r="C18" s="182"/>
       <c r="D18" s="49"/>
-      <c r="E18" s="197"/>
+      <c r="E18" s="131"/>
     </row>
-    <row r="19" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="131"/>
-      <c r="B19" s="143"/>
-      <c r="C19" s="165"/>
+    <row r="19" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="150"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="182"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="197"/>
+      <c r="E19" s="131"/>
     </row>
-    <row r="20" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="131"/>
-      <c r="B20" s="143"/>
-      <c r="C20" s="165"/>
+    <row r="20" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="150"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="182"/>
       <c r="D20" s="49"/>
-      <c r="E20" s="197"/>
+      <c r="E20" s="131"/>
     </row>
-    <row r="21" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="131"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="165"/>
+    <row r="21" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="150"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="182"/>
       <c r="D21" s="49"/>
-      <c r="E21" s="197"/>
+      <c r="E21" s="131"/>
     </row>
-    <row r="22" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="131"/>
-      <c r="B22" s="143"/>
-      <c r="C22" s="165"/>
+    <row r="22" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="150"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="182"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="197"/>
+      <c r="E22" s="131"/>
     </row>
-    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="131"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="165"/>
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="150"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="182"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="197"/>
+      <c r="E23" s="131"/>
     </row>
-    <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
@@ -30643,9 +30667,9 @@
       <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="197"/>
+      <c r="E24" s="131"/>
     </row>
-    <row r="25" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30658,9 +30682,9 @@
       <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="E25" s="197"/>
+      <c r="E25" s="131"/>
     </row>
-    <row r="26" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30671,18 +30695,18 @@
       <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="197"/>
+      <c r="E26" s="131"/>
     </row>
-    <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="197"/>
+      <c r="E27" s="131"/>
     </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30695,9 +30719,9 @@
       <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="197"/>
+      <c r="E28" s="131"/>
     </row>
-    <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="85"/>
       <c r="B29" s="84"/>
       <c r="C29" s="70" t="s">
@@ -30706,9 +30730,9 @@
       <c r="D29" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="197"/>
+      <c r="E29" s="131"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30717,9 +30741,9 @@
       <c r="D30" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="E30" s="197"/>
+      <c r="E30" s="131"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30728,13 +30752,13 @@
       <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="197"/>
+      <c r="E31" s="131"/>
     </row>
-    <row r="32" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="149" t="s">
+    <row r="32" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="166" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="152" t="s">
+      <c r="B32" s="169" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30743,41 +30767,41 @@
       <c r="D32" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="E32" s="197"/>
+      <c r="E32" s="131"/>
     </row>
-    <row r="33" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="150"/>
-      <c r="B33" s="153"/>
+    <row r="33" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="167"/>
+      <c r="B33" s="170"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
-      <c r="E33" s="197"/>
+      <c r="E33" s="131"/>
     </row>
-    <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="150"/>
-      <c r="B34" s="153"/>
+    <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="167"/>
+      <c r="B34" s="170"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
-      <c r="E34" s="197"/>
+      <c r="E34" s="131"/>
     </row>
-    <row r="35" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="150"/>
-      <c r="B35" s="153"/>
+    <row r="35" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="167"/>
+      <c r="B35" s="170"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
-      <c r="E35" s="197"/>
+      <c r="E35" s="131"/>
     </row>
-    <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="151"/>
-      <c r="B36" s="154"/>
+    <row r="36" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="168"/>
+      <c r="B36" s="171"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="197"/>
+      <c r="E36" s="131"/>
     </row>
-    <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>27</v>
       </c>
@@ -30788,22 +30812,22 @@
       <c r="D37" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="197"/>
+      <c r="E37" s="131"/>
     </row>
-    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
-      <c r="E38" s="197"/>
+      <c r="E38" s="131"/>
     </row>
-    <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="135" t="s">
+    <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30812,119 +30836,119 @@
       <c r="D39" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="E39" s="197"/>
+      <c r="E39" s="131"/>
     </row>
-    <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="135"/>
-      <c r="B40" s="134"/>
+    <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="154"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="197"/>
+      <c r="E40" s="131"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="133" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="134" t="s">
+      <c r="B41" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="155" t="s">
+      <c r="C41" s="172" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="131" t="s">
+      <c r="D41" s="150" t="s">
         <v>228</v>
       </c>
-      <c r="E41" s="197"/>
+      <c r="E41" s="131"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="133"/>
-      <c r="B42" s="134"/>
-      <c r="C42" s="155"/>
-      <c r="D42" s="131"/>
-      <c r="E42" s="197"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="152"/>
+      <c r="B42" s="153"/>
+      <c r="C42" s="172"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="131"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="133"/>
-      <c r="B43" s="134"/>
-      <c r="C43" s="155" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="152"/>
+      <c r="B43" s="153"/>
+      <c r="C43" s="172" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="148" t="s">
+      <c r="D43" s="162" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="197"/>
+      <c r="E43" s="131"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="133"/>
-      <c r="B44" s="134"/>
-      <c r="C44" s="155"/>
-      <c r="D44" s="148"/>
-      <c r="E44" s="197"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="152"/>
+      <c r="B44" s="153"/>
+      <c r="C44" s="172"/>
+      <c r="D44" s="162"/>
+      <c r="E44" s="131"/>
     </row>
-    <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="147" t="s">
+    <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="143" t="s">
+      <c r="B45" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="159"/>
+      <c r="C45" s="176"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="197"/>
+      <c r="E45" s="131"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="147"/>
-      <c r="B46" s="143"/>
-      <c r="C46" s="160"/>
-      <c r="D46" s="156" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="161"/>
+      <c r="B46" s="156"/>
+      <c r="C46" s="177"/>
+      <c r="D46" s="173" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="197"/>
+      <c r="E46" s="131"/>
     </row>
-    <row r="47" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="147"/>
-      <c r="B47" s="143"/>
-      <c r="C47" s="160"/>
-      <c r="D47" s="157"/>
-      <c r="E47" s="197"/>
+    <row r="47" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="161"/>
+      <c r="B47" s="156"/>
+      <c r="C47" s="177"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="131"/>
     </row>
-    <row r="48" spans="1:5" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="147"/>
-      <c r="B48" s="143"/>
-      <c r="C48" s="161"/>
-      <c r="D48" s="157"/>
-      <c r="E48" s="197"/>
+    <row r="48" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="161"/>
+      <c r="B48" s="156"/>
+      <c r="C48" s="178"/>
+      <c r="D48" s="174"/>
+      <c r="E48" s="131"/>
     </row>
-    <row r="49" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="147"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="146"/>
-      <c r="D49" s="157"/>
-      <c r="E49" s="197"/>
+    <row r="49" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="161"/>
+      <c r="B49" s="156"/>
+      <c r="C49" s="160"/>
+      <c r="D49" s="174"/>
+      <c r="E49" s="131"/>
     </row>
-    <row r="50" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="147"/>
-      <c r="B50" s="143"/>
-      <c r="C50" s="146"/>
-      <c r="D50" s="158"/>
-      <c r="E50" s="197"/>
+    <row r="50" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="161"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="175"/>
+      <c r="E50" s="131"/>
     </row>
-    <row r="51" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
-      <c r="E51" s="197"/>
+      <c r="E51" s="131"/>
     </row>
-    <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
@@ -30935,13 +30959,13 @@
       <c r="D52" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="197"/>
+      <c r="E52" s="131"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="143" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="143" t="s">
+      <c r="B53" s="156" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30950,191 +30974,191 @@
       <c r="D53" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="197"/>
+      <c r="E53" s="131"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="156"/>
+      <c r="B54" s="156"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
       <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="197"/>
+      <c r="E54" s="131"/>
     </row>
-    <row r="55" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="143"/>
-      <c r="B55" s="143"/>
+    <row r="55" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="156"/>
+      <c r="B55" s="156"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="197"/>
+      <c r="E55" s="131"/>
     </row>
-    <row r="56" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="143"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="162" t="s">
+    <row r="56" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="156"/>
+      <c r="B56" s="156"/>
+      <c r="C56" s="179" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="E56" s="197"/>
+      <c r="E56" s="131"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="143"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="162"/>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="156"/>
+      <c r="B57" s="156"/>
+      <c r="C57" s="179"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="197"/>
+      <c r="E57" s="131"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="143"/>
-      <c r="B58" s="143"/>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="156"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
       <c r="D58" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E58" s="197"/>
+      <c r="E58" s="131"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="143"/>
-      <c r="B59" s="143"/>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="156"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
       <c r="D59" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="197"/>
+      <c r="E59" s="131"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="143"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="162" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="156"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="179" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="197"/>
+      <c r="E60" s="131"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="143"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="162"/>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="156"/>
+      <c r="B61" s="156"/>
+      <c r="C61" s="179"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="197"/>
+      <c r="E61" s="131"/>
     </row>
-    <row r="62" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="143"/>
-      <c r="B62" s="143"/>
-      <c r="C62" s="162"/>
+    <row r="62" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="156"/>
+      <c r="B62" s="156"/>
+      <c r="C62" s="179"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="E62" s="197"/>
+      <c r="E62" s="131"/>
     </row>
-    <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="143"/>
-      <c r="B63" s="143"/>
-      <c r="C63" s="155" t="s">
+    <row r="63" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="156"/>
+      <c r="B63" s="156"/>
+      <c r="C63" s="172" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="E63" s="197"/>
+      <c r="E63" s="131"/>
     </row>
-    <row r="64" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="143"/>
-      <c r="B64" s="143"/>
-      <c r="C64" s="155"/>
-      <c r="D64" s="148" t="s">
+    <row r="64" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="156"/>
+      <c r="B64" s="156"/>
+      <c r="C64" s="172"/>
+      <c r="D64" s="162" t="s">
         <v>220</v>
       </c>
-      <c r="E64" s="197"/>
+      <c r="E64" s="131"/>
     </row>
-    <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="143"/>
-      <c r="B65" s="143"/>
-      <c r="C65" s="155"/>
-      <c r="D65" s="148"/>
-      <c r="E65" s="197"/>
+    <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="156"/>
+      <c r="B65" s="156"/>
+      <c r="C65" s="172"/>
+      <c r="D65" s="162"/>
+      <c r="E65" s="131"/>
     </row>
-    <row r="66" spans="1:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="143"/>
-      <c r="B66" s="143"/>
-      <c r="C66" s="155"/>
-      <c r="D66" s="148"/>
-      <c r="E66" s="197"/>
+    <row r="66" spans="1:5" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="156"/>
+      <c r="B66" s="156"/>
+      <c r="C66" s="172"/>
+      <c r="D66" s="162"/>
+      <c r="E66" s="131"/>
     </row>
-    <row r="67" spans="1:5" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="143"/>
-      <c r="B67" s="143"/>
-      <c r="C67" s="155"/>
-      <c r="D67" s="148"/>
-      <c r="E67" s="197"/>
+    <row r="67" spans="1:5" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="156"/>
+      <c r="B67" s="156"/>
+      <c r="C67" s="172"/>
+      <c r="D67" s="162"/>
+      <c r="E67" s="131"/>
     </row>
-    <row r="68" spans="1:5" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
-      <c r="E68" s="197"/>
+      <c r="E68" s="131"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -31150,23 +31174,23 @@
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="B53:B67"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="C45:C48"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C56:C57"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="A4:A9"/>
@@ -31183,22 +31207,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -31208,164 +31232,164 @@
       <c r="C1" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="181" t="s">
+      <c r="D1" s="116" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
-      <c r="D2" s="182"/>
+      <c r="D2" s="117"/>
       <c r="E2" s="58"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="131" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="162" t="s">
+      <c r="B3" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="58"/>
-      <c r="D3" s="183" t="s">
+      <c r="D3" s="118" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="194">
+      <c r="E3" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="131"/>
-      <c r="B4" s="162"/>
+    <row r="4" spans="1:5" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="150"/>
+      <c r="B4" s="179"/>
       <c r="C4" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="184" t="s">
+      <c r="D4" s="119" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="193">
+      <c r="E4" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="162"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="185" t="s">
+      <c r="D5" s="120" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="193">
+      <c r="E5" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="162"/>
+      <c r="B6" s="179"/>
       <c r="C6" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="185" t="s">
+      <c r="D6" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="193">
+      <c r="E6" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="173" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="190" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="162"/>
+      <c r="B7" s="179"/>
       <c r="C7" s="58"/>
-      <c r="D7" s="186" t="s">
+      <c r="D7" s="121" t="s">
         <v>261</v>
       </c>
-      <c r="E7" s="194">
+      <c r="E7" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="174"/>
-      <c r="B8" s="162"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="191"/>
+      <c r="B8" s="179"/>
       <c r="C8" s="58"/>
-      <c r="D8" s="183" t="s">
+      <c r="D8" s="118" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="194">
+      <c r="E8" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="162"/>
+      <c r="B9" s="179"/>
       <c r="C9" s="58"/>
-      <c r="D9" s="185" t="s">
+      <c r="D9" s="120" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="193">
+      <c r="E9" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="187"/>
+      <c r="D10" s="122"/>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="170" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="187" t="s">
         <v>237</v>
       </c>
-      <c r="B11" s="162" t="s">
+      <c r="B11" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" t="s">
         <v>258</v>
       </c>
-      <c r="E11" s="194">
+      <c r="E11" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="171"/>
-      <c r="B12" s="162"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="188"/>
+      <c r="B12" s="179"/>
       <c r="C12" s="58"/>
-      <c r="D12" s="183" t="s">
+      <c r="D12" s="118" t="s">
         <v>252</v>
       </c>
-      <c r="E12" s="193">
+      <c r="E12" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="172"/>
-      <c r="B13" s="162"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="189"/>
+      <c r="B13" s="179"/>
       <c r="C13" s="58"/>
-      <c r="D13" s="183" t="s">
+      <c r="D13" s="118" t="s">
         <v>254</v>
       </c>
-      <c r="E13" s="193">
+      <c r="E13" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="96" t="s">
         <v>27</v>
       </c>
@@ -31373,55 +31397,55 @@
         <v>234</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="183" t="s">
+      <c r="D14" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="E14" s="194">
+      <c r="E14" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="162" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="179" t="s">
         <v>222</v>
       </c>
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="175" t="s">
+      <c r="C15" s="198" t="s">
         <v>239</v>
       </c>
-      <c r="D15" s="188" t="s">
+      <c r="D15" s="123" t="s">
         <v>241</v>
       </c>
-      <c r="E15" s="193">
+      <c r="E15" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="162"/>
-      <c r="B16" s="162"/>
-      <c r="C16" s="176"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="179"/>
+      <c r="B16" s="179"/>
+      <c r="C16" s="199"/>
       <c r="D16" s="113" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="194">
+      <c r="E16" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="162"/>
-      <c r="B17" s="162"/>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="179"/>
+      <c r="B17" s="179"/>
       <c r="C17" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="189" t="s">
+      <c r="D17" s="124" t="s">
         <v>242</v>
       </c>
-      <c r="E17" s="193">
+      <c r="E17" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="110" t="s">
         <v>280</v>
       </c>
@@ -31429,49 +31453,49 @@
       <c r="C18" s="61" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="183" t="s">
+      <c r="D18" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="E18" s="194">
+      <c r="E18" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
-      <c r="D19" s="182"/>
+      <c r="D19" s="117"/>
       <c r="E19" s="58"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="173" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="190" t="s">
         <v>260</v>
       </c>
-      <c r="B20" s="162" t="s">
+      <c r="B20" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C20" s="58"/>
-      <c r="D20" s="186" t="s">
+      <c r="D20" s="121" t="s">
         <v>261</v>
       </c>
-      <c r="E20" s="194">
+      <c r="E20" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="174"/>
-      <c r="B21" s="162"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="191"/>
+      <c r="B21" s="179"/>
       <c r="C21" s="58"/>
-      <c r="D21" s="183" t="s">
+      <c r="D21" s="118" t="s">
         <v>257</v>
       </c>
-      <c r="E21" s="194">
+      <c r="E21" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="102" t="s">
         <v>243</v>
       </c>
@@ -31481,345 +31505,383 @@
       <c r="C22" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="190" t="s">
+      <c r="D22" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="193">
+      <c r="E22" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="177" t="s">
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="192" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="168" t="s">
+      <c r="B23" s="185" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="D23" s="183" t="s">
+      <c r="D23" s="118" t="s">
         <v>251</v>
       </c>
-      <c r="E23" s="193">
+      <c r="E23" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="178"/>
-      <c r="B24" s="180"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="193"/>
+      <c r="B24" s="195"/>
       <c r="C24" t="s">
         <v>270</v>
       </c>
-      <c r="D24" s="183" t="s">
+      <c r="D24" s="118" t="s">
         <v>251</v>
       </c>
-      <c r="E24" s="194">
+      <c r="E24" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="178"/>
-      <c r="B25" s="180"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="193"/>
+      <c r="B25" s="195"/>
       <c r="C25" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="D25" s="183" t="s">
+      <c r="D25" s="118" t="s">
         <v>251</v>
       </c>
-      <c r="E25" s="194">
+      <c r="E25" s="128">
         <v>43270</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="178"/>
-      <c r="B26" s="180"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="193"/>
+      <c r="B26" s="195"/>
       <c r="C26" s="112" t="s">
         <v>277</v>
       </c>
       <c r="D26" s="113" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="194">
+      <c r="E26" s="130">
         <v>43270</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="179"/>
-      <c r="B27" s="169"/>
-      <c r="C27" s="98" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="193"/>
+      <c r="B27" s="195"/>
+      <c r="C27" s="58" t="s">
+        <v>284</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" s="127">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="193"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>286</v>
+      </c>
+      <c r="E28" s="127">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="194"/>
+      <c r="B29" s="186"/>
+      <c r="C29" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="D27" s="190" t="s">
+      <c r="D29" s="125" t="s">
         <v>245</v>
       </c>
-      <c r="E27" s="193">
+      <c r="E29" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
+    <row r="30" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="182"/>
-      <c r="E28" s="58"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="58"/>
     </row>
-    <row r="29" spans="1:5" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="109"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="186" t="s">
+    <row r="31" spans="1:5" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="109"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="121" t="s">
         <v>261</v>
       </c>
-      <c r="E29" s="58"/>
+      <c r="E31" s="58"/>
     </row>
-    <row r="30" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="131" t="s">
+    <row r="32" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="162" t="s">
+      <c r="B32" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C30" s="107" t="s">
+      <c r="C32" s="107" t="s">
         <v>246</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D32" s="118" t="s">
         <v>253</v>
       </c>
-      <c r="E30" s="193">
+      <c r="E32" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="131"/>
-      <c r="B31" s="162"/>
-      <c r="C31" s="107">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="150"/>
+      <c r="B33" s="179"/>
+      <c r="C33" s="107">
         <v>10.1</v>
       </c>
-      <c r="D31" s="183" t="s">
+      <c r="D33" s="118" t="s">
         <v>272</v>
       </c>
-      <c r="E31" s="193">
+      <c r="E33" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="131"/>
-      <c r="B32" s="162"/>
-      <c r="C32" s="107">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="150"/>
+      <c r="B34" s="179"/>
+      <c r="C34" s="107">
         <v>10.199999999999999</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D34" s="118" t="s">
         <v>272</v>
       </c>
-      <c r="E32" s="193">
+      <c r="E34" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="131" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="150" t="s">
         <v>247</v>
       </c>
-      <c r="B33" s="162" t="s">
+      <c r="B35" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="162"/>
-      <c r="D33" s="191" t="s">
+      <c r="C35" s="179"/>
+      <c r="D35" s="200" t="s">
         <v>261</v>
       </c>
-      <c r="E33" s="195">
+      <c r="E35" s="196">
         <v>43270</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="131"/>
-      <c r="B34" s="162"/>
-      <c r="C34" s="162"/>
-      <c r="D34" s="191"/>
-      <c r="E34" s="196"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="150"/>
+      <c r="B36" s="179"/>
+      <c r="C36" s="179"/>
+      <c r="D36" s="200"/>
+      <c r="E36" s="197"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="106" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="106" t="s">
         <v>262</v>
-      </c>
-      <c r="B35" s="107" t="s">
-        <v>234</v>
-      </c>
-      <c r="C35" s="107" t="s">
-        <v>250</v>
-      </c>
-      <c r="D35" s="192" t="s">
-        <v>251</v>
-      </c>
-      <c r="E35" s="193">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="100" t="s">
-        <v>248</v>
-      </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="105"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="58"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="58" t="s">
-        <v>249</v>
       </c>
       <c r="B37" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="104" t="s">
-        <v>265</v>
-      </c>
-      <c r="D37" s="183" t="s">
-        <v>267</v>
-      </c>
-      <c r="E37" s="193">
+      <c r="C37" s="107" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" s="126" t="s">
+        <v>251</v>
+      </c>
+      <c r="E37" s="127">
         <v>43244</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="108" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="108"/>
-      <c r="C38" s="108"/>
-      <c r="D38" s="114"/>
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="100" t="s">
+        <v>248</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="115"/>
       <c r="E38" s="58"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="166" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="168" t="s">
-        <v>271</v>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39" s="107" t="s">
+        <v>234</v>
       </c>
       <c r="C39" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="D39" s="183" t="s">
+      <c r="D39" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="E39" s="193">
+      <c r="E39" s="127">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="58" t="s">
+        <v>287</v>
+      </c>
+      <c r="B40" s="129" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" s="104" t="s">
+        <v>288</v>
+      </c>
+      <c r="D40" s="118" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" s="127">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="108" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="108"/>
+      <c r="C41" s="108"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="58"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="183" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="185" t="s">
+        <v>271</v>
+      </c>
+      <c r="C42" s="104" t="s">
+        <v>265</v>
+      </c>
+      <c r="D42" s="118" t="s">
+        <v>267</v>
+      </c>
+      <c r="E42" s="127">
         <v>43259</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="167"/>
-      <c r="B40" s="169"/>
-      <c r="C40" s="104" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="184"/>
+      <c r="B43" s="186"/>
+      <c r="C43" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="D40" s="183" t="s">
+      <c r="D43" s="118" t="s">
         <v>266</v>
       </c>
-      <c r="E40" s="193">
+      <c r="E43" s="127">
         <v>43259</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="103" t="s">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="107" t="s">
+      <c r="B44" s="107" t="s">
         <v>271</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C44" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D41" s="183" t="s">
+      <c r="D44" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="193">
+      <c r="E44" s="127">
         <v>43259</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="103" t="s">
+    <row r="45" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="107" t="s">
+      <c r="B45" s="107" t="s">
         <v>271</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C45" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D42" s="183" t="s">
+      <c r="D45" s="118" t="s">
         <v>263</v>
       </c>
-      <c r="E42" s="193">
+      <c r="E45" s="127">
         <v>43259</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="108" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="108" t="s">
         <v>273</v>
       </c>
-      <c r="B43" s="108"/>
-      <c r="C43" s="108"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="58"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="58"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="58"/>
-      <c r="B44" s="107" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="58"/>
+      <c r="B47" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C47" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="192" t="s">
+      <c r="D47" s="126" t="s">
         <v>274</v>
       </c>
-      <c r="E44" s="193">
+      <c r="E47" s="127">
         <v>43265</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="108" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="108" t="s">
         <v>279</v>
       </c>
-      <c r="B45" s="108"/>
-      <c r="C45" s="108"/>
-      <c r="D45" s="114"/>
-      <c r="E45" s="58"/>
+      <c r="B48" s="108"/>
+      <c r="C48" s="108"/>
+      <c r="D48" s="114"/>
+      <c r="E48" s="58"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="58"/>
-      <c r="B46" s="111" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="58"/>
+      <c r="B49" s="111" t="s">
         <v>234</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="C49" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="192" t="s">
+      <c r="D49" s="126" t="s">
         <v>274</v>
       </c>
-      <c r="E46" s="194">
+      <c r="E49" s="128">
         <v>43270</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E35:E36"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A11:A13"/>
@@ -31827,6 +31889,11 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"merging branches 2 and 3"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\userdatadubc11\homedir\pbarre02\Desktop_vdi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMOD_Documentation\paye-employers-documentation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
+    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -3274,7 +3274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3521,15 +3521,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3539,23 +3530,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3563,20 +3542,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3605,6 +3572,24 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4199,16 +4184,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4228,21 +4213,21 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="132" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="131">
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="126">
         <v>43056</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -4255,24 +4240,24 @@
       <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="131"/>
+      <c r="E3" s="126"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="131"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -4285,12 +4270,12 @@
       <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="131"/>
+      <c r="E5" s="126"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -4303,16 +4288,16 @@
       <c r="D6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="131"/>
+      <c r="E6" s="126"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="135" t="s">
+    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="138">
+      <c r="B7" s="133">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4321,86 +4306,86 @@
       <c r="D7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="131"/>
+      <c r="E7" s="126"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
-      <c r="B8" s="139"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="131"/>
+      <c r="B8" s="134"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="131"/>
+      <c r="E8" s="126"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="136"/>
-      <c r="B9" s="139"/>
+    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="131"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="131"/>
+      <c r="E9" s="126"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="136"/>
-      <c r="B10" s="139"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="131"/>
+      <c r="B10" s="134"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="131"/>
+      <c r="E10" s="126"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="136"/>
-      <c r="B11" s="139"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="131"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="131"/>
+      <c r="E11" s="126"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="140"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="132"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="131"/>
+      <c r="E12" s="126"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="143" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="138">
+      <c r="B13" s="133">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4409,26 +4394,26 @@
       <c r="D13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="126"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="144"/>
-      <c r="B14" s="140"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="139"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="131"/>
+      <c r="E14" s="126"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4441,12 +4426,12 @@
       <c r="D15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="131"/>
+      <c r="E15" s="126"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4459,24 +4444,24 @@
       <c r="D16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="131"/>
+      <c r="E16" s="126"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="132" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="133"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="131"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="126"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4489,12 +4474,12 @@
       <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="131"/>
+      <c r="E18" s="126"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4507,28 +4492,28 @@
       <c r="D19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="131"/>
+      <c r="E19" s="126"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="132" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="133"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="131"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="126"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="145" t="s">
+    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="142">
+      <c r="B21" s="137">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4537,23 +4522,23 @@
       <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="131"/>
+      <c r="E21" s="126"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="146"/>
-      <c r="B22" s="140"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="141"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="131"/>
+      <c r="E22" s="126"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4566,22 +4551,22 @@
       <c r="D23" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="131"/>
+      <c r="E23" s="126"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="132" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="131"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="126"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="141" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="142">
+      <c r="B25" s="137">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4590,110 +4575,110 @@
       <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="131"/>
+      <c r="E25" s="126"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="136"/>
-      <c r="B26" s="139"/>
+    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="131"/>
+      <c r="B26" s="134"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="131"/>
+      <c r="E26" s="126"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="136"/>
-      <c r="B27" s="139"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="131"/>
+      <c r="B27" s="134"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="131"/>
+      <c r="E27" s="126"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="136"/>
-      <c r="B28" s="139"/>
+    <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="131"/>
+      <c r="B28" s="134"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="131"/>
+      <c r="E28" s="126"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="136"/>
-      <c r="B29" s="139"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="131"/>
+      <c r="B29" s="134"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="131"/>
+      <c r="E29" s="126"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="136"/>
-      <c r="B30" s="139"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="131"/>
+      <c r="B30" s="134"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="131"/>
+      <c r="E30" s="126"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="136"/>
-      <c r="B31" s="139"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="131"/>
+      <c r="B31" s="134"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="131"/>
+      <c r="E31" s="126"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="137"/>
-      <c r="B32" s="140"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="132"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="131"/>
+      <c r="E32" s="126"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4706,9 +4691,9 @@
       <c r="D33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="131"/>
+      <c r="E33" s="126"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4721,9 +4706,9 @@
       <c r="D34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="131"/>
+      <c r="E34" s="126"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4736,9 +4721,9 @@
       <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="131"/>
+      <c r="E35" s="126"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4751,9 +4736,9 @@
       <c r="D36" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="131"/>
+      <c r="E36" s="126"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4766,9 +4751,9 @@
       <c r="D37" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="131"/>
+      <c r="E37" s="126"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4781,9 +4766,9 @@
       <c r="D38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="131"/>
+      <c r="E38" s="126"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4796,9 +4781,9 @@
       <c r="D39" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="131"/>
+      <c r="E39" s="126"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4811,18 +4796,18 @@
       <c r="D40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="131"/>
+      <c r="E40" s="126"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="132" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="133"/>
-      <c r="C41" s="133"/>
-      <c r="D41" s="134"/>
-      <c r="E41" s="131"/>
+      <c r="B41" s="128"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="126"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4835,9 +4820,9 @@
       <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="131"/>
+      <c r="E42" s="126"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4850,9 +4835,9 @@
       <c r="D43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="131"/>
+      <c r="E43" s="126"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4865,9 +4850,9 @@
       <c r="D44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="131"/>
+      <c r="E44" s="126"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4880,7 +4865,7 @@
       <c r="D45" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="131"/>
+      <c r="E45" s="126"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -4930,16 +4915,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4956,18 +4941,18 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="158">
+      <c r="E2" s="153">
         <v>43140</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -4978,9 +4963,9 @@
       <c r="D3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="158"/>
+      <c r="E3" s="153"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -4991,9 +4976,9 @@
       <c r="D4" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="158"/>
+      <c r="E4" s="153"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -5004,22 +4989,22 @@
       <c r="D5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="158"/>
+      <c r="E5" s="153"/>
     </row>
-    <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="158"/>
+      <c r="E6" s="153"/>
     </row>
-    <row r="7" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="152" t="s">
+    <row r="7" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5028,68 +5013,68 @@
       <c r="D7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="158"/>
+      <c r="E7" s="153"/>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="152"/>
-      <c r="B8" s="153"/>
+    <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="147"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="158"/>
+      <c r="E8" s="153"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="152"/>
-      <c r="B9" s="153"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="147"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="158"/>
+      <c r="E9" s="153"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
-      <c r="B10" s="153"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="147"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="158"/>
+      <c r="E10" s="153"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="152"/>
-      <c r="B11" s="153"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="147"/>
+      <c r="B11" s="148"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="158"/>
+      <c r="E11" s="153"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
-      <c r="B12" s="153"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="147"/>
+      <c r="B12" s="148"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="158"/>
+      <c r="E12" s="153"/>
     </row>
-    <row r="13" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="155" t="s">
+    <row r="13" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="153" t="s">
+      <c r="B13" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5098,35 +5083,35 @@
       <c r="D13" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="158"/>
+      <c r="E13" s="153"/>
     </row>
-    <row r="14" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
-      <c r="B14" s="153"/>
+    <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="150"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="158"/>
+      <c r="E14" s="153"/>
     </row>
-    <row r="15" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
-      <c r="B15" s="153"/>
+    <row r="15" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="150"/>
+      <c r="B15" s="148"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="158"/>
+      <c r="E15" s="153"/>
     </row>
-    <row r="16" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="150" t="s">
+    <row r="16" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="151" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5135,108 +5120,108 @@
       <c r="D16" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="158"/>
+      <c r="E16" s="153"/>
     </row>
-    <row r="17" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
-      <c r="B17" s="156"/>
+    <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="145"/>
+      <c r="B17" s="151"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="158"/>
+      <c r="E17" s="153"/>
     </row>
-    <row r="18" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="156"/>
+    <row r="18" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="145"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="158"/>
+      <c r="E18" s="153"/>
     </row>
-    <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="150"/>
-      <c r="B19" s="156"/>
+    <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="145"/>
+      <c r="B19" s="151"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="158"/>
+      <c r="E19" s="153"/>
     </row>
-    <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150"/>
-      <c r="B20" s="156"/>
+    <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="145"/>
+      <c r="B20" s="151"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="158"/>
+      <c r="E20" s="153"/>
     </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
-      <c r="B21" s="156"/>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="145"/>
+      <c r="B21" s="151"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="158"/>
+      <c r="E21" s="153"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="156"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="145"/>
+      <c r="B22" s="151"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="158"/>
+      <c r="E22" s="153"/>
     </row>
-    <row r="23" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="156"/>
+    <row r="23" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="145"/>
+      <c r="B23" s="151"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="E23" s="158"/>
+      <c r="E23" s="153"/>
     </row>
-    <row r="24" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
-      <c r="B24" s="156"/>
-      <c r="C24" s="150" t="s">
+    <row r="24" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="145"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="145" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="157" t="s">
+      <c r="D24" s="152" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="158"/>
+      <c r="E24" s="153"/>
     </row>
-    <row r="25" spans="1:5" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
-      <c r="B25" s="156"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="158"/>
+    <row r="25" spans="1:5" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="145"/>
+      <c r="B25" s="151"/>
+      <c r="C25" s="145"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="153"/>
     </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="152" t="s">
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="147" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="153" t="s">
+      <c r="B26" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5245,18 +5230,18 @@
       <c r="D26" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="158"/>
+      <c r="E26" s="153"/>
     </row>
-    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="152"/>
-      <c r="B27" s="153"/>
+    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="147"/>
+      <c r="B27" s="148"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="158"/>
+      <c r="E27" s="153"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -5267,117 +5252,117 @@
       <c r="D28" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="158"/>
+      <c r="E28" s="153"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="158"/>
+      <c r="E29" s="153"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="154" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="153" t="s">
+      <c r="B30" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="150" t="s">
+      <c r="C30" s="145" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="151" t="s">
+      <c r="D30" s="146" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="158"/>
+      <c r="E30" s="153"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="154"/>
-      <c r="B31" s="153"/>
-      <c r="C31" s="150"/>
-      <c r="D31" s="151"/>
-      <c r="E31" s="158"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="149"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="145"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="153"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="154"/>
-      <c r="B32" s="153"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="149"/>
+      <c r="B32" s="148"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="158"/>
+      <c r="E32" s="153"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="154"/>
-      <c r="B33" s="153"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="149"/>
+      <c r="B33" s="148"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="158"/>
+      <c r="E33" s="153"/>
     </row>
-    <row r="34" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="154"/>
-      <c r="B34" s="153"/>
+    <row r="34" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="149"/>
+      <c r="B34" s="148"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="158"/>
+      <c r="E34" s="153"/>
     </row>
-    <row r="35" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="154"/>
-      <c r="B35" s="153"/>
+    <row r="35" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="149"/>
+      <c r="B35" s="148"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="158"/>
+      <c r="E35" s="153"/>
     </row>
-    <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="154"/>
-      <c r="B36" s="153"/>
+    <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="149"/>
+      <c r="B36" s="148"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
       <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="158"/>
+      <c r="E36" s="153"/>
     </row>
-    <row r="37" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="154"/>
-      <c r="B37" s="153"/>
-      <c r="C37" s="147" t="s">
+    <row r="37" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="149"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="142" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="149" t="s">
+      <c r="D37" s="144" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="158"/>
+      <c r="E37" s="153"/>
     </row>
-    <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="154"/>
-      <c r="B38" s="153"/>
-      <c r="C38" s="148"/>
-      <c r="D38" s="149"/>
-      <c r="E38" s="158"/>
+    <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="149"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="153"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="152" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B39" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5386,18 +5371,18 @@
       <c r="D39" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="158"/>
+      <c r="E39" s="153"/>
     </row>
-    <row r="40" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="152"/>
-      <c r="B40" s="153"/>
+    <row r="40" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="147"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="158"/>
+      <c r="E40" s="153"/>
     </row>
-    <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -5408,99 +5393,99 @@
       <c r="D41" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="158"/>
+      <c r="E41" s="153"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="158"/>
+      <c r="E42" s="153"/>
     </row>
-    <row r="43" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="154" t="s">
+    <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="153" t="s">
+      <c r="B43" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="158"/>
+      <c r="E43" s="153"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="154"/>
-      <c r="B44" s="153"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="149"/>
+      <c r="B44" s="148"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D44" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="158"/>
+      <c r="E44" s="153"/>
     </row>
-    <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="163" t="s">
+    <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="158" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="153" t="s">
+      <c r="B45" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="158"/>
+      <c r="E45" s="153"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="164"/>
-      <c r="B46" s="153"/>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="159"/>
+      <c r="B46" s="148"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="158"/>
+      <c r="E46" s="153"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="164"/>
-      <c r="B47" s="153"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="159"/>
+      <c r="B47" s="148"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="158"/>
+      <c r="E47" s="153"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="165"/>
-      <c r="B48" s="153"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="160"/>
+      <c r="B48" s="148"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="158"/>
+      <c r="E48" s="153"/>
     </row>
-    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A49" s="156" t="s">
+    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A49" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="156" t="s">
+      <c r="B49" s="151" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="158"/>
+      <c r="E49" s="153"/>
       <c r="H49" s="42"/>
       <c r="L49" s="42"/>
       <c r="P49" s="42"/>
@@ -9597,16 +9582,16 @@
       <c r="XEZ49" s="42"/>
       <c r="XFD49" s="42"/>
     </row>
-    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="156"/>
-      <c r="B50" s="156"/>
+    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="151"/>
+      <c r="B50" s="151"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="158"/>
+      <c r="E50" s="153"/>
       <c r="H50" s="42"/>
       <c r="L50" s="42"/>
       <c r="P50" s="42"/>
@@ -13703,16 +13688,16 @@
       <c r="XEZ50" s="42"/>
       <c r="XFD50" s="42"/>
     </row>
-    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A51" s="156"/>
-      <c r="B51" s="156"/>
+    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A51" s="151"/>
+      <c r="B51" s="151"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="E51" s="158"/>
+      <c r="E51" s="153"/>
       <c r="H51" s="42"/>
       <c r="L51" s="42"/>
       <c r="P51" s="42"/>
@@ -17809,16 +17794,16 @@
       <c r="XEZ51" s="42"/>
       <c r="XFD51" s="42"/>
     </row>
-    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A52" s="156"/>
-      <c r="B52" s="156"/>
+    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A52" s="151"/>
+      <c r="B52" s="151"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="158"/>
+      <c r="E52" s="153"/>
       <c r="H52" s="42"/>
       <c r="L52" s="42"/>
       <c r="P52" s="42"/>
@@ -21915,16 +21900,16 @@
       <c r="XEZ52" s="42"/>
       <c r="XFD52" s="42"/>
     </row>
-    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A53" s="156"/>
-      <c r="B53" s="156"/>
-      <c r="C53" s="160" t="s">
+    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A53" s="151"/>
+      <c r="B53" s="151"/>
+      <c r="C53" s="155" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="151" t="s">
+      <c r="D53" s="146" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="158"/>
+      <c r="E53" s="153"/>
       <c r="H53" s="42"/>
       <c r="L53" s="42"/>
       <c r="P53" s="42"/>
@@ -26021,12 +26006,12 @@
       <c r="XEZ53" s="42"/>
       <c r="XFD53" s="42"/>
     </row>
-    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="156"/>
-      <c r="B54" s="156"/>
-      <c r="C54" s="160"/>
-      <c r="D54" s="151"/>
-      <c r="E54" s="158"/>
+    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="151"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="155"/>
+      <c r="D54" s="146"/>
+      <c r="E54" s="153"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -30123,16 +30108,16 @@
       <c r="XEZ54" s="42"/>
       <c r="XFD54" s="42"/>
     </row>
-    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
-      <c r="E55" s="158"/>
+      <c r="E55" s="153"/>
     </row>
-    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -30143,13 +30128,13 @@
       <c r="D56" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="158"/>
+      <c r="E56" s="153"/>
     </row>
-    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A57" s="161" t="s">
+    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A57" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="156" t="s">
+      <c r="B57" s="151" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30158,221 +30143,221 @@
       <c r="D57" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="158"/>
+      <c r="E57" s="153"/>
     </row>
-    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="161"/>
-      <c r="B58" s="156"/>
+    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="156"/>
+      <c r="B58" s="151"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="E58" s="158"/>
+      <c r="E58" s="153"/>
     </row>
-    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A59" s="161"/>
-      <c r="B59" s="156"/>
+    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A59" s="156"/>
+      <c r="B59" s="151"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D59" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="158"/>
+      <c r="E59" s="153"/>
     </row>
-    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="161"/>
-      <c r="B60" s="156"/>
+    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="156"/>
+      <c r="B60" s="151"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D60" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="158"/>
+      <c r="E60" s="153"/>
     </row>
-    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A61" s="161"/>
-      <c r="B61" s="156"/>
+    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A61" s="156"/>
+      <c r="B61" s="151"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="158"/>
+      <c r="E61" s="153"/>
     </row>
-    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A62" s="161"/>
-      <c r="B62" s="156"/>
+    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A62" s="156"/>
+      <c r="B62" s="151"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="158"/>
+      <c r="E62" s="153"/>
     </row>
-    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A63" s="161"/>
-      <c r="B63" s="156"/>
+    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A63" s="156"/>
+      <c r="B63" s="151"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D63" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="158"/>
+      <c r="E63" s="153"/>
     </row>
-    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A64" s="161"/>
-      <c r="B64" s="156"/>
+    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A64" s="156"/>
+      <c r="B64" s="151"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="158"/>
+      <c r="E64" s="153"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="161"/>
-      <c r="B65" s="156"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="156"/>
+      <c r="B65" s="151"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="158"/>
+      <c r="E65" s="153"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="161"/>
-      <c r="B66" s="156"/>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="156"/>
+      <c r="B66" s="151"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="158"/>
+      <c r="E66" s="153"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="161"/>
-      <c r="B67" s="156"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="156"/>
+      <c r="B67" s="151"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E67" s="158"/>
+      <c r="E67" s="153"/>
     </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="161"/>
-      <c r="B68" s="156"/>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="156"/>
+      <c r="B68" s="151"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="158"/>
+      <c r="E68" s="153"/>
     </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="161"/>
-      <c r="B69" s="156"/>
+    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="156"/>
+      <c r="B69" s="151"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E69" s="158"/>
+      <c r="E69" s="153"/>
     </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="161"/>
-      <c r="B70" s="156"/>
+    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="156"/>
+      <c r="B70" s="151"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="158"/>
+      <c r="E70" s="153"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="161"/>
-      <c r="B71" s="156"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="156"/>
+      <c r="B71" s="151"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="158"/>
+      <c r="E71" s="153"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="161"/>
-      <c r="B72" s="156"/>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="156"/>
+      <c r="B72" s="151"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="158"/>
+      <c r="E72" s="153"/>
     </row>
-    <row r="73" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="161"/>
-      <c r="B73" s="156"/>
+    <row r="73" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="156"/>
+      <c r="B73" s="151"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="158"/>
+      <c r="E73" s="153"/>
     </row>
-    <row r="74" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="161"/>
-      <c r="B74" s="156"/>
+    <row r="74" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="156"/>
+      <c r="B74" s="151"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="E74" s="158"/>
+      <c r="E74" s="153"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="161"/>
-      <c r="B75" s="156"/>
-      <c r="C75" s="159"/>
-      <c r="D75" s="162" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="156"/>
+      <c r="B75" s="151"/>
+      <c r="C75" s="154"/>
+      <c r="D75" s="157" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="158"/>
+      <c r="E75" s="153"/>
     </row>
-    <row r="76" spans="1:5" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="161"/>
-      <c r="B76" s="156"/>
-      <c r="C76" s="159"/>
-      <c r="D76" s="162"/>
-      <c r="E76" s="158"/>
+    <row r="76" spans="1:5" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="156"/>
+      <c r="B76" s="151"/>
+      <c r="C76" s="154"/>
+      <c r="D76" s="157"/>
+      <c r="E76" s="153"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
-      <c r="E77" s="158"/>
+      <c r="E77" s="153"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -30442,16 +30427,16 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
-    <col min="4" max="4" width="80.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30468,31 +30453,31 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="131">
+      <c r="E2" s="126">
         <v>43179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="131"/>
+      <c r="E3" s="126"/>
     </row>
-    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="152" t="s">
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30501,160 +30486,160 @@
       <c r="D4" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="131"/>
+      <c r="E4" s="126"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="181" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="147"/>
+      <c r="B5" s="148"/>
+      <c r="C5" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="180" t="s">
+      <c r="D5" s="175" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="131"/>
+      <c r="E5" s="126"/>
     </row>
-    <row r="6" spans="1:5" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="152"/>
-      <c r="B6" s="153"/>
-      <c r="C6" s="181"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="131"/>
+    <row r="6" spans="1:5" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="147"/>
+      <c r="B6" s="148"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="175"/>
+      <c r="E6" s="126"/>
     </row>
-    <row r="7" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="152"/>
-      <c r="B7" s="153"/>
+    <row r="7" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="147"/>
+      <c r="B7" s="148"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
-      <c r="E7" s="131"/>
+      <c r="E7" s="126"/>
     </row>
-    <row r="8" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="152"/>
-      <c r="B8" s="153"/>
+    <row r="8" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="147"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
-      <c r="E8" s="131"/>
+      <c r="E8" s="126"/>
     </row>
-    <row r="9" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="152"/>
-      <c r="B9" s="153"/>
+    <row r="9" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="147"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
-      <c r="E9" s="131"/>
+      <c r="E9" s="126"/>
     </row>
-    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="155" t="s">
+    <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="172"/>
-      <c r="D10" s="180" t="s">
+      <c r="C10" s="167"/>
+      <c r="D10" s="175" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="131"/>
+      <c r="E10" s="126"/>
     </row>
-    <row r="11" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="155"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="172"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="131"/>
+    <row r="11" spans="1:5" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="150"/>
+      <c r="B11" s="148"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="126"/>
     </row>
-    <row r="12" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="155"/>
-      <c r="B12" s="153"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="180"/>
-      <c r="E12" s="131"/>
+    <row r="12" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="150"/>
+      <c r="B12" s="148"/>
+      <c r="C12" s="167"/>
+      <c r="D12" s="175"/>
+      <c r="E12" s="126"/>
     </row>
-    <row r="13" spans="1:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="150" t="s">
+    <row r="13" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="151" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="182"/>
-      <c r="D13" s="180" t="s">
+      <c r="C13" s="177"/>
+      <c r="D13" s="175" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="126"/>
     </row>
-    <row r="14" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="150"/>
-      <c r="B14" s="156"/>
-      <c r="C14" s="182"/>
-      <c r="D14" s="180"/>
-      <c r="E14" s="131"/>
+    <row r="14" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="145"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="177"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="126"/>
     </row>
-    <row r="15" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
-      <c r="B15" s="156"/>
-      <c r="C15" s="182"/>
+    <row r="15" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="145"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="177"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="131"/>
+      <c r="E15" s="126"/>
     </row>
-    <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="150"/>
-      <c r="B16" s="156"/>
-      <c r="C16" s="182"/>
+    <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="145"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="177"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="131"/>
+      <c r="E16" s="126"/>
     </row>
-    <row r="17" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
-      <c r="B17" s="156"/>
-      <c r="C17" s="182"/>
+    <row r="17" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="145"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="177"/>
       <c r="D17" s="49"/>
-      <c r="E17" s="131"/>
+      <c r="E17" s="126"/>
     </row>
-    <row r="18" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="156"/>
-      <c r="C18" s="182"/>
+    <row r="18" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="145"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="177"/>
       <c r="D18" s="49"/>
-      <c r="E18" s="131"/>
+      <c r="E18" s="126"/>
     </row>
-    <row r="19" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="150"/>
-      <c r="B19" s="156"/>
-      <c r="C19" s="182"/>
+    <row r="19" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="145"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="177"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="131"/>
+      <c r="E19" s="126"/>
     </row>
-    <row r="20" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150"/>
-      <c r="B20" s="156"/>
-      <c r="C20" s="182"/>
+    <row r="20" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="145"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="177"/>
       <c r="D20" s="49"/>
-      <c r="E20" s="131"/>
+      <c r="E20" s="126"/>
     </row>
-    <row r="21" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
-      <c r="B21" s="156"/>
-      <c r="C21" s="182"/>
+    <row r="21" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="145"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="177"/>
       <c r="D21" s="49"/>
-      <c r="E21" s="131"/>
+      <c r="E21" s="126"/>
     </row>
-    <row r="22" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="156"/>
-      <c r="C22" s="182"/>
+    <row r="22" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="145"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="177"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="131"/>
+      <c r="E22" s="126"/>
     </row>
-    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="156"/>
-      <c r="C23" s="182"/>
+    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="145"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="177"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="131"/>
+      <c r="E23" s="126"/>
     </row>
-    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
@@ -30667,9 +30652,9 @@
       <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="131"/>
+      <c r="E24" s="126"/>
     </row>
-    <row r="25" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30682,9 +30667,9 @@
       <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="E25" s="131"/>
+      <c r="E25" s="126"/>
     </row>
-    <row r="26" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30695,18 +30680,18 @@
       <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="131"/>
+      <c r="E26" s="126"/>
     </row>
-    <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="131"/>
+      <c r="E27" s="126"/>
     </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30719,9 +30704,9 @@
       <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="131"/>
+      <c r="E28" s="126"/>
     </row>
-    <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="85"/>
       <c r="B29" s="84"/>
       <c r="C29" s="70" t="s">
@@ -30730,9 +30715,9 @@
       <c r="D29" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="131"/>
+      <c r="E29" s="126"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30741,9 +30726,9 @@
       <c r="D30" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="E30" s="131"/>
+      <c r="E30" s="126"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30752,13 +30737,13 @@
       <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="131"/>
+      <c r="E31" s="126"/>
     </row>
-    <row r="32" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="166" t="s">
+    <row r="32" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="161" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="169" t="s">
+      <c r="B32" s="164" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30767,41 +30752,41 @@
       <c r="D32" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="E32" s="131"/>
+      <c r="E32" s="126"/>
     </row>
-    <row r="33" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="167"/>
-      <c r="B33" s="170"/>
+    <row r="33" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="162"/>
+      <c r="B33" s="165"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
-      <c r="E33" s="131"/>
+      <c r="E33" s="126"/>
     </row>
-    <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="167"/>
-      <c r="B34" s="170"/>
+    <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="162"/>
+      <c r="B34" s="165"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
-      <c r="E34" s="131"/>
+      <c r="E34" s="126"/>
     </row>
-    <row r="35" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="167"/>
-      <c r="B35" s="170"/>
+    <row r="35" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="162"/>
+      <c r="B35" s="165"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
-      <c r="E35" s="131"/>
+      <c r="E35" s="126"/>
     </row>
-    <row r="36" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="168"/>
-      <c r="B36" s="171"/>
+    <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="163"/>
+      <c r="B36" s="166"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="131"/>
+      <c r="E36" s="126"/>
     </row>
-    <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
         <v>27</v>
       </c>
@@ -30812,22 +30797,22 @@
       <c r="D37" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="131"/>
+      <c r="E37" s="126"/>
     </row>
-    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
-      <c r="E38" s="131"/>
+      <c r="E38" s="126"/>
     </row>
-    <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="154" t="s">
+    <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B39" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30836,119 +30821,119 @@
       <c r="D39" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="E39" s="131"/>
+      <c r="E39" s="126"/>
     </row>
-    <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="154"/>
-      <c r="B40" s="153"/>
+    <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="149"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="131"/>
+      <c r="E40" s="126"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="152" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="153" t="s">
+      <c r="B41" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="172" t="s">
+      <c r="C41" s="167" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="150" t="s">
+      <c r="D41" s="145" t="s">
         <v>228</v>
       </c>
-      <c r="E41" s="131"/>
+      <c r="E41" s="126"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="152"/>
-      <c r="B42" s="153"/>
-      <c r="C42" s="172"/>
-      <c r="D42" s="150"/>
-      <c r="E42" s="131"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="147"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="167"/>
+      <c r="D42" s="145"/>
+      <c r="E42" s="126"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="152"/>
-      <c r="B43" s="153"/>
-      <c r="C43" s="172" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="147"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="167" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="162" t="s">
+      <c r="D43" s="157" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="131"/>
+      <c r="E43" s="126"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="152"/>
-      <c r="B44" s="153"/>
-      <c r="C44" s="172"/>
-      <c r="D44" s="162"/>
-      <c r="E44" s="131"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="147"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="167"/>
+      <c r="D44" s="157"/>
+      <c r="E44" s="126"/>
     </row>
-    <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="161" t="s">
+    <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="151" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="176"/>
+      <c r="C45" s="171"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="131"/>
+      <c r="E45" s="126"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="161"/>
-      <c r="B46" s="156"/>
-      <c r="C46" s="177"/>
-      <c r="D46" s="173" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="156"/>
+      <c r="B46" s="151"/>
+      <c r="C46" s="172"/>
+      <c r="D46" s="168" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="131"/>
+      <c r="E46" s="126"/>
     </row>
-    <row r="47" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="161"/>
-      <c r="B47" s="156"/>
-      <c r="C47" s="177"/>
-      <c r="D47" s="174"/>
-      <c r="E47" s="131"/>
+    <row r="47" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="156"/>
+      <c r="B47" s="151"/>
+      <c r="C47" s="172"/>
+      <c r="D47" s="169"/>
+      <c r="E47" s="126"/>
     </row>
-    <row r="48" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="161"/>
-      <c r="B48" s="156"/>
-      <c r="C48" s="178"/>
-      <c r="D48" s="174"/>
-      <c r="E48" s="131"/>
+    <row r="48" spans="1:5" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="156"/>
+      <c r="B48" s="151"/>
+      <c r="C48" s="173"/>
+      <c r="D48" s="169"/>
+      <c r="E48" s="126"/>
     </row>
-    <row r="49" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="161"/>
-      <c r="B49" s="156"/>
-      <c r="C49" s="160"/>
-      <c r="D49" s="174"/>
-      <c r="E49" s="131"/>
+    <row r="49" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="156"/>
+      <c r="B49" s="151"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="169"/>
+      <c r="E49" s="126"/>
     </row>
-    <row r="50" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="161"/>
-      <c r="B50" s="156"/>
-      <c r="C50" s="160"/>
-      <c r="D50" s="175"/>
-      <c r="E50" s="131"/>
+    <row r="50" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="156"/>
+      <c r="B50" s="151"/>
+      <c r="C50" s="155"/>
+      <c r="D50" s="170"/>
+      <c r="E50" s="126"/>
     </row>
-    <row r="51" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
-      <c r="E51" s="131"/>
+      <c r="E51" s="126"/>
     </row>
-    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
@@ -30959,13 +30944,13 @@
       <c r="D52" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="131"/>
+      <c r="E52" s="126"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="156" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="156" t="s">
+      <c r="B53" s="151" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30974,191 +30959,191 @@
       <c r="D53" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="131"/>
+      <c r="E53" s="126"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="156"/>
-      <c r="B54" s="156"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="151"/>
+      <c r="B54" s="151"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
       <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="131"/>
+      <c r="E54" s="126"/>
     </row>
-    <row r="55" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="156"/>
-      <c r="B55" s="156"/>
+    <row r="55" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="151"/>
+      <c r="B55" s="151"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="131"/>
+      <c r="E55" s="126"/>
     </row>
-    <row r="56" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="156"/>
-      <c r="B56" s="156"/>
-      <c r="C56" s="179" t="s">
+    <row r="56" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="151"/>
+      <c r="B56" s="151"/>
+      <c r="C56" s="174" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="E56" s="131"/>
+      <c r="E56" s="126"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="156"/>
-      <c r="B57" s="156"/>
-      <c r="C57" s="179"/>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="151"/>
+      <c r="B57" s="151"/>
+      <c r="C57" s="174"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="131"/>
+      <c r="E57" s="126"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="156"/>
-      <c r="B58" s="156"/>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="151"/>
+      <c r="B58" s="151"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
       <c r="D58" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E58" s="131"/>
+      <c r="E58" s="126"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="156"/>
-      <c r="B59" s="156"/>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="151"/>
+      <c r="B59" s="151"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
       <c r="D59" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="131"/>
+      <c r="E59" s="126"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="156"/>
-      <c r="B60" s="156"/>
-      <c r="C60" s="179" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="151"/>
+      <c r="B60" s="151"/>
+      <c r="C60" s="174" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="131"/>
+      <c r="E60" s="126"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="156"/>
-      <c r="B61" s="156"/>
-      <c r="C61" s="179"/>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="151"/>
+      <c r="B61" s="151"/>
+      <c r="C61" s="174"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="131"/>
+      <c r="E61" s="126"/>
     </row>
-    <row r="62" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="156"/>
-      <c r="B62" s="156"/>
-      <c r="C62" s="179"/>
+    <row r="62" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="151"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="174"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="E62" s="131"/>
+      <c r="E62" s="126"/>
     </row>
-    <row r="63" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="156"/>
-      <c r="B63" s="156"/>
-      <c r="C63" s="172" t="s">
+    <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="151"/>
+      <c r="B63" s="151"/>
+      <c r="C63" s="167" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="E63" s="131"/>
+      <c r="E63" s="126"/>
     </row>
-    <row r="64" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="156"/>
-      <c r="B64" s="156"/>
-      <c r="C64" s="172"/>
-      <c r="D64" s="162" t="s">
+    <row r="64" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="151"/>
+      <c r="B64" s="151"/>
+      <c r="C64" s="167"/>
+      <c r="D64" s="157" t="s">
         <v>220</v>
       </c>
-      <c r="E64" s="131"/>
+      <c r="E64" s="126"/>
     </row>
-    <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="156"/>
-      <c r="B65" s="156"/>
-      <c r="C65" s="172"/>
-      <c r="D65" s="162"/>
-      <c r="E65" s="131"/>
+    <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="151"/>
+      <c r="B65" s="151"/>
+      <c r="C65" s="167"/>
+      <c r="D65" s="157"/>
+      <c r="E65" s="126"/>
     </row>
-    <row r="66" spans="1:5" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="156"/>
-      <c r="B66" s="156"/>
-      <c r="C66" s="172"/>
-      <c r="D66" s="162"/>
-      <c r="E66" s="131"/>
+    <row r="66" spans="1:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="151"/>
+      <c r="B66" s="151"/>
+      <c r="C66" s="167"/>
+      <c r="D66" s="157"/>
+      <c r="E66" s="126"/>
     </row>
-    <row r="67" spans="1:5" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="156"/>
-      <c r="B67" s="156"/>
-      <c r="C67" s="172"/>
-      <c r="D67" s="162"/>
-      <c r="E67" s="131"/>
+    <row r="67" spans="1:5" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="151"/>
+      <c r="B67" s="151"/>
+      <c r="C67" s="167"/>
+      <c r="D67" s="157"/>
+      <c r="E67" s="126"/>
     </row>
-    <row r="68" spans="1:5" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
-      <c r="E68" s="131"/>
+      <c r="E68" s="126"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -31209,20 +31194,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -31232,647 +31217,648 @@
       <c r="C1" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="105" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
-      <c r="D2" s="117"/>
+      <c r="D2" s="106"/>
       <c r="E2" s="58"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="150" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="174" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="58"/>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="107" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="128">
+      <c r="E3" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="150"/>
-      <c r="B4" s="179"/>
-      <c r="C4" s="101" t="s">
+    <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="145"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="124" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="108" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="127">
+      <c r="E4" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="179"/>
-      <c r="C5" s="101" t="s">
+      <c r="B5" s="174"/>
+      <c r="C5" s="124" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="109" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="127">
+      <c r="E5" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="179"/>
-      <c r="C6" s="101" t="s">
+      <c r="B6" s="174"/>
+      <c r="C6" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="127">
+      <c r="E6" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="190" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="185" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="179"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="58"/>
-      <c r="D7" s="121" t="s">
+      <c r="D7" s="110" t="s">
         <v>261</v>
       </c>
-      <c r="E7" s="128">
+      <c r="E7" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="191"/>
-      <c r="B8" s="179"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="186"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="58"/>
-      <c r="D8" s="118" t="s">
+      <c r="D8" s="107" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="128">
+      <c r="E8" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="179"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="58"/>
-      <c r="D9" s="120" t="s">
+      <c r="D9" s="109" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="127">
+      <c r="E9" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="122"/>
+      <c r="D10" s="111"/>
       <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="187" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="182" t="s">
         <v>237</v>
       </c>
-      <c r="B11" s="179" t="s">
+      <c r="B11" s="174" t="s">
         <v>234</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" t="s">
         <v>258</v>
       </c>
-      <c r="E11" s="128">
+      <c r="E11" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="188"/>
-      <c r="B12" s="179"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="183"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="58"/>
-      <c r="D12" s="118" t="s">
+      <c r="D12" s="107" t="s">
         <v>252</v>
       </c>
-      <c r="E12" s="127">
+      <c r="E12" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="189"/>
-      <c r="B13" s="179"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="184"/>
+      <c r="B13" s="174"/>
       <c r="C13" s="58"/>
-      <c r="D13" s="118" t="s">
+      <c r="D13" s="107" t="s">
         <v>254</v>
       </c>
-      <c r="E13" s="127">
+      <c r="E13" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="96" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="120" t="s">
         <v>234</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="118" t="s">
+      <c r="D14" s="107" t="s">
         <v>238</v>
       </c>
-      <c r="E14" s="128">
+      <c r="E14" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="179" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="174" t="s">
         <v>222</v>
       </c>
-      <c r="B15" s="179" t="s">
+      <c r="B15" s="174" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="198" t="s">
+      <c r="C15" s="193" t="s">
         <v>239</v>
       </c>
-      <c r="D15" s="123" t="s">
+      <c r="D15" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="E15" s="127">
+      <c r="E15" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="179"/>
-      <c r="B16" s="179"/>
-      <c r="C16" s="199"/>
-      <c r="D16" s="113" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="174"/>
+      <c r="B16" s="174"/>
+      <c r="C16" s="194"/>
+      <c r="D16" s="104" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="128">
+      <c r="E16" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="179"/>
-      <c r="B17" s="179"/>
-      <c r="C17" s="99" t="s">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="174"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="96" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="124" t="s">
+      <c r="D17" s="113" t="s">
         <v>242</v>
       </c>
-      <c r="E17" s="127">
+      <c r="E17" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="110" t="s">
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="121" t="s">
         <v>280</v>
       </c>
       <c r="B18" s="58"/>
       <c r="C18" s="61" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="118" t="s">
+      <c r="D18" s="107" t="s">
         <v>281</v>
       </c>
-      <c r="E18" s="128">
+      <c r="E18" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
-      <c r="D19" s="117"/>
+      <c r="D19" s="106"/>
       <c r="E19" s="58"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="190" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="185" t="s">
         <v>260</v>
       </c>
-      <c r="B20" s="179" t="s">
+      <c r="B20" s="174" t="s">
         <v>234</v>
       </c>
       <c r="C20" s="58"/>
-      <c r="D20" s="121" t="s">
+      <c r="D20" s="110" t="s">
         <v>261</v>
       </c>
-      <c r="E20" s="128">
+      <c r="E20" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="191"/>
-      <c r="B21" s="179"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="186"/>
+      <c r="B21" s="174"/>
       <c r="C21" s="58"/>
-      <c r="D21" s="118" t="s">
+      <c r="D21" s="107" t="s">
         <v>257</v>
       </c>
-      <c r="E21" s="128">
+      <c r="E21" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="102" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="98" t="s">
         <v>243</v>
       </c>
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="120" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="97" t="s">
+      <c r="C22" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="125" t="s">
+      <c r="D22" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="127">
+      <c r="E22" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="192" t="s">
+    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="185" t="s">
+      <c r="B23" s="180" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="D23" s="118" t="s">
+      <c r="D23" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="E23" s="127">
+      <c r="E23" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="193"/>
-      <c r="B24" s="195"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="188"/>
+      <c r="B24" s="190"/>
       <c r="C24" t="s">
         <v>270</v>
       </c>
-      <c r="D24" s="118" t="s">
+      <c r="D24" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="E24" s="128">
+      <c r="E24" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="193"/>
-      <c r="B25" s="195"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="188"/>
+      <c r="B25" s="190"/>
       <c r="C25" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="D25" s="118" t="s">
+      <c r="D25" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="E25" s="128">
+      <c r="E25" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="193"/>
-      <c r="B26" s="195"/>
-      <c r="C26" s="112" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="188"/>
+      <c r="B26" s="190"/>
+      <c r="C26" s="103" t="s">
         <v>277</v>
       </c>
-      <c r="D26" s="113" t="s">
+      <c r="D26" s="104" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="130">
+      <c r="E26" s="125">
         <v>43270</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="193"/>
-      <c r="B27" s="195"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="188"/>
+      <c r="B27" s="190"/>
       <c r="C27" s="58" t="s">
         <v>284</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="E27" s="127">
+      <c r="E27" s="116">
         <v>43279</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="193"/>
-      <c r="B28" s="195"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="188"/>
+      <c r="B28" s="190"/>
       <c r="C28" s="58" t="s">
         <v>285</v>
       </c>
       <c r="D28" s="58" t="s">
         <v>286</v>
       </c>
-      <c r="E28" s="127">
+      <c r="E28" s="116">
         <v>43279</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="194"/>
-      <c r="B29" s="186"/>
-      <c r="C29" s="98" t="s">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="189"/>
+      <c r="B29" s="181"/>
+      <c r="C29" s="95" t="s">
         <v>244</v>
       </c>
-      <c r="D29" s="125" t="s">
+      <c r="D29" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="E29" s="127">
+      <c r="E29" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
-      <c r="D30" s="117"/>
+      <c r="D30" s="106"/>
       <c r="E30" s="58"/>
     </row>
-    <row r="31" spans="1:5" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
+    <row r="31" spans="1:5" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="102"/>
       <c r="B31" s="67"/>
       <c r="C31" s="58"/>
-      <c r="D31" s="121" t="s">
+      <c r="D31" s="110" t="s">
         <v>261</v>
       </c>
       <c r="E31" s="58"/>
     </row>
-    <row r="32" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="150" t="s">
+    <row r="32" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="179" t="s">
+      <c r="B32" s="174" t="s">
         <v>234</v>
       </c>
-      <c r="C32" s="107" t="s">
+      <c r="C32" s="124" t="s">
         <v>246</v>
       </c>
-      <c r="D32" s="118" t="s">
+      <c r="D32" s="107" t="s">
         <v>253</v>
       </c>
-      <c r="E32" s="127">
+      <c r="E32" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="150"/>
-      <c r="B33" s="179"/>
-      <c r="C33" s="107">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="145"/>
+      <c r="B33" s="174"/>
+      <c r="C33" s="124">
         <v>10.1</v>
       </c>
-      <c r="D33" s="118" t="s">
+      <c r="D33" s="107" t="s">
         <v>272</v>
       </c>
-      <c r="E33" s="127">
+      <c r="E33" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="150"/>
-      <c r="B34" s="179"/>
-      <c r="C34" s="107">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="145"/>
+      <c r="B34" s="174"/>
+      <c r="C34" s="124">
         <v>10.199999999999999</v>
       </c>
-      <c r="D34" s="118" t="s">
+      <c r="D34" s="107" t="s">
         <v>272</v>
       </c>
-      <c r="E34" s="127">
+      <c r="E34" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="150" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="145" t="s">
         <v>247</v>
       </c>
-      <c r="B35" s="179" t="s">
+      <c r="B35" s="174" t="s">
         <v>234</v>
       </c>
-      <c r="C35" s="179"/>
-      <c r="D35" s="200" t="s">
+      <c r="C35" s="174"/>
+      <c r="D35" s="195" t="s">
         <v>261</v>
       </c>
-      <c r="E35" s="196">
+      <c r="E35" s="191">
         <v>43270</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="150"/>
-      <c r="B36" s="179"/>
-      <c r="C36" s="179"/>
-      <c r="D36" s="200"/>
-      <c r="E36" s="197"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="145"/>
+      <c r="B36" s="174"/>
+      <c r="C36" s="174"/>
+      <c r="D36" s="195"/>
+      <c r="E36" s="192"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="106" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="123" t="s">
         <v>262</v>
       </c>
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="107" t="s">
+      <c r="C37" s="124" t="s">
         <v>250</v>
       </c>
-      <c r="D37" s="126" t="s">
+      <c r="D37" s="115" t="s">
         <v>251</v>
       </c>
-      <c r="E37" s="127">
+      <c r="E37" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="100" t="s">
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="97" t="s">
         <v>248</v>
       </c>
       <c r="B38" s="39"/>
-      <c r="C38" s="105"/>
-      <c r="D38" s="115"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="119"/>
       <c r="E38" s="58"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="104" t="s">
+      <c r="C39" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="D39" s="118" t="s">
+      <c r="D39" s="107" t="s">
         <v>267</v>
       </c>
-      <c r="E39" s="127">
+      <c r="E39" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A40" s="58" t="s">
         <v>287</v>
       </c>
-      <c r="B40" s="129" t="s">
+      <c r="B40" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C40" s="104" t="s">
+      <c r="C40" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="D40" s="118" t="s">
+      <c r="D40" s="107" t="s">
         <v>289</v>
       </c>
-      <c r="E40" s="127">
+      <c r="E40" s="116">
         <v>43280</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="108" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="108"/>
-      <c r="C41" s="108"/>
-      <c r="D41" s="114"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="118"/>
       <c r="E41" s="58"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="183" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="178" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="185" t="s">
+      <c r="B42" s="180" t="s">
         <v>271</v>
       </c>
-      <c r="C42" s="104" t="s">
+      <c r="C42" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="D42" s="118" t="s">
+      <c r="D42" s="107" t="s">
         <v>267</v>
       </c>
-      <c r="E42" s="127">
+      <c r="E42" s="116">
         <v>43259</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
-      <c r="B43" s="186"/>
-      <c r="C43" s="104" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="179"/>
+      <c r="B43" s="181"/>
+      <c r="C43" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="D43" s="118" t="s">
+      <c r="D43" s="107" t="s">
         <v>266</v>
       </c>
-      <c r="E43" s="127">
+      <c r="E43" s="116">
         <v>43259</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="103" t="s">
+    <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="107" t="s">
+      <c r="B44" s="124" t="s">
         <v>271</v>
       </c>
       <c r="C44" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D44" s="118" t="s">
+      <c r="D44" s="107" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="127">
+      <c r="E44" s="116">
         <v>43259</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="103" t="s">
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="124" t="s">
         <v>271</v>
       </c>
       <c r="C45" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D45" s="118" t="s">
+      <c r="D45" s="107" t="s">
         <v>263</v>
       </c>
-      <c r="E45" s="127">
+      <c r="E45" s="116">
         <v>43259</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="108" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="101" t="s">
         <v>273</v>
       </c>
-      <c r="B46" s="108"/>
-      <c r="C46" s="108"/>
-      <c r="D46" s="114"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="118"/>
       <c r="E46" s="58"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="58"/>
-      <c r="B47" s="107" t="s">
+      <c r="B47" s="124" t="s">
         <v>234</v>
       </c>
       <c r="C47" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="126" t="s">
+      <c r="D47" s="115" t="s">
         <v>274</v>
       </c>
-      <c r="E47" s="127">
+      <c r="E47" s="116">
         <v>43265</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="108" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="B48" s="108"/>
-      <c r="C48" s="108"/>
-      <c r="D48" s="114"/>
+      <c r="B48" s="101"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="118"/>
       <c r="E48" s="58"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="58"/>
-      <c r="B49" s="111" t="s">
+      <c r="B49" s="124" t="s">
         <v>234</v>
       </c>
       <c r="C49" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="126" t="s">
+      <c r="D49" s="115" t="s">
         <v>274</v>
       </c>
-      <c r="E49" s="128">
+      <c r="E49" s="117">
         <v>43270</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B42:B43"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C35:C36"/>
@@ -31880,8 +31866,6 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A11:A13"/>
@@ -31894,6 +31878,7 @@
     <mergeCell ref="B23:B29"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"SOAP lookup by range and HTTP Compression docs"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="296">
   <si>
     <t>Document</t>
   </si>
@@ -2681,6 +2681,24 @@
   <si>
     <t>New section</t>
   </si>
+  <si>
+    <t>code 2048</t>
+  </si>
+  <si>
+    <t>code 3008 - 3012</t>
+  </si>
+  <si>
+    <t>code 4004</t>
+  </si>
+  <si>
+    <t>SOAP Lookup RPNs by Range Guide</t>
+  </si>
+  <si>
+    <t>listOfEmployeesSampleCSV</t>
+  </si>
+  <si>
+    <t>The number format in the DIR_MRK column was changed from ‘Date’ to ‘General’</t>
+  </si>
 </sst>
 </file>
 
@@ -3274,7 +3292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3585,9 +3603,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3596,6 +3611,16 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3645,35 +3670,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3687,8 +3685,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3701,6 +3714,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3723,6 +3748,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3741,38 +3778,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3789,7 +3799,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3805,6 +3821,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4214,13 +4242,13 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="126">
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="129">
         <v>43056</v>
       </c>
       <c r="F2" s="2"/>
@@ -4240,19 +4268,19 @@
       <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="126"/>
+      <c r="E3" s="129"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="126"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="129"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -4270,7 +4298,7 @@
       <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="126"/>
+      <c r="E5" s="129"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -4288,16 +4316,16 @@
       <c r="D6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="126"/>
+      <c r="E6" s="129"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="133">
+      <c r="B7" s="136">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4306,86 +4334,86 @@
       <c r="D7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="126"/>
+      <c r="E7" s="129"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="131"/>
-      <c r="B8" s="134"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="126"/>
+      <c r="E8" s="129"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="131"/>
-      <c r="B9" s="134"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="137"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="126"/>
+      <c r="E9" s="129"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="131"/>
-      <c r="B10" s="134"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="126"/>
+      <c r="E10" s="129"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="131"/>
-      <c r="B11" s="134"/>
+      <c r="A11" s="134"/>
+      <c r="B11" s="137"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="126"/>
+      <c r="E11" s="129"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
-      <c r="B12" s="135"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="126"/>
+      <c r="E12" s="129"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="133">
+      <c r="B13" s="136">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4394,21 +4422,21 @@
       <c r="D13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="126"/>
+      <c r="E13" s="129"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="139"/>
-      <c r="B14" s="135"/>
+      <c r="A14" s="142"/>
+      <c r="B14" s="138"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="126"/>
+      <c r="E14" s="129"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -4426,7 +4454,7 @@
       <c r="D15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="126"/>
+      <c r="E15" s="129"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -4444,19 +4472,19 @@
       <c r="D16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="126"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="127" t="s">
+      <c r="A17" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="128"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="126"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="129"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -4474,7 +4502,7 @@
       <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="126"/>
+      <c r="E18" s="129"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -4492,28 +4520,28 @@
       <c r="D19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="126"/>
+      <c r="E19" s="129"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="127" t="s">
+      <c r="A20" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="128"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="126"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="129"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="140" t="s">
+      <c r="A21" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="137">
+      <c r="B21" s="140">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4522,21 +4550,21 @@
       <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="126"/>
+      <c r="E21" s="129"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="141"/>
-      <c r="B22" s="135"/>
+      <c r="A22" s="144"/>
+      <c r="B22" s="138"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="126"/>
+      <c r="E22" s="129"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
@@ -4551,22 +4579,22 @@
       <c r="D23" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="126"/>
+      <c r="E23" s="129"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="127" t="s">
+      <c r="A24" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="126"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="129"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="136" t="s">
+      <c r="A25" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="137">
+      <c r="B25" s="140">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4575,105 +4603,105 @@
       <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="126"/>
+      <c r="E25" s="129"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="131"/>
-      <c r="B26" s="134"/>
+      <c r="A26" s="134"/>
+      <c r="B26" s="137"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="126"/>
+      <c r="E26" s="129"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="131"/>
-      <c r="B27" s="134"/>
+      <c r="A27" s="134"/>
+      <c r="B27" s="137"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="126"/>
+      <c r="E27" s="129"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="131"/>
-      <c r="B28" s="134"/>
+      <c r="A28" s="134"/>
+      <c r="B28" s="137"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="126"/>
+      <c r="E28" s="129"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="131"/>
-      <c r="B29" s="134"/>
+      <c r="A29" s="134"/>
+      <c r="B29" s="137"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="126"/>
+      <c r="E29" s="129"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="131"/>
-      <c r="B30" s="134"/>
+      <c r="A30" s="134"/>
+      <c r="B30" s="137"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="126"/>
+      <c r="E30" s="129"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="131"/>
-      <c r="B31" s="134"/>
+      <c r="A31" s="134"/>
+      <c r="B31" s="137"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="126"/>
+      <c r="E31" s="129"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="132"/>
-      <c r="B32" s="135"/>
+      <c r="A32" s="135"/>
+      <c r="B32" s="138"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="126"/>
+      <c r="E32" s="129"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -4691,7 +4719,7 @@
       <c r="D33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="126"/>
+      <c r="E33" s="129"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
@@ -4706,7 +4734,7 @@
       <c r="D34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="126"/>
+      <c r="E34" s="129"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
@@ -4721,7 +4749,7 @@
       <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="126"/>
+      <c r="E35" s="129"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
@@ -4736,7 +4764,7 @@
       <c r="D36" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="126"/>
+      <c r="E36" s="129"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
@@ -4751,7 +4779,7 @@
       <c r="D37" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="126"/>
+      <c r="E37" s="129"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
@@ -4766,7 +4794,7 @@
       <c r="D38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="126"/>
+      <c r="E38" s="129"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
@@ -4781,7 +4809,7 @@
       <c r="D39" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="126"/>
+      <c r="E39" s="129"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
@@ -4796,16 +4824,16 @@
       <c r="D40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="126"/>
+      <c r="E40" s="129"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="127" t="s">
+      <c r="A41" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="128"/>
-      <c r="C41" s="128"/>
-      <c r="D41" s="129"/>
-      <c r="E41" s="126"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="129"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4820,7 +4848,7 @@
       <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="126"/>
+      <c r="E42" s="129"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
@@ -4835,7 +4863,7 @@
       <c r="D43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="126"/>
+      <c r="E43" s="129"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
@@ -4850,7 +4878,7 @@
       <c r="D44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="126"/>
+      <c r="E44" s="129"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
@@ -4865,7 +4893,7 @@
       <c r="D45" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="126"/>
+      <c r="E45" s="129"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -4948,7 +4976,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="153">
+      <c r="E2" s="147">
         <v>43140</v>
       </c>
     </row>
@@ -4963,7 +4991,7 @@
       <c r="D3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="153"/>
+      <c r="E3" s="147"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
@@ -4976,7 +5004,7 @@
       <c r="D4" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="153"/>
+      <c r="E4" s="147"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
@@ -4989,7 +5017,7 @@
       <c r="D5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="153"/>
+      <c r="E5" s="147"/>
     </row>
     <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
@@ -4998,13 +5026,13 @@
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="153"/>
+      <c r="E6" s="147"/>
     </row>
     <row r="7" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5013,68 +5041,68 @@
       <c r="D7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="153"/>
+      <c r="E7" s="147"/>
     </row>
     <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="147"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="160"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="153"/>
+      <c r="E8" s="147"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="147"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="161"/>
+      <c r="B9" s="160"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="153"/>
+      <c r="E9" s="147"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="147"/>
-      <c r="B10" s="148"/>
+      <c r="A10" s="161"/>
+      <c r="B10" s="160"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="153"/>
+      <c r="E10" s="147"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="147"/>
-      <c r="B11" s="148"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="160"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="153"/>
+      <c r="E11" s="147"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="147"/>
-      <c r="B12" s="148"/>
+      <c r="A12" s="161"/>
+      <c r="B12" s="160"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="153"/>
+      <c r="E12" s="147"/>
     </row>
     <row r="13" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="163" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5083,35 +5111,35 @@
       <c r="D13" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="153"/>
+      <c r="E13" s="147"/>
     </row>
     <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="150"/>
-      <c r="B14" s="148"/>
+      <c r="A14" s="163"/>
+      <c r="B14" s="160"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="153"/>
+      <c r="E14" s="147"/>
     </row>
     <row r="15" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="150"/>
-      <c r="B15" s="148"/>
+      <c r="A15" s="163"/>
+      <c r="B15" s="160"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="153"/>
+      <c r="E15" s="147"/>
     </row>
     <row r="16" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5120,108 +5148,108 @@
       <c r="D16" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="153"/>
+      <c r="E16" s="147"/>
     </row>
     <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="145"/>
-      <c r="B17" s="151"/>
+      <c r="B17" s="155"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="153"/>
+      <c r="E17" s="147"/>
     </row>
     <row r="18" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="145"/>
-      <c r="B18" s="151"/>
+      <c r="B18" s="155"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="153"/>
+      <c r="E18" s="147"/>
     </row>
     <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="145"/>
-      <c r="B19" s="151"/>
+      <c r="B19" s="155"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="153"/>
+      <c r="E19" s="147"/>
     </row>
     <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="145"/>
-      <c r="B20" s="151"/>
+      <c r="B20" s="155"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="153"/>
+      <c r="E20" s="147"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="145"/>
-      <c r="B21" s="151"/>
+      <c r="B21" s="155"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="153"/>
+      <c r="E21" s="147"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="145"/>
-      <c r="B22" s="151"/>
+      <c r="B22" s="155"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="153"/>
+      <c r="E22" s="147"/>
     </row>
     <row r="23" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="145"/>
-      <c r="B23" s="151"/>
+      <c r="B23" s="155"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="E23" s="153"/>
+      <c r="E23" s="147"/>
     </row>
     <row r="24" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="145"/>
-      <c r="B24" s="151"/>
+      <c r="B24" s="155"/>
       <c r="C24" s="145" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="152" t="s">
+      <c r="D24" s="146" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="153"/>
+      <c r="E24" s="147"/>
     </row>
     <row r="25" spans="1:5" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="145"/>
-      <c r="B25" s="151"/>
+      <c r="B25" s="155"/>
       <c r="C25" s="145"/>
-      <c r="D25" s="152"/>
-      <c r="E25" s="153"/>
+      <c r="D25" s="146"/>
+      <c r="E25" s="147"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="161" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5230,16 +5258,16 @@
       <c r="D26" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="153"/>
+      <c r="E26" s="147"/>
     </row>
     <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="147"/>
-      <c r="B27" s="148"/>
+      <c r="A27" s="161"/>
+      <c r="B27" s="160"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="153"/>
+      <c r="E27" s="147"/>
     </row>
     <row r="28" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
@@ -5252,7 +5280,7 @@
       <c r="D28" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="153"/>
+      <c r="E28" s="147"/>
     </row>
     <row r="29" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
@@ -5261,108 +5289,108 @@
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="153"/>
+      <c r="E29" s="147"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="149" t="s">
+      <c r="A30" s="162" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="145" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="146" t="s">
+      <c r="D30" s="150" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="153"/>
+      <c r="E30" s="147"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="149"/>
-      <c r="B31" s="148"/>
+      <c r="A31" s="162"/>
+      <c r="B31" s="160"/>
       <c r="C31" s="145"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="153"/>
+      <c r="D31" s="150"/>
+      <c r="E31" s="147"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="149"/>
-      <c r="B32" s="148"/>
+      <c r="A32" s="162"/>
+      <c r="B32" s="160"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="153"/>
+      <c r="E32" s="147"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="149"/>
-      <c r="B33" s="148"/>
+      <c r="A33" s="162"/>
+      <c r="B33" s="160"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="153"/>
+      <c r="E33" s="147"/>
     </row>
     <row r="34" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="149"/>
-      <c r="B34" s="148"/>
+      <c r="A34" s="162"/>
+      <c r="B34" s="160"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="153"/>
+      <c r="E34" s="147"/>
     </row>
     <row r="35" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="149"/>
-      <c r="B35" s="148"/>
+      <c r="A35" s="162"/>
+      <c r="B35" s="160"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="153"/>
+      <c r="E35" s="147"/>
     </row>
     <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="149"/>
-      <c r="B36" s="148"/>
+      <c r="A36" s="162"/>
+      <c r="B36" s="160"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
       <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="153"/>
+      <c r="E36" s="147"/>
     </row>
     <row r="37" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="149"/>
-      <c r="B37" s="148"/>
-      <c r="C37" s="142" t="s">
+      <c r="A37" s="162"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="144" t="s">
+      <c r="D37" s="153" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="153"/>
+      <c r="E37" s="147"/>
     </row>
     <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="149"/>
-      <c r="B38" s="148"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="153"/>
+      <c r="A38" s="162"/>
+      <c r="B38" s="160"/>
+      <c r="C38" s="152"/>
+      <c r="D38" s="153"/>
+      <c r="E38" s="147"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="147" t="s">
+      <c r="A39" s="161" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5371,16 +5399,16 @@
       <c r="D39" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="153"/>
+      <c r="E39" s="147"/>
     </row>
     <row r="40" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="147"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="161"/>
+      <c r="B40" s="160"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="153"/>
+      <c r="E40" s="147"/>
     </row>
     <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
@@ -5393,7 +5421,7 @@
       <c r="D41" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="153"/>
+      <c r="E41" s="147"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
@@ -5402,90 +5430,90 @@
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="153"/>
+      <c r="E42" s="147"/>
     </row>
     <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="149" t="s">
+      <c r="A43" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="148" t="s">
+      <c r="B43" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="153"/>
+      <c r="E43" s="147"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="149"/>
-      <c r="B44" s="148"/>
+      <c r="A44" s="162"/>
+      <c r="B44" s="160"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D44" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="153"/>
+      <c r="E44" s="147"/>
     </row>
     <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="158" t="s">
+      <c r="A45" s="157" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="153"/>
+      <c r="E45" s="147"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="159"/>
-      <c r="B46" s="148"/>
+      <c r="A46" s="158"/>
+      <c r="B46" s="160"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="153"/>
+      <c r="E46" s="147"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="159"/>
-      <c r="B47" s="148"/>
+      <c r="A47" s="158"/>
+      <c r="B47" s="160"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="153"/>
+      <c r="E47" s="147"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="160"/>
-      <c r="B48" s="148"/>
+      <c r="A48" s="159"/>
+      <c r="B48" s="160"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="153"/>
+      <c r="E48" s="147"/>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="151" t="s">
+      <c r="A49" s="155" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="151" t="s">
+      <c r="B49" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="153"/>
+      <c r="E49" s="147"/>
       <c r="H49" s="42"/>
       <c r="L49" s="42"/>
       <c r="P49" s="42"/>
@@ -9583,15 +9611,15 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="151"/>
-      <c r="B50" s="151"/>
+      <c r="A50" s="155"/>
+      <c r="B50" s="155"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="153"/>
+      <c r="E50" s="147"/>
       <c r="H50" s="42"/>
       <c r="L50" s="42"/>
       <c r="P50" s="42"/>
@@ -13689,15 +13717,15 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="151"/>
-      <c r="B51" s="151"/>
+      <c r="A51" s="155"/>
+      <c r="B51" s="155"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="E51" s="153"/>
+      <c r="E51" s="147"/>
       <c r="H51" s="42"/>
       <c r="L51" s="42"/>
       <c r="P51" s="42"/>
@@ -17795,15 +17823,15 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="151"/>
-      <c r="B52" s="151"/>
+      <c r="A52" s="155"/>
+      <c r="B52" s="155"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="153"/>
+      <c r="E52" s="147"/>
       <c r="H52" s="42"/>
       <c r="L52" s="42"/>
       <c r="P52" s="42"/>
@@ -21901,15 +21929,15 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="151"/>
-      <c r="B53" s="151"/>
-      <c r="C53" s="155" t="s">
+      <c r="A53" s="155"/>
+      <c r="B53" s="155"/>
+      <c r="C53" s="149" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="146" t="s">
+      <c r="D53" s="150" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="153"/>
+      <c r="E53" s="147"/>
       <c r="H53" s="42"/>
       <c r="L53" s="42"/>
       <c r="P53" s="42"/>
@@ -26007,11 +26035,11 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="151"/>
-      <c r="B54" s="151"/>
-      <c r="C54" s="155"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="153"/>
+      <c r="A54" s="155"/>
+      <c r="B54" s="155"/>
+      <c r="C54" s="149"/>
+      <c r="D54" s="150"/>
+      <c r="E54" s="147"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -30115,7 +30143,7 @@
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
-      <c r="E55" s="153"/>
+      <c r="E55" s="147"/>
     </row>
     <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
@@ -30128,13 +30156,13 @@
       <c r="D56" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="153"/>
+      <c r="E56" s="147"/>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="156" t="s">
+      <c r="A57" s="154" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30143,204 +30171,204 @@
       <c r="D57" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="153"/>
+      <c r="E57" s="147"/>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="156"/>
-      <c r="B58" s="151"/>
+      <c r="A58" s="154"/>
+      <c r="B58" s="155"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="E58" s="153"/>
+      <c r="E58" s="147"/>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="156"/>
-      <c r="B59" s="151"/>
+      <c r="A59" s="154"/>
+      <c r="B59" s="155"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D59" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="153"/>
+      <c r="E59" s="147"/>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="156"/>
-      <c r="B60" s="151"/>
+      <c r="A60" s="154"/>
+      <c r="B60" s="155"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D60" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="153"/>
+      <c r="E60" s="147"/>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="156"/>
-      <c r="B61" s="151"/>
+      <c r="A61" s="154"/>
+      <c r="B61" s="155"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="153"/>
+      <c r="E61" s="147"/>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="156"/>
-      <c r="B62" s="151"/>
+      <c r="A62" s="154"/>
+      <c r="B62" s="155"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="153"/>
+      <c r="E62" s="147"/>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="156"/>
-      <c r="B63" s="151"/>
+      <c r="A63" s="154"/>
+      <c r="B63" s="155"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D63" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="153"/>
+      <c r="E63" s="147"/>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="156"/>
-      <c r="B64" s="151"/>
+      <c r="A64" s="154"/>
+      <c r="B64" s="155"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="153"/>
+      <c r="E64" s="147"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="156"/>
-      <c r="B65" s="151"/>
+      <c r="A65" s="154"/>
+      <c r="B65" s="155"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="153"/>
+      <c r="E65" s="147"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="156"/>
-      <c r="B66" s="151"/>
+      <c r="A66" s="154"/>
+      <c r="B66" s="155"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="153"/>
+      <c r="E66" s="147"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="156"/>
-      <c r="B67" s="151"/>
+      <c r="A67" s="154"/>
+      <c r="B67" s="155"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E67" s="153"/>
+      <c r="E67" s="147"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="156"/>
-      <c r="B68" s="151"/>
+      <c r="A68" s="154"/>
+      <c r="B68" s="155"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="153"/>
+      <c r="E68" s="147"/>
     </row>
     <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="156"/>
-      <c r="B69" s="151"/>
+      <c r="A69" s="154"/>
+      <c r="B69" s="155"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E69" s="153"/>
+      <c r="E69" s="147"/>
     </row>
     <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="156"/>
-      <c r="B70" s="151"/>
+      <c r="A70" s="154"/>
+      <c r="B70" s="155"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="153"/>
+      <c r="E70" s="147"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="156"/>
-      <c r="B71" s="151"/>
+      <c r="A71" s="154"/>
+      <c r="B71" s="155"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="153"/>
+      <c r="E71" s="147"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="156"/>
-      <c r="B72" s="151"/>
+      <c r="A72" s="154"/>
+      <c r="B72" s="155"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="153"/>
+      <c r="E72" s="147"/>
     </row>
     <row r="73" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="156"/>
-      <c r="B73" s="151"/>
+      <c r="A73" s="154"/>
+      <c r="B73" s="155"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="153"/>
+      <c r="E73" s="147"/>
     </row>
     <row r="74" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="156"/>
-      <c r="B74" s="151"/>
+      <c r="A74" s="154"/>
+      <c r="B74" s="155"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="E74" s="153"/>
+      <c r="E74" s="147"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="156"/>
-      <c r="B75" s="151"/>
-      <c r="C75" s="154"/>
-      <c r="D75" s="157" t="s">
+      <c r="A75" s="154"/>
+      <c r="B75" s="155"/>
+      <c r="C75" s="148"/>
+      <c r="D75" s="156" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="153"/>
+      <c r="E75" s="147"/>
     </row>
     <row r="76" spans="1:5" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="156"/>
-      <c r="B76" s="151"/>
-      <c r="C76" s="154"/>
-      <c r="D76" s="157"/>
-      <c r="E76" s="153"/>
+      <c r="A76" s="154"/>
+      <c r="B76" s="155"/>
+      <c r="C76" s="148"/>
+      <c r="D76" s="156"/>
+      <c r="E76" s="147"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30349,7 +30377,7 @@
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
-      <c r="E77" s="153"/>
+      <c r="E77" s="147"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="48"/>
@@ -30387,6 +30415,15 @@
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="B16:B25"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="A57:A76"/>
     <mergeCell ref="B57:B76"/>
     <mergeCell ref="D75:D76"/>
@@ -30400,19 +30437,10 @@
     <mergeCell ref="C75:C76"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B16:B25"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30460,7 +30488,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="126">
+      <c r="E2" s="129">
         <v>43179</v>
       </c>
     </row>
@@ -30471,13 +30499,13 @@
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="126"/>
+      <c r="E3" s="129"/>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30486,158 +30514,158 @@
       <c r="D4" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="126"/>
+      <c r="E4" s="129"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="147"/>
-      <c r="B5" s="148"/>
-      <c r="C5" s="176" t="s">
+      <c r="A5" s="161"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="173" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="172" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="126"/>
+      <c r="E5" s="129"/>
     </row>
     <row r="6" spans="1:5" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="147"/>
-      <c r="B6" s="148"/>
-      <c r="C6" s="176"/>
-      <c r="D6" s="175"/>
-      <c r="E6" s="126"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="129"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="147"/>
-      <c r="B7" s="148"/>
+      <c r="A7" s="161"/>
+      <c r="B7" s="160"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
-      <c r="E7" s="126"/>
+      <c r="E7" s="129"/>
     </row>
     <row r="8" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="147"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="160"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
-      <c r="E8" s="126"/>
+      <c r="E8" s="129"/>
     </row>
     <row r="9" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="147"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="161"/>
+      <c r="B9" s="160"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
-      <c r="E9" s="126"/>
+      <c r="E9" s="129"/>
     </row>
     <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="163" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="167"/>
-      <c r="D10" s="175" t="s">
+      <c r="C10" s="170"/>
+      <c r="D10" s="172" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="126"/>
+      <c r="E10" s="129"/>
     </row>
     <row r="11" spans="1:5" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="150"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="167"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="126"/>
+      <c r="A11" s="163"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="129"/>
     </row>
     <row r="12" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="150"/>
-      <c r="B12" s="148"/>
-      <c r="C12" s="167"/>
-      <c r="D12" s="175"/>
-      <c r="E12" s="126"/>
+      <c r="A12" s="163"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="172"/>
+      <c r="E12" s="129"/>
     </row>
     <row r="13" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="151" t="s">
+      <c r="B13" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="175" t="s">
+      <c r="C13" s="174"/>
+      <c r="D13" s="172" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="126"/>
+      <c r="E13" s="129"/>
     </row>
     <row r="14" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="145"/>
-      <c r="B14" s="151"/>
-      <c r="C14" s="177"/>
-      <c r="D14" s="175"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="155"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="172"/>
+      <c r="E14" s="129"/>
     </row>
     <row r="15" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="145"/>
-      <c r="B15" s="151"/>
-      <c r="C15" s="177"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="174"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="126"/>
+      <c r="E15" s="129"/>
     </row>
     <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="145"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="177"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="174"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="126"/>
+      <c r="E16" s="129"/>
     </row>
     <row r="17" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="145"/>
-      <c r="B17" s="151"/>
-      <c r="C17" s="177"/>
+      <c r="B17" s="155"/>
+      <c r="C17" s="174"/>
       <c r="D17" s="49"/>
-      <c r="E17" s="126"/>
+      <c r="E17" s="129"/>
     </row>
     <row r="18" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="145"/>
-      <c r="B18" s="151"/>
-      <c r="C18" s="177"/>
+      <c r="B18" s="155"/>
+      <c r="C18" s="174"/>
       <c r="D18" s="49"/>
-      <c r="E18" s="126"/>
+      <c r="E18" s="129"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="145"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="177"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="174"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="126"/>
+      <c r="E19" s="129"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="145"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="177"/>
+      <c r="B20" s="155"/>
+      <c r="C20" s="174"/>
       <c r="D20" s="49"/>
-      <c r="E20" s="126"/>
+      <c r="E20" s="129"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="145"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="177"/>
+      <c r="B21" s="155"/>
+      <c r="C21" s="174"/>
       <c r="D21" s="49"/>
-      <c r="E21" s="126"/>
+      <c r="E21" s="129"/>
     </row>
     <row r="22" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="145"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="177"/>
+      <c r="B22" s="155"/>
+      <c r="C22" s="174"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="126"/>
+      <c r="E22" s="129"/>
     </row>
     <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="145"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="177"/>
+      <c r="B23" s="155"/>
+      <c r="C23" s="174"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="126"/>
+      <c r="E23" s="129"/>
     </row>
     <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
@@ -30652,7 +30680,7 @@
       <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="126"/>
+      <c r="E24" s="129"/>
     </row>
     <row r="25" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
@@ -30667,7 +30695,7 @@
       <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="E25" s="126"/>
+      <c r="E25" s="129"/>
     </row>
     <row r="26" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
@@ -30680,7 +30708,7 @@
       <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="126"/>
+      <c r="E26" s="129"/>
     </row>
     <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
@@ -30689,7 +30717,7 @@
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="126"/>
+      <c r="E27" s="129"/>
     </row>
     <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
@@ -30704,7 +30732,7 @@
       <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="126"/>
+      <c r="E28" s="129"/>
     </row>
     <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="85"/>
@@ -30715,7 +30743,7 @@
       <c r="D29" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="126"/>
+      <c r="E29" s="129"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
@@ -30726,7 +30754,7 @@
       <c r="D30" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="E30" s="126"/>
+      <c r="E30" s="129"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
@@ -30737,13 +30765,13 @@
       <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="126"/>
+      <c r="E31" s="129"/>
     </row>
     <row r="32" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="161" t="s">
+      <c r="A32" s="164" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="167" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30752,39 +30780,39 @@
       <c r="D32" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="E32" s="126"/>
+      <c r="E32" s="129"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="162"/>
-      <c r="B33" s="165"/>
+      <c r="A33" s="165"/>
+      <c r="B33" s="168"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
-      <c r="E33" s="126"/>
+      <c r="E33" s="129"/>
     </row>
     <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="162"/>
-      <c r="B34" s="165"/>
+      <c r="A34" s="165"/>
+      <c r="B34" s="168"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
-      <c r="E34" s="126"/>
+      <c r="E34" s="129"/>
     </row>
     <row r="35" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="162"/>
-      <c r="B35" s="165"/>
+      <c r="A35" s="165"/>
+      <c r="B35" s="168"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
-      <c r="E35" s="126"/>
+      <c r="E35" s="129"/>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="163"/>
-      <c r="B36" s="166"/>
+      <c r="A36" s="166"/>
+      <c r="B36" s="169"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="126"/>
+      <c r="E36" s="129"/>
     </row>
     <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
@@ -30797,7 +30825,7 @@
       <c r="D37" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="126"/>
+      <c r="E37" s="129"/>
     </row>
     <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
@@ -30806,13 +30834,13 @@
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
-      <c r="E38" s="126"/>
+      <c r="E38" s="129"/>
     </row>
     <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="149" t="s">
+      <c r="A39" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30821,108 +30849,108 @@
       <c r="D39" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="E39" s="126"/>
+      <c r="E39" s="129"/>
     </row>
     <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="149"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="162"/>
+      <c r="B40" s="160"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="126"/>
+      <c r="E40" s="129"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="147" t="s">
+      <c r="A41" s="161" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="167" t="s">
+      <c r="C41" s="170" t="s">
         <v>194</v>
       </c>
       <c r="D41" s="145" t="s">
         <v>228</v>
       </c>
-      <c r="E41" s="126"/>
+      <c r="E41" s="129"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="147"/>
-      <c r="B42" s="148"/>
-      <c r="C42" s="167"/>
+      <c r="A42" s="161"/>
+      <c r="B42" s="160"/>
+      <c r="C42" s="170"/>
       <c r="D42" s="145"/>
-      <c r="E42" s="126"/>
+      <c r="E42" s="129"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="147"/>
-      <c r="B43" s="148"/>
-      <c r="C43" s="167" t="s">
+      <c r="A43" s="161"/>
+      <c r="B43" s="160"/>
+      <c r="C43" s="170" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="157" t="s">
+      <c r="D43" s="156" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="126"/>
+      <c r="E43" s="129"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="147"/>
-      <c r="B44" s="148"/>
-      <c r="C44" s="167"/>
-      <c r="D44" s="157"/>
-      <c r="E44" s="126"/>
+      <c r="A44" s="161"/>
+      <c r="B44" s="160"/>
+      <c r="C44" s="170"/>
+      <c r="D44" s="156"/>
+      <c r="E44" s="129"/>
     </row>
     <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="156" t="s">
+      <c r="A45" s="154" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="151" t="s">
+      <c r="B45" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="171"/>
+      <c r="C45" s="178"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="126"/>
+      <c r="E45" s="129"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="156"/>
-      <c r="B46" s="151"/>
-      <c r="C46" s="172"/>
-      <c r="D46" s="168" t="s">
+      <c r="A46" s="154"/>
+      <c r="B46" s="155"/>
+      <c r="C46" s="179"/>
+      <c r="D46" s="175" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="126"/>
+      <c r="E46" s="129"/>
     </row>
     <row r="47" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="156"/>
-      <c r="B47" s="151"/>
-      <c r="C47" s="172"/>
-      <c r="D47" s="169"/>
-      <c r="E47" s="126"/>
+      <c r="A47" s="154"/>
+      <c r="B47" s="155"/>
+      <c r="C47" s="179"/>
+      <c r="D47" s="176"/>
+      <c r="E47" s="129"/>
     </row>
     <row r="48" spans="1:5" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="156"/>
-      <c r="B48" s="151"/>
-      <c r="C48" s="173"/>
-      <c r="D48" s="169"/>
-      <c r="E48" s="126"/>
+      <c r="A48" s="154"/>
+      <c r="B48" s="155"/>
+      <c r="C48" s="180"/>
+      <c r="D48" s="176"/>
+      <c r="E48" s="129"/>
     </row>
     <row r="49" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="156"/>
-      <c r="B49" s="151"/>
-      <c r="C49" s="155"/>
-      <c r="D49" s="169"/>
-      <c r="E49" s="126"/>
+      <c r="A49" s="154"/>
+      <c r="B49" s="155"/>
+      <c r="C49" s="149"/>
+      <c r="D49" s="176"/>
+      <c r="E49" s="129"/>
     </row>
     <row r="50" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="156"/>
-      <c r="B50" s="151"/>
-      <c r="C50" s="155"/>
-      <c r="D50" s="170"/>
-      <c r="E50" s="126"/>
+      <c r="A50" s="154"/>
+      <c r="B50" s="155"/>
+      <c r="C50" s="149"/>
+      <c r="D50" s="177"/>
+      <c r="E50" s="129"/>
     </row>
     <row r="51" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30931,7 +30959,7 @@
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
-      <c r="E51" s="126"/>
+      <c r="E51" s="129"/>
     </row>
     <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
@@ -30944,13 +30972,13 @@
       <c r="D52" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="126"/>
+      <c r="E52" s="129"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="151" t="s">
+      <c r="A53" s="155" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="151" t="s">
+      <c r="B53" s="155" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30959,148 +30987,148 @@
       <c r="D53" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="126"/>
+      <c r="E53" s="129"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="151"/>
-      <c r="B54" s="151"/>
+      <c r="A54" s="155"/>
+      <c r="B54" s="155"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
       <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="126"/>
+      <c r="E54" s="129"/>
     </row>
     <row r="55" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="151"/>
-      <c r="B55" s="151"/>
+      <c r="A55" s="155"/>
+      <c r="B55" s="155"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="126"/>
+      <c r="E55" s="129"/>
     </row>
     <row r="56" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="151"/>
-      <c r="B56" s="151"/>
-      <c r="C56" s="174" t="s">
+      <c r="A56" s="155"/>
+      <c r="B56" s="155"/>
+      <c r="C56" s="171" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="E56" s="126"/>
+      <c r="E56" s="129"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="151"/>
-      <c r="B57" s="151"/>
-      <c r="C57" s="174"/>
+      <c r="A57" s="155"/>
+      <c r="B57" s="155"/>
+      <c r="C57" s="171"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="126"/>
+      <c r="E57" s="129"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="151"/>
-      <c r="B58" s="151"/>
+      <c r="A58" s="155"/>
+      <c r="B58" s="155"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
       <c r="D58" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E58" s="126"/>
+      <c r="E58" s="129"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="151"/>
-      <c r="B59" s="151"/>
+      <c r="A59" s="155"/>
+      <c r="B59" s="155"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
       <c r="D59" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="126"/>
+      <c r="E59" s="129"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="151"/>
-      <c r="B60" s="151"/>
-      <c r="C60" s="174" t="s">
+      <c r="A60" s="155"/>
+      <c r="B60" s="155"/>
+      <c r="C60" s="171" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="126"/>
+      <c r="E60" s="129"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="151"/>
-      <c r="B61" s="151"/>
-      <c r="C61" s="174"/>
+      <c r="A61" s="155"/>
+      <c r="B61" s="155"/>
+      <c r="C61" s="171"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="126"/>
+      <c r="E61" s="129"/>
     </row>
     <row r="62" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="151"/>
-      <c r="B62" s="151"/>
-      <c r="C62" s="174"/>
+      <c r="A62" s="155"/>
+      <c r="B62" s="155"/>
+      <c r="C62" s="171"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="E62" s="126"/>
+      <c r="E62" s="129"/>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="151"/>
-      <c r="B63" s="151"/>
-      <c r="C63" s="167" t="s">
+      <c r="A63" s="155"/>
+      <c r="B63" s="155"/>
+      <c r="C63" s="170" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="E63" s="126"/>
+      <c r="E63" s="129"/>
     </row>
     <row r="64" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="151"/>
-      <c r="B64" s="151"/>
-      <c r="C64" s="167"/>
-      <c r="D64" s="157" t="s">
+      <c r="A64" s="155"/>
+      <c r="B64" s="155"/>
+      <c r="C64" s="170"/>
+      <c r="D64" s="156" t="s">
         <v>220</v>
       </c>
-      <c r="E64" s="126"/>
+      <c r="E64" s="129"/>
     </row>
     <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="151"/>
-      <c r="B65" s="151"/>
-      <c r="C65" s="167"/>
-      <c r="D65" s="157"/>
-      <c r="E65" s="126"/>
+      <c r="A65" s="155"/>
+      <c r="B65" s="155"/>
+      <c r="C65" s="170"/>
+      <c r="D65" s="156"/>
+      <c r="E65" s="129"/>
     </row>
     <row r="66" spans="1:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="151"/>
-      <c r="B66" s="151"/>
-      <c r="C66" s="167"/>
-      <c r="D66" s="157"/>
-      <c r="E66" s="126"/>
+      <c r="A66" s="155"/>
+      <c r="B66" s="155"/>
+      <c r="C66" s="170"/>
+      <c r="D66" s="156"/>
+      <c r="E66" s="129"/>
     </row>
     <row r="67" spans="1:5" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="151"/>
-      <c r="B67" s="151"/>
-      <c r="C67" s="167"/>
-      <c r="D67" s="157"/>
-      <c r="E67" s="126"/>
+      <c r="A67" s="155"/>
+      <c r="B67" s="155"/>
+      <c r="C67" s="170"/>
+      <c r="D67" s="156"/>
+      <c r="E67" s="129"/>
     </row>
     <row r="68" spans="1:5" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
-      <c r="E68" s="126"/>
+      <c r="E68" s="129"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
@@ -31150,6 +31178,10 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="E2:E68"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C5:C6"/>
@@ -31162,20 +31194,16 @@
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="C45:C48"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C63:C67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B53:B67"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="C43:C44"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C63:C67"/>
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="A4:A9"/>
@@ -31192,10 +31220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31237,7 +31265,7 @@
       <c r="A3" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="174" t="s">
+      <c r="B3" s="171" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="58"/>
@@ -31250,8 +31278,8 @@
     </row>
     <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="145"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="124" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="123" t="s">
         <v>235</v>
       </c>
       <c r="D4" s="108" t="s">
@@ -31265,8 +31293,8 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="174"/>
-      <c r="C5" s="124" t="s">
+      <c r="B5" s="171"/>
+      <c r="C5" s="123" t="s">
         <v>235</v>
       </c>
       <c r="D5" s="109" t="s">
@@ -31280,8 +31308,8 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="124" t="s">
+      <c r="B6" s="171"/>
+      <c r="C6" s="123" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="109" t="s">
@@ -31292,10 +31320,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="183" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="58"/>
       <c r="D7" s="110" t="s">
         <v>261</v>
@@ -31305,8 +31333,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="186"/>
-      <c r="B8" s="174"/>
+      <c r="A8" s="184"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="58"/>
       <c r="D8" s="107" t="s">
         <v>276</v>
@@ -31316,501 +31344,495 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="A9" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="171"/>
+      <c r="C9" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="116">
+        <v>43299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="109" t="s">
+      <c r="B10" s="171"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="109" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="116">
+      <c r="E10" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+    <row r="11" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="58"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="182" t="s">
-        <v>237</v>
-      </c>
-      <c r="B11" s="174" t="s">
-        <v>234</v>
-      </c>
-      <c r="C11" s="58"/>
-      <c r="D11" t="s">
-        <v>258</v>
-      </c>
-      <c r="E11" s="117">
-        <v>43270</v>
-      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="183"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="197" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="171" t="s">
+        <v>234</v>
+      </c>
       <c r="C12" s="58"/>
-      <c r="D12" s="107" t="s">
-        <v>252</v>
-      </c>
-      <c r="E12" s="116">
-        <v>43244</v>
+      <c r="D12" t="s">
+        <v>258</v>
+      </c>
+      <c r="E12" s="117">
+        <v>43270</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="184"/>
-      <c r="B13" s="174"/>
+      <c r="A13" s="198"/>
+      <c r="B13" s="171"/>
       <c r="C13" s="58"/>
       <c r="D13" s="107" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E13" s="116">
         <v>43244</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="120" t="s">
-        <v>234</v>
-      </c>
+      <c r="A14" s="199"/>
+      <c r="B14" s="171"/>
       <c r="C14" s="58"/>
       <c r="D14" s="107" t="s">
-        <v>238</v>
-      </c>
-      <c r="E14" s="117">
-        <v>43270</v>
+        <v>254</v>
+      </c>
+      <c r="E14" s="116">
+        <v>43244</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="174" t="s">
-        <v>222</v>
-      </c>
-      <c r="B15" s="174" t="s">
+      <c r="A15" s="126" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="120" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="193" t="s">
-        <v>239</v>
-      </c>
-      <c r="D15" s="112" t="s">
-        <v>241</v>
-      </c>
-      <c r="E15" s="116">
-        <v>43244</v>
+      <c r="C15" s="58"/>
+      <c r="D15" s="107" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="117">
+        <v>43270</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="174"/>
-      <c r="B16" s="174"/>
-      <c r="C16" s="194"/>
-      <c r="D16" s="104" t="s">
+      <c r="A16" s="145" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" s="171" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="193" t="s">
+        <v>239</v>
+      </c>
+      <c r="D16" s="112" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" s="116">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="145"/>
+      <c r="B17" s="171"/>
+      <c r="C17" s="194"/>
+      <c r="D17" s="104" t="s">
         <v>278</v>
       </c>
-      <c r="E16" s="117">
+      <c r="E17" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="174"/>
-      <c r="B17" s="174"/>
-      <c r="C17" s="96" t="s">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="145"/>
+      <c r="B18" s="171"/>
+      <c r="C18" s="96" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="113" t="s">
+      <c r="D18" s="113" t="s">
         <v>242</v>
       </c>
-      <c r="E17" s="116">
+      <c r="E18" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="121" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="58" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19" s="127" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="58"/>
+      <c r="E19" s="116">
+        <v>43299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="121" t="s">
         <v>280</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="61" t="s">
+      <c r="B20" s="58"/>
+      <c r="C20" s="61" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="107" t="s">
+      <c r="D20" s="107" t="s">
         <v>281</v>
-      </c>
-      <c r="E18" s="117">
-        <v>43270</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="58"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="185" t="s">
-        <v>260</v>
-      </c>
-      <c r="B20" s="174" t="s">
-        <v>234</v>
-      </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="110" t="s">
-        <v>261</v>
       </c>
       <c r="E20" s="117">
         <v>43270</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="186"/>
-      <c r="B21" s="174"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="107" t="s">
-        <v>257</v>
-      </c>
-      <c r="E21" s="117">
-        <v>43270</v>
-      </c>
+    <row r="21" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="58"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="98" t="s">
-        <v>243</v>
-      </c>
-      <c r="B22" s="120" t="s">
+      <c r="A22" s="183" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" s="171" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="124" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="114" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="116">
-        <v>43244</v>
+      <c r="C22" s="58"/>
+      <c r="D22" s="110" t="s">
+        <v>261</v>
+      </c>
+      <c r="E22" s="117">
+        <v>43270</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="187" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="180" t="s">
-        <v>234</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>268</v>
-      </c>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="184"/>
+      <c r="B23" s="171"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="107" t="s">
-        <v>251</v>
-      </c>
-      <c r="E23" s="116">
-        <v>43244</v>
+        <v>257</v>
+      </c>
+      <c r="E23" s="117">
+        <v>43270</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="188"/>
-      <c r="B24" s="190"/>
-      <c r="C24" t="s">
-        <v>270</v>
-      </c>
-      <c r="D24" s="107" t="s">
-        <v>251</v>
-      </c>
-      <c r="E24" s="117">
-        <v>43270</v>
+      <c r="A24" s="98" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="120" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="123" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="114" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="116">
+        <v>43244</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="188"/>
-      <c r="B25" s="190"/>
+    <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="185" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="188" t="s">
+        <v>234</v>
+      </c>
       <c r="C25" s="58" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D25" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="E25" s="117">
-        <v>43270</v>
+      <c r="E25" s="116">
+        <v>43244</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="188"/>
-      <c r="B26" s="190"/>
-      <c r="C26" s="103" t="s">
-        <v>277</v>
-      </c>
-      <c r="D26" s="104" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="125">
+      <c r="A26" s="186"/>
+      <c r="B26" s="189"/>
+      <c r="C26" t="s">
+        <v>270</v>
+      </c>
+      <c r="D26" s="107" t="s">
+        <v>251</v>
+      </c>
+      <c r="E26" s="117">
         <v>43270</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="188"/>
-      <c r="B27" s="190"/>
+      <c r="A27" s="186"/>
+      <c r="B27" s="189"/>
       <c r="C27" s="58" t="s">
-        <v>284</v>
-      </c>
-      <c r="D27" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D27" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="E27" s="116">
-        <v>43279</v>
+      <c r="E27" s="117">
+        <v>43270</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="188"/>
-      <c r="B28" s="190"/>
-      <c r="C28" s="58" t="s">
+      <c r="A28" s="186"/>
+      <c r="B28" s="189"/>
+      <c r="C28" s="103" t="s">
+        <v>277</v>
+      </c>
+      <c r="D28" s="104" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="124">
+        <v>43270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="186"/>
+      <c r="B29" s="189"/>
+      <c r="C29" s="58" t="s">
+        <v>284</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E29" s="116">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="186"/>
+      <c r="B30" s="189"/>
+      <c r="C30" s="58" t="s">
         <v>285</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D30" s="58" t="s">
         <v>286</v>
       </c>
-      <c r="E28" s="116">
+      <c r="E30" s="116">
         <v>43279</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="189"/>
-      <c r="B29" s="181"/>
-      <c r="C29" s="95" t="s">
-        <v>244</v>
-      </c>
-      <c r="D29" s="114" t="s">
-        <v>245</v>
-      </c>
-      <c r="E29" s="116">
-        <v>43244</v>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="186"/>
+      <c r="B31" s="189"/>
+      <c r="C31" s="125" t="s">
+        <v>290</v>
+      </c>
+      <c r="D31" s="125" t="s">
+        <v>251</v>
+      </c>
+      <c r="E31" s="116">
+        <v>43299</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="58"/>
-    </row>
-    <row r="31" spans="1:5" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="102"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="110" t="s">
-        <v>261</v>
-      </c>
-      <c r="E31" s="58"/>
-    </row>
-    <row r="32" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="145" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="174" t="s">
-        <v>234</v>
-      </c>
-      <c r="C32" s="124" t="s">
-        <v>246</v>
-      </c>
-      <c r="D32" s="107" t="s">
-        <v>253</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="186"/>
+      <c r="B32" s="189"/>
+      <c r="C32" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" s="125" t="s">
+        <v>251</v>
       </c>
       <c r="E32" s="116">
-        <v>43244</v>
+        <v>43299</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="145"/>
-      <c r="B33" s="174"/>
-      <c r="C33" s="124">
-        <v>10.1</v>
-      </c>
-      <c r="D33" s="107" t="s">
-        <v>272</v>
+      <c r="A33" s="186"/>
+      <c r="B33" s="189"/>
+      <c r="C33" s="125" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" s="125" t="s">
+        <v>102</v>
       </c>
       <c r="E33" s="116">
-        <v>43244</v>
+        <v>43299</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="145"/>
-      <c r="B34" s="174"/>
-      <c r="C34" s="124">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D34" s="107" t="s">
-        <v>272</v>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="187"/>
+      <c r="B34" s="190"/>
+      <c r="C34" s="95" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" s="114" t="s">
+        <v>245</v>
       </c>
       <c r="E34" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="145" t="s">
-        <v>247</v>
-      </c>
-      <c r="B35" s="174" t="s">
+    <row r="35" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="58"/>
+    </row>
+    <row r="36" spans="1:5" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="102"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="110" t="s">
+        <v>261</v>
+      </c>
+      <c r="E36" s="58"/>
+    </row>
+    <row r="37" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="145" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="171" t="s">
         <v>234</v>
       </c>
-      <c r="C35" s="174"/>
-      <c r="D35" s="195" t="s">
-        <v>261</v>
-      </c>
-      <c r="E35" s="191">
-        <v>43270</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="145"/>
-      <c r="B36" s="174"/>
-      <c r="C36" s="174"/>
-      <c r="D36" s="195"/>
-      <c r="E36" s="192"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="B37" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C37" s="124" t="s">
-        <v>250</v>
-      </c>
-      <c r="D37" s="115" t="s">
-        <v>251</v>
+      <c r="C37" s="123" t="s">
+        <v>246</v>
+      </c>
+      <c r="D37" s="107" t="s">
+        <v>253</v>
       </c>
       <c r="E37" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="97" t="s">
-        <v>248</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="58"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="145"/>
+      <c r="B38" s="171"/>
+      <c r="C38" s="123">
+        <v>10.1</v>
+      </c>
+      <c r="D38" s="107" t="s">
+        <v>272</v>
+      </c>
+      <c r="E38" s="116">
+        <v>43244</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B39" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C39" s="100" t="s">
-        <v>265</v>
+      <c r="A39" s="145"/>
+      <c r="B39" s="171"/>
+      <c r="C39" s="123">
+        <v>10.199999999999999</v>
       </c>
       <c r="D39" s="107" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="E39" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="58" t="s">
-        <v>287</v>
-      </c>
-      <c r="B40" s="124" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="145" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" s="171" t="s">
         <v>234</v>
       </c>
-      <c r="C40" s="100" t="s">
-        <v>288</v>
-      </c>
-      <c r="D40" s="107" t="s">
-        <v>289</v>
-      </c>
-      <c r="E40" s="116">
-        <v>43280</v>
+      <c r="C40" s="171"/>
+      <c r="D40" s="195" t="s">
+        <v>261</v>
+      </c>
+      <c r="E40" s="191">
+        <v>43270</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="101" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="58"/>
+      <c r="A41" s="145"/>
+      <c r="B41" s="171"/>
+      <c r="C41" s="171"/>
+      <c r="D41" s="195"/>
+      <c r="E41" s="192"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="178" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="180" t="s">
-        <v>271</v>
-      </c>
-      <c r="C42" s="100" t="s">
+      <c r="A42" s="122" t="s">
+        <v>262</v>
+      </c>
+      <c r="B42" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="123" t="s">
+        <v>250</v>
+      </c>
+      <c r="D42" s="115" t="s">
+        <v>251</v>
+      </c>
+      <c r="E42" s="116">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="97" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" s="39"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="58"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="D42" s="107" t="s">
+      <c r="D44" s="107" t="s">
         <v>267</v>
       </c>
-      <c r="E42" s="116">
-        <v>43259</v>
+      <c r="E44" s="116">
+        <v>43244</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="179"/>
-      <c r="B43" s="181"/>
-      <c r="C43" s="100" t="s">
-        <v>265</v>
-      </c>
-      <c r="D43" s="107" t="s">
-        <v>266</v>
-      </c>
-      <c r="E43" s="116">
-        <v>43259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="124" t="s">
-        <v>271</v>
-      </c>
-      <c r="C44" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D44" s="107" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="116">
-        <v>43259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="124" t="s">
-        <v>271</v>
-      </c>
-      <c r="C45" s="61" t="s">
-        <v>264</v>
+    <row r="45" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="58" t="s">
+        <v>287</v>
+      </c>
+      <c r="B45" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="100" t="s">
+        <v>288</v>
       </c>
       <c r="D45" s="107" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="E45" s="116">
-        <v>43259</v>
+        <v>43280</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="101" t="s">
-        <v>273</v>
+        <v>56</v>
       </c>
       <c r="B46" s="101"/>
       <c r="C46" s="101"/>
@@ -31818,67 +31840,155 @@
       <c r="E46" s="58"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="58"/>
-      <c r="B47" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C47" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="115" t="s">
-        <v>274</v>
+      <c r="A47" s="181" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="188" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" s="100" t="s">
+        <v>265</v>
+      </c>
+      <c r="D47" s="107" t="s">
+        <v>267</v>
       </c>
       <c r="E47" s="116">
-        <v>43265</v>
+        <v>43259</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="101" t="s">
+      <c r="A48" s="182"/>
+      <c r="B48" s="190"/>
+      <c r="C48" s="100" t="s">
+        <v>265</v>
+      </c>
+      <c r="D48" s="107" t="s">
+        <v>266</v>
+      </c>
+      <c r="E48" s="116">
+        <v>43259</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="123" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D49" s="107" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="116">
+        <v>43259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="58" t="s">
+        <v>294</v>
+      </c>
+      <c r="B50" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50" s="58"/>
+      <c r="D50" s="196" t="s">
+        <v>295</v>
+      </c>
+      <c r="E50" s="116">
+        <v>43299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="123" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D51" s="107" t="s">
+        <v>263</v>
+      </c>
+      <c r="E51" s="116">
+        <v>43259</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="101" t="s">
+        <v>273</v>
+      </c>
+      <c r="B52" s="101"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="118"/>
+      <c r="E52" s="58"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="58"/>
+      <c r="B53" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="E53" s="116">
+        <v>43265</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="B48" s="101"/>
-      <c r="C48" s="101"/>
-      <c r="D48" s="118"/>
-      <c r="E48" s="58"/>
+      <c r="B54" s="101"/>
+      <c r="C54" s="101"/>
+      <c r="D54" s="118"/>
+      <c r="E54" s="58"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="58"/>
-      <c r="B49" s="124" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="58"/>
+      <c r="B55" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C49" s="58" t="s">
+      <c r="C55" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="115" t="s">
+      <c r="D55" s="115" t="s">
         <v>274</v>
       </c>
-      <c r="E49" s="117">
+      <c r="E55" s="117">
         <v>43270</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B47:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Changes to Examples Overview and Self-service Guide"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -19,15 +19,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="299">
   <si>
     <t>Document</t>
   </si>
@@ -2699,6 +2699,15 @@
   <si>
     <t>The number format in the DIR_MRK column was changed from ‘Date’ to ‘General’</t>
   </si>
+  <si>
+    <t>Section 5.9 Figure 26</t>
+  </si>
+  <si>
+    <t>Changed to New RPN request structure.</t>
+  </si>
+  <si>
+    <t>Section 6.1</t>
+  </si>
 </sst>
 </file>
 
@@ -2818,7 +2827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2837,8 +2846,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -3288,11 +3303,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3622,6 +3648,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3670,8 +3702,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3697,35 +3759,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3745,43 +3810,34 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3808,31 +3864,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4242,13 +4291,13 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="129">
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="131">
         <v>43056</v>
       </c>
       <c r="F2" s="2"/>
@@ -4268,19 +4317,19 @@
       <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="129"/>
+      <c r="E3" s="131"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="129"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="131"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -4298,7 +4347,7 @@
       <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="129"/>
+      <c r="E5" s="131"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -4316,16 +4365,16 @@
       <c r="D6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="129"/>
+      <c r="E6" s="131"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="136">
+      <c r="B7" s="138">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4334,86 +4383,86 @@
       <c r="D7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="129"/>
+      <c r="E7" s="131"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="134"/>
-      <c r="B8" s="137"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="129"/>
+      <c r="E8" s="131"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="134"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="136"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="129"/>
+      <c r="E9" s="131"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="134"/>
-      <c r="B10" s="137"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="129"/>
+      <c r="E10" s="131"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="134"/>
-      <c r="B11" s="137"/>
+      <c r="A11" s="136"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="129"/>
+      <c r="E11" s="131"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="135"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="129"/>
+      <c r="E12" s="131"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="136">
+      <c r="B13" s="138">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4422,21 +4471,21 @@
       <c r="D13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="129"/>
+      <c r="E13" s="131"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="142"/>
-      <c r="B14" s="138"/>
+      <c r="A14" s="144"/>
+      <c r="B14" s="140"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="129"/>
+      <c r="E14" s="131"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -4454,7 +4503,7 @@
       <c r="D15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="129"/>
+      <c r="E15" s="131"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -4472,19 +4521,19 @@
       <c r="D16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="129"/>
+      <c r="E16" s="131"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="132"/>
-      <c r="E17" s="129"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="131"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -4502,7 +4551,7 @@
       <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="129"/>
+      <c r="E18" s="131"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -4520,28 +4569,28 @@
       <c r="D19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="129"/>
+      <c r="E19" s="131"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="130" t="s">
+      <c r="A20" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="132"/>
-      <c r="E20" s="129"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="131"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="140">
+      <c r="B21" s="142">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4550,21 +4599,21 @@
       <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="129"/>
+      <c r="E21" s="131"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="144"/>
-      <c r="B22" s="138"/>
+      <c r="A22" s="146"/>
+      <c r="B22" s="140"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="129"/>
+      <c r="E22" s="131"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
@@ -4579,22 +4628,22 @@
       <c r="D23" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="129"/>
+      <c r="E23" s="131"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="130" t="s">
+      <c r="A24" s="132" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="129"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="131"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="139" t="s">
+      <c r="A25" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="140">
+      <c r="B25" s="142">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4603,105 +4652,105 @@
       <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="129"/>
+      <c r="E25" s="131"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="134"/>
-      <c r="B26" s="137"/>
+      <c r="A26" s="136"/>
+      <c r="B26" s="139"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="129"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="134"/>
-      <c r="B27" s="137"/>
+      <c r="A27" s="136"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="129"/>
+      <c r="E27" s="131"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="134"/>
-      <c r="B28" s="137"/>
+      <c r="A28" s="136"/>
+      <c r="B28" s="139"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="129"/>
+      <c r="E28" s="131"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="134"/>
-      <c r="B29" s="137"/>
+      <c r="A29" s="136"/>
+      <c r="B29" s="139"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="129"/>
+      <c r="E29" s="131"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="134"/>
-      <c r="B30" s="137"/>
+      <c r="A30" s="136"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="129"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="134"/>
-      <c r="B31" s="137"/>
+      <c r="A31" s="136"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="129"/>
+      <c r="E31" s="131"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="135"/>
-      <c r="B32" s="138"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="140"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="129"/>
+      <c r="E32" s="131"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -4719,7 +4768,7 @@
       <c r="D33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="129"/>
+      <c r="E33" s="131"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
@@ -4734,7 +4783,7 @@
       <c r="D34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="129"/>
+      <c r="E34" s="131"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
@@ -4749,7 +4798,7 @@
       <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="129"/>
+      <c r="E35" s="131"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
@@ -4764,7 +4813,7 @@
       <c r="D36" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="129"/>
+      <c r="E36" s="131"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
@@ -4779,7 +4828,7 @@
       <c r="D37" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="129"/>
+      <c r="E37" s="131"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
@@ -4794,7 +4843,7 @@
       <c r="D38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="129"/>
+      <c r="E38" s="131"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
@@ -4809,7 +4858,7 @@
       <c r="D39" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="129"/>
+      <c r="E39" s="131"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
@@ -4824,16 +4873,16 @@
       <c r="D40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="129"/>
+      <c r="E40" s="131"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="130" t="s">
+      <c r="A41" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="131"/>
-      <c r="C41" s="131"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="129"/>
+      <c r="B41" s="133"/>
+      <c r="C41" s="133"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="131"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4848,7 +4897,7 @@
       <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="129"/>
+      <c r="E42" s="131"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
@@ -4863,7 +4912,7 @@
       <c r="D43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="129"/>
+      <c r="E43" s="131"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
@@ -4878,7 +4927,7 @@
       <c r="D44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="129"/>
+      <c r="E44" s="131"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
@@ -4893,11 +4942,11 @@
       <c r="D45" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="129"/>
+      <c r="E45" s="131"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4907,7 +4956,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4976,7 +5025,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="147">
+      <c r="E2" s="159">
         <v>43140</v>
       </c>
     </row>
@@ -4991,7 +5040,7 @@
       <c r="D3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="147"/>
+      <c r="E3" s="159"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
@@ -5004,7 +5053,7 @@
       <c r="D4" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="147"/>
+      <c r="E4" s="159"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
@@ -5017,7 +5066,7 @@
       <c r="D5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="147"/>
+      <c r="E5" s="159"/>
     </row>
     <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
@@ -5026,13 +5075,13 @@
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="147"/>
+      <c r="E6" s="159"/>
     </row>
     <row r="7" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="161" t="s">
+      <c r="A7" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5041,68 +5090,68 @@
       <c r="D7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="147"/>
+      <c r="E7" s="159"/>
     </row>
     <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="161"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="147"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="147"/>
+      <c r="E8" s="159"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="161"/>
-      <c r="B9" s="160"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="147"/>
+      <c r="E9" s="159"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="161"/>
-      <c r="B10" s="160"/>
+      <c r="A10" s="147"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="147"/>
+      <c r="E10" s="159"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="161"/>
-      <c r="B11" s="160"/>
+      <c r="A11" s="147"/>
+      <c r="B11" s="148"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="147"/>
+      <c r="E11" s="159"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="161"/>
-      <c r="B12" s="160"/>
+      <c r="A12" s="147"/>
+      <c r="B12" s="148"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="147"/>
+      <c r="E12" s="159"/>
     </row>
     <row r="13" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="163" t="s">
+      <c r="A13" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5111,35 +5160,35 @@
       <c r="D13" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="147"/>
+      <c r="E13" s="159"/>
     </row>
     <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="163"/>
-      <c r="B14" s="160"/>
+      <c r="A14" s="150"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="147"/>
+      <c r="E14" s="159"/>
     </row>
     <row r="15" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="163"/>
-      <c r="B15" s="160"/>
+      <c r="A15" s="150"/>
+      <c r="B15" s="148"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="147"/>
+      <c r="E15" s="159"/>
     </row>
     <row r="16" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="145" t="s">
+      <c r="A16" s="151" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5148,108 +5197,108 @@
       <c r="D16" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="147"/>
+      <c r="E16" s="159"/>
     </row>
     <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="145"/>
-      <c r="B17" s="155"/>
+      <c r="A17" s="151"/>
+      <c r="B17" s="152"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="147"/>
+      <c r="E17" s="159"/>
     </row>
     <row r="18" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="145"/>
-      <c r="B18" s="155"/>
+      <c r="A18" s="151"/>
+      <c r="B18" s="152"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="147"/>
+      <c r="E18" s="159"/>
     </row>
     <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="145"/>
-      <c r="B19" s="155"/>
+      <c r="A19" s="151"/>
+      <c r="B19" s="152"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="147"/>
+      <c r="E19" s="159"/>
     </row>
     <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="145"/>
-      <c r="B20" s="155"/>
+      <c r="A20" s="151"/>
+      <c r="B20" s="152"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="147"/>
+      <c r="E20" s="159"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="145"/>
-      <c r="B21" s="155"/>
+      <c r="A21" s="151"/>
+      <c r="B21" s="152"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="147"/>
+      <c r="E21" s="159"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="145"/>
-      <c r="B22" s="155"/>
+      <c r="A22" s="151"/>
+      <c r="B22" s="152"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="147"/>
+      <c r="E22" s="159"/>
     </row>
     <row r="23" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="145"/>
-      <c r="B23" s="155"/>
+      <c r="A23" s="151"/>
+      <c r="B23" s="152"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="E23" s="147"/>
+      <c r="E23" s="159"/>
     </row>
     <row r="24" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="145"/>
-      <c r="B24" s="155"/>
-      <c r="C24" s="145" t="s">
+      <c r="A24" s="151"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="146" t="s">
+      <c r="D24" s="158" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="147"/>
+      <c r="E24" s="159"/>
     </row>
     <row r="25" spans="1:5" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="145"/>
-      <c r="B25" s="155"/>
-      <c r="C25" s="145"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="147"/>
+      <c r="A25" s="151"/>
+      <c r="B25" s="152"/>
+      <c r="C25" s="151"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="159"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="161" t="s">
+      <c r="A26" s="147" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="160" t="s">
+      <c r="B26" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5258,16 +5307,16 @@
       <c r="D26" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="147"/>
+      <c r="E26" s="159"/>
     </row>
     <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="161"/>
-      <c r="B27" s="160"/>
+      <c r="A27" s="147"/>
+      <c r="B27" s="148"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="147"/>
+      <c r="E27" s="159"/>
     </row>
     <row r="28" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
@@ -5280,7 +5329,7 @@
       <c r="D28" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="147"/>
+      <c r="E28" s="159"/>
     </row>
     <row r="29" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
@@ -5289,108 +5338,108 @@
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="147"/>
+      <c r="E29" s="159"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="162" t="s">
+      <c r="A30" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="160" t="s">
+      <c r="B30" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="145" t="s">
+      <c r="C30" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="150" t="s">
+      <c r="D30" s="162" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="147"/>
+      <c r="E30" s="159"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="162"/>
-      <c r="B31" s="160"/>
-      <c r="C31" s="145"/>
-      <c r="D31" s="150"/>
-      <c r="E31" s="147"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="151"/>
+      <c r="D31" s="162"/>
+      <c r="E31" s="159"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="162"/>
-      <c r="B32" s="160"/>
+      <c r="A32" s="149"/>
+      <c r="B32" s="148"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="147"/>
+      <c r="E32" s="159"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="162"/>
-      <c r="B33" s="160"/>
+      <c r="A33" s="149"/>
+      <c r="B33" s="148"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="147"/>
+      <c r="E33" s="159"/>
     </row>
     <row r="34" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="162"/>
-      <c r="B34" s="160"/>
+      <c r="A34" s="149"/>
+      <c r="B34" s="148"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="147"/>
+      <c r="E34" s="159"/>
     </row>
     <row r="35" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="162"/>
-      <c r="B35" s="160"/>
+      <c r="A35" s="149"/>
+      <c r="B35" s="148"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="147"/>
+      <c r="E35" s="159"/>
     </row>
     <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="162"/>
-      <c r="B36" s="160"/>
+      <c r="A36" s="149"/>
+      <c r="B36" s="148"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
       <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="147"/>
+      <c r="E36" s="159"/>
     </row>
     <row r="37" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="162"/>
-      <c r="B37" s="160"/>
-      <c r="C37" s="151" t="s">
+      <c r="A37" s="149"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="163" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="153" t="s">
+      <c r="D37" s="165" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="147"/>
+      <c r="E37" s="159"/>
     </row>
     <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="162"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="153"/>
-      <c r="E38" s="147"/>
+      <c r="A38" s="149"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="159"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="161" t="s">
+      <c r="A39" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5399,16 +5448,16 @@
       <c r="D39" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="147"/>
+      <c r="E39" s="159"/>
     </row>
     <row r="40" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="161"/>
-      <c r="B40" s="160"/>
+      <c r="A40" s="147"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="147"/>
+      <c r="E40" s="159"/>
     </row>
     <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
@@ -5421,7 +5470,7 @@
       <c r="D41" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="147"/>
+      <c r="E41" s="159"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
@@ -5430,90 +5479,90 @@
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="147"/>
+      <c r="E42" s="159"/>
     </row>
     <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="162" t="s">
+      <c r="A43" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="160" t="s">
+      <c r="B43" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="147"/>
+      <c r="E43" s="159"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="162"/>
-      <c r="B44" s="160"/>
+      <c r="A44" s="149"/>
+      <c r="B44" s="148"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D44" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="147"/>
+      <c r="E44" s="159"/>
     </row>
     <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="157" t="s">
+      <c r="A45" s="155" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="160" t="s">
+      <c r="B45" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="147"/>
+      <c r="E45" s="159"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="158"/>
-      <c r="B46" s="160"/>
+      <c r="A46" s="156"/>
+      <c r="B46" s="148"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="147"/>
+      <c r="E46" s="159"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="158"/>
-      <c r="B47" s="160"/>
+      <c r="A47" s="156"/>
+      <c r="B47" s="148"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="147"/>
+      <c r="E47" s="159"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="159"/>
-      <c r="B48" s="160"/>
+      <c r="A48" s="157"/>
+      <c r="B48" s="148"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="147"/>
+      <c r="E48" s="159"/>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="155" t="s">
+      <c r="A49" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="155" t="s">
+      <c r="B49" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="147"/>
+      <c r="E49" s="159"/>
       <c r="H49" s="42"/>
       <c r="L49" s="42"/>
       <c r="P49" s="42"/>
@@ -9611,15 +9660,15 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="155"/>
-      <c r="B50" s="155"/>
+      <c r="A50" s="152"/>
+      <c r="B50" s="152"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="147"/>
+      <c r="E50" s="159"/>
       <c r="H50" s="42"/>
       <c r="L50" s="42"/>
       <c r="P50" s="42"/>
@@ -13717,15 +13766,15 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="155"/>
-      <c r="B51" s="155"/>
+      <c r="A51" s="152"/>
+      <c r="B51" s="152"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="E51" s="147"/>
+      <c r="E51" s="159"/>
       <c r="H51" s="42"/>
       <c r="L51" s="42"/>
       <c r="P51" s="42"/>
@@ -17823,15 +17872,15 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="155"/>
-      <c r="B52" s="155"/>
+      <c r="A52" s="152"/>
+      <c r="B52" s="152"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="147"/>
+      <c r="E52" s="159"/>
       <c r="H52" s="42"/>
       <c r="L52" s="42"/>
       <c r="P52" s="42"/>
@@ -21929,15 +21978,15 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="155"/>
-      <c r="B53" s="155"/>
-      <c r="C53" s="149" t="s">
+      <c r="A53" s="152"/>
+      <c r="B53" s="152"/>
+      <c r="C53" s="161" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="150" t="s">
+      <c r="D53" s="162" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="147"/>
+      <c r="E53" s="159"/>
       <c r="H53" s="42"/>
       <c r="L53" s="42"/>
       <c r="P53" s="42"/>
@@ -26035,11 +26084,11 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="155"/>
-      <c r="B54" s="155"/>
-      <c r="C54" s="149"/>
-      <c r="D54" s="150"/>
-      <c r="E54" s="147"/>
+      <c r="A54" s="152"/>
+      <c r="B54" s="152"/>
+      <c r="C54" s="161"/>
+      <c r="D54" s="162"/>
+      <c r="E54" s="159"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -30143,7 +30192,7 @@
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
-      <c r="E55" s="147"/>
+      <c r="E55" s="159"/>
     </row>
     <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
@@ -30156,13 +30205,13 @@
       <c r="D56" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="147"/>
+      <c r="E56" s="159"/>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="154" t="s">
+      <c r="A57" s="153" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="155" t="s">
+      <c r="B57" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30171,204 +30220,204 @@
       <c r="D57" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="147"/>
+      <c r="E57" s="159"/>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="154"/>
-      <c r="B58" s="155"/>
+      <c r="A58" s="153"/>
+      <c r="B58" s="152"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="E58" s="147"/>
+      <c r="E58" s="159"/>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="154"/>
-      <c r="B59" s="155"/>
+      <c r="A59" s="153"/>
+      <c r="B59" s="152"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D59" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="147"/>
+      <c r="E59" s="159"/>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="154"/>
-      <c r="B60" s="155"/>
+      <c r="A60" s="153"/>
+      <c r="B60" s="152"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D60" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="147"/>
+      <c r="E60" s="159"/>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="154"/>
-      <c r="B61" s="155"/>
+      <c r="A61" s="153"/>
+      <c r="B61" s="152"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="147"/>
+      <c r="E61" s="159"/>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="154"/>
-      <c r="B62" s="155"/>
+      <c r="A62" s="153"/>
+      <c r="B62" s="152"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="147"/>
+      <c r="E62" s="159"/>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="154"/>
-      <c r="B63" s="155"/>
+      <c r="A63" s="153"/>
+      <c r="B63" s="152"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D63" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="147"/>
+      <c r="E63" s="159"/>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="154"/>
-      <c r="B64" s="155"/>
+      <c r="A64" s="153"/>
+      <c r="B64" s="152"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="147"/>
+      <c r="E64" s="159"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="154"/>
-      <c r="B65" s="155"/>
+      <c r="A65" s="153"/>
+      <c r="B65" s="152"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="147"/>
+      <c r="E65" s="159"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="154"/>
-      <c r="B66" s="155"/>
+      <c r="A66" s="153"/>
+      <c r="B66" s="152"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="147"/>
+      <c r="E66" s="159"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="154"/>
-      <c r="B67" s="155"/>
+      <c r="A67" s="153"/>
+      <c r="B67" s="152"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E67" s="147"/>
+      <c r="E67" s="159"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="154"/>
-      <c r="B68" s="155"/>
+      <c r="A68" s="153"/>
+      <c r="B68" s="152"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="147"/>
+      <c r="E68" s="159"/>
     </row>
     <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="154"/>
-      <c r="B69" s="155"/>
+      <c r="A69" s="153"/>
+      <c r="B69" s="152"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E69" s="147"/>
+      <c r="E69" s="159"/>
     </row>
     <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="154"/>
-      <c r="B70" s="155"/>
+      <c r="A70" s="153"/>
+      <c r="B70" s="152"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="147"/>
+      <c r="E70" s="159"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="154"/>
-      <c r="B71" s="155"/>
+      <c r="A71" s="153"/>
+      <c r="B71" s="152"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="147"/>
+      <c r="E71" s="159"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="154"/>
-      <c r="B72" s="155"/>
+      <c r="A72" s="153"/>
+      <c r="B72" s="152"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="147"/>
+      <c r="E72" s="159"/>
     </row>
     <row r="73" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="154"/>
-      <c r="B73" s="155"/>
+      <c r="A73" s="153"/>
+      <c r="B73" s="152"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="147"/>
+      <c r="E73" s="159"/>
     </row>
     <row r="74" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="154"/>
-      <c r="B74" s="155"/>
+      <c r="A74" s="153"/>
+      <c r="B74" s="152"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="E74" s="147"/>
+      <c r="E74" s="159"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="154"/>
-      <c r="B75" s="155"/>
-      <c r="C75" s="148"/>
-      <c r="D75" s="156" t="s">
+      <c r="A75" s="153"/>
+      <c r="B75" s="152"/>
+      <c r="C75" s="160"/>
+      <c r="D75" s="154" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="147"/>
+      <c r="E75" s="159"/>
     </row>
     <row r="76" spans="1:5" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="154"/>
-      <c r="B76" s="155"/>
-      <c r="C76" s="148"/>
-      <c r="D76" s="156"/>
-      <c r="E76" s="147"/>
+      <c r="A76" s="153"/>
+      <c r="B76" s="152"/>
+      <c r="C76" s="160"/>
+      <c r="D76" s="154"/>
+      <c r="E76" s="159"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30377,7 +30426,7 @@
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
-      <c r="E77" s="147"/>
+      <c r="E77" s="159"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="48"/>
@@ -30393,8 +30442,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30403,13 +30452,30 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="31">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E2:E77"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30424,23 +30490,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E2:E77"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30488,7 +30537,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="129">
+      <c r="E2" s="131">
         <v>43179</v>
       </c>
     </row>
@@ -30499,13 +30548,13 @@
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="129"/>
+      <c r="E3" s="131"/>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30514,158 +30563,158 @@
       <c r="D4" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="129"/>
+      <c r="E4" s="131"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="161"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="173" t="s">
+      <c r="A5" s="147"/>
+      <c r="B5" s="148"/>
+      <c r="C5" s="167" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="172" t="s">
+      <c r="D5" s="166" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="129"/>
+      <c r="E5" s="131"/>
     </row>
     <row r="6" spans="1:5" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="161"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="173"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="129"/>
+      <c r="A6" s="147"/>
+      <c r="B6" s="148"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="166"/>
+      <c r="E6" s="131"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="161"/>
-      <c r="B7" s="160"/>
+      <c r="A7" s="147"/>
+      <c r="B7" s="148"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
-      <c r="E7" s="129"/>
+      <c r="E7" s="131"/>
     </row>
     <row r="8" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="161"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="147"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
-      <c r="E8" s="129"/>
+      <c r="E8" s="131"/>
     </row>
     <row r="9" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="161"/>
-      <c r="B9" s="160"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
-      <c r="E9" s="129"/>
+      <c r="E9" s="131"/>
     </row>
     <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="163" t="s">
+      <c r="A10" s="150" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="160" t="s">
+      <c r="B10" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="170"/>
-      <c r="D10" s="172" t="s">
+      <c r="C10" s="169"/>
+      <c r="D10" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="129"/>
+      <c r="E10" s="131"/>
     </row>
     <row r="11" spans="1:5" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="163"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="129"/>
+      <c r="A11" s="150"/>
+      <c r="B11" s="148"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="166"/>
+      <c r="E11" s="131"/>
     </row>
     <row r="12" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="163"/>
-      <c r="B12" s="160"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="172"/>
-      <c r="E12" s="129"/>
+      <c r="A12" s="150"/>
+      <c r="B12" s="148"/>
+      <c r="C12" s="169"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="131"/>
     </row>
     <row r="13" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="145" t="s">
+      <c r="A13" s="151" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="174"/>
-      <c r="D13" s="172" t="s">
+      <c r="C13" s="168"/>
+      <c r="D13" s="166" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="129"/>
+      <c r="E13" s="131"/>
     </row>
     <row r="14" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="145"/>
-      <c r="B14" s="155"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="172"/>
-      <c r="E14" s="129"/>
+      <c r="A14" s="151"/>
+      <c r="B14" s="152"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="166"/>
+      <c r="E14" s="131"/>
     </row>
     <row r="15" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="145"/>
-      <c r="B15" s="155"/>
-      <c r="C15" s="174"/>
+      <c r="A15" s="151"/>
+      <c r="B15" s="152"/>
+      <c r="C15" s="168"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="129"/>
+      <c r="E15" s="131"/>
     </row>
     <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="145"/>
-      <c r="B16" s="155"/>
-      <c r="C16" s="174"/>
+      <c r="A16" s="151"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="168"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="129"/>
+      <c r="E16" s="131"/>
     </row>
     <row r="17" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="145"/>
-      <c r="B17" s="155"/>
-      <c r="C17" s="174"/>
+      <c r="A17" s="151"/>
+      <c r="B17" s="152"/>
+      <c r="C17" s="168"/>
       <c r="D17" s="49"/>
-      <c r="E17" s="129"/>
+      <c r="E17" s="131"/>
     </row>
     <row r="18" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="145"/>
-      <c r="B18" s="155"/>
-      <c r="C18" s="174"/>
+      <c r="A18" s="151"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="168"/>
       <c r="D18" s="49"/>
-      <c r="E18" s="129"/>
+      <c r="E18" s="131"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="145"/>
-      <c r="B19" s="155"/>
-      <c r="C19" s="174"/>
+      <c r="A19" s="151"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="168"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="129"/>
+      <c r="E19" s="131"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="145"/>
-      <c r="B20" s="155"/>
-      <c r="C20" s="174"/>
+      <c r="A20" s="151"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="168"/>
       <c r="D20" s="49"/>
-      <c r="E20" s="129"/>
+      <c r="E20" s="131"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="145"/>
-      <c r="B21" s="155"/>
-      <c r="C21" s="174"/>
+      <c r="A21" s="151"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="168"/>
       <c r="D21" s="49"/>
-      <c r="E21" s="129"/>
+      <c r="E21" s="131"/>
     </row>
     <row r="22" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="145"/>
-      <c r="B22" s="155"/>
-      <c r="C22" s="174"/>
+      <c r="A22" s="151"/>
+      <c r="B22" s="152"/>
+      <c r="C22" s="168"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="129"/>
+      <c r="E22" s="131"/>
     </row>
     <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="145"/>
-      <c r="B23" s="155"/>
-      <c r="C23" s="174"/>
+      <c r="A23" s="151"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="168"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="129"/>
+      <c r="E23" s="131"/>
     </row>
     <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
@@ -30680,7 +30729,7 @@
       <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="129"/>
+      <c r="E24" s="131"/>
     </row>
     <row r="25" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
@@ -30695,7 +30744,7 @@
       <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="E25" s="129"/>
+      <c r="E25" s="131"/>
     </row>
     <row r="26" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
@@ -30708,7 +30757,7 @@
       <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="129"/>
+      <c r="E26" s="131"/>
     </row>
     <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
@@ -30717,7 +30766,7 @@
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="129"/>
+      <c r="E27" s="131"/>
     </row>
     <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
@@ -30732,7 +30781,7 @@
       <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="129"/>
+      <c r="E28" s="131"/>
     </row>
     <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="85"/>
@@ -30743,7 +30792,7 @@
       <c r="D29" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="129"/>
+      <c r="E29" s="131"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
@@ -30754,7 +30803,7 @@
       <c r="D30" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="E30" s="129"/>
+      <c r="E30" s="131"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
@@ -30765,13 +30814,13 @@
       <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="129"/>
+      <c r="E31" s="131"/>
     </row>
     <row r="32" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="164" t="s">
+      <c r="A32" s="177" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="167" t="s">
+      <c r="B32" s="180" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30780,39 +30829,39 @@
       <c r="D32" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="E32" s="129"/>
+      <c r="E32" s="131"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="165"/>
-      <c r="B33" s="168"/>
+      <c r="A33" s="178"/>
+      <c r="B33" s="181"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
-      <c r="E33" s="129"/>
+      <c r="E33" s="131"/>
     </row>
     <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="165"/>
-      <c r="B34" s="168"/>
+      <c r="A34" s="178"/>
+      <c r="B34" s="181"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
-      <c r="E34" s="129"/>
+      <c r="E34" s="131"/>
     </row>
     <row r="35" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="165"/>
-      <c r="B35" s="168"/>
+      <c r="A35" s="178"/>
+      <c r="B35" s="181"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
-      <c r="E35" s="129"/>
+      <c r="E35" s="131"/>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="166"/>
-      <c r="B36" s="169"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="182"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="129"/>
+      <c r="E36" s="131"/>
     </row>
     <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
@@ -30825,7 +30874,7 @@
       <c r="D37" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="129"/>
+      <c r="E37" s="131"/>
     </row>
     <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
@@ -30834,13 +30883,13 @@
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
-      <c r="E38" s="129"/>
+      <c r="E38" s="131"/>
     </row>
     <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="162" t="s">
+      <c r="A39" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30849,108 +30898,108 @@
       <c r="D39" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="E39" s="129"/>
+      <c r="E39" s="131"/>
     </row>
     <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="162"/>
-      <c r="B40" s="160"/>
+      <c r="A40" s="149"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="129"/>
+      <c r="E40" s="131"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="160" t="s">
+      <c r="B41" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="170" t="s">
+      <c r="C41" s="169" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="145" t="s">
+      <c r="D41" s="151" t="s">
         <v>228</v>
       </c>
-      <c r="E41" s="129"/>
+      <c r="E41" s="131"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="161"/>
-      <c r="B42" s="160"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="145"/>
-      <c r="E42" s="129"/>
+      <c r="A42" s="147"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="151"/>
+      <c r="E42" s="131"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="161"/>
-      <c r="B43" s="160"/>
-      <c r="C43" s="170" t="s">
+      <c r="A43" s="147"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="169" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="156" t="s">
+      <c r="D43" s="154" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="129"/>
+      <c r="E43" s="131"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="161"/>
-      <c r="B44" s="160"/>
-      <c r="C44" s="170"/>
-      <c r="D44" s="156"/>
-      <c r="E44" s="129"/>
+      <c r="A44" s="147"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="169"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="131"/>
     </row>
     <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="154" t="s">
+      <c r="A45" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="155" t="s">
+      <c r="B45" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="178"/>
+      <c r="C45" s="173"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="129"/>
+      <c r="E45" s="131"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="154"/>
-      <c r="B46" s="155"/>
-      <c r="C46" s="179"/>
-      <c r="D46" s="175" t="s">
+      <c r="A46" s="153"/>
+      <c r="B46" s="152"/>
+      <c r="C46" s="174"/>
+      <c r="D46" s="170" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="129"/>
+      <c r="E46" s="131"/>
     </row>
     <row r="47" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="154"/>
-      <c r="B47" s="155"/>
-      <c r="C47" s="179"/>
-      <c r="D47" s="176"/>
-      <c r="E47" s="129"/>
+      <c r="A47" s="153"/>
+      <c r="B47" s="152"/>
+      <c r="C47" s="174"/>
+      <c r="D47" s="171"/>
+      <c r="E47" s="131"/>
     </row>
     <row r="48" spans="1:5" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="154"/>
-      <c r="B48" s="155"/>
-      <c r="C48" s="180"/>
-      <c r="D48" s="176"/>
-      <c r="E48" s="129"/>
+      <c r="A48" s="153"/>
+      <c r="B48" s="152"/>
+      <c r="C48" s="175"/>
+      <c r="D48" s="171"/>
+      <c r="E48" s="131"/>
     </row>
     <row r="49" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="154"/>
-      <c r="B49" s="155"/>
-      <c r="C49" s="149"/>
-      <c r="D49" s="176"/>
-      <c r="E49" s="129"/>
+      <c r="A49" s="153"/>
+      <c r="B49" s="152"/>
+      <c r="C49" s="161"/>
+      <c r="D49" s="171"/>
+      <c r="E49" s="131"/>
     </row>
     <row r="50" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="154"/>
-      <c r="B50" s="155"/>
-      <c r="C50" s="149"/>
-      <c r="D50" s="177"/>
-      <c r="E50" s="129"/>
+      <c r="A50" s="153"/>
+      <c r="B50" s="152"/>
+      <c r="C50" s="161"/>
+      <c r="D50" s="172"/>
+      <c r="E50" s="131"/>
     </row>
     <row r="51" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30959,7 +31008,7 @@
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
-      <c r="E51" s="129"/>
+      <c r="E51" s="131"/>
     </row>
     <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
@@ -30972,13 +31021,13 @@
       <c r="D52" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="129"/>
+      <c r="E52" s="131"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="155" t="s">
+      <c r="B53" s="152" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30987,148 +31036,148 @@
       <c r="D53" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="129"/>
+      <c r="E53" s="131"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="155"/>
-      <c r="B54" s="155"/>
+      <c r="A54" s="152"/>
+      <c r="B54" s="152"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
       <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="129"/>
+      <c r="E54" s="131"/>
     </row>
     <row r="55" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="155"/>
-      <c r="B55" s="155"/>
+      <c r="A55" s="152"/>
+      <c r="B55" s="152"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="129"/>
+      <c r="E55" s="131"/>
     </row>
     <row r="56" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="155"/>
-      <c r="B56" s="155"/>
-      <c r="C56" s="171" t="s">
+      <c r="A56" s="152"/>
+      <c r="B56" s="152"/>
+      <c r="C56" s="176" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="E56" s="129"/>
+      <c r="E56" s="131"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="155"/>
-      <c r="B57" s="155"/>
-      <c r="C57" s="171"/>
+      <c r="A57" s="152"/>
+      <c r="B57" s="152"/>
+      <c r="C57" s="176"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="129"/>
+      <c r="E57" s="131"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="155"/>
-      <c r="B58" s="155"/>
+      <c r="A58" s="152"/>
+      <c r="B58" s="152"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
       <c r="D58" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E58" s="129"/>
+      <c r="E58" s="131"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="155"/>
-      <c r="B59" s="155"/>
+      <c r="A59" s="152"/>
+      <c r="B59" s="152"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
       <c r="D59" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="129"/>
+      <c r="E59" s="131"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="155"/>
-      <c r="B60" s="155"/>
-      <c r="C60" s="171" t="s">
+      <c r="A60" s="152"/>
+      <c r="B60" s="152"/>
+      <c r="C60" s="176" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="129"/>
+      <c r="E60" s="131"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="155"/>
-      <c r="B61" s="155"/>
-      <c r="C61" s="171"/>
+      <c r="A61" s="152"/>
+      <c r="B61" s="152"/>
+      <c r="C61" s="176"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="129"/>
+      <c r="E61" s="131"/>
     </row>
     <row r="62" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="155"/>
-      <c r="B62" s="155"/>
-      <c r="C62" s="171"/>
+      <c r="A62" s="152"/>
+      <c r="B62" s="152"/>
+      <c r="C62" s="176"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="E62" s="129"/>
+      <c r="E62" s="131"/>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="155"/>
-      <c r="B63" s="155"/>
-      <c r="C63" s="170" t="s">
+      <c r="A63" s="152"/>
+      <c r="B63" s="152"/>
+      <c r="C63" s="169" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="E63" s="129"/>
+      <c r="E63" s="131"/>
     </row>
     <row r="64" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="155"/>
-      <c r="B64" s="155"/>
-      <c r="C64" s="170"/>
-      <c r="D64" s="156" t="s">
+      <c r="A64" s="152"/>
+      <c r="B64" s="152"/>
+      <c r="C64" s="169"/>
+      <c r="D64" s="154" t="s">
         <v>220</v>
       </c>
-      <c r="E64" s="129"/>
+      <c r="E64" s="131"/>
     </row>
     <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="155"/>
-      <c r="B65" s="155"/>
-      <c r="C65" s="170"/>
-      <c r="D65" s="156"/>
-      <c r="E65" s="129"/>
+      <c r="A65" s="152"/>
+      <c r="B65" s="152"/>
+      <c r="C65" s="169"/>
+      <c r="D65" s="154"/>
+      <c r="E65" s="131"/>
     </row>
     <row r="66" spans="1:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="155"/>
-      <c r="B66" s="155"/>
-      <c r="C66" s="170"/>
-      <c r="D66" s="156"/>
-      <c r="E66" s="129"/>
+      <c r="A66" s="152"/>
+      <c r="B66" s="152"/>
+      <c r="C66" s="169"/>
+      <c r="D66" s="154"/>
+      <c r="E66" s="131"/>
     </row>
     <row r="67" spans="1:5" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="155"/>
-      <c r="B67" s="155"/>
-      <c r="C67" s="170"/>
-      <c r="D67" s="156"/>
-      <c r="E67" s="129"/>
+      <c r="A67" s="152"/>
+      <c r="B67" s="152"/>
+      <c r="C67" s="169"/>
+      <c r="D67" s="154"/>
+      <c r="E67" s="131"/>
     </row>
     <row r="68" spans="1:5" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
-      <c r="E68" s="129"/>
+      <c r="E68" s="131"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
@@ -31178,6 +31227,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C63:C67"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
@@ -31194,24 +31261,6 @@
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="C45:C48"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="B53:B67"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C63:C67"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31220,10 +31269,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31262,10 +31311,10 @@
       <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="58"/>
@@ -31277,8 +31326,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="145"/>
-      <c r="B4" s="171"/>
+      <c r="A4" s="151"/>
+      <c r="B4" s="176"/>
       <c r="C4" s="123" t="s">
         <v>235</v>
       </c>
@@ -31293,7 +31342,7 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="171"/>
+      <c r="B5" s="176"/>
       <c r="C5" s="123" t="s">
         <v>235</v>
       </c>
@@ -31308,7 +31357,7 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="171"/>
+      <c r="B6" s="176"/>
       <c r="C6" s="123" t="s">
         <v>22</v>
       </c>
@@ -31320,10 +31369,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="183" t="s">
+      <c r="A7" s="193" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="171"/>
+      <c r="B7" s="176"/>
       <c r="C7" s="58"/>
       <c r="D7" s="110" t="s">
         <v>261</v>
@@ -31333,8 +31382,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="184"/>
-      <c r="B8" s="171"/>
+      <c r="A8" s="194"/>
+      <c r="B8" s="176"/>
       <c r="C8" s="58"/>
       <c r="D8" s="107" t="s">
         <v>276</v>
@@ -31347,7 +31396,7 @@
       <c r="A9" t="s">
         <v>293</v>
       </c>
-      <c r="B9" s="171"/>
+      <c r="B9" s="176"/>
       <c r="C9" s="58" t="s">
         <v>30</v>
       </c>
@@ -31360,7 +31409,7 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="171"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="58"/>
       <c r="D10" s="109" t="s">
         <v>259</v>
@@ -31379,10 +31428,10 @@
       <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="197" t="s">
+      <c r="A12" s="190" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="171" t="s">
+      <c r="B12" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C12" s="58"/>
@@ -31394,8 +31443,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="198"/>
-      <c r="B13" s="171"/>
+      <c r="A13" s="191"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="58"/>
       <c r="D13" s="107" t="s">
         <v>252</v>
@@ -31405,8 +31454,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="199"/>
-      <c r="B14" s="171"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="58"/>
       <c r="D14" s="107" t="s">
         <v>254</v>
@@ -31431,13 +31480,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="145" t="s">
+      <c r="A16" s="151" t="s">
         <v>222</v>
       </c>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="176" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="193" t="s">
+      <c r="C16" s="185" t="s">
         <v>239</v>
       </c>
       <c r="D16" s="112" t="s">
@@ -31448,9 +31497,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="145"/>
-      <c r="B17" s="171"/>
-      <c r="C17" s="194"/>
+      <c r="A17" s="151"/>
+      <c r="B17" s="176"/>
+      <c r="C17" s="186"/>
       <c r="D17" s="104" t="s">
         <v>278</v>
       </c>
@@ -31459,8 +31508,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="145"/>
-      <c r="B18" s="171"/>
+      <c r="A18" s="151"/>
+      <c r="B18" s="176"/>
       <c r="C18" s="96" t="s">
         <v>240</v>
       </c>
@@ -31511,10 +31560,10 @@
       <c r="E21" s="58"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="183" t="s">
+      <c r="A22" s="193" t="s">
         <v>260</v>
       </c>
-      <c r="B22" s="171" t="s">
+      <c r="B22" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C22" s="58"/>
@@ -31526,8 +31575,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="184"/>
-      <c r="B23" s="171"/>
+      <c r="A23" s="194"/>
+      <c r="B23" s="176"/>
       <c r="C23" s="58"/>
       <c r="D23" s="107" t="s">
         <v>257</v>
@@ -31554,10 +31603,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="185" t="s">
+      <c r="A25" s="195" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="188" t="s">
+      <c r="B25" s="198" t="s">
         <v>234</v>
       </c>
       <c r="C25" s="58" t="s">
@@ -31571,8 +31620,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="186"/>
-      <c r="B26" s="189"/>
+      <c r="A26" s="196"/>
+      <c r="B26" s="199"/>
       <c r="C26" t="s">
         <v>270</v>
       </c>
@@ -31584,8 +31633,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="186"/>
-      <c r="B27" s="189"/>
+      <c r="A27" s="196"/>
+      <c r="B27" s="199"/>
       <c r="C27" s="58" t="s">
         <v>269</v>
       </c>
@@ -31597,8 +31646,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="186"/>
-      <c r="B28" s="189"/>
+      <c r="A28" s="196"/>
+      <c r="B28" s="199"/>
       <c r="C28" s="103" t="s">
         <v>277</v>
       </c>
@@ -31610,8 +31659,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="186"/>
-      <c r="B29" s="189"/>
+      <c r="A29" s="196"/>
+      <c r="B29" s="199"/>
       <c r="C29" s="58" t="s">
         <v>284</v>
       </c>
@@ -31623,8 +31672,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="186"/>
-      <c r="B30" s="189"/>
+      <c r="A30" s="196"/>
+      <c r="B30" s="199"/>
       <c r="C30" s="58" t="s">
         <v>285</v>
       </c>
@@ -31636,8 +31685,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="186"/>
-      <c r="B31" s="189"/>
+      <c r="A31" s="196"/>
+      <c r="B31" s="199"/>
       <c r="C31" s="125" t="s">
         <v>290</v>
       </c>
@@ -31649,8 +31698,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="186"/>
-      <c r="B32" s="189"/>
+      <c r="A32" s="196"/>
+      <c r="B32" s="199"/>
       <c r="C32" s="125" t="s">
         <v>291</v>
       </c>
@@ -31662,8 +31711,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="186"/>
-      <c r="B33" s="189"/>
+      <c r="A33" s="196"/>
+      <c r="B33" s="199"/>
       <c r="C33" s="125" t="s">
         <v>292</v>
       </c>
@@ -31675,8 +31724,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="187"/>
-      <c r="B34" s="190"/>
+      <c r="A34" s="197"/>
+      <c r="B34" s="200"/>
       <c r="C34" s="95" t="s">
         <v>244</v>
       </c>
@@ -31706,204 +31755,198 @@
       <c r="E36" s="58"/>
     </row>
     <row r="37" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="145" t="s">
+      <c r="A37" s="176" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="171" t="s">
+      <c r="B37" s="176" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="123" t="s">
+      <c r="C37" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="E37" s="116">
+      <c r="E37" s="203">
         <v>43244</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="145"/>
-      <c r="B38" s="171"/>
-      <c r="C38" s="123">
+      <c r="A38" s="176"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="129">
         <v>10.1</v>
       </c>
-      <c r="D38" s="107" t="s">
+      <c r="D38" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="E38" s="116">
+      <c r="E38" s="203">
         <v>43244</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="145"/>
-      <c r="B39" s="171"/>
-      <c r="C39" s="123">
+      <c r="A39" s="176"/>
+      <c r="B39" s="176"/>
+      <c r="C39" s="129">
         <v>10.199999999999999</v>
       </c>
-      <c r="D39" s="107" t="s">
+      <c r="D39" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="E39" s="116">
+      <c r="E39" s="203">
         <v>43244</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="145" t="s">
-        <v>247</v>
-      </c>
-      <c r="B40" s="171" t="s">
-        <v>234</v>
-      </c>
-      <c r="C40" s="171"/>
-      <c r="D40" s="195" t="s">
-        <v>261</v>
-      </c>
-      <c r="E40" s="191">
-        <v>43270</v>
+      <c r="A40" s="176"/>
+      <c r="B40" s="176"/>
+      <c r="C40" s="205" t="s">
+        <v>296</v>
+      </c>
+      <c r="D40" s="206" t="s">
+        <v>297</v>
+      </c>
+      <c r="E40" s="116">
+        <v>43299</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="145"/>
-      <c r="B41" s="171"/>
-      <c r="C41" s="171"/>
-      <c r="D41" s="195"/>
-      <c r="E41" s="192"/>
+      <c r="A41" s="151" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" s="176" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="200"/>
+      <c r="D41" s="204" t="s">
+        <v>261</v>
+      </c>
+      <c r="E41" s="183">
+        <v>43270</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="122" t="s">
+      <c r="A42" s="151"/>
+      <c r="B42" s="176"/>
+      <c r="C42" s="176"/>
+      <c r="D42" s="187"/>
+      <c r="E42" s="184"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="122" t="s">
         <v>262</v>
       </c>
-      <c r="B42" s="123" t="s">
+      <c r="B43" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C42" s="123" t="s">
+      <c r="C43" s="123" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="115" t="s">
+      <c r="D43" s="115" t="s">
         <v>251</v>
       </c>
-      <c r="E42" s="116">
+      <c r="E43" s="116">
         <v>43244</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="97" t="s">
+    <row r="44" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="97" t="s">
         <v>248</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="58"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="58"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="58" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="58" t="s">
         <v>249</v>
-      </c>
-      <c r="B44" s="123" t="s">
-        <v>234</v>
-      </c>
-      <c r="C44" s="100" t="s">
-        <v>265</v>
-      </c>
-      <c r="D44" s="107" t="s">
-        <v>267</v>
-      </c>
-      <c r="E44" s="116">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="58" t="s">
-        <v>287</v>
       </c>
       <c r="B45" s="123" t="s">
         <v>234</v>
       </c>
       <c r="C45" s="100" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="D45" s="107" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="E45" s="116">
-        <v>43280</v>
+        <v>43244</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="101" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="101"/>
-      <c r="C46" s="101"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="58"/>
+      <c r="A46" s="207" t="s">
+        <v>287</v>
+      </c>
+      <c r="B46" s="201" t="s">
+        <v>234</v>
+      </c>
+      <c r="C46" s="206" t="s">
+        <v>298</v>
+      </c>
+      <c r="D46" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E46" s="116">
+        <v>43299</v>
+      </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="181" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="188" t="s">
-        <v>271</v>
-      </c>
+    <row r="47" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="208"/>
+      <c r="B47" s="202"/>
       <c r="C47" s="100" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="D47" s="107" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="E47" s="116">
-        <v>43259</v>
+        <v>43280</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="182"/>
-      <c r="B48" s="190"/>
-      <c r="C48" s="100" t="s">
+      <c r="A48" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="101"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="118"/>
+      <c r="E48" s="58"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="188" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="198" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" s="100" t="s">
         <v>265</v>
       </c>
-      <c r="D48" s="107" t="s">
-        <v>266</v>
-      </c>
-      <c r="E48" s="116">
-        <v>43259</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="123" t="s">
-        <v>271</v>
-      </c>
-      <c r="C49" s="61" t="s">
-        <v>264</v>
-      </c>
       <c r="D49" s="107" t="s">
-        <v>100</v>
+        <v>267</v>
       </c>
       <c r="E49" s="116">
         <v>43259</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="58" t="s">
-        <v>294</v>
-      </c>
-      <c r="B50" s="128" t="s">
-        <v>271</v>
-      </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="196" t="s">
-        <v>295</v>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="189"/>
+      <c r="B50" s="200"/>
+      <c r="C50" s="100" t="s">
+        <v>265</v>
+      </c>
+      <c r="D50" s="107" t="s">
+        <v>266</v>
       </c>
       <c r="E50" s="116">
-        <v>43299</v>
+        <v>43259</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="99" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="123" t="s">
         <v>271</v>
@@ -31912,39 +31955,47 @@
         <v>264</v>
       </c>
       <c r="D51" s="107" t="s">
-        <v>263</v>
+        <v>100</v>
       </c>
       <c r="E51" s="116">
         <v>43259</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="101" t="s">
-        <v>273</v>
-      </c>
-      <c r="B52" s="101"/>
-      <c r="C52" s="101"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="58"/>
+    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="58" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52" s="128" t="s">
+        <v>271</v>
+      </c>
+      <c r="C52" s="58"/>
+      <c r="D52" s="130" t="s">
+        <v>295</v>
+      </c>
+      <c r="E52" s="116">
+        <v>43299</v>
+      </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="58"/>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="99" t="s">
+        <v>60</v>
+      </c>
       <c r="B53" s="123" t="s">
-        <v>234</v>
-      </c>
-      <c r="C53" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="115" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="C53" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="107" t="s">
+        <v>263</v>
       </c>
       <c r="E53" s="116">
-        <v>43265</v>
+        <v>43259</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="101" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B54" s="101"/>
       <c r="C54" s="101"/>
@@ -31962,20 +32013,40 @@
       <c r="D55" s="115" t="s">
         <v>274</v>
       </c>
-      <c r="E55" s="117">
+      <c r="E55" s="116">
+        <v>43265</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="B56" s="101"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="58"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="58"/>
+      <c r="B57" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="E57" s="117">
         <v>43270</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A40:A41"/>
+  <mergeCells count="23">
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A41:A42"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="A12:A14"/>
@@ -31983,12 +32054,18 @@
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A37:A39"/>
     <mergeCell ref="A25:A34"/>
     <mergeCell ref="B25:B34"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B37:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Merging Release Candidate 3 with Release Candidate 2
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -19,9 +19,9 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -3654,6 +3654,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3702,38 +3707,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3759,6 +3734,60 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3767,9 +3796,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3789,41 +3815,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3864,24 +3866,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4291,13 +4291,13 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="131">
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="134">
         <v>43056</v>
       </c>
       <c r="F2" s="2"/>
@@ -4317,19 +4317,19 @@
       <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="131"/>
+      <c r="E3" s="134"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="131"/>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="134"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -4347,7 +4347,7 @@
       <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="131"/>
+      <c r="E5" s="134"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -4365,16 +4365,16 @@
       <c r="D6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="131"/>
+      <c r="E6" s="134"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="138">
+      <c r="B7" s="141">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4383,86 +4383,86 @@
       <c r="D7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="131"/>
+      <c r="E7" s="134"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="136"/>
-      <c r="B8" s="139"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="131"/>
+      <c r="E8" s="134"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="136"/>
-      <c r="B9" s="139"/>
+      <c r="A9" s="139"/>
+      <c r="B9" s="142"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="131"/>
+      <c r="E9" s="134"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="136"/>
-      <c r="B10" s="139"/>
+      <c r="A10" s="139"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="131"/>
+      <c r="E10" s="134"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="136"/>
-      <c r="B11" s="139"/>
+      <c r="A11" s="139"/>
+      <c r="B11" s="142"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="131"/>
+      <c r="E11" s="134"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="137"/>
-      <c r="B12" s="140"/>
+      <c r="A12" s="140"/>
+      <c r="B12" s="143"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="131"/>
+      <c r="E12" s="134"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="138">
+      <c r="B13" s="141">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4471,21 +4471,21 @@
       <c r="D13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="134"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="144"/>
-      <c r="B14" s="140"/>
+      <c r="A14" s="147"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="131"/>
+      <c r="E14" s="134"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -4503,7 +4503,7 @@
       <c r="D15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="131"/>
+      <c r="E15" s="134"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -4521,19 +4521,19 @@
       <c r="D16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="131"/>
+      <c r="E16" s="134"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="132" t="s">
+      <c r="A17" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="133"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="131"/>
+      <c r="B17" s="136"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="134"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -4551,7 +4551,7 @@
       <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="131"/>
+      <c r="E18" s="134"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -4569,28 +4569,28 @@
       <c r="D19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="131"/>
+      <c r="E19" s="134"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="132" t="s">
+      <c r="A20" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="133"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="131"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="134"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="145" t="s">
+      <c r="A21" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="142">
+      <c r="B21" s="145">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4599,21 +4599,21 @@
       <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="131"/>
+      <c r="E21" s="134"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="146"/>
-      <c r="B22" s="140"/>
+      <c r="A22" s="149"/>
+      <c r="B22" s="143"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="131"/>
+      <c r="E22" s="134"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
@@ -4628,22 +4628,22 @@
       <c r="D23" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="131"/>
+      <c r="E23" s="134"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="132" t="s">
+      <c r="A24" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="131"/>
+      <c r="B24" s="136"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="134"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="141" t="s">
+      <c r="A25" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="142">
+      <c r="B25" s="145">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4652,105 +4652,105 @@
       <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="131"/>
+      <c r="E25" s="134"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="136"/>
-      <c r="B26" s="139"/>
+      <c r="A26" s="139"/>
+      <c r="B26" s="142"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="131"/>
+      <c r="E26" s="134"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="136"/>
-      <c r="B27" s="139"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="142"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="131"/>
+      <c r="E27" s="134"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="136"/>
-      <c r="B28" s="139"/>
+      <c r="A28" s="139"/>
+      <c r="B28" s="142"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="131"/>
+      <c r="E28" s="134"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="136"/>
-      <c r="B29" s="139"/>
+      <c r="A29" s="139"/>
+      <c r="B29" s="142"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="131"/>
+      <c r="E29" s="134"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="136"/>
-      <c r="B30" s="139"/>
+      <c r="A30" s="139"/>
+      <c r="B30" s="142"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="131"/>
+      <c r="E30" s="134"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="136"/>
-      <c r="B31" s="139"/>
+      <c r="A31" s="139"/>
+      <c r="B31" s="142"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="131"/>
+      <c r="E31" s="134"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="137"/>
-      <c r="B32" s="140"/>
+      <c r="A32" s="140"/>
+      <c r="B32" s="143"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="131"/>
+      <c r="E32" s="134"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -4768,7 +4768,7 @@
       <c r="D33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="131"/>
+      <c r="E33" s="134"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
@@ -4783,7 +4783,7 @@
       <c r="D34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="131"/>
+      <c r="E34" s="134"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
@@ -4798,7 +4798,7 @@
       <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="131"/>
+      <c r="E35" s="134"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
@@ -4813,7 +4813,7 @@
       <c r="D36" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="131"/>
+      <c r="E36" s="134"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
@@ -4828,7 +4828,7 @@
       <c r="D37" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="131"/>
+      <c r="E37" s="134"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
@@ -4843,7 +4843,7 @@
       <c r="D38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="131"/>
+      <c r="E38" s="134"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
@@ -4858,7 +4858,7 @@
       <c r="D39" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="131"/>
+      <c r="E39" s="134"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
@@ -4873,16 +4873,16 @@
       <c r="D40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="131"/>
+      <c r="E40" s="134"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="132" t="s">
+      <c r="A41" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="133"/>
-      <c r="C41" s="133"/>
-      <c r="D41" s="134"/>
-      <c r="E41" s="131"/>
+      <c r="B41" s="136"/>
+      <c r="C41" s="136"/>
+      <c r="D41" s="137"/>
+      <c r="E41" s="134"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4897,7 +4897,7 @@
       <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="131"/>
+      <c r="E42" s="134"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
@@ -4912,7 +4912,7 @@
       <c r="D43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="131"/>
+      <c r="E43" s="134"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
@@ -4927,7 +4927,7 @@
       <c r="D44" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="131"/>
+      <c r="E44" s="134"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
@@ -4942,11 +4942,11 @@
       <c r="D45" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="131"/>
+      <c r="E45" s="134"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4956,7 +4956,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5025,7 +5025,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="159">
+      <c r="E2" s="152">
         <v>43140</v>
       </c>
     </row>
@@ -5040,7 +5040,7 @@
       <c r="D3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="159"/>
+      <c r="E3" s="152"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
@@ -5053,7 +5053,7 @@
       <c r="D4" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="159"/>
+      <c r="E4" s="152"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
@@ -5066,7 +5066,7 @@
       <c r="D5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="159"/>
+      <c r="E5" s="152"/>
     </row>
     <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
@@ -5075,13 +5075,13 @@
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="159"/>
+      <c r="E6" s="152"/>
     </row>
     <row r="7" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="165" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5090,68 +5090,68 @@
       <c r="D7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="159"/>
+      <c r="E7" s="152"/>
     </row>
     <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="147"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="166"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="159"/>
+      <c r="E8" s="152"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="147"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="166"/>
+      <c r="B9" s="165"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="159"/>
+      <c r="E9" s="152"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="147"/>
-      <c r="B10" s="148"/>
+      <c r="A10" s="166"/>
+      <c r="B10" s="165"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="159"/>
+      <c r="E10" s="152"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="147"/>
-      <c r="B11" s="148"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="159"/>
+      <c r="E11" s="152"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="147"/>
-      <c r="B12" s="148"/>
+      <c r="A12" s="166"/>
+      <c r="B12" s="165"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="159"/>
+      <c r="E12" s="152"/>
     </row>
     <row r="13" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="168" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="165" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5160,35 +5160,35 @@
       <c r="D13" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="159"/>
+      <c r="E13" s="152"/>
     </row>
     <row r="14" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="150"/>
-      <c r="B14" s="148"/>
+      <c r="A14" s="168"/>
+      <c r="B14" s="165"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="159"/>
+      <c r="E14" s="152"/>
     </row>
     <row r="15" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="150"/>
-      <c r="B15" s="148"/>
+      <c r="A15" s="168"/>
+      <c r="B15" s="165"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="159"/>
+      <c r="E15" s="152"/>
     </row>
     <row r="16" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="152" t="s">
+      <c r="B16" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5197,108 +5197,108 @@
       <c r="D16" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="E16" s="159"/>
+      <c r="E16" s="152"/>
     </row>
     <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="151"/>
-      <c r="B17" s="152"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="160"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="159"/>
+      <c r="E17" s="152"/>
     </row>
     <row r="18" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="151"/>
-      <c r="B18" s="152"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="160"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="159"/>
+      <c r="E18" s="152"/>
     </row>
     <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="151"/>
-      <c r="B19" s="152"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="160"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="E19" s="159"/>
+      <c r="E19" s="152"/>
     </row>
     <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="151"/>
-      <c r="B20" s="152"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="160"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="159"/>
+      <c r="E20" s="152"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="151"/>
-      <c r="B21" s="152"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="160"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="159"/>
+      <c r="E21" s="152"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="151"/>
-      <c r="B22" s="152"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="160"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="159"/>
+      <c r="E22" s="152"/>
     </row>
     <row r="23" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="151"/>
-      <c r="B23" s="152"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="160"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="E23" s="159"/>
+      <c r="E23" s="152"/>
     </row>
     <row r="24" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="151"/>
-      <c r="B24" s="152"/>
-      <c r="C24" s="151" t="s">
+      <c r="A24" s="150"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="150" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="158" t="s">
+      <c r="D24" s="151" t="s">
         <v>162</v>
       </c>
-      <c r="E24" s="159"/>
+      <c r="E24" s="152"/>
     </row>
     <row r="25" spans="1:5" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="151"/>
-      <c r="B25" s="152"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="158"/>
-      <c r="E25" s="159"/>
+      <c r="A25" s="150"/>
+      <c r="B25" s="160"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="151"/>
+      <c r="E25" s="152"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="147" t="s">
+      <c r="A26" s="166" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="165" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5307,16 +5307,16 @@
       <c r="D26" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="E26" s="159"/>
+      <c r="E26" s="152"/>
     </row>
     <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="147"/>
-      <c r="B27" s="148"/>
+      <c r="A27" s="166"/>
+      <c r="B27" s="165"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="159"/>
+      <c r="E27" s="152"/>
     </row>
     <row r="28" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
@@ -5329,7 +5329,7 @@
       <c r="D28" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="159"/>
+      <c r="E28" s="152"/>
     </row>
     <row r="29" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
@@ -5338,108 +5338,108 @@
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
-      <c r="E29" s="159"/>
+      <c r="E29" s="152"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="149" t="s">
+      <c r="A30" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="165" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="151" t="s">
+      <c r="C30" s="150" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="162" t="s">
+      <c r="D30" s="155" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="159"/>
+      <c r="E30" s="152"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="149"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="151"/>
-      <c r="D31" s="162"/>
-      <c r="E31" s="159"/>
+      <c r="A31" s="167"/>
+      <c r="B31" s="165"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="152"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="149"/>
-      <c r="B32" s="148"/>
+      <c r="A32" s="167"/>
+      <c r="B32" s="165"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="159"/>
+      <c r="E32" s="152"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="149"/>
-      <c r="B33" s="148"/>
+      <c r="A33" s="167"/>
+      <c r="B33" s="165"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="159"/>
+      <c r="E33" s="152"/>
     </row>
     <row r="34" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="149"/>
-      <c r="B34" s="148"/>
+      <c r="A34" s="167"/>
+      <c r="B34" s="165"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="159"/>
+      <c r="E34" s="152"/>
     </row>
     <row r="35" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="149"/>
-      <c r="B35" s="148"/>
+      <c r="A35" s="167"/>
+      <c r="B35" s="165"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="159"/>
+      <c r="E35" s="152"/>
     </row>
     <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="149"/>
-      <c r="B36" s="148"/>
+      <c r="A36" s="167"/>
+      <c r="B36" s="165"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
       <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="159"/>
+      <c r="E36" s="152"/>
     </row>
     <row r="37" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="149"/>
-      <c r="B37" s="148"/>
-      <c r="C37" s="163" t="s">
+      <c r="A37" s="167"/>
+      <c r="B37" s="165"/>
+      <c r="C37" s="156" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="165" t="s">
+      <c r="D37" s="158" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="159"/>
+      <c r="E37" s="152"/>
     </row>
     <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="149"/>
-      <c r="B38" s="148"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="159"/>
+      <c r="A38" s="167"/>
+      <c r="B38" s="165"/>
+      <c r="C38" s="157"/>
+      <c r="D38" s="158"/>
+      <c r="E38" s="152"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="147" t="s">
+      <c r="A39" s="166" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="165" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5448,16 +5448,16 @@
       <c r="D39" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="159"/>
+      <c r="E39" s="152"/>
     </row>
     <row r="40" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="147"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="166"/>
+      <c r="B40" s="165"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E40" s="159"/>
+      <c r="E40" s="152"/>
     </row>
     <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
@@ -5470,7 +5470,7 @@
       <c r="D41" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="159"/>
+      <c r="E41" s="152"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
@@ -5479,90 +5479,90 @@
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="159"/>
+      <c r="E42" s="152"/>
     </row>
     <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="149" t="s">
+      <c r="A43" s="167" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="148" t="s">
+      <c r="B43" s="165" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="159"/>
+      <c r="E43" s="152"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="149"/>
-      <c r="B44" s="148"/>
+      <c r="A44" s="167"/>
+      <c r="B44" s="165"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D44" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E44" s="159"/>
+      <c r="E44" s="152"/>
     </row>
     <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="155" t="s">
+      <c r="A45" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="165" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="159"/>
+      <c r="E45" s="152"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="156"/>
-      <c r="B46" s="148"/>
+      <c r="A46" s="163"/>
+      <c r="B46" s="165"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="159"/>
+      <c r="E46" s="152"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="156"/>
-      <c r="B47" s="148"/>
+      <c r="A47" s="163"/>
+      <c r="B47" s="165"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="159"/>
+      <c r="E47" s="152"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="157"/>
-      <c r="B48" s="148"/>
+      <c r="A48" s="164"/>
+      <c r="B48" s="165"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="159"/>
+      <c r="E48" s="152"/>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="152" t="s">
+      <c r="A49" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="152" t="s">
+      <c r="B49" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="159"/>
+      <c r="E49" s="152"/>
       <c r="H49" s="42"/>
       <c r="L49" s="42"/>
       <c r="P49" s="42"/>
@@ -9660,15 +9660,15 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="152"/>
-      <c r="B50" s="152"/>
+      <c r="A50" s="160"/>
+      <c r="B50" s="160"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="159"/>
+      <c r="E50" s="152"/>
       <c r="H50" s="42"/>
       <c r="L50" s="42"/>
       <c r="P50" s="42"/>
@@ -13766,15 +13766,15 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="152"/>
-      <c r="B51" s="152"/>
+      <c r="A51" s="160"/>
+      <c r="B51" s="160"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="E51" s="159"/>
+      <c r="E51" s="152"/>
       <c r="H51" s="42"/>
       <c r="L51" s="42"/>
       <c r="P51" s="42"/>
@@ -17872,15 +17872,15 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="152"/>
-      <c r="B52" s="152"/>
+      <c r="A52" s="160"/>
+      <c r="B52" s="160"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="159"/>
+      <c r="E52" s="152"/>
       <c r="H52" s="42"/>
       <c r="L52" s="42"/>
       <c r="P52" s="42"/>
@@ -21978,15 +21978,15 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="152"/>
-      <c r="B53" s="152"/>
-      <c r="C53" s="161" t="s">
+      <c r="A53" s="160"/>
+      <c r="B53" s="160"/>
+      <c r="C53" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="162" t="s">
+      <c r="D53" s="155" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="159"/>
+      <c r="E53" s="152"/>
       <c r="H53" s="42"/>
       <c r="L53" s="42"/>
       <c r="P53" s="42"/>
@@ -26084,11 +26084,11 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152"/>
-      <c r="B54" s="152"/>
-      <c r="C54" s="161"/>
-      <c r="D54" s="162"/>
-      <c r="E54" s="159"/>
+      <c r="A54" s="160"/>
+      <c r="B54" s="160"/>
+      <c r="C54" s="154"/>
+      <c r="D54" s="155"/>
+      <c r="E54" s="152"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -30192,7 +30192,7 @@
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
-      <c r="E55" s="159"/>
+      <c r="E55" s="152"/>
     </row>
     <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
@@ -30205,13 +30205,13 @@
       <c r="D56" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="159"/>
+      <c r="E56" s="152"/>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="153" t="s">
+      <c r="A57" s="159" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="152" t="s">
+      <c r="B57" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30220,204 +30220,204 @@
       <c r="D57" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="159"/>
+      <c r="E57" s="152"/>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="153"/>
-      <c r="B58" s="152"/>
+      <c r="A58" s="159"/>
+      <c r="B58" s="160"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="E58" s="159"/>
+      <c r="E58" s="152"/>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="153"/>
-      <c r="B59" s="152"/>
+      <c r="A59" s="159"/>
+      <c r="B59" s="160"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D59" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="159"/>
+      <c r="E59" s="152"/>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="153"/>
-      <c r="B60" s="152"/>
+      <c r="A60" s="159"/>
+      <c r="B60" s="160"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D60" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="159"/>
+      <c r="E60" s="152"/>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="153"/>
-      <c r="B61" s="152"/>
+      <c r="A61" s="159"/>
+      <c r="B61" s="160"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="159"/>
+      <c r="E61" s="152"/>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="153"/>
-      <c r="B62" s="152"/>
+      <c r="A62" s="159"/>
+      <c r="B62" s="160"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="159"/>
+      <c r="E62" s="152"/>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="153"/>
-      <c r="B63" s="152"/>
+      <c r="A63" s="159"/>
+      <c r="B63" s="160"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D63" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="159"/>
+      <c r="E63" s="152"/>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="153"/>
-      <c r="B64" s="152"/>
+      <c r="A64" s="159"/>
+      <c r="B64" s="160"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="159"/>
+      <c r="E64" s="152"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="153"/>
-      <c r="B65" s="152"/>
+      <c r="A65" s="159"/>
+      <c r="B65" s="160"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="E65" s="159"/>
+      <c r="E65" s="152"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="153"/>
-      <c r="B66" s="152"/>
+      <c r="A66" s="159"/>
+      <c r="B66" s="160"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="159"/>
+      <c r="E66" s="152"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="153"/>
-      <c r="B67" s="152"/>
+      <c r="A67" s="159"/>
+      <c r="B67" s="160"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E67" s="159"/>
+      <c r="E67" s="152"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="153"/>
-      <c r="B68" s="152"/>
+      <c r="A68" s="159"/>
+      <c r="B68" s="160"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="159"/>
+      <c r="E68" s="152"/>
     </row>
     <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="153"/>
-      <c r="B69" s="152"/>
+      <c r="A69" s="159"/>
+      <c r="B69" s="160"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E69" s="159"/>
+      <c r="E69" s="152"/>
     </row>
     <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="153"/>
-      <c r="B70" s="152"/>
+      <c r="A70" s="159"/>
+      <c r="B70" s="160"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="159"/>
+      <c r="E70" s="152"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="153"/>
-      <c r="B71" s="152"/>
+      <c r="A71" s="159"/>
+      <c r="B71" s="160"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="159"/>
+      <c r="E71" s="152"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="153"/>
-      <c r="B72" s="152"/>
+      <c r="A72" s="159"/>
+      <c r="B72" s="160"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="159"/>
+      <c r="E72" s="152"/>
     </row>
     <row r="73" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="153"/>
-      <c r="B73" s="152"/>
+      <c r="A73" s="159"/>
+      <c r="B73" s="160"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="159"/>
+      <c r="E73" s="152"/>
     </row>
     <row r="74" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="153"/>
-      <c r="B74" s="152"/>
+      <c r="A74" s="159"/>
+      <c r="B74" s="160"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="E74" s="159"/>
+      <c r="E74" s="152"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="153"/>
-      <c r="B75" s="152"/>
-      <c r="C75" s="160"/>
-      <c r="D75" s="154" t="s">
+      <c r="A75" s="159"/>
+      <c r="B75" s="160"/>
+      <c r="C75" s="153"/>
+      <c r="D75" s="161" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="159"/>
+      <c r="E75" s="152"/>
     </row>
     <row r="76" spans="1:5" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="153"/>
-      <c r="B76" s="152"/>
-      <c r="C76" s="160"/>
-      <c r="D76" s="154"/>
-      <c r="E76" s="159"/>
+      <c r="A76" s="159"/>
+      <c r="B76" s="160"/>
+      <c r="C76" s="153"/>
+      <c r="D76" s="161"/>
+      <c r="E76" s="152"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30426,7 +30426,7 @@
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
-      <c r="E77" s="159"/>
+      <c r="E77" s="152"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="48"/>
@@ -30442,8 +30442,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30452,30 +30452,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="31">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E2:E77"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30490,6 +30473,23 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E2:E77"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30537,7 +30537,7 @@
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
-      <c r="E2" s="131">
+      <c r="E2" s="134">
         <v>43179</v>
       </c>
     </row>
@@ -30548,13 +30548,13 @@
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="131"/>
+      <c r="E3" s="134"/>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="165" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30563,158 +30563,158 @@
       <c r="D4" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="131"/>
+      <c r="E4" s="134"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="147"/>
-      <c r="B5" s="148"/>
-      <c r="C5" s="167" t="s">
+      <c r="A5" s="166"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="178" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="166" t="s">
+      <c r="D5" s="177" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="131"/>
+      <c r="E5" s="134"/>
     </row>
     <row r="6" spans="1:5" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="147"/>
-      <c r="B6" s="148"/>
-      <c r="C6" s="167"/>
-      <c r="D6" s="166"/>
-      <c r="E6" s="131"/>
+      <c r="A6" s="166"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="177"/>
+      <c r="E6" s="134"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="147"/>
-      <c r="B7" s="148"/>
+      <c r="A7" s="166"/>
+      <c r="B7" s="165"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
-      <c r="E7" s="131"/>
+      <c r="E7" s="134"/>
     </row>
     <row r="8" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="147"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="166"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
-      <c r="E8" s="131"/>
+      <c r="E8" s="134"/>
     </row>
     <row r="9" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="147"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="166"/>
+      <c r="B9" s="165"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
-      <c r="E9" s="131"/>
+      <c r="E9" s="134"/>
     </row>
     <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="168" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="165" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="169"/>
-      <c r="D10" s="166" t="s">
+      <c r="C10" s="175"/>
+      <c r="D10" s="177" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="131"/>
+      <c r="E10" s="134"/>
     </row>
     <row r="11" spans="1:5" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="150"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="169"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="131"/>
+      <c r="A11" s="168"/>
+      <c r="B11" s="165"/>
+      <c r="C11" s="175"/>
+      <c r="D11" s="177"/>
+      <c r="E11" s="134"/>
     </row>
     <row r="12" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="150"/>
-      <c r="B12" s="148"/>
-      <c r="C12" s="169"/>
-      <c r="D12" s="166"/>
-      <c r="E12" s="131"/>
+      <c r="A12" s="168"/>
+      <c r="B12" s="165"/>
+      <c r="C12" s="175"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="134"/>
     </row>
     <row r="13" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="168"/>
-      <c r="D13" s="166" t="s">
+      <c r="C13" s="179"/>
+      <c r="D13" s="177" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="134"/>
     </row>
     <row r="14" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="151"/>
-      <c r="B14" s="152"/>
-      <c r="C14" s="168"/>
-      <c r="D14" s="166"/>
-      <c r="E14" s="131"/>
+      <c r="A14" s="150"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="134"/>
     </row>
     <row r="15" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="151"/>
-      <c r="B15" s="152"/>
-      <c r="C15" s="168"/>
+      <c r="A15" s="150"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="179"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="131"/>
+      <c r="E15" s="134"/>
     </row>
     <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="151"/>
-      <c r="B16" s="152"/>
-      <c r="C16" s="168"/>
+      <c r="A16" s="150"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="179"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="131"/>
+      <c r="E16" s="134"/>
     </row>
     <row r="17" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="151"/>
-      <c r="B17" s="152"/>
-      <c r="C17" s="168"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="179"/>
       <c r="D17" s="49"/>
-      <c r="E17" s="131"/>
+      <c r="E17" s="134"/>
     </row>
     <row r="18" spans="1:5" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="151"/>
-      <c r="B18" s="152"/>
-      <c r="C18" s="168"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="179"/>
       <c r="D18" s="49"/>
-      <c r="E18" s="131"/>
+      <c r="E18" s="134"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="151"/>
-      <c r="B19" s="152"/>
-      <c r="C19" s="168"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="179"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="131"/>
+      <c r="E19" s="134"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="151"/>
-      <c r="B20" s="152"/>
-      <c r="C20" s="168"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="179"/>
       <c r="D20" s="49"/>
-      <c r="E20" s="131"/>
+      <c r="E20" s="134"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="151"/>
-      <c r="B21" s="152"/>
-      <c r="C21" s="168"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="179"/>
       <c r="D21" s="49"/>
-      <c r="E21" s="131"/>
+      <c r="E21" s="134"/>
     </row>
     <row r="22" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="151"/>
-      <c r="B22" s="152"/>
-      <c r="C22" s="168"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="179"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="131"/>
+      <c r="E22" s="134"/>
     </row>
     <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="151"/>
-      <c r="B23" s="152"/>
-      <c r="C23" s="168"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="179"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="131"/>
+      <c r="E23" s="134"/>
     </row>
     <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
@@ -30729,7 +30729,7 @@
       <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="131"/>
+      <c r="E24" s="134"/>
     </row>
     <row r="25" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
@@ -30744,7 +30744,7 @@
       <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="E25" s="131"/>
+      <c r="E25" s="134"/>
     </row>
     <row r="26" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
@@ -30757,7 +30757,7 @@
       <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="131"/>
+      <c r="E26" s="134"/>
     </row>
     <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
@@ -30766,7 +30766,7 @@
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
-      <c r="E27" s="131"/>
+      <c r="E27" s="134"/>
     </row>
     <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
@@ -30781,7 +30781,7 @@
       <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="131"/>
+      <c r="E28" s="134"/>
     </row>
     <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="85"/>
@@ -30792,7 +30792,7 @@
       <c r="D29" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="131"/>
+      <c r="E29" s="134"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
@@ -30803,7 +30803,7 @@
       <c r="D30" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="E30" s="131"/>
+      <c r="E30" s="134"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
@@ -30814,13 +30814,13 @@
       <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="E31" s="131"/>
+      <c r="E31" s="134"/>
     </row>
     <row r="32" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="177" t="s">
+      <c r="A32" s="169" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="180" t="s">
+      <c r="B32" s="172" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30829,39 +30829,39 @@
       <c r="D32" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="E32" s="131"/>
+      <c r="E32" s="134"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="178"/>
-      <c r="B33" s="181"/>
+      <c r="A33" s="170"/>
+      <c r="B33" s="173"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
-      <c r="E33" s="131"/>
+      <c r="E33" s="134"/>
     </row>
     <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="178"/>
-      <c r="B34" s="181"/>
+      <c r="A34" s="170"/>
+      <c r="B34" s="173"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
-      <c r="E34" s="131"/>
+      <c r="E34" s="134"/>
     </row>
     <row r="35" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="178"/>
-      <c r="B35" s="181"/>
+      <c r="A35" s="170"/>
+      <c r="B35" s="173"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
-      <c r="E35" s="131"/>
+      <c r="E35" s="134"/>
     </row>
     <row r="36" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="179"/>
-      <c r="B36" s="182"/>
+      <c r="A36" s="171"/>
+      <c r="B36" s="174"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="E36" s="131"/>
+      <c r="E36" s="134"/>
     </row>
     <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
@@ -30874,7 +30874,7 @@
       <c r="D37" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="131"/>
+      <c r="E37" s="134"/>
     </row>
     <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
@@ -30883,13 +30883,13 @@
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
-      <c r="E38" s="131"/>
+      <c r="E38" s="134"/>
     </row>
     <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="149" t="s">
+      <c r="A39" s="167" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="165" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30898,108 +30898,108 @@
       <c r="D39" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="E39" s="131"/>
+      <c r="E39" s="134"/>
     </row>
     <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="149"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="167"/>
+      <c r="B40" s="165"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="131"/>
+      <c r="E40" s="134"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="147" t="s">
+      <c r="A41" s="166" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="165" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="169" t="s">
+      <c r="C41" s="175" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="151" t="s">
+      <c r="D41" s="150" t="s">
         <v>228</v>
       </c>
-      <c r="E41" s="131"/>
+      <c r="E41" s="134"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="147"/>
-      <c r="B42" s="148"/>
-      <c r="C42" s="169"/>
-      <c r="D42" s="151"/>
-      <c r="E42" s="131"/>
+      <c r="A42" s="166"/>
+      <c r="B42" s="165"/>
+      <c r="C42" s="175"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="134"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="147"/>
-      <c r="B43" s="148"/>
-      <c r="C43" s="169" t="s">
+      <c r="A43" s="166"/>
+      <c r="B43" s="165"/>
+      <c r="C43" s="175" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="154" t="s">
+      <c r="D43" s="161" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="131"/>
+      <c r="E43" s="134"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="147"/>
-      <c r="B44" s="148"/>
-      <c r="C44" s="169"/>
-      <c r="D44" s="154"/>
-      <c r="E44" s="131"/>
+      <c r="A44" s="166"/>
+      <c r="B44" s="165"/>
+      <c r="C44" s="175"/>
+      <c r="D44" s="161"/>
+      <c r="E44" s="134"/>
     </row>
     <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="153" t="s">
+      <c r="A45" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="152" t="s">
+      <c r="B45" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="173"/>
+      <c r="C45" s="183"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="131"/>
+      <c r="E45" s="134"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="153"/>
-      <c r="B46" s="152"/>
-      <c r="C46" s="174"/>
-      <c r="D46" s="170" t="s">
+      <c r="A46" s="159"/>
+      <c r="B46" s="160"/>
+      <c r="C46" s="184"/>
+      <c r="D46" s="180" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="131"/>
+      <c r="E46" s="134"/>
     </row>
     <row r="47" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="153"/>
-      <c r="B47" s="152"/>
-      <c r="C47" s="174"/>
-      <c r="D47" s="171"/>
-      <c r="E47" s="131"/>
+      <c r="A47" s="159"/>
+      <c r="B47" s="160"/>
+      <c r="C47" s="184"/>
+      <c r="D47" s="181"/>
+      <c r="E47" s="134"/>
     </row>
     <row r="48" spans="1:5" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="153"/>
-      <c r="B48" s="152"/>
-      <c r="C48" s="175"/>
-      <c r="D48" s="171"/>
-      <c r="E48" s="131"/>
+      <c r="A48" s="159"/>
+      <c r="B48" s="160"/>
+      <c r="C48" s="185"/>
+      <c r="D48" s="181"/>
+      <c r="E48" s="134"/>
     </row>
     <row r="49" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="153"/>
-      <c r="B49" s="152"/>
-      <c r="C49" s="161"/>
-      <c r="D49" s="171"/>
-      <c r="E49" s="131"/>
+      <c r="A49" s="159"/>
+      <c r="B49" s="160"/>
+      <c r="C49" s="154"/>
+      <c r="D49" s="181"/>
+      <c r="E49" s="134"/>
     </row>
     <row r="50" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="153"/>
-      <c r="B50" s="152"/>
-      <c r="C50" s="161"/>
-      <c r="D50" s="172"/>
-      <c r="E50" s="131"/>
+      <c r="A50" s="159"/>
+      <c r="B50" s="160"/>
+      <c r="C50" s="154"/>
+      <c r="D50" s="182"/>
+      <c r="E50" s="134"/>
     </row>
     <row r="51" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -31008,7 +31008,7 @@
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
-      <c r="E51" s="131"/>
+      <c r="E51" s="134"/>
     </row>
     <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
@@ -31021,13 +31021,13 @@
       <c r="D52" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="131"/>
+      <c r="E52" s="134"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="152" t="s">
+      <c r="A53" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="152" t="s">
+      <c r="B53" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31036,148 +31036,148 @@
       <c r="D53" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="131"/>
+      <c r="E53" s="134"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="152"/>
-      <c r="B54" s="152"/>
+      <c r="A54" s="160"/>
+      <c r="B54" s="160"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
       <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="131"/>
+      <c r="E54" s="134"/>
     </row>
     <row r="55" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="152"/>
-      <c r="B55" s="152"/>
+      <c r="A55" s="160"/>
+      <c r="B55" s="160"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="131"/>
+      <c r="E55" s="134"/>
     </row>
     <row r="56" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="152"/>
-      <c r="B56" s="152"/>
+      <c r="A56" s="160"/>
+      <c r="B56" s="160"/>
       <c r="C56" s="176" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="E56" s="131"/>
+      <c r="E56" s="134"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="152"/>
-      <c r="B57" s="152"/>
+      <c r="A57" s="160"/>
+      <c r="B57" s="160"/>
       <c r="C57" s="176"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="131"/>
+      <c r="E57" s="134"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="152"/>
-      <c r="B58" s="152"/>
+      <c r="A58" s="160"/>
+      <c r="B58" s="160"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
       <c r="D58" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E58" s="131"/>
+      <c r="E58" s="134"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="152"/>
-      <c r="B59" s="152"/>
+      <c r="A59" s="160"/>
+      <c r="B59" s="160"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
       <c r="D59" s="79" t="s">
         <v>215</v>
       </c>
-      <c r="E59" s="131"/>
+      <c r="E59" s="134"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="152"/>
-      <c r="B60" s="152"/>
+      <c r="A60" s="160"/>
+      <c r="B60" s="160"/>
       <c r="C60" s="176" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="131"/>
+      <c r="E60" s="134"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="152"/>
-      <c r="B61" s="152"/>
+      <c r="A61" s="160"/>
+      <c r="B61" s="160"/>
       <c r="C61" s="176"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="131"/>
+      <c r="E61" s="134"/>
     </row>
     <row r="62" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="152"/>
-      <c r="B62" s="152"/>
+      <c r="A62" s="160"/>
+      <c r="B62" s="160"/>
       <c r="C62" s="176"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="E62" s="131"/>
+      <c r="E62" s="134"/>
     </row>
     <row r="63" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="152"/>
-      <c r="B63" s="152"/>
-      <c r="C63" s="169" t="s">
+      <c r="A63" s="160"/>
+      <c r="B63" s="160"/>
+      <c r="C63" s="175" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="E63" s="131"/>
+      <c r="E63" s="134"/>
     </row>
     <row r="64" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="152"/>
-      <c r="B64" s="152"/>
-      <c r="C64" s="169"/>
-      <c r="D64" s="154" t="s">
+      <c r="A64" s="160"/>
+      <c r="B64" s="160"/>
+      <c r="C64" s="175"/>
+      <c r="D64" s="161" t="s">
         <v>220</v>
       </c>
-      <c r="E64" s="131"/>
+      <c r="E64" s="134"/>
     </row>
     <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="152"/>
-      <c r="B65" s="152"/>
-      <c r="C65" s="169"/>
-      <c r="D65" s="154"/>
-      <c r="E65" s="131"/>
+      <c r="A65" s="160"/>
+      <c r="B65" s="160"/>
+      <c r="C65" s="175"/>
+      <c r="D65" s="161"/>
+      <c r="E65" s="134"/>
     </row>
     <row r="66" spans="1:5" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="152"/>
-      <c r="B66" s="152"/>
-      <c r="C66" s="169"/>
-      <c r="D66" s="154"/>
-      <c r="E66" s="131"/>
+      <c r="A66" s="160"/>
+      <c r="B66" s="160"/>
+      <c r="C66" s="175"/>
+      <c r="D66" s="161"/>
+      <c r="E66" s="134"/>
     </row>
     <row r="67" spans="1:5" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="152"/>
-      <c r="B67" s="152"/>
-      <c r="C67" s="169"/>
-      <c r="D67" s="154"/>
-      <c r="E67" s="131"/>
+      <c r="A67" s="160"/>
+      <c r="B67" s="160"/>
+      <c r="C67" s="175"/>
+      <c r="D67" s="161"/>
+      <c r="E67" s="134"/>
     </row>
     <row r="68" spans="1:5" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
-      <c r="E68" s="131"/>
+      <c r="E68" s="134"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
@@ -31227,24 +31227,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="B53:B67"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C63:C67"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
@@ -31261,6 +31243,24 @@
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="C45:C48"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31311,7 +31311,7 @@
       <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="150" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="176" t="s">
@@ -31326,7 +31326,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="151"/>
+      <c r="A4" s="150"/>
       <c r="B4" s="176"/>
       <c r="C4" s="123" t="s">
         <v>235</v>
@@ -31369,7 +31369,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="193" t="s">
+      <c r="A7" s="195" t="s">
         <v>275</v>
       </c>
       <c r="B7" s="176"/>
@@ -31382,7 +31382,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="194"/>
+      <c r="A8" s="196"/>
       <c r="B8" s="176"/>
       <c r="C8" s="58"/>
       <c r="D8" s="107" t="s">
@@ -31428,7 +31428,7 @@
       <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="190" t="s">
+      <c r="A12" s="192" t="s">
         <v>237</v>
       </c>
       <c r="B12" s="176" t="s">
@@ -31443,7 +31443,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="191"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="176"/>
       <c r="C13" s="58"/>
       <c r="D13" s="107" t="s">
@@ -31454,7 +31454,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="192"/>
+      <c r="A14" s="194"/>
       <c r="B14" s="176"/>
       <c r="C14" s="58"/>
       <c r="D14" s="107" t="s">
@@ -31480,13 +31480,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="150" t="s">
         <v>222</v>
       </c>
       <c r="B16" s="176" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="185" t="s">
+      <c r="C16" s="205" t="s">
         <v>239</v>
       </c>
       <c r="D16" s="112" t="s">
@@ -31497,9 +31497,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="151"/>
+      <c r="A17" s="150"/>
       <c r="B17" s="176"/>
-      <c r="C17" s="186"/>
+      <c r="C17" s="206"/>
       <c r="D17" s="104" t="s">
         <v>278</v>
       </c>
@@ -31508,7 +31508,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="151"/>
+      <c r="A18" s="150"/>
       <c r="B18" s="176"/>
       <c r="C18" s="96" t="s">
         <v>240</v>
@@ -31560,7 +31560,7 @@
       <c r="E21" s="58"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="193" t="s">
+      <c r="A22" s="195" t="s">
         <v>260</v>
       </c>
       <c r="B22" s="176" t="s">
@@ -31575,7 +31575,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="194"/>
+      <c r="A23" s="196"/>
       <c r="B23" s="176"/>
       <c r="C23" s="58"/>
       <c r="D23" s="107" t="s">
@@ -31603,10 +31603,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="197" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="198" t="s">
+      <c r="B25" s="200" t="s">
         <v>234</v>
       </c>
       <c r="C25" s="58" t="s">
@@ -31620,8 +31620,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="196"/>
-      <c r="B26" s="199"/>
+      <c r="A26" s="198"/>
+      <c r="B26" s="201"/>
       <c r="C26" t="s">
         <v>270</v>
       </c>
@@ -31633,8 +31633,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="196"/>
-      <c r="B27" s="199"/>
+      <c r="A27" s="198"/>
+      <c r="B27" s="201"/>
       <c r="C27" s="58" t="s">
         <v>269</v>
       </c>
@@ -31646,8 +31646,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="196"/>
-      <c r="B28" s="199"/>
+      <c r="A28" s="198"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="103" t="s">
         <v>277</v>
       </c>
@@ -31659,8 +31659,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="196"/>
-      <c r="B29" s="199"/>
+      <c r="A29" s="198"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="58" t="s">
         <v>284</v>
       </c>
@@ -31672,8 +31672,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="196"/>
-      <c r="B30" s="199"/>
+      <c r="A30" s="198"/>
+      <c r="B30" s="201"/>
       <c r="C30" s="58" t="s">
         <v>285</v>
       </c>
@@ -31685,8 +31685,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="196"/>
-      <c r="B31" s="199"/>
+      <c r="A31" s="198"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="125" t="s">
         <v>290</v>
       </c>
@@ -31698,8 +31698,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="196"/>
-      <c r="B32" s="199"/>
+      <c r="A32" s="198"/>
+      <c r="B32" s="201"/>
       <c r="C32" s="125" t="s">
         <v>291</v>
       </c>
@@ -31711,8 +31711,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="196"/>
-      <c r="B33" s="199"/>
+      <c r="A33" s="198"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="125" t="s">
         <v>292</v>
       </c>
@@ -31724,8 +31724,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="197"/>
-      <c r="B34" s="200"/>
+      <c r="A34" s="199"/>
+      <c r="B34" s="202"/>
       <c r="C34" s="95" t="s">
         <v>244</v>
       </c>
@@ -31767,7 +31767,7 @@
       <c r="D37" s="58" t="s">
         <v>253</v>
       </c>
-      <c r="E37" s="203">
+      <c r="E37" s="131">
         <v>43244</v>
       </c>
     </row>
@@ -31780,7 +31780,7 @@
       <c r="D38" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="E38" s="203">
+      <c r="E38" s="131">
         <v>43244</v>
       </c>
     </row>
@@ -31793,17 +31793,17 @@
       <c r="D39" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="E39" s="203">
+      <c r="E39" s="131">
         <v>43244</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="176"/>
       <c r="B40" s="176"/>
-      <c r="C40" s="205" t="s">
+      <c r="C40" s="132" t="s">
         <v>296</v>
       </c>
-      <c r="D40" s="206" t="s">
+      <c r="D40" s="133" t="s">
         <v>297</v>
       </c>
       <c r="E40" s="116">
@@ -31811,26 +31811,26 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="151" t="s">
+      <c r="A41" s="150" t="s">
         <v>247</v>
       </c>
       <c r="B41" s="176" t="s">
         <v>234</v>
       </c>
-      <c r="C41" s="200"/>
-      <c r="D41" s="204" t="s">
+      <c r="C41" s="202"/>
+      <c r="D41" s="207" t="s">
         <v>261</v>
       </c>
-      <c r="E41" s="183">
+      <c r="E41" s="203">
         <v>43270</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="151"/>
+      <c r="A42" s="150"/>
       <c r="B42" s="176"/>
       <c r="C42" s="176"/>
-      <c r="D42" s="187"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="208"/>
+      <c r="E42" s="204"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="122" t="s">
@@ -31876,13 +31876,13 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="207" t="s">
+      <c r="A46" s="186" t="s">
         <v>287</v>
       </c>
-      <c r="B46" s="201" t="s">
+      <c r="B46" s="188" t="s">
         <v>234</v>
       </c>
-      <c r="C46" s="206" t="s">
+      <c r="C46" s="133" t="s">
         <v>298</v>
       </c>
       <c r="D46" s="58" t="s">
@@ -31893,8 +31893,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="208"/>
-      <c r="B47" s="202"/>
+      <c r="A47" s="187"/>
+      <c r="B47" s="189"/>
       <c r="C47" s="100" t="s">
         <v>288</v>
       </c>
@@ -31915,10 +31915,10 @@
       <c r="E48" s="58"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="188" t="s">
+      <c r="A49" s="190" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="198" t="s">
+      <c r="B49" s="200" t="s">
         <v>271</v>
       </c>
       <c r="C49" s="100" t="s">
@@ -31932,8 +31932,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="189"/>
-      <c r="B50" s="200"/>
+      <c r="A50" s="191"/>
+      <c r="B50" s="202"/>
       <c r="C50" s="100" t="s">
         <v>265</v>
       </c>
@@ -32043,6 +32043,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B37:B40"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="A49:A50"/>
@@ -32059,13 +32066,6 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B37:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"REST Integration Guide Doc"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008"/>
+    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="303">
   <si>
     <t>Document</t>
   </si>
@@ -2652,9 +2652,6 @@
     <t>REST Request Authentication Presentation</t>
   </si>
   <si>
-    <t>REST_Web_Service_Integration_Guide_Sample_Http_Messages</t>
-  </si>
-  <si>
     <t>updated header's Request-target</t>
   </si>
   <si>
@@ -2704,6 +2701,24 @@
   </si>
   <si>
     <t>Section 6.1</t>
+  </si>
+  <si>
+    <t>REST Web Service Integration Guide Sample Http Messages</t>
+  </si>
+  <si>
+    <t>HTTP Method Override</t>
+  </si>
+  <si>
+    <t>Samples added</t>
+  </si>
+  <si>
+    <t>HTTP request example updated to include Digest and Signature elements.</t>
+  </si>
+  <si>
+    <t>pensionTracingNumber</t>
+  </si>
+  <si>
+    <t>Data item number changed from 38 to 39</t>
   </si>
 </sst>
 </file>
@@ -3601,9 +3616,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3612,9 +3624,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3626,6 +3635,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3671,38 +3700,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3725,38 +3724,35 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3776,8 +3772,38 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3827,10 +3853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3839,31 +3862,23 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4238,7 +4253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -4268,12 +4283,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="119"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4296,12 +4311,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="119"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="125"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4341,10 +4356,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="123">
+      <c r="B7" s="129">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4358,8 +4373,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="121"/>
-      <c r="B8" s="124"/>
+      <c r="A8" s="127"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4371,8 +4386,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="121"/>
-      <c r="B9" s="124"/>
+      <c r="A9" s="127"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4384,8 +4399,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="121"/>
-      <c r="B10" s="124"/>
+      <c r="A10" s="127"/>
+      <c r="B10" s="130"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4397,8 +4412,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="121"/>
-      <c r="B11" s="124"/>
+      <c r="A11" s="127"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4410,8 +4425,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="122"/>
-      <c r="B12" s="125"/>
+      <c r="A12" s="128"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4423,10 +4438,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="123">
+      <c r="B13" s="129">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4440,8 +4455,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="129"/>
-      <c r="B14" s="125"/>
+      <c r="A14" s="135"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4487,12 +4502,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="117" t="s">
+      <c r="A17" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="119"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="125"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4532,21 +4547,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="117" t="s">
+      <c r="A20" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="119"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="124"/>
+      <c r="D20" s="125"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="130" t="s">
+      <c r="A21" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="127">
+      <c r="B21" s="133">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4560,8 +4575,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="131"/>
-      <c r="B22" s="125"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="131"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4584,18 +4599,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="117" t="s">
+      <c r="A24" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="118"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="119"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="125"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="126" t="s">
+      <c r="A25" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="127">
+      <c r="B25" s="133">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4609,8 +4624,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="121"/>
-      <c r="B26" s="124"/>
+      <c r="A26" s="127"/>
+      <c r="B26" s="130"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4622,8 +4637,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="121"/>
-      <c r="B27" s="124"/>
+      <c r="A27" s="127"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4635,8 +4650,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="121"/>
-      <c r="B28" s="124"/>
+      <c r="A28" s="127"/>
+      <c r="B28" s="130"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4648,8 +4663,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="121"/>
-      <c r="B29" s="124"/>
+      <c r="A29" s="127"/>
+      <c r="B29" s="130"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4661,8 +4676,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="121"/>
-      <c r="B30" s="124"/>
+      <c r="A30" s="127"/>
+      <c r="B30" s="130"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4674,8 +4689,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="121"/>
-      <c r="B31" s="124"/>
+      <c r="A31" s="127"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4687,8 +4702,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="122"/>
-      <c r="B32" s="125"/>
+      <c r="A32" s="128"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4812,12 +4827,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="117" t="s">
+      <c r="A41" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="118"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="119"/>
+      <c r="B41" s="124"/>
+      <c r="C41" s="124"/>
+      <c r="D41" s="125"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4877,7 +4892,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4887,7 +4902,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4997,10 +5012,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="132" t="s">
+      <c r="A7" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5011,8 +5026,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="153"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5021,8 +5036,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="153"/>
+      <c r="B9" s="152"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5031,8 +5046,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="132"/>
-      <c r="B10" s="133"/>
+      <c r="A10" s="153"/>
+      <c r="B10" s="152"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5041,8 +5056,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="132"/>
-      <c r="B11" s="133"/>
+      <c r="A11" s="153"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5051,8 +5066,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
-      <c r="B12" s="133"/>
+      <c r="A12" s="153"/>
+      <c r="B12" s="152"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5061,10 +5076,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="135" t="s">
+      <c r="A13" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="133" t="s">
+      <c r="B13" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5075,8 +5090,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
-      <c r="B14" s="133"/>
+      <c r="A14" s="155"/>
+      <c r="B14" s="152"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5085,8 +5100,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="135"/>
-      <c r="B15" s="133"/>
+      <c r="A15" s="155"/>
+      <c r="B15" s="152"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5095,10 +5110,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="136" t="s">
+      <c r="A16" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="137" t="s">
+      <c r="B16" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5109,8 +5124,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="136"/>
-      <c r="B17" s="137"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="147"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5119,8 +5134,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="137"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="147"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5129,8 +5144,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136"/>
-      <c r="B19" s="137"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="147"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5139,8 +5154,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="136"/>
-      <c r="B20" s="137"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="147"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5149,8 +5164,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="136"/>
-      <c r="B21" s="137"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="147"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5159,8 +5174,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="136"/>
-      <c r="B22" s="137"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="147"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5169,8 +5184,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="136"/>
-      <c r="B23" s="137"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="147"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5179,26 +5194,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="136"/>
-      <c r="B24" s="137"/>
-      <c r="C24" s="136" t="s">
+      <c r="A24" s="138"/>
+      <c r="B24" s="147"/>
+      <c r="C24" s="138" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="143" t="s">
+      <c r="D24" s="139" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="136"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="143"/>
+      <c r="A25" s="138"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="139"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="132" t="s">
+      <c r="A26" s="153" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="133" t="s">
+      <c r="B26" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5209,8 +5224,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="132"/>
-      <c r="B27" s="133"/>
+      <c r="A27" s="153"/>
+      <c r="B27" s="152"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5237,28 +5252,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="134" t="s">
+      <c r="A30" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="133" t="s">
+      <c r="B30" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="136" t="s">
+      <c r="C30" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="146" t="s">
+      <c r="D30" s="142" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="134"/>
-      <c r="B31" s="133"/>
-      <c r="C31" s="136"/>
-      <c r="D31" s="146"/>
+      <c r="A31" s="154"/>
+      <c r="B31" s="152"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="142"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="134"/>
-      <c r="B32" s="133"/>
+      <c r="A32" s="154"/>
+      <c r="B32" s="152"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5267,8 +5282,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="134"/>
-      <c r="B33" s="133"/>
+      <c r="A33" s="154"/>
+      <c r="B33" s="152"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5277,8 +5292,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="134"/>
-      <c r="B34" s="133"/>
+      <c r="A34" s="154"/>
+      <c r="B34" s="152"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5287,8 +5302,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="134"/>
-      <c r="B35" s="133"/>
+      <c r="A35" s="154"/>
+      <c r="B35" s="152"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5297,8 +5312,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="134"/>
-      <c r="B36" s="133"/>
+      <c r="A36" s="154"/>
+      <c r="B36" s="152"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5307,26 +5322,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="134"/>
-      <c r="B37" s="133"/>
-      <c r="C37" s="147" t="s">
+      <c r="A37" s="154"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="143" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="149" t="s">
+      <c r="D37" s="145" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="134"/>
-      <c r="B38" s="133"/>
-      <c r="C38" s="148"/>
-      <c r="D38" s="149"/>
+      <c r="A38" s="154"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="144"/>
+      <c r="D38" s="145"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="132" t="s">
+      <c r="A39" s="153" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="133" t="s">
+      <c r="B39" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5337,8 +5352,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="132"/>
-      <c r="B40" s="133"/>
+      <c r="A40" s="153"/>
+      <c r="B40" s="152"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5365,10 +5380,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="134" t="s">
+      <c r="A43" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5377,8 +5392,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="134"/>
-      <c r="B44" s="133"/>
+      <c r="A44" s="154"/>
+      <c r="B44" s="152"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5387,10 +5402,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="140" t="s">
+      <c r="A45" s="149" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5399,8 +5414,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="141"/>
-      <c r="B46" s="133"/>
+      <c r="A46" s="150"/>
+      <c r="B46" s="152"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5409,8 +5424,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="141"/>
-      <c r="B47" s="133"/>
+      <c r="A47" s="150"/>
+      <c r="B47" s="152"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5419,8 +5434,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="142"/>
-      <c r="B48" s="133"/>
+      <c r="A48" s="151"/>
+      <c r="B48" s="152"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5429,10 +5444,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="137" t="s">
+      <c r="A49" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="137" t="s">
+      <c r="B49" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9536,8 +9551,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="137"/>
-      <c r="B50" s="137"/>
+      <c r="A50" s="147"/>
+      <c r="B50" s="147"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13641,8 +13656,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="137"/>
-      <c r="B51" s="137"/>
+      <c r="A51" s="147"/>
+      <c r="B51" s="147"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17746,8 +17761,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="137"/>
-      <c r="B52" s="137"/>
+      <c r="A52" s="147"/>
+      <c r="B52" s="147"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21851,12 +21866,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="137"/>
-      <c r="B53" s="137"/>
-      <c r="C53" s="145" t="s">
+      <c r="A53" s="147"/>
+      <c r="B53" s="147"/>
+      <c r="C53" s="141" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="146" t="s">
+      <c r="D53" s="142" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25956,10 +25971,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="137"/>
-      <c r="C54" s="145"/>
-      <c r="D54" s="146"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="147"/>
+      <c r="C54" s="141"/>
+      <c r="D54" s="142"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30077,10 +30092,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="138" t="s">
+      <c r="A57" s="146" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="137" t="s">
+      <c r="B57" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30091,8 +30106,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="138"/>
-      <c r="B58" s="137"/>
+      <c r="A58" s="146"/>
+      <c r="B58" s="147"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30101,8 +30116,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="138"/>
-      <c r="B59" s="137"/>
+      <c r="A59" s="146"/>
+      <c r="B59" s="147"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30111,8 +30126,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="138"/>
-      <c r="B60" s="137"/>
+      <c r="A60" s="146"/>
+      <c r="B60" s="147"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30121,8 +30136,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="138"/>
-      <c r="B61" s="137"/>
+      <c r="A61" s="146"/>
+      <c r="B61" s="147"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30131,8 +30146,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="138"/>
-      <c r="B62" s="137"/>
+      <c r="A62" s="146"/>
+      <c r="B62" s="147"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30141,8 +30156,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="138"/>
-      <c r="B63" s="137"/>
+      <c r="A63" s="146"/>
+      <c r="B63" s="147"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30151,16 +30166,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="138"/>
-      <c r="B64" s="137"/>
+      <c r="A64" s="146"/>
+      <c r="B64" s="147"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="138"/>
-      <c r="B65" s="137"/>
+      <c r="A65" s="146"/>
+      <c r="B65" s="147"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30169,16 +30184,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="138"/>
-      <c r="B66" s="137"/>
+      <c r="A66" s="146"/>
+      <c r="B66" s="147"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="138"/>
-      <c r="B67" s="137"/>
+      <c r="A67" s="146"/>
+      <c r="B67" s="147"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30187,8 +30202,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="138"/>
-      <c r="B68" s="137"/>
+      <c r="A68" s="146"/>
+      <c r="B68" s="147"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30197,8 +30212,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="138"/>
-      <c r="B69" s="137"/>
+      <c r="A69" s="146"/>
+      <c r="B69" s="147"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30207,8 +30222,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="138"/>
-      <c r="B70" s="137"/>
+      <c r="A70" s="146"/>
+      <c r="B70" s="147"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30217,8 +30232,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="138"/>
-      <c r="B71" s="137"/>
+      <c r="A71" s="146"/>
+      <c r="B71" s="147"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30227,8 +30242,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="138"/>
-      <c r="B72" s="137"/>
+      <c r="A72" s="146"/>
+      <c r="B72" s="147"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30237,16 +30252,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="138"/>
-      <c r="B73" s="137"/>
+      <c r="A73" s="146"/>
+      <c r="B73" s="147"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="138"/>
-      <c r="B74" s="137"/>
+      <c r="A74" s="146"/>
+      <c r="B74" s="147"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30255,18 +30270,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="138"/>
-      <c r="B75" s="137"/>
-      <c r="C75" s="144"/>
-      <c r="D75" s="139" t="s">
+      <c r="A75" s="146"/>
+      <c r="B75" s="147"/>
+      <c r="C75" s="140"/>
+      <c r="D75" s="148" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="138"/>
-      <c r="B76" s="137"/>
-      <c r="C76" s="144"/>
-      <c r="D76" s="139"/>
+      <c r="A76" s="146"/>
+      <c r="B76" s="147"/>
+      <c r="C76" s="140"/>
+      <c r="D76" s="148"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30290,8 +30305,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30300,29 +30315,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30337,6 +30336,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30390,10 +30405,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="152" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30404,133 +30419,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="132"/>
-      <c r="B5" s="133"/>
-      <c r="C5" s="151" t="s">
+      <c r="A5" s="153"/>
+      <c r="B5" s="152"/>
+      <c r="C5" s="165" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="150" t="s">
+      <c r="D5" s="164" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="132"/>
-      <c r="B6" s="133"/>
-      <c r="C6" s="151"/>
-      <c r="D6" s="150"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="164"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="132"/>
-      <c r="B7" s="133"/>
+      <c r="A7" s="153"/>
+      <c r="B7" s="152"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="153"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="153"/>
+      <c r="B9" s="152"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="135" t="s">
+      <c r="A10" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="153"/>
-      <c r="D10" s="150" t="s">
+      <c r="C10" s="162"/>
+      <c r="D10" s="164" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="135"/>
-      <c r="B11" s="133"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="150"/>
+      <c r="A11" s="155"/>
+      <c r="B11" s="152"/>
+      <c r="C11" s="162"/>
+      <c r="D11" s="164"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="135"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="153"/>
-      <c r="D12" s="150"/>
+      <c r="A12" s="155"/>
+      <c r="B12" s="152"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="164"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="152"/>
-      <c r="D13" s="150" t="s">
+      <c r="C13" s="166"/>
+      <c r="D13" s="164" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="136"/>
-      <c r="B14" s="137"/>
-      <c r="C14" s="152"/>
-      <c r="D14" s="150"/>
+      <c r="A14" s="138"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="166"/>
+      <c r="D14" s="164"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="136"/>
-      <c r="B15" s="137"/>
-      <c r="C15" s="152"/>
+      <c r="A15" s="138"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="166"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="136"/>
-      <c r="B16" s="137"/>
-      <c r="C16" s="152"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="166"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="136"/>
-      <c r="B17" s="137"/>
-      <c r="C17" s="152"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="166"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="137"/>
-      <c r="C18" s="152"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="147"/>
+      <c r="C18" s="166"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136"/>
-      <c r="B19" s="137"/>
-      <c r="C19" s="152"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="166"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="136"/>
-      <c r="B20" s="137"/>
-      <c r="C20" s="152"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="166"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="136"/>
-      <c r="B21" s="137"/>
-      <c r="C21" s="152"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="166"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="136"/>
-      <c r="B22" s="137"/>
-      <c r="C22" s="152"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="166"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="136"/>
-      <c r="B23" s="137"/>
-      <c r="C23" s="152"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="166"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30628,10 +30643,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="161" t="s">
+      <c r="A32" s="156" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="159" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30642,26 +30657,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="162"/>
-      <c r="B33" s="165"/>
+      <c r="A33" s="157"/>
+      <c r="B33" s="160"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="162"/>
-      <c r="B34" s="165"/>
+      <c r="A34" s="157"/>
+      <c r="B34" s="160"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="162"/>
-      <c r="B35" s="165"/>
+      <c r="A35" s="157"/>
+      <c r="B35" s="160"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="163"/>
-      <c r="B36" s="166"/>
+      <c r="A36" s="158"/>
+      <c r="B36" s="161"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30690,10 +30705,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="134" t="s">
+      <c r="A39" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="133" t="s">
+      <c r="B39" s="152" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30704,8 +30719,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="134"/>
-      <c r="B40" s="133"/>
+      <c r="A40" s="154"/>
+      <c r="B40" s="152"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30714,84 +30729,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="132" t="s">
+      <c r="A41" s="153" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="133" t="s">
+      <c r="B41" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="153" t="s">
+      <c r="C41" s="162" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="136" t="s">
+      <c r="D41" s="138" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="132"/>
-      <c r="B42" s="133"/>
-      <c r="C42" s="153"/>
-      <c r="D42" s="136"/>
+      <c r="A42" s="153"/>
+      <c r="B42" s="152"/>
+      <c r="C42" s="162"/>
+      <c r="D42" s="138"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="132"/>
-      <c r="B43" s="133"/>
-      <c r="C43" s="153" t="s">
+      <c r="A43" s="153"/>
+      <c r="B43" s="152"/>
+      <c r="C43" s="162" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="139" t="s">
+      <c r="D43" s="148" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="132"/>
-      <c r="B44" s="133"/>
-      <c r="C44" s="153"/>
-      <c r="D44" s="139"/>
+      <c r="A44" s="153"/>
+      <c r="B44" s="152"/>
+      <c r="C44" s="162"/>
+      <c r="D44" s="148"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="138" t="s">
+      <c r="A45" s="146" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="137" t="s">
+      <c r="B45" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="157"/>
+      <c r="C45" s="170"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="138"/>
-      <c r="B46" s="137"/>
-      <c r="C46" s="158"/>
-      <c r="D46" s="154" t="s">
+      <c r="A46" s="146"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="171"/>
+      <c r="D46" s="167" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="138"/>
-      <c r="B47" s="137"/>
-      <c r="C47" s="158"/>
-      <c r="D47" s="155"/>
+      <c r="A47" s="146"/>
+      <c r="B47" s="147"/>
+      <c r="C47" s="171"/>
+      <c r="D47" s="168"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="138"/>
-      <c r="B48" s="137"/>
-      <c r="C48" s="159"/>
-      <c r="D48" s="155"/>
+      <c r="A48" s="146"/>
+      <c r="B48" s="147"/>
+      <c r="C48" s="172"/>
+      <c r="D48" s="168"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="138"/>
-      <c r="B49" s="137"/>
-      <c r="C49" s="145"/>
-      <c r="D49" s="155"/>
+      <c r="A49" s="146"/>
+      <c r="B49" s="147"/>
+      <c r="C49" s="141"/>
+      <c r="D49" s="168"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="138"/>
-      <c r="B50" s="137"/>
-      <c r="C50" s="145"/>
-      <c r="D50" s="156"/>
+      <c r="A50" s="146"/>
+      <c r="B50" s="147"/>
+      <c r="C50" s="141"/>
+      <c r="D50" s="169"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30814,10 +30829,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="137" t="s">
+      <c r="A53" s="147" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="137" t="s">
+      <c r="B53" s="147" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30828,8 +30843,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="137"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="147"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30838,8 +30853,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="137"/>
-      <c r="B55" s="137"/>
+      <c r="A55" s="147"/>
+      <c r="B55" s="147"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30848,9 +30863,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="137"/>
-      <c r="B56" s="137"/>
-      <c r="C56" s="160" t="s">
+      <c r="A56" s="147"/>
+      <c r="B56" s="147"/>
+      <c r="C56" s="163" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30858,16 +30873,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="137"/>
-      <c r="B57" s="137"/>
-      <c r="C57" s="160"/>
+      <c r="A57" s="147"/>
+      <c r="B57" s="147"/>
+      <c r="C57" s="163"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="137"/>
-      <c r="B58" s="137"/>
+      <c r="A58" s="147"/>
+      <c r="B58" s="147"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30876,8 +30891,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="137"/>
-      <c r="B59" s="137"/>
+      <c r="A59" s="147"/>
+      <c r="B59" s="147"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30886,9 +30901,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="137"/>
-      <c r="B60" s="137"/>
-      <c r="C60" s="160" t="s">
+      <c r="A60" s="147"/>
+      <c r="B60" s="147"/>
+      <c r="C60" s="163" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30896,25 +30911,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="137"/>
-      <c r="B61" s="137"/>
-      <c r="C61" s="160"/>
+      <c r="A61" s="147"/>
+      <c r="B61" s="147"/>
+      <c r="C61" s="163"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="137"/>
-      <c r="B62" s="137"/>
-      <c r="C62" s="160"/>
+      <c r="A62" s="147"/>
+      <c r="B62" s="147"/>
+      <c r="C62" s="163"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="137"/>
-      <c r="B63" s="137"/>
-      <c r="C63" s="153" t="s">
+      <c r="A63" s="147"/>
+      <c r="B63" s="147"/>
+      <c r="C63" s="162" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30922,30 +30937,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="137"/>
-      <c r="B64" s="137"/>
-      <c r="C64" s="153"/>
-      <c r="D64" s="139" t="s">
+      <c r="A64" s="147"/>
+      <c r="B64" s="147"/>
+      <c r="C64" s="162"/>
+      <c r="D64" s="148" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="137"/>
-      <c r="B65" s="137"/>
-      <c r="C65" s="153"/>
-      <c r="D65" s="139"/>
+      <c r="A65" s="147"/>
+      <c r="B65" s="147"/>
+      <c r="C65" s="162"/>
+      <c r="D65" s="148"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="137"/>
-      <c r="B66" s="137"/>
-      <c r="C66" s="153"/>
-      <c r="D66" s="139"/>
+      <c r="A66" s="147"/>
+      <c r="B66" s="147"/>
+      <c r="C66" s="162"/>
+      <c r="D66" s="148"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="137"/>
-      <c r="B67" s="137"/>
-      <c r="C67" s="153"/>
-      <c r="D67" s="139"/>
+      <c r="A67" s="147"/>
+      <c r="B67" s="147"/>
+      <c r="C67" s="162"/>
+      <c r="D67" s="148"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31001,24 +31016,10 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="B53:B67"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C45:C48"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
@@ -31030,10 +31031,24 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31042,9 +31057,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -31063,7 +31078,7 @@
       <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="184" t="s">
+      <c r="C1" s="115" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="57" t="s">
@@ -31079,10 +31094,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="163" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="101"/>
@@ -31091,12 +31106,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="185" t="s">
+      <c r="A4" s="138"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="116" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="195" t="s">
+      <c r="D4" s="121" t="s">
         <v>256</v>
       </c>
     </row>
@@ -31104,11 +31119,11 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="160"/>
-      <c r="C5" s="185" t="s">
+      <c r="B5" s="163"/>
+      <c r="C5" s="116" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="114" t="s">
         <v>236</v>
       </c>
     </row>
@@ -31116,27 +31131,27 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="160"/>
-      <c r="C6" s="185" t="s">
+      <c r="B6" s="163"/>
+      <c r="C6" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="116" t="s">
+      <c r="D6" s="114" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="177" t="s">
+      <c r="A7" s="182" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="160"/>
+      <c r="B7" s="163"/>
       <c r="C7" s="101"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="178"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="183"/>
+      <c r="B8" s="163"/>
       <c r="C8" s="101"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
@@ -31144,9 +31159,9 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B9" s="160"/>
+        <v>291</v>
+      </c>
+      <c r="B9" s="163"/>
       <c r="C9" s="101" t="s">
         <v>30</v>
       </c>
@@ -31156,9 +31171,9 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="160"/>
+      <c r="B10" s="163"/>
       <c r="C10" s="101"/>
-      <c r="D10" s="116" t="s">
+      <c r="D10" s="114" t="s">
         <v>259</v>
       </c>
     </row>
@@ -31171,10 +31186,10 @@
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="174" t="s">
+      <c r="A12" s="179" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="160" t="s">
+      <c r="B12" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C12" s="101"/>
@@ -31183,509 +31198,530 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="175"/>
-      <c r="B13" s="160"/>
+      <c r="A13" s="180"/>
+      <c r="B13" s="197"/>
       <c r="C13" s="101"/>
       <c r="D13" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="176"/>
-      <c r="B14" s="160"/>
+      <c r="A14" s="180"/>
+      <c r="B14" s="197"/>
       <c r="C14" s="101"/>
       <c r="D14" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="101"/>
+      <c r="A15" s="181"/>
+      <c r="B15" s="176"/>
+      <c r="C15" s="58" t="s">
+        <v>301</v>
+      </c>
       <c r="D15" s="58" t="s">
-        <v>238</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="136" t="s">
-        <v>222</v>
-      </c>
-      <c r="B16" s="160" t="s">
+      <c r="A16" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="186" t="s">
-        <v>239</v>
-      </c>
-      <c r="D16" s="196" t="s">
-        <v>241</v>
+      <c r="C16" s="101"/>
+      <c r="D16" s="58" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="136"/>
-      <c r="B17" s="160"/>
-      <c r="C17" s="187"/>
-      <c r="D17" s="110" t="s">
+      <c r="A17" s="138" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="163" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="190" t="s">
+        <v>239</v>
+      </c>
+      <c r="D17" s="122" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="138"/>
+      <c r="B18" s="163"/>
+      <c r="C18" s="191"/>
+      <c r="D18" s="109" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="160"/>
-      <c r="C18" s="188" t="s">
-        <v>240</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="58" t="s">
-        <v>292</v>
-      </c>
-      <c r="B19" s="112" t="s">
+      <c r="A19" s="138"/>
+      <c r="B19" s="163"/>
+      <c r="C19" s="195" t="s">
+        <v>240</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="138"/>
+      <c r="B20" s="163"/>
+      <c r="C20" s="196"/>
+      <c r="D20" s="61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="147" t="s">
+        <v>297</v>
+      </c>
+      <c r="B21" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="101" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="58"/>
+      <c r="C21" s="58" t="s">
+        <v>298</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>299</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="107" t="s">
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="147"/>
+      <c r="B22" s="163"/>
+      <c r="C22" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="58" t="s">
         <v>280</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="103" t="s">
-        <v>282</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>281</v>
-      </c>
     </row>
-    <row r="21" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39" t="s">
+    <row r="23" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="44"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="177" t="s">
-        <v>260</v>
-      </c>
-      <c r="B22" s="160" t="s">
-        <v>234</v>
-      </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="79" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="178"/>
-      <c r="B23" s="160"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="58" t="s">
-        <v>257</v>
-      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="B24" s="106" t="s">
+      <c r="A24" s="182" t="s">
+        <v>260</v>
+      </c>
+      <c r="B24" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C24" s="185" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>30</v>
+      <c r="C24" s="101"/>
+      <c r="D24" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="179" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="182" t="s">
-        <v>234</v>
-      </c>
-      <c r="C25" s="101" t="s">
-        <v>268</v>
-      </c>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="183"/>
+      <c r="B25" s="163"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="58" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="180"/>
-      <c r="B26" s="183"/>
-      <c r="C26" t="s">
-        <v>270</v>
-      </c>
-      <c r="D26" s="58" t="s">
-        <v>251</v>
+      <c r="A26" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="116" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="114" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="180"/>
-      <c r="B27" s="183"/>
+    <row r="27" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="184" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="187" t="s">
+        <v>234</v>
+      </c>
       <c r="C27" s="101" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="180"/>
-      <c r="B28" s="183"/>
-      <c r="C28" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D28" s="110" t="s">
-        <v>102</v>
+      <c r="A28" s="185"/>
+      <c r="B28" s="188"/>
+      <c r="C28" t="s">
+        <v>270</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="180"/>
-      <c r="B29" s="183"/>
+      <c r="A29" s="185"/>
+      <c r="B29" s="188"/>
       <c r="C29" s="101" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="180"/>
-      <c r="B30" s="183"/>
-      <c r="C30" s="101" t="s">
-        <v>284</v>
-      </c>
-      <c r="D30" s="58" t="s">
-        <v>285</v>
+      <c r="A30" s="185"/>
+      <c r="B30" s="188"/>
+      <c r="C30" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D30" s="109" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="180"/>
-      <c r="B31" s="183"/>
-      <c r="C31" s="104" t="s">
-        <v>289</v>
-      </c>
-      <c r="D31" s="110" t="s">
+      <c r="A31" s="185"/>
+      <c r="B31" s="188"/>
+      <c r="C31" s="101" t="s">
+        <v>282</v>
+      </c>
+      <c r="D31" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="180"/>
-      <c r="B32" s="183"/>
-      <c r="C32" s="104" t="s">
-        <v>290</v>
-      </c>
-      <c r="D32" s="110" t="s">
-        <v>251</v>
+      <c r="A32" s="185"/>
+      <c r="B32" s="188"/>
+      <c r="C32" s="101" t="s">
+        <v>283</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="180"/>
-      <c r="B33" s="183"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="188"/>
       <c r="C33" s="104" t="s">
-        <v>291</v>
-      </c>
-      <c r="D33" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" s="109" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="185"/>
+      <c r="B34" s="188"/>
+      <c r="C34" s="104" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" s="109" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="185"/>
+      <c r="B35" s="188"/>
+      <c r="C35" s="104" t="s">
+        <v>290</v>
+      </c>
+      <c r="D35" s="109" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="181"/>
-      <c r="B34" s="167"/>
-      <c r="C34" s="189" t="s">
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="186"/>
+      <c r="B36" s="189"/>
+      <c r="C36" s="117" t="s">
         <v>244</v>
       </c>
-      <c r="D34" s="116" t="s">
+      <c r="D36" s="114" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39" t="s">
+    <row r="37" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="44"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="44"/>
     </row>
-    <row r="36" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="101"/>
-      <c r="D36" s="79" t="s">
+    <row r="38" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="99"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="160" t="s">
+    <row r="39" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="163" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="160" t="s">
+      <c r="B39" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="185" t="s">
+      <c r="C39" s="116" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="58" t="s">
+      <c r="D39" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="160"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="185">
-        <v>10.1</v>
-      </c>
-      <c r="D38" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="160"/>
-      <c r="B39" s="160"/>
-      <c r="C39" s="185">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D39" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="160"/>
-      <c r="B40" s="160"/>
-      <c r="C40" s="190" t="s">
-        <v>295</v>
-      </c>
-      <c r="D40" s="114" t="s">
-        <v>296</v>
+      <c r="A40" s="163"/>
+      <c r="B40" s="163"/>
+      <c r="C40" s="116">
+        <v>10.1</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="136" t="s">
-        <v>247</v>
-      </c>
-      <c r="B41" s="160" t="s">
-        <v>234</v>
-      </c>
-      <c r="C41" s="191"/>
-      <c r="D41" s="197" t="s">
-        <v>261</v>
+      <c r="A41" s="163"/>
+      <c r="B41" s="163"/>
+      <c r="C41" s="116">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="136"/>
-      <c r="B42" s="160"/>
-      <c r="C42" s="192"/>
-      <c r="D42" s="197"/>
+      <c r="A42" s="163"/>
+      <c r="B42" s="163"/>
+      <c r="C42" s="118" t="s">
+        <v>294</v>
+      </c>
+      <c r="D42" s="112" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="108" t="s">
-        <v>262</v>
-      </c>
-      <c r="B43" s="109" t="s">
+      <c r="A43" s="138" t="s">
+        <v>247</v>
+      </c>
+      <c r="B43" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C43" s="185" t="s">
-        <v>250</v>
-      </c>
-      <c r="D43" s="110" t="s">
-        <v>251</v>
+      <c r="C43" s="192"/>
+      <c r="D43" s="194" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="105"/>
-      <c r="D44" s="98"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="138"/>
+      <c r="B44" s="163"/>
+      <c r="C44" s="193"/>
+      <c r="D44" s="194"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="58" t="s">
+      <c r="A45" s="107" t="s">
+        <v>262</v>
+      </c>
+      <c r="B45" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="116" t="s">
+        <v>250</v>
+      </c>
+      <c r="D45" s="109" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" s="39"/>
+      <c r="C46" s="105"/>
+      <c r="D46" s="98"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="B45" s="109" t="s">
+      <c r="B47" s="108" t="s">
         <v>234</v>
       </c>
-      <c r="C45" s="193" t="s">
+      <c r="C47" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D45" s="58" t="s">
+      <c r="D47" s="58" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="168" t="s">
-        <v>286</v>
-      </c>
-      <c r="B46" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="C46" s="194" t="s">
-        <v>297</v>
-      </c>
-      <c r="D46" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="169"/>
-      <c r="B47" s="171"/>
-      <c r="C47" s="193" t="s">
-        <v>287</v>
-      </c>
-      <c r="D47" s="58" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="98"/>
-      <c r="C48" s="115"/>
-      <c r="D48" s="98"/>
+      <c r="A48" s="173" t="s">
+        <v>285</v>
+      </c>
+      <c r="B48" s="175" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48" s="120" t="s">
+        <v>296</v>
+      </c>
+      <c r="D48" s="58" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="172" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="182" t="s">
-        <v>271</v>
-      </c>
-      <c r="C49" s="193" t="s">
-        <v>265</v>
+    <row r="49" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="174"/>
+      <c r="B49" s="176"/>
+      <c r="C49" s="119" t="s">
+        <v>286</v>
       </c>
       <c r="D49" s="58" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="173"/>
-      <c r="B50" s="167"/>
-      <c r="C50" s="193" t="s">
+      <c r="A50" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="98"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="98"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="177" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="187" t="s">
+        <v>271</v>
+      </c>
+      <c r="C51" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="D50" s="58" t="s">
+      <c r="D51" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="178"/>
+      <c r="B52" s="189"/>
+      <c r="C52" s="119" t="s">
+        <v>265</v>
+      </c>
+      <c r="D52" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="97" t="s">
+    <row r="53" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="109" t="s">
-        <v>271</v>
-      </c>
-      <c r="C51" s="103" t="s">
-        <v>264</v>
-      </c>
-      <c r="D51" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="58" t="s">
-        <v>293</v>
-      </c>
-      <c r="B52" s="113" t="s">
-        <v>271</v>
-      </c>
-      <c r="C52" s="101"/>
-      <c r="D52" s="61" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="109" t="s">
+      <c r="B53" s="108" t="s">
         <v>271</v>
       </c>
       <c r="C53" s="103" t="s">
         <v>264</v>
       </c>
       <c r="D53" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="58" t="s">
+        <v>292</v>
+      </c>
+      <c r="B54" s="111" t="s">
+        <v>271</v>
+      </c>
+      <c r="C54" s="101"/>
+      <c r="D54" s="61" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="108" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" s="103" t="s">
+        <v>264</v>
+      </c>
+      <c r="D55" s="58" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B54" s="98"/>
-      <c r="C54" s="115"/>
-      <c r="D54" s="98"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="58"/>
-      <c r="B55" s="109" t="s">
-        <v>234</v>
-      </c>
-      <c r="C55" s="101" t="s">
-        <v>30</v>
-      </c>
-      <c r="D55" s="110" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="98" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B56" s="98"/>
-      <c r="C56" s="115"/>
+      <c r="C56" s="113"/>
       <c r="D56" s="98"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="58"/>
-      <c r="B57" s="109" t="s">
+      <c r="B57" s="108" t="s">
         <v>234</v>
       </c>
       <c r="C57" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="110" t="s">
+      <c r="D57" s="109" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B58" s="98"/>
+      <c r="C58" s="113"/>
+      <c r="D58" s="98"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="58"/>
+      <c r="B59" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" s="109" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A41:A42"/>
+  <mergeCells count="25">
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B36"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B51:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Removal of validation code 3008"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -19,9 +19,9 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2679,9 +2679,6 @@
     <t>code 2048</t>
   </si>
   <si>
-    <t>code 3008 - 3012</t>
-  </si>
-  <si>
     <t>code 4004</t>
   </si>
   <si>
@@ -2719,6 +2716,9 @@
   </si>
   <si>
     <t>Data item number changed from 38 to 39</t>
+  </si>
+  <si>
+    <t>code 3009 - 3012</t>
   </si>
 </sst>
 </file>
@@ -3700,8 +3700,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3724,35 +3754,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3772,38 +3805,44 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3811,25 +3850,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3854,30 +3878,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4892,7 +4892,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4902,7 +4902,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5012,10 +5012,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="153" t="s">
+      <c r="A7" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5026,8 +5026,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="153"/>
-      <c r="B8" s="152"/>
+      <c r="A8" s="138"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5036,8 +5036,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="153"/>
-      <c r="B9" s="152"/>
+      <c r="A9" s="138"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5046,8 +5046,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="153"/>
-      <c r="B10" s="152"/>
+      <c r="A10" s="138"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5056,8 +5056,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="153"/>
-      <c r="B11" s="152"/>
+      <c r="A11" s="138"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5066,8 +5066,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="153"/>
-      <c r="B12" s="152"/>
+      <c r="A12" s="138"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5076,10 +5076,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="155" t="s">
+      <c r="A13" s="141" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5090,8 +5090,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="155"/>
-      <c r="B14" s="152"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5100,8 +5100,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="155"/>
-      <c r="B15" s="152"/>
+      <c r="A15" s="141"/>
+      <c r="B15" s="139"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5110,10 +5110,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="138" t="s">
+      <c r="A16" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5124,8 +5124,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="138"/>
-      <c r="B17" s="147"/>
+      <c r="A17" s="142"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5134,8 +5134,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="138"/>
-      <c r="B18" s="147"/>
+      <c r="A18" s="142"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5144,8 +5144,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="138"/>
-      <c r="B19" s="147"/>
+      <c r="A19" s="142"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5154,8 +5154,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="138"/>
-      <c r="B20" s="147"/>
+      <c r="A20" s="142"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5164,8 +5164,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="138"/>
-      <c r="B21" s="147"/>
+      <c r="A21" s="142"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5174,8 +5174,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="138"/>
-      <c r="B22" s="147"/>
+      <c r="A22" s="142"/>
+      <c r="B22" s="143"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5184,8 +5184,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="138"/>
-      <c r="B23" s="147"/>
+      <c r="A23" s="142"/>
+      <c r="B23" s="143"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5194,26 +5194,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="138"/>
-      <c r="B24" s="147"/>
-      <c r="C24" s="138" t="s">
+      <c r="A24" s="142"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="142" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="139" t="s">
+      <c r="D24" s="149" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="138"/>
-      <c r="B25" s="147"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="139"/>
+      <c r="A25" s="142"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="142"/>
+      <c r="D25" s="149"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="153" t="s">
+      <c r="A26" s="138" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="152" t="s">
+      <c r="B26" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5224,8 +5224,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="153"/>
-      <c r="B27" s="152"/>
+      <c r="A27" s="138"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5252,28 +5252,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="154" t="s">
+      <c r="A30" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="152" t="s">
+      <c r="B30" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="138" t="s">
+      <c r="C30" s="142" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="142" t="s">
+      <c r="D30" s="152" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="154"/>
-      <c r="B31" s="152"/>
-      <c r="C31" s="138"/>
-      <c r="D31" s="142"/>
+      <c r="A31" s="140"/>
+      <c r="B31" s="139"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="152"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="154"/>
-      <c r="B32" s="152"/>
+      <c r="A32" s="140"/>
+      <c r="B32" s="139"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5282,8 +5282,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="154"/>
-      <c r="B33" s="152"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="139"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5292,8 +5292,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="154"/>
-      <c r="B34" s="152"/>
+      <c r="A34" s="140"/>
+      <c r="B34" s="139"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5302,8 +5302,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="154"/>
-      <c r="B35" s="152"/>
+      <c r="A35" s="140"/>
+      <c r="B35" s="139"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5312,8 +5312,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="154"/>
-      <c r="B36" s="152"/>
+      <c r="A36" s="140"/>
+      <c r="B36" s="139"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5322,26 +5322,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="154"/>
-      <c r="B37" s="152"/>
-      <c r="C37" s="143" t="s">
+      <c r="A37" s="140"/>
+      <c r="B37" s="139"/>
+      <c r="C37" s="153" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="145" t="s">
+      <c r="D37" s="155" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="154"/>
-      <c r="B38" s="152"/>
-      <c r="C38" s="144"/>
-      <c r="D38" s="145"/>
+      <c r="A38" s="140"/>
+      <c r="B38" s="139"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="155"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="153" t="s">
+      <c r="A39" s="138" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5352,8 +5352,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="153"/>
-      <c r="B40" s="152"/>
+      <c r="A40" s="138"/>
+      <c r="B40" s="139"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5380,10 +5380,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="154" t="s">
+      <c r="A43" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="152" t="s">
+      <c r="B43" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5392,8 +5392,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="154"/>
-      <c r="B44" s="152"/>
+      <c r="A44" s="140"/>
+      <c r="B44" s="139"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5402,10 +5402,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="149" t="s">
+      <c r="A45" s="146" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="152" t="s">
+      <c r="B45" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5414,8 +5414,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="150"/>
-      <c r="B46" s="152"/>
+      <c r="A46" s="147"/>
+      <c r="B46" s="139"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5424,8 +5424,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="150"/>
-      <c r="B47" s="152"/>
+      <c r="A47" s="147"/>
+      <c r="B47" s="139"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5434,8 +5434,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="151"/>
-      <c r="B48" s="152"/>
+      <c r="A48" s="148"/>
+      <c r="B48" s="139"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5444,10 +5444,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="147" t="s">
+      <c r="A49" s="143" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="147" t="s">
+      <c r="B49" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9551,8 +9551,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="147"/>
-      <c r="B50" s="147"/>
+      <c r="A50" s="143"/>
+      <c r="B50" s="143"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13656,8 +13656,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="147"/>
-      <c r="B51" s="147"/>
+      <c r="A51" s="143"/>
+      <c r="B51" s="143"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17761,8 +17761,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="147"/>
-      <c r="B52" s="147"/>
+      <c r="A52" s="143"/>
+      <c r="B52" s="143"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21866,12 +21866,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="147"/>
-      <c r="B53" s="147"/>
-      <c r="C53" s="141" t="s">
+      <c r="A53" s="143"/>
+      <c r="B53" s="143"/>
+      <c r="C53" s="151" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="142" t="s">
+      <c r="D53" s="152" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25971,10 +25971,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="147"/>
-      <c r="B54" s="147"/>
-      <c r="C54" s="141"/>
-      <c r="D54" s="142"/>
+      <c r="A54" s="143"/>
+      <c r="B54" s="143"/>
+      <c r="C54" s="151"/>
+      <c r="D54" s="152"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30092,10 +30092,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="146" t="s">
+      <c r="A57" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="147" t="s">
+      <c r="B57" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30106,8 +30106,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="146"/>
-      <c r="B58" s="147"/>
+      <c r="A58" s="144"/>
+      <c r="B58" s="143"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30116,8 +30116,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="146"/>
-      <c r="B59" s="147"/>
+      <c r="A59" s="144"/>
+      <c r="B59" s="143"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30126,8 +30126,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="146"/>
-      <c r="B60" s="147"/>
+      <c r="A60" s="144"/>
+      <c r="B60" s="143"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30136,8 +30136,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="146"/>
-      <c r="B61" s="147"/>
+      <c r="A61" s="144"/>
+      <c r="B61" s="143"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30146,8 +30146,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="146"/>
-      <c r="B62" s="147"/>
+      <c r="A62" s="144"/>
+      <c r="B62" s="143"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30156,8 +30156,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="146"/>
-      <c r="B63" s="147"/>
+      <c r="A63" s="144"/>
+      <c r="B63" s="143"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30166,16 +30166,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="146"/>
-      <c r="B64" s="147"/>
+      <c r="A64" s="144"/>
+      <c r="B64" s="143"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="146"/>
-      <c r="B65" s="147"/>
+      <c r="A65" s="144"/>
+      <c r="B65" s="143"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30184,16 +30184,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="146"/>
-      <c r="B66" s="147"/>
+      <c r="A66" s="144"/>
+      <c r="B66" s="143"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="146"/>
-      <c r="B67" s="147"/>
+      <c r="A67" s="144"/>
+      <c r="B67" s="143"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30202,8 +30202,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="146"/>
-      <c r="B68" s="147"/>
+      <c r="A68" s="144"/>
+      <c r="B68" s="143"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30212,8 +30212,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="146"/>
-      <c r="B69" s="147"/>
+      <c r="A69" s="144"/>
+      <c r="B69" s="143"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30222,8 +30222,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="146"/>
-      <c r="B70" s="147"/>
+      <c r="A70" s="144"/>
+      <c r="B70" s="143"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30232,8 +30232,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="146"/>
-      <c r="B71" s="147"/>
+      <c r="A71" s="144"/>
+      <c r="B71" s="143"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30242,8 +30242,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="146"/>
-      <c r="B72" s="147"/>
+      <c r="A72" s="144"/>
+      <c r="B72" s="143"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30252,16 +30252,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="146"/>
-      <c r="B73" s="147"/>
+      <c r="A73" s="144"/>
+      <c r="B73" s="143"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="146"/>
-      <c r="B74" s="147"/>
+      <c r="A74" s="144"/>
+      <c r="B74" s="143"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30270,18 +30270,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="146"/>
-      <c r="B75" s="147"/>
-      <c r="C75" s="140"/>
-      <c r="D75" s="148" t="s">
+      <c r="A75" s="144"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="150"/>
+      <c r="D75" s="145" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="146"/>
-      <c r="B76" s="147"/>
-      <c r="C76" s="140"/>
-      <c r="D76" s="148"/>
+      <c r="A76" s="144"/>
+      <c r="B76" s="143"/>
+      <c r="C76" s="150"/>
+      <c r="D76" s="145"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30305,8 +30305,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30315,13 +30315,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30336,22 +30352,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30405,10 +30405,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="139" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30419,133 +30419,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="153"/>
-      <c r="B5" s="152"/>
-      <c r="C5" s="165" t="s">
+      <c r="A5" s="138"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="163" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="164" t="s">
+      <c r="D5" s="162" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="153"/>
-      <c r="B6" s="152"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="164"/>
+      <c r="A6" s="138"/>
+      <c r="B6" s="139"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="162"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="153"/>
-      <c r="B7" s="152"/>
+      <c r="A7" s="138"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="153"/>
-      <c r="B8" s="152"/>
+      <c r="A8" s="138"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="153"/>
-      <c r="B9" s="152"/>
+      <c r="A9" s="138"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="155" t="s">
+      <c r="A10" s="141" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="152" t="s">
+      <c r="B10" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="162"/>
-      <c r="D10" s="164" t="s">
+      <c r="C10" s="165"/>
+      <c r="D10" s="162" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="155"/>
-      <c r="B11" s="152"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="164"/>
+      <c r="A11" s="141"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="162"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="155"/>
-      <c r="B12" s="152"/>
-      <c r="C12" s="162"/>
-      <c r="D12" s="164"/>
+      <c r="A12" s="141"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="162"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="143" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="166"/>
-      <c r="D13" s="164" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="162" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="138"/>
-      <c r="B14" s="147"/>
-      <c r="C14" s="166"/>
-      <c r="D14" s="164"/>
+      <c r="A14" s="142"/>
+      <c r="B14" s="143"/>
+      <c r="C14" s="164"/>
+      <c r="D14" s="162"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="138"/>
-      <c r="B15" s="147"/>
-      <c r="C15" s="166"/>
+      <c r="A15" s="142"/>
+      <c r="B15" s="143"/>
+      <c r="C15" s="164"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="138"/>
-      <c r="B16" s="147"/>
-      <c r="C16" s="166"/>
+      <c r="A16" s="142"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="164"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="138"/>
-      <c r="B17" s="147"/>
-      <c r="C17" s="166"/>
+      <c r="A17" s="142"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="164"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="138"/>
-      <c r="B18" s="147"/>
-      <c r="C18" s="166"/>
+      <c r="A18" s="142"/>
+      <c r="B18" s="143"/>
+      <c r="C18" s="164"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="138"/>
-      <c r="B19" s="147"/>
-      <c r="C19" s="166"/>
+      <c r="A19" s="142"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="164"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="138"/>
-      <c r="B20" s="147"/>
-      <c r="C20" s="166"/>
+      <c r="A20" s="142"/>
+      <c r="B20" s="143"/>
+      <c r="C20" s="164"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="138"/>
-      <c r="B21" s="147"/>
-      <c r="C21" s="166"/>
+      <c r="A21" s="142"/>
+      <c r="B21" s="143"/>
+      <c r="C21" s="164"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="138"/>
-      <c r="B22" s="147"/>
-      <c r="C22" s="166"/>
+      <c r="A22" s="142"/>
+      <c r="B22" s="143"/>
+      <c r="C22" s="164"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="138"/>
-      <c r="B23" s="147"/>
-      <c r="C23" s="166"/>
+      <c r="A23" s="142"/>
+      <c r="B23" s="143"/>
+      <c r="C23" s="164"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30643,10 +30643,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="156" t="s">
+      <c r="A32" s="167" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="159" t="s">
+      <c r="B32" s="170" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30657,26 +30657,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="157"/>
-      <c r="B33" s="160"/>
+      <c r="A33" s="168"/>
+      <c r="B33" s="171"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="157"/>
-      <c r="B34" s="160"/>
+      <c r="A34" s="168"/>
+      <c r="B34" s="171"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="157"/>
-      <c r="B35" s="160"/>
+      <c r="A35" s="168"/>
+      <c r="B35" s="171"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="158"/>
-      <c r="B36" s="161"/>
+      <c r="A36" s="169"/>
+      <c r="B36" s="172"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30705,10 +30705,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="154" t="s">
+      <c r="A39" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="139" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30719,8 +30719,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="154"/>
-      <c r="B40" s="152"/>
+      <c r="A40" s="140"/>
+      <c r="B40" s="139"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30729,84 +30729,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="153" t="s">
+      <c r="A41" s="138" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="152" t="s">
+      <c r="B41" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="162" t="s">
+      <c r="C41" s="165" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="138" t="s">
+      <c r="D41" s="142" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="153"/>
-      <c r="B42" s="152"/>
-      <c r="C42" s="162"/>
-      <c r="D42" s="138"/>
+      <c r="A42" s="138"/>
+      <c r="B42" s="139"/>
+      <c r="C42" s="165"/>
+      <c r="D42" s="142"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="153"/>
-      <c r="B43" s="152"/>
-      <c r="C43" s="162" t="s">
+      <c r="A43" s="138"/>
+      <c r="B43" s="139"/>
+      <c r="C43" s="165" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="148" t="s">
+      <c r="D43" s="145" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="153"/>
-      <c r="B44" s="152"/>
-      <c r="C44" s="162"/>
-      <c r="D44" s="148"/>
+      <c r="A44" s="138"/>
+      <c r="B44" s="139"/>
+      <c r="C44" s="165"/>
+      <c r="D44" s="145"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="146" t="s">
+      <c r="A45" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="147" t="s">
+      <c r="B45" s="143" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="170"/>
+      <c r="C45" s="159"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="146"/>
-      <c r="B46" s="147"/>
-      <c r="C46" s="171"/>
-      <c r="D46" s="167" t="s">
+      <c r="A46" s="144"/>
+      <c r="B46" s="143"/>
+      <c r="C46" s="160"/>
+      <c r="D46" s="156" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="146"/>
-      <c r="B47" s="147"/>
-      <c r="C47" s="171"/>
-      <c r="D47" s="168"/>
+      <c r="A47" s="144"/>
+      <c r="B47" s="143"/>
+      <c r="C47" s="160"/>
+      <c r="D47" s="157"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="146"/>
-      <c r="B48" s="147"/>
-      <c r="C48" s="172"/>
-      <c r="D48" s="168"/>
+      <c r="A48" s="144"/>
+      <c r="B48" s="143"/>
+      <c r="C48" s="161"/>
+      <c r="D48" s="157"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="146"/>
-      <c r="B49" s="147"/>
-      <c r="C49" s="141"/>
-      <c r="D49" s="168"/>
+      <c r="A49" s="144"/>
+      <c r="B49" s="143"/>
+      <c r="C49" s="151"/>
+      <c r="D49" s="157"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="146"/>
-      <c r="B50" s="147"/>
-      <c r="C50" s="141"/>
-      <c r="D50" s="169"/>
+      <c r="A50" s="144"/>
+      <c r="B50" s="143"/>
+      <c r="C50" s="151"/>
+      <c r="D50" s="158"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30829,10 +30829,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="147" t="s">
+      <c r="A53" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="147" t="s">
+      <c r="B53" s="143" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30843,8 +30843,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="147"/>
-      <c r="B54" s="147"/>
+      <c r="A54" s="143"/>
+      <c r="B54" s="143"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30853,8 +30853,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="147"/>
-      <c r="B55" s="147"/>
+      <c r="A55" s="143"/>
+      <c r="B55" s="143"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30863,9 +30863,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="147"/>
-      <c r="B56" s="147"/>
-      <c r="C56" s="163" t="s">
+      <c r="A56" s="143"/>
+      <c r="B56" s="143"/>
+      <c r="C56" s="166" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30873,16 +30873,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="147"/>
-      <c r="B57" s="147"/>
-      <c r="C57" s="163"/>
+      <c r="A57" s="143"/>
+      <c r="B57" s="143"/>
+      <c r="C57" s="166"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="147"/>
-      <c r="B58" s="147"/>
+      <c r="A58" s="143"/>
+      <c r="B58" s="143"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30891,8 +30891,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="147"/>
-      <c r="B59" s="147"/>
+      <c r="A59" s="143"/>
+      <c r="B59" s="143"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30901,9 +30901,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="147"/>
-      <c r="B60" s="147"/>
-      <c r="C60" s="163" t="s">
+      <c r="A60" s="143"/>
+      <c r="B60" s="143"/>
+      <c r="C60" s="166" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30911,25 +30911,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="147"/>
-      <c r="B61" s="147"/>
-      <c r="C61" s="163"/>
+      <c r="A61" s="143"/>
+      <c r="B61" s="143"/>
+      <c r="C61" s="166"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="147"/>
-      <c r="B62" s="147"/>
-      <c r="C62" s="163"/>
+      <c r="A62" s="143"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="166"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="147"/>
-      <c r="B63" s="147"/>
-      <c r="C63" s="162" t="s">
+      <c r="A63" s="143"/>
+      <c r="B63" s="143"/>
+      <c r="C63" s="165" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30937,30 +30937,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="147"/>
-      <c r="B64" s="147"/>
-      <c r="C64" s="162"/>
-      <c r="D64" s="148" t="s">
+      <c r="A64" s="143"/>
+      <c r="B64" s="143"/>
+      <c r="C64" s="165"/>
+      <c r="D64" s="145" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="147"/>
-      <c r="B65" s="147"/>
-      <c r="C65" s="162"/>
-      <c r="D65" s="148"/>
+      <c r="A65" s="143"/>
+      <c r="B65" s="143"/>
+      <c r="C65" s="165"/>
+      <c r="D65" s="145"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="147"/>
-      <c r="B66" s="147"/>
-      <c r="C66" s="162"/>
-      <c r="D66" s="148"/>
+      <c r="A66" s="143"/>
+      <c r="B66" s="143"/>
+      <c r="C66" s="165"/>
+      <c r="D66" s="145"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="147"/>
-      <c r="B67" s="147"/>
-      <c r="C67" s="162"/>
-      <c r="D67" s="148"/>
+      <c r="A67" s="143"/>
+      <c r="B67" s="143"/>
+      <c r="C67" s="165"/>
+      <c r="D67" s="145"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31016,6 +31016,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31024,31 +31041,14 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B41:B44"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B53:B67"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31059,8 +31059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31094,10 +31094,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="166" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="101"/>
@@ -31106,8 +31106,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="138"/>
-      <c r="B4" s="163"/>
+      <c r="A4" s="142"/>
+      <c r="B4" s="166"/>
       <c r="C4" s="116" t="s">
         <v>235</v>
       </c>
@@ -31119,7 +31119,7 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="163"/>
+      <c r="B5" s="166"/>
       <c r="C5" s="116" t="s">
         <v>235</v>
       </c>
@@ -31131,7 +31131,7 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="163"/>
+      <c r="B6" s="166"/>
       <c r="C6" s="116" t="s">
         <v>22</v>
       </c>
@@ -31140,18 +31140,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="182" t="s">
+      <c r="A7" s="190" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="163"/>
+      <c r="B7" s="166"/>
       <c r="C7" s="101"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="183"/>
-      <c r="B8" s="163"/>
+      <c r="A8" s="191"/>
+      <c r="B8" s="166"/>
       <c r="C8" s="101"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
@@ -31159,9 +31159,9 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B9" s="163"/>
+        <v>290</v>
+      </c>
+      <c r="B9" s="166"/>
       <c r="C9" s="101" t="s">
         <v>30</v>
       </c>
@@ -31171,7 +31171,7 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="163"/>
+      <c r="B10" s="166"/>
       <c r="C10" s="101"/>
       <c r="D10" s="114" t="s">
         <v>259</v>
@@ -31186,10 +31186,10 @@
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="179" t="s">
+      <c r="A12" s="173" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="175" t="s">
+      <c r="B12" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C12" s="101"/>
@@ -31198,29 +31198,29 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="180"/>
-      <c r="B13" s="197"/>
+      <c r="A13" s="174"/>
+      <c r="B13" s="177"/>
       <c r="C13" s="101"/>
       <c r="D13" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="180"/>
-      <c r="B14" s="197"/>
+      <c r="A14" s="174"/>
+      <c r="B14" s="177"/>
       <c r="C14" s="101"/>
       <c r="D14" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="181"/>
-      <c r="B15" s="176"/>
+      <c r="A15" s="175"/>
+      <c r="B15" s="178"/>
       <c r="C15" s="58" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" s="58" t="s">
         <v>301</v>
-      </c>
-      <c r="D15" s="58" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -31236,13 +31236,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="138" t="s">
+      <c r="A17" s="142" t="s">
         <v>222</v>
       </c>
-      <c r="B17" s="163" t="s">
+      <c r="B17" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C17" s="190" t="s">
+      <c r="C17" s="179" t="s">
         <v>239</v>
       </c>
       <c r="D17" s="122" t="s">
@@ -31250,48 +31250,48 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="138"/>
-      <c r="B18" s="163"/>
-      <c r="C18" s="191"/>
+      <c r="A18" s="142"/>
+      <c r="B18" s="166"/>
+      <c r="C18" s="180"/>
       <c r="D18" s="109" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="138"/>
-      <c r="B19" s="163"/>
-      <c r="C19" s="195" t="s">
+      <c r="A19" s="142"/>
+      <c r="B19" s="166"/>
+      <c r="C19" s="184" t="s">
         <v>240</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="138"/>
-      <c r="B20" s="163"/>
-      <c r="C20" s="196"/>
+      <c r="A20" s="142"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="185"/>
       <c r="D20" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="147" t="s">
+      <c r="A21" s="143" t="s">
+        <v>296</v>
+      </c>
+      <c r="B21" s="166" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B21" s="163" t="s">
-        <v>234</v>
-      </c>
-      <c r="C21" s="58" t="s">
+      <c r="D21" s="58" t="s">
         <v>298</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="147"/>
-      <c r="B22" s="163"/>
+      <c r="A22" s="143"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="61" t="s">
         <v>281</v>
       </c>
@@ -31308,10 +31308,10 @@
       <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="182" t="s">
+      <c r="A24" s="190" t="s">
         <v>260</v>
       </c>
-      <c r="B24" s="163" t="s">
+      <c r="B24" s="166" t="s">
         <v>234</v>
       </c>
       <c r="C24" s="101"/>
@@ -31320,8 +31320,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="183"/>
-      <c r="B25" s="163"/>
+      <c r="A25" s="191"/>
+      <c r="B25" s="166"/>
       <c r="C25" s="101"/>
       <c r="D25" s="58" t="s">
         <v>257</v>
@@ -31342,10 +31342,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="184" t="s">
+      <c r="A27" s="192" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="187" t="s">
+      <c r="B27" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="101" t="s">
@@ -31356,8 +31356,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="185"/>
-      <c r="B28" s="188"/>
+      <c r="A28" s="193"/>
+      <c r="B28" s="196"/>
       <c r="C28" t="s">
         <v>270</v>
       </c>
@@ -31366,8 +31366,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="185"/>
-      <c r="B29" s="188"/>
+      <c r="A29" s="193"/>
+      <c r="B29" s="196"/>
       <c r="C29" s="101" t="s">
         <v>269</v>
       </c>
@@ -31376,8 +31376,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="185"/>
-      <c r="B30" s="188"/>
+      <c r="A30" s="193"/>
+      <c r="B30" s="196"/>
       <c r="C30" s="100" t="s">
         <v>277</v>
       </c>
@@ -31386,8 +31386,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="185"/>
-      <c r="B31" s="188"/>
+      <c r="A31" s="193"/>
+      <c r="B31" s="196"/>
       <c r="C31" s="101" t="s">
         <v>282</v>
       </c>
@@ -31396,8 +31396,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="185"/>
-      <c r="B32" s="188"/>
+      <c r="A32" s="193"/>
+      <c r="B32" s="196"/>
       <c r="C32" s="101" t="s">
         <v>283</v>
       </c>
@@ -31406,8 +31406,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="185"/>
-      <c r="B33" s="188"/>
+      <c r="A33" s="193"/>
+      <c r="B33" s="196"/>
       <c r="C33" s="104" t="s">
         <v>288</v>
       </c>
@@ -31416,28 +31416,28 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="185"/>
-      <c r="B34" s="188"/>
+      <c r="A34" s="193"/>
+      <c r="B34" s="196"/>
       <c r="C34" s="104" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="D34" s="109" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="185"/>
-      <c r="B35" s="188"/>
+      <c r="A35" s="193"/>
+      <c r="B35" s="196"/>
       <c r="C35" s="104" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D35" s="109" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="186"/>
-      <c r="B36" s="189"/>
+      <c r="A36" s="194"/>
+      <c r="B36" s="197"/>
       <c r="C36" s="117" t="s">
         <v>244</v>
       </c>
@@ -31462,10 +31462,10 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="163" t="s">
+      <c r="A39" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="163" t="s">
+      <c r="B39" s="166" t="s">
         <v>234</v>
       </c>
       <c r="C39" s="116" t="s">
@@ -31476,8 +31476,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="163"/>
-      <c r="B40" s="163"/>
+      <c r="A40" s="166"/>
+      <c r="B40" s="166"/>
       <c r="C40" s="116">
         <v>10.1</v>
       </c>
@@ -31486,8 +31486,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="163"/>
-      <c r="B41" s="163"/>
+      <c r="A41" s="166"/>
+      <c r="B41" s="166"/>
       <c r="C41" s="116">
         <v>10.199999999999999</v>
       </c>
@@ -31496,32 +31496,32 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="163"/>
-      <c r="B42" s="163"/>
+      <c r="A42" s="166"/>
+      <c r="B42" s="166"/>
       <c r="C42" s="118" t="s">
+        <v>293</v>
+      </c>
+      <c r="D42" s="112" t="s">
         <v>294</v>
-      </c>
-      <c r="D42" s="112" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="138" t="s">
+      <c r="A43" s="142" t="s">
         <v>247</v>
       </c>
-      <c r="B43" s="163" t="s">
+      <c r="B43" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C43" s="192"/>
-      <c r="D43" s="194" t="s">
+      <c r="C43" s="181"/>
+      <c r="D43" s="183" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="138"/>
-      <c r="B44" s="163"/>
-      <c r="C44" s="193"/>
-      <c r="D44" s="194"/>
+      <c r="A44" s="142"/>
+      <c r="B44" s="166"/>
+      <c r="C44" s="182"/>
+      <c r="D44" s="183"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="107" t="s">
@@ -31560,22 +31560,22 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="173" t="s">
+      <c r="A48" s="186" t="s">
         <v>285</v>
       </c>
-      <c r="B48" s="175" t="s">
+      <c r="B48" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C48" s="120" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D48" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="174"/>
-      <c r="B49" s="176"/>
+      <c r="A49" s="187"/>
+      <c r="B49" s="178"/>
       <c r="C49" s="119" t="s">
         <v>286</v>
       </c>
@@ -31592,10 +31592,10 @@
       <c r="D50" s="98"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="177" t="s">
+      <c r="A51" s="188" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="187" t="s">
+      <c r="B51" s="195" t="s">
         <v>271</v>
       </c>
       <c r="C51" s="119" t="s">
@@ -31606,8 +31606,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="178"/>
-      <c r="B52" s="189"/>
+      <c r="A52" s="189"/>
+      <c r="B52" s="197"/>
       <c r="C52" s="119" t="s">
         <v>265</v>
       </c>
@@ -31631,14 +31631,14 @@
     </row>
     <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B54" s="111" t="s">
         <v>271</v>
       </c>
       <c r="C54" s="101"/>
       <c r="D54" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -31697,17 +31697,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C19:C20"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="A51:A52"/>
@@ -31722,6 +31711,17 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C19:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"PITSelfServiceGuide and REST endpoint name corrections"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="307">
   <si>
     <t>Document</t>
   </si>
@@ -2720,6 +2720,18 @@
   <si>
     <t>code 3009 - 3012</t>
   </si>
+  <si>
+    <t>Create Temporary RPN</t>
+  </si>
+  <si>
+    <t>Corrected to 'Create New RPN'</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>Added Returns &amp; Reconciliations endpoints</t>
+  </si>
 </sst>
 </file>
 
@@ -3341,7 +3353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3622,9 +3634,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3772,6 +3781,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3780,12 +3795,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3805,24 +3814,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3835,20 +3826,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3879,6 +3882,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4283,12 +4301,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="125"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4311,12 +4329,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="125"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="124"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4356,10 +4374,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="129">
+      <c r="B7" s="128">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4373,8 +4391,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="127"/>
-      <c r="B8" s="130"/>
+      <c r="A8" s="126"/>
+      <c r="B8" s="129"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4386,8 +4404,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="127"/>
-      <c r="B9" s="130"/>
+      <c r="A9" s="126"/>
+      <c r="B9" s="129"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4399,8 +4417,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="127"/>
-      <c r="B10" s="130"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="129"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4412,8 +4430,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="127"/>
-      <c r="B11" s="130"/>
+      <c r="A11" s="126"/>
+      <c r="B11" s="129"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4425,8 +4443,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="128"/>
-      <c r="B12" s="131"/>
+      <c r="A12" s="127"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4438,10 +4456,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="129">
+      <c r="B13" s="128">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4455,8 +4473,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
-      <c r="B14" s="131"/>
+      <c r="A14" s="134"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4502,12 +4520,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="123" t="s">
+      <c r="A17" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="124"/>
-      <c r="C17" s="124"/>
-      <c r="D17" s="125"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="124"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4547,21 +4565,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="123" t="s">
+      <c r="A20" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="124"/>
-      <c r="C20" s="124"/>
-      <c r="D20" s="125"/>
+      <c r="B20" s="123"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="124"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="136" t="s">
+      <c r="A21" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="133">
+      <c r="B21" s="132">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4575,8 +4593,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="137"/>
-      <c r="B22" s="131"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="130"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4599,18 +4617,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="123" t="s">
+      <c r="A24" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="124"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="125"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="124"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="132" t="s">
+      <c r="A25" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="133">
+      <c r="B25" s="132">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4624,8 +4642,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="127"/>
-      <c r="B26" s="130"/>
+      <c r="A26" s="126"/>
+      <c r="B26" s="129"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4637,8 +4655,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="127"/>
-      <c r="B27" s="130"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="129"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4650,8 +4668,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="127"/>
-      <c r="B28" s="130"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="129"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4663,8 +4681,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="127"/>
-      <c r="B29" s="130"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="129"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4676,8 +4694,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="127"/>
-      <c r="B30" s="130"/>
+      <c r="A30" s="126"/>
+      <c r="B30" s="129"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4689,8 +4707,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="127"/>
-      <c r="B31" s="130"/>
+      <c r="A31" s="126"/>
+      <c r="B31" s="129"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4702,8 +4720,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="128"/>
-      <c r="B32" s="131"/>
+      <c r="A32" s="127"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4827,12 +4845,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="123" t="s">
+      <c r="A41" s="122" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="124"/>
-      <c r="C41" s="124"/>
-      <c r="D41" s="125"/>
+      <c r="B41" s="123"/>
+      <c r="C41" s="123"/>
+      <c r="D41" s="124"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -5012,10 +5030,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="138" t="s">
+      <c r="A7" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="139" t="s">
+      <c r="B7" s="138" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5026,8 +5044,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="138"/>
-      <c r="B8" s="139"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="138"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5036,8 +5054,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="138"/>
-      <c r="B9" s="139"/>
+      <c r="A9" s="137"/>
+      <c r="B9" s="138"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5046,8 +5064,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="138"/>
-      <c r="B10" s="139"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="138"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5056,8 +5074,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="138"/>
-      <c r="B11" s="139"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="138"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5066,8 +5084,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="138"/>
-      <c r="B12" s="139"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5076,10 +5094,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="140" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="138" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5090,8 +5108,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="141"/>
-      <c r="B14" s="139"/>
+      <c r="A14" s="140"/>
+      <c r="B14" s="138"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5100,8 +5118,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="141"/>
-      <c r="B15" s="139"/>
+      <c r="A15" s="140"/>
+      <c r="B15" s="138"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5110,10 +5128,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5124,8 +5142,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="142"/>
-      <c r="B17" s="143"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="142"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5134,8 +5152,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="142"/>
-      <c r="B18" s="143"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="142"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5144,8 +5162,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="142"/>
-      <c r="B19" s="143"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5154,8 +5172,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="142"/>
-      <c r="B20" s="143"/>
+      <c r="A20" s="141"/>
+      <c r="B20" s="142"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5164,8 +5182,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="142"/>
-      <c r="B21" s="143"/>
+      <c r="A21" s="141"/>
+      <c r="B21" s="142"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5174,8 +5192,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="142"/>
-      <c r="B22" s="143"/>
+      <c r="A22" s="141"/>
+      <c r="B22" s="142"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5184,8 +5202,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="142"/>
-      <c r="B23" s="143"/>
+      <c r="A23" s="141"/>
+      <c r="B23" s="142"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5194,26 +5212,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="142"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="142" t="s">
+      <c r="A24" s="141"/>
+      <c r="B24" s="142"/>
+      <c r="C24" s="141" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="149" t="s">
+      <c r="D24" s="148" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="142"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="142"/>
-      <c r="D25" s="149"/>
+      <c r="A25" s="141"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="148"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="138" t="s">
+      <c r="A26" s="137" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="139" t="s">
+      <c r="B26" s="138" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5224,8 +5242,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="138"/>
-      <c r="B27" s="139"/>
+      <c r="A27" s="137"/>
+      <c r="B27" s="138"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5252,28 +5270,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="140" t="s">
+      <c r="A30" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="139" t="s">
+      <c r="B30" s="138" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="142" t="s">
+      <c r="C30" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="152" t="s">
+      <c r="D30" s="151" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="140"/>
-      <c r="B31" s="139"/>
-      <c r="C31" s="142"/>
-      <c r="D31" s="152"/>
+      <c r="A31" s="139"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="151"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="140"/>
-      <c r="B32" s="139"/>
+      <c r="A32" s="139"/>
+      <c r="B32" s="138"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5282,8 +5300,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="140"/>
-      <c r="B33" s="139"/>
+      <c r="A33" s="139"/>
+      <c r="B33" s="138"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5292,8 +5310,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="140"/>
-      <c r="B34" s="139"/>
+      <c r="A34" s="139"/>
+      <c r="B34" s="138"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5302,8 +5320,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="140"/>
-      <c r="B35" s="139"/>
+      <c r="A35" s="139"/>
+      <c r="B35" s="138"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5312,8 +5330,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="140"/>
-      <c r="B36" s="139"/>
+      <c r="A36" s="139"/>
+      <c r="B36" s="138"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5322,26 +5340,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="140"/>
-      <c r="B37" s="139"/>
-      <c r="C37" s="153" t="s">
+      <c r="A37" s="139"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="152" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="155" t="s">
+      <c r="D37" s="154" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="140"/>
-      <c r="B38" s="139"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="155"/>
+      <c r="A38" s="139"/>
+      <c r="B38" s="138"/>
+      <c r="C38" s="153"/>
+      <c r="D38" s="154"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="138" t="s">
+      <c r="A39" s="137" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="139" t="s">
+      <c r="B39" s="138" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5352,8 +5370,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="138"/>
-      <c r="B40" s="139"/>
+      <c r="A40" s="137"/>
+      <c r="B40" s="138"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5380,10 +5398,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="140" t="s">
+      <c r="A43" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="139" t="s">
+      <c r="B43" s="138" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5392,8 +5410,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="140"/>
-      <c r="B44" s="139"/>
+      <c r="A44" s="139"/>
+      <c r="B44" s="138"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5402,10 +5420,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="146" t="s">
+      <c r="A45" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="139" t="s">
+      <c r="B45" s="138" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5414,8 +5432,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="147"/>
-      <c r="B46" s="139"/>
+      <c r="A46" s="146"/>
+      <c r="B46" s="138"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5424,8 +5442,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="147"/>
-      <c r="B47" s="139"/>
+      <c r="A47" s="146"/>
+      <c r="B47" s="138"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5434,8 +5452,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="148"/>
-      <c r="B48" s="139"/>
+      <c r="A48" s="147"/>
+      <c r="B48" s="138"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5444,10 +5462,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="143" t="s">
+      <c r="A49" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="143" t="s">
+      <c r="B49" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9551,8 +9569,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="143"/>
-      <c r="B50" s="143"/>
+      <c r="A50" s="142"/>
+      <c r="B50" s="142"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13656,8 +13674,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="143"/>
-      <c r="B51" s="143"/>
+      <c r="A51" s="142"/>
+      <c r="B51" s="142"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17761,8 +17779,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="143"/>
-      <c r="B52" s="143"/>
+      <c r="A52" s="142"/>
+      <c r="B52" s="142"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21866,12 +21884,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="143"/>
-      <c r="B53" s="143"/>
-      <c r="C53" s="151" t="s">
+      <c r="A53" s="142"/>
+      <c r="B53" s="142"/>
+      <c r="C53" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="152" t="s">
+      <c r="D53" s="151" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25971,10 +25989,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="151"/>
-      <c r="D54" s="152"/>
+      <c r="A54" s="142"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="150"/>
+      <c r="D54" s="151"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30092,10 +30110,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="144" t="s">
+      <c r="A57" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="143" t="s">
+      <c r="B57" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30106,8 +30124,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="144"/>
-      <c r="B58" s="143"/>
+      <c r="A58" s="143"/>
+      <c r="B58" s="142"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30116,8 +30134,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="144"/>
-      <c r="B59" s="143"/>
+      <c r="A59" s="143"/>
+      <c r="B59" s="142"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30126,8 +30144,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="144"/>
-      <c r="B60" s="143"/>
+      <c r="A60" s="143"/>
+      <c r="B60" s="142"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30136,8 +30154,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="144"/>
-      <c r="B61" s="143"/>
+      <c r="A61" s="143"/>
+      <c r="B61" s="142"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30146,8 +30164,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="144"/>
-      <c r="B62" s="143"/>
+      <c r="A62" s="143"/>
+      <c r="B62" s="142"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30156,8 +30174,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="144"/>
-      <c r="B63" s="143"/>
+      <c r="A63" s="143"/>
+      <c r="B63" s="142"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30166,16 +30184,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="144"/>
-      <c r="B64" s="143"/>
+      <c r="A64" s="143"/>
+      <c r="B64" s="142"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="144"/>
-      <c r="B65" s="143"/>
+      <c r="A65" s="143"/>
+      <c r="B65" s="142"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30184,16 +30202,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="144"/>
-      <c r="B66" s="143"/>
+      <c r="A66" s="143"/>
+      <c r="B66" s="142"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="144"/>
-      <c r="B67" s="143"/>
+      <c r="A67" s="143"/>
+      <c r="B67" s="142"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30202,8 +30220,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="144"/>
-      <c r="B68" s="143"/>
+      <c r="A68" s="143"/>
+      <c r="B68" s="142"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30212,8 +30230,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="144"/>
-      <c r="B69" s="143"/>
+      <c r="A69" s="143"/>
+      <c r="B69" s="142"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30222,8 +30240,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="144"/>
-      <c r="B70" s="143"/>
+      <c r="A70" s="143"/>
+      <c r="B70" s="142"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30232,8 +30250,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="144"/>
-      <c r="B71" s="143"/>
+      <c r="A71" s="143"/>
+      <c r="B71" s="142"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30242,8 +30260,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="144"/>
-      <c r="B72" s="143"/>
+      <c r="A72" s="143"/>
+      <c r="B72" s="142"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30252,16 +30270,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="144"/>
-      <c r="B73" s="143"/>
+      <c r="A73" s="143"/>
+      <c r="B73" s="142"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="144"/>
-      <c r="B74" s="143"/>
+      <c r="A74" s="143"/>
+      <c r="B74" s="142"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30270,18 +30288,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="144"/>
-      <c r="B75" s="143"/>
-      <c r="C75" s="150"/>
-      <c r="D75" s="145" t="s">
+      <c r="A75" s="143"/>
+      <c r="B75" s="142"/>
+      <c r="C75" s="149"/>
+      <c r="D75" s="144" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="144"/>
-      <c r="B76" s="143"/>
-      <c r="C76" s="150"/>
-      <c r="D76" s="145"/>
+      <c r="A76" s="143"/>
+      <c r="B76" s="142"/>
+      <c r="C76" s="149"/>
+      <c r="D76" s="144"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30405,10 +30423,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="138" t="s">
+      <c r="A4" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="138" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30419,133 +30437,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="138"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="163" t="s">
+      <c r="A5" s="137"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="164" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="162" t="s">
+      <c r="D5" s="163" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="138"/>
-      <c r="B6" s="139"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="162"/>
+      <c r="A6" s="137"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="163"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="138"/>
-      <c r="B7" s="139"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="138"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="138"/>
-      <c r="B8" s="139"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="138"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="138"/>
-      <c r="B9" s="139"/>
+      <c r="A9" s="137"/>
+      <c r="B9" s="138"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="141" t="s">
+      <c r="A10" s="140" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="138" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="162" t="s">
+      <c r="C10" s="162"/>
+      <c r="D10" s="163" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="141"/>
-      <c r="B11" s="139"/>
-      <c r="C11" s="165"/>
-      <c r="D11" s="162"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="162"/>
+      <c r="D11" s="163"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="141"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="165"/>
-      <c r="D12" s="162"/>
+      <c r="A12" s="140"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="163"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="142" t="s">
+      <c r="A13" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="143" t="s">
+      <c r="B13" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="162" t="s">
+      <c r="C13" s="165"/>
+      <c r="D13" s="163" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="142"/>
-      <c r="B14" s="143"/>
-      <c r="C14" s="164"/>
-      <c r="D14" s="162"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="142"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="163"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="142"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="164"/>
+      <c r="A15" s="141"/>
+      <c r="B15" s="142"/>
+      <c r="C15" s="165"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="142"/>
-      <c r="B16" s="143"/>
-      <c r="C16" s="164"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="142"/>
+      <c r="C16" s="165"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="142"/>
-      <c r="B17" s="143"/>
-      <c r="C17" s="164"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="142"/>
+      <c r="C17" s="165"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="142"/>
-      <c r="B18" s="143"/>
-      <c r="C18" s="164"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="165"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="142"/>
-      <c r="B19" s="143"/>
-      <c r="C19" s="164"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="165"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="142"/>
-      <c r="B20" s="143"/>
-      <c r="C20" s="164"/>
+      <c r="A20" s="141"/>
+      <c r="B20" s="142"/>
+      <c r="C20" s="165"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="142"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="164"/>
+      <c r="A21" s="141"/>
+      <c r="B21" s="142"/>
+      <c r="C21" s="165"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="142"/>
-      <c r="B22" s="143"/>
-      <c r="C22" s="164"/>
+      <c r="A22" s="141"/>
+      <c r="B22" s="142"/>
+      <c r="C22" s="165"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="142"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="164"/>
+      <c r="A23" s="141"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="165"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30643,10 +30661,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="167" t="s">
+      <c r="A32" s="166" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="170" t="s">
+      <c r="B32" s="169" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30657,26 +30675,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="168"/>
-      <c r="B33" s="171"/>
+      <c r="A33" s="167"/>
+      <c r="B33" s="170"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="168"/>
-      <c r="B34" s="171"/>
+      <c r="A34" s="167"/>
+      <c r="B34" s="170"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="168"/>
-      <c r="B35" s="171"/>
+      <c r="A35" s="167"/>
+      <c r="B35" s="170"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="169"/>
-      <c r="B36" s="172"/>
+      <c r="A36" s="168"/>
+      <c r="B36" s="171"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30705,10 +30723,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="140" t="s">
+      <c r="A39" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="139" t="s">
+      <c r="B39" s="138" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30719,8 +30737,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="140"/>
-      <c r="B40" s="139"/>
+      <c r="A40" s="139"/>
+      <c r="B40" s="138"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30729,84 +30747,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="138" t="s">
+      <c r="A41" s="137" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="139" t="s">
+      <c r="B41" s="138" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="165" t="s">
+      <c r="C41" s="162" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="142" t="s">
+      <c r="D41" s="141" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="138"/>
-      <c r="B42" s="139"/>
-      <c r="C42" s="165"/>
-      <c r="D42" s="142"/>
+      <c r="A42" s="137"/>
+      <c r="B42" s="138"/>
+      <c r="C42" s="162"/>
+      <c r="D42" s="141"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="138"/>
-      <c r="B43" s="139"/>
-      <c r="C43" s="165" t="s">
+      <c r="A43" s="137"/>
+      <c r="B43" s="138"/>
+      <c r="C43" s="162" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="145" t="s">
+      <c r="D43" s="144" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="138"/>
-      <c r="B44" s="139"/>
-      <c r="C44" s="165"/>
-      <c r="D44" s="145"/>
+      <c r="A44" s="137"/>
+      <c r="B44" s="138"/>
+      <c r="C44" s="162"/>
+      <c r="D44" s="144"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="144" t="s">
+      <c r="A45" s="143" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="143" t="s">
+      <c r="B45" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="159"/>
+      <c r="C45" s="158"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="144"/>
-      <c r="B46" s="143"/>
-      <c r="C46" s="160"/>
-      <c r="D46" s="156" t="s">
+      <c r="A46" s="143"/>
+      <c r="B46" s="142"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="155" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="144"/>
-      <c r="B47" s="143"/>
-      <c r="C47" s="160"/>
-      <c r="D47" s="157"/>
+      <c r="A47" s="143"/>
+      <c r="B47" s="142"/>
+      <c r="C47" s="159"/>
+      <c r="D47" s="156"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="144"/>
-      <c r="B48" s="143"/>
-      <c r="C48" s="161"/>
-      <c r="D48" s="157"/>
+      <c r="A48" s="143"/>
+      <c r="B48" s="142"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="156"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="144"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="151"/>
-      <c r="D49" s="157"/>
+      <c r="A49" s="143"/>
+      <c r="B49" s="142"/>
+      <c r="C49" s="150"/>
+      <c r="D49" s="156"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="144"/>
-      <c r="B50" s="143"/>
-      <c r="C50" s="151"/>
-      <c r="D50" s="158"/>
+      <c r="A50" s="143"/>
+      <c r="B50" s="142"/>
+      <c r="C50" s="150"/>
+      <c r="D50" s="157"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30829,10 +30847,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="143" t="s">
+      <c r="A53" s="142" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="143" t="s">
+      <c r="B53" s="142" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30843,8 +30861,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
+      <c r="A54" s="142"/>
+      <c r="B54" s="142"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30853,8 +30871,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="143"/>
-      <c r="B55" s="143"/>
+      <c r="A55" s="142"/>
+      <c r="B55" s="142"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30863,9 +30881,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="143"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="166" t="s">
+      <c r="A56" s="142"/>
+      <c r="B56" s="142"/>
+      <c r="C56" s="161" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30873,16 +30891,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="143"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="166"/>
+      <c r="A57" s="142"/>
+      <c r="B57" s="142"/>
+      <c r="C57" s="161"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="143"/>
-      <c r="B58" s="143"/>
+      <c r="A58" s="142"/>
+      <c r="B58" s="142"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30891,8 +30909,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="143"/>
-      <c r="B59" s="143"/>
+      <c r="A59" s="142"/>
+      <c r="B59" s="142"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30901,9 +30919,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="143"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="166" t="s">
+      <c r="A60" s="142"/>
+      <c r="B60" s="142"/>
+      <c r="C60" s="161" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30911,25 +30929,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="143"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="166"/>
+      <c r="A61" s="142"/>
+      <c r="B61" s="142"/>
+      <c r="C61" s="161"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="143"/>
-      <c r="B62" s="143"/>
-      <c r="C62" s="166"/>
+      <c r="A62" s="142"/>
+      <c r="B62" s="142"/>
+      <c r="C62" s="161"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="143"/>
-      <c r="B63" s="143"/>
-      <c r="C63" s="165" t="s">
+      <c r="A63" s="142"/>
+      <c r="B63" s="142"/>
+      <c r="C63" s="162" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30937,30 +30955,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="143"/>
-      <c r="B64" s="143"/>
-      <c r="C64" s="165"/>
-      <c r="D64" s="145" t="s">
+      <c r="A64" s="142"/>
+      <c r="B64" s="142"/>
+      <c r="C64" s="162"/>
+      <c r="D64" s="144" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="143"/>
-      <c r="B65" s="143"/>
-      <c r="C65" s="165"/>
-      <c r="D65" s="145"/>
+      <c r="A65" s="142"/>
+      <c r="B65" s="142"/>
+      <c r="C65" s="162"/>
+      <c r="D65" s="144"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="143"/>
-      <c r="B66" s="143"/>
-      <c r="C66" s="165"/>
-      <c r="D66" s="145"/>
+      <c r="A66" s="142"/>
+      <c r="B66" s="142"/>
+      <c r="C66" s="162"/>
+      <c r="D66" s="144"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="143"/>
-      <c r="B67" s="143"/>
-      <c r="C67" s="165"/>
-      <c r="D67" s="145"/>
+      <c r="A67" s="142"/>
+      <c r="B67" s="142"/>
+      <c r="C67" s="162"/>
+      <c r="D67" s="144"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31057,10 +31075,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31078,7 +31096,7 @@
       <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="114" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="57" t="s">
@@ -31094,10 +31112,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="166" t="s">
+      <c r="B3" s="161" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="101"/>
@@ -31106,12 +31124,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="142"/>
-      <c r="B4" s="166"/>
-      <c r="C4" s="116" t="s">
+      <c r="A4" s="141"/>
+      <c r="B4" s="161"/>
+      <c r="C4" s="115" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="120" t="s">
         <v>256</v>
       </c>
     </row>
@@ -31119,11 +31137,11 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="166"/>
-      <c r="C5" s="116" t="s">
+      <c r="B5" s="161"/>
+      <c r="C5" s="115" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>236</v>
       </c>
     </row>
@@ -31131,27 +31149,27 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="166"/>
-      <c r="C6" s="116" t="s">
+      <c r="B6" s="161"/>
+      <c r="C6" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="113" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="190" t="s">
+      <c r="A7" s="187" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="166"/>
+      <c r="B7" s="161"/>
       <c r="C7" s="101"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="191"/>
-      <c r="B8" s="166"/>
+      <c r="A8" s="188"/>
+      <c r="B8" s="161"/>
       <c r="C8" s="101"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
@@ -31161,7 +31179,7 @@
       <c r="A9" t="s">
         <v>290</v>
       </c>
-      <c r="B9" s="166"/>
+      <c r="B9" s="161"/>
       <c r="C9" s="101" t="s">
         <v>30</v>
       </c>
@@ -31171,9 +31189,9 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="166"/>
+      <c r="B10" s="161"/>
       <c r="C10" s="101"/>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="113" t="s">
         <v>259</v>
       </c>
     </row>
@@ -31186,10 +31204,10 @@
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="195" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="176" t="s">
+      <c r="B12" s="183" t="s">
         <v>234</v>
       </c>
       <c r="C12" s="101"/>
@@ -31198,24 +31216,24 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="174"/>
-      <c r="B13" s="177"/>
+      <c r="A13" s="196"/>
+      <c r="B13" s="198"/>
       <c r="C13" s="101"/>
       <c r="D13" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="174"/>
-      <c r="B14" s="177"/>
+      <c r="A14" s="196"/>
+      <c r="B14" s="198"/>
       <c r="C14" s="101"/>
       <c r="D14" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="175"/>
-      <c r="B15" s="178"/>
+      <c r="A15" s="197"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="58" t="s">
         <v>300</v>
       </c>
@@ -31224,426 +31242,420 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="110" t="s">
+      <c r="A16" s="178" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="161" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="58" t="s">
-        <v>238</v>
+      <c r="C16" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D16" s="109" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="142" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="166" t="s">
-        <v>234</v>
-      </c>
-      <c r="C17" s="179" t="s">
-        <v>239</v>
-      </c>
-      <c r="D17" s="122" t="s">
-        <v>241</v>
+      <c r="A17" s="179"/>
+      <c r="B17" s="161"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="142"/>
-      <c r="B18" s="166"/>
-      <c r="C18" s="180"/>
-      <c r="D18" s="109" t="s">
-        <v>278</v>
+      <c r="A18" s="141" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="161" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="172" t="s">
+        <v>239</v>
+      </c>
+      <c r="D18" s="121" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="142"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="184" t="s">
+      <c r="A19" s="141"/>
+      <c r="B19" s="161"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="109" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="141"/>
+      <c r="B20" s="161"/>
+      <c r="C20" s="176" t="s">
         <v>240</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D20" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="142"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="185"/>
-      <c r="D20" s="61" t="s">
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="141"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="143" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="142" t="s">
         <v>296</v>
       </c>
-      <c r="B21" s="166" t="s">
+      <c r="B22" s="161" t="s">
         <v>234</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C22" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D22" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="143"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="61" t="s">
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="142"/>
+      <c r="B23" s="161"/>
+      <c r="C23" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D23" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
+    <row r="24" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="44"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="190" t="s">
-        <v>260</v>
-      </c>
-      <c r="B24" s="166" t="s">
-        <v>234</v>
-      </c>
-      <c r="C24" s="101"/>
-      <c r="D24" s="79" t="s">
-        <v>261</v>
-      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="44"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="191"/>
-      <c r="B25" s="166"/>
+      <c r="A25" s="187" t="s">
+        <v>260</v>
+      </c>
+      <c r="B25" s="161" t="s">
+        <v>234</v>
+      </c>
       <c r="C25" s="101"/>
-      <c r="D25" s="58" t="s">
-        <v>257</v>
+      <c r="D25" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="188"/>
+      <c r="B26" s="161"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B26" s="106" t="s">
+      <c r="B27" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="116" t="s">
+      <c r="C27" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="114" t="s">
+      <c r="D27" s="113" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="192" t="s">
+    <row r="28" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="195" t="s">
+      <c r="B28" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="101" t="s">
+      <c r="C28" s="101" t="s">
         <v>268</v>
-      </c>
-      <c r="D27" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="193"/>
-      <c r="B28" s="196"/>
-      <c r="C28" t="s">
-        <v>270</v>
       </c>
       <c r="D28" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="193"/>
-      <c r="B29" s="196"/>
-      <c r="C29" s="101" t="s">
-        <v>269</v>
+      <c r="A29" s="190"/>
+      <c r="B29" s="193"/>
+      <c r="C29" t="s">
+        <v>270</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="193"/>
-      <c r="B30" s="196"/>
-      <c r="C30" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D30" s="109" t="s">
-        <v>102</v>
+      <c r="A30" s="190"/>
+      <c r="B30" s="193"/>
+      <c r="C30" s="101" t="s">
+        <v>269</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="193"/>
-      <c r="B31" s="196"/>
-      <c r="C31" s="101" t="s">
-        <v>282</v>
-      </c>
-      <c r="D31" s="58" t="s">
-        <v>251</v>
+      <c r="A31" s="190"/>
+      <c r="B31" s="193"/>
+      <c r="C31" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31" s="109" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="193"/>
-      <c r="B32" s="196"/>
+      <c r="A32" s="190"/>
+      <c r="B32" s="193"/>
       <c r="C32" s="101" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="193"/>
-      <c r="B33" s="196"/>
-      <c r="C33" s="104" t="s">
-        <v>288</v>
-      </c>
-      <c r="D33" s="109" t="s">
-        <v>251</v>
+      <c r="A33" s="190"/>
+      <c r="B33" s="193"/>
+      <c r="C33" s="101" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="193"/>
-      <c r="B34" s="196"/>
+      <c r="A34" s="190"/>
+      <c r="B34" s="193"/>
       <c r="C34" s="104" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D34" s="109" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="193"/>
-      <c r="B35" s="196"/>
+      <c r="A35" s="190"/>
+      <c r="B35" s="193"/>
       <c r="C35" s="104" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" s="109" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="190"/>
+      <c r="B36" s="193"/>
+      <c r="C36" s="104" t="s">
         <v>289</v>
       </c>
-      <c r="D35" s="109" t="s">
+      <c r="D36" s="109" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="194"/>
-      <c r="B36" s="197"/>
-      <c r="C36" s="117" t="s">
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="191"/>
+      <c r="B37" s="194"/>
+      <c r="C37" s="116" t="s">
         <v>244</v>
       </c>
-      <c r="D36" s="114" t="s">
+      <c r="D37" s="113" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39" t="s">
+    <row r="38" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="102"/>
-      <c r="D37" s="44"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="102"/>
+      <c r="D38" s="44"/>
     </row>
-    <row r="38" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="99"/>
-      <c r="B38" s="67"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="79" t="s">
+    <row r="39" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="99"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="166" t="s">
+    <row r="40" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="161" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="166" t="s">
+      <c r="B40" s="161" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="116" t="s">
+      <c r="C40" s="115" t="s">
         <v>246</v>
       </c>
-      <c r="D39" s="58" t="s">
+      <c r="D40" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="166"/>
-      <c r="B40" s="166"/>
-      <c r="C40" s="116">
-        <v>10.1</v>
-      </c>
-      <c r="D40" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="166"/>
-      <c r="B41" s="166"/>
-      <c r="C41" s="116">
-        <v>10.199999999999999</v>
+      <c r="A41" s="161"/>
+      <c r="B41" s="161"/>
+      <c r="C41" s="115">
+        <v>10.1</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="166"/>
-      <c r="B42" s="166"/>
-      <c r="C42" s="118" t="s">
-        <v>293</v>
-      </c>
-      <c r="D42" s="112" t="s">
-        <v>294</v>
+      <c r="A42" s="161"/>
+      <c r="B42" s="161"/>
+      <c r="C42" s="115">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="142" t="s">
-        <v>247</v>
-      </c>
-      <c r="B43" s="166" t="s">
-        <v>234</v>
-      </c>
-      <c r="C43" s="181"/>
-      <c r="D43" s="183" t="s">
-        <v>261</v>
+      <c r="A43" s="161"/>
+      <c r="B43" s="161"/>
+      <c r="C43" s="117" t="s">
+        <v>293</v>
+      </c>
+      <c r="D43" s="111" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="142"/>
-      <c r="B44" s="166"/>
-      <c r="C44" s="182"/>
-      <c r="D44" s="183"/>
+      <c r="A44" s="141" t="s">
+        <v>247</v>
+      </c>
+      <c r="B44" s="161" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="174"/>
+      <c r="D44" s="180" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="107" t="s">
+      <c r="A45" s="141"/>
+      <c r="B45" s="161"/>
+      <c r="C45" s="175"/>
+      <c r="D45" s="180"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="107" t="s">
         <v>262</v>
       </c>
-      <c r="B45" s="108" t="s">
+      <c r="B46" s="108" t="s">
         <v>234</v>
       </c>
-      <c r="C45" s="116" t="s">
+      <c r="C46" s="115" t="s">
         <v>250</v>
       </c>
-      <c r="D45" s="109" t="s">
+      <c r="D46" s="109" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="95" t="s">
+    <row r="47" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="105"/>
-      <c r="D46" s="98"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B47" s="108" t="s">
-        <v>234</v>
-      </c>
-      <c r="C47" s="119" t="s">
-        <v>265</v>
-      </c>
-      <c r="D47" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="B47" s="39"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="98"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="186" t="s">
+      <c r="A48" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B48" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48" s="118" t="s">
+        <v>265</v>
+      </c>
+      <c r="D48" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="181" t="s">
         <v>285</v>
       </c>
-      <c r="B48" s="176" t="s">
+      <c r="B49" s="183" t="s">
         <v>234</v>
       </c>
-      <c r="C48" s="120" t="s">
+      <c r="C49" s="119" t="s">
         <v>295</v>
       </c>
-      <c r="D48" s="58" t="s">
+      <c r="D49" s="58" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="187"/>
-      <c r="B49" s="178"/>
-      <c r="C49" s="119" t="s">
-        <v>286</v>
-      </c>
-      <c r="D49" s="58" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="98"/>
-      <c r="C50" s="113"/>
-      <c r="D50" s="98"/>
+      <c r="A50" s="199"/>
+      <c r="B50" s="198"/>
+      <c r="C50" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50" s="109" t="s">
+        <v>306</v>
+      </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="188" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="195" t="s">
-        <v>271</v>
-      </c>
-      <c r="C51" s="119" t="s">
-        <v>265</v>
+    <row r="51" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="182"/>
+      <c r="B51" s="184"/>
+      <c r="C51" s="118" t="s">
+        <v>286</v>
       </c>
       <c r="D51" s="58" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="189"/>
-      <c r="B52" s="197"/>
-      <c r="C52" s="119" t="s">
+      <c r="A52" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="98"/>
+      <c r="C52" s="112"/>
+      <c r="D52" s="98"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="185" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="192" t="s">
+        <v>271</v>
+      </c>
+      <c r="C53" s="118" t="s">
         <v>265</v>
       </c>
-      <c r="D52" s="58" t="s">
+      <c r="D53" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="186"/>
+      <c r="B54" s="194"/>
+      <c r="C54" s="118" t="s">
+        <v>265</v>
+      </c>
+      <c r="D54" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="97" t="s">
+    <row r="55" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B53" s="108" t="s">
-        <v>271</v>
-      </c>
-      <c r="C53" s="103" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B54" s="111" t="s">
-        <v>271</v>
-      </c>
-      <c r="C54" s="101"/>
-      <c r="D54" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="97" t="s">
-        <v>60</v>
       </c>
       <c r="B55" s="108" t="s">
         <v>271</v>
@@ -31652,35 +31664,41 @@
         <v>264</v>
       </c>
       <c r="D55" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B56" s="110" t="s">
+        <v>271</v>
+      </c>
+      <c r="C56" s="101"/>
+      <c r="D56" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="108" t="s">
+        <v>271</v>
+      </c>
+      <c r="C57" s="103" t="s">
+        <v>264</v>
+      </c>
+      <c r="D57" s="58" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B56" s="98"/>
-      <c r="C56" s="113"/>
-      <c r="D56" s="98"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="58"/>
-      <c r="B57" s="108" t="s">
-        <v>234</v>
-      </c>
-      <c r="C57" s="101" t="s">
-        <v>30</v>
-      </c>
-      <c r="D57" s="109" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="98" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B58" s="98"/>
-      <c r="C58" s="113"/>
+      <c r="C58" s="112"/>
       <c r="D58" s="98"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -31695,33 +31713,55 @@
         <v>274</v>
       </c>
     </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B60" s="98"/>
+      <c r="C60" s="112"/>
+      <c r="D60" s="98"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="58"/>
+      <c r="B61" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="C61" s="101" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="109" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A43:A44"/>
+  <mergeCells count="27">
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A44:A45"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B10"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B36"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"updated validation rules and Error Message Guide"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -19,15 +19,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="313">
   <si>
     <t>Document</t>
   </si>
@@ -2747,6 +2747,9 @@
   <si>
     <t>Error Response and Error Response Message</t>
   </si>
+  <si>
+    <t>code 3012</t>
+  </si>
 </sst>
 </file>
 
@@ -3348,7 +3351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3663,6 +3666,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3708,38 +3717,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3762,6 +3741,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3782,51 +3821,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3873,14 +3867,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4285,12 +4300,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="124"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4313,12 +4328,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="124"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="126"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4358,10 +4373,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="128">
+      <c r="B7" s="130">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4375,8 +4390,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="126"/>
-      <c r="B8" s="129"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4388,8 +4403,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="126"/>
-      <c r="B9" s="129"/>
+      <c r="A9" s="128"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4401,8 +4416,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="126"/>
-      <c r="B10" s="129"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4414,8 +4429,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="126"/>
-      <c r="B11" s="129"/>
+      <c r="A11" s="128"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4427,8 +4442,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
-      <c r="B12" s="130"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="132"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4440,10 +4455,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="135" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="128">
+      <c r="B13" s="130">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4457,8 +4472,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="134"/>
-      <c r="B14" s="130"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4504,12 +4519,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="124" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="124"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="126"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4549,21 +4564,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="123"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="124"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="126"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="132">
+      <c r="B21" s="134">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4577,8 +4592,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="136"/>
-      <c r="B22" s="130"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4601,18 +4616,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="122" t="s">
+      <c r="A24" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="124"/>
+      <c r="B24" s="125"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="126"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="131" t="s">
+      <c r="A25" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="132">
+      <c r="B25" s="134">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4626,8 +4641,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="126"/>
-      <c r="B26" s="129"/>
+      <c r="A26" s="128"/>
+      <c r="B26" s="131"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4639,8 +4654,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="126"/>
-      <c r="B27" s="129"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="131"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4652,8 +4667,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="126"/>
-      <c r="B28" s="129"/>
+      <c r="A28" s="128"/>
+      <c r="B28" s="131"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4665,8 +4680,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="126"/>
-      <c r="B29" s="129"/>
+      <c r="A29" s="128"/>
+      <c r="B29" s="131"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4678,8 +4693,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="126"/>
-      <c r="B30" s="129"/>
+      <c r="A30" s="128"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4691,8 +4706,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="126"/>
-      <c r="B31" s="129"/>
+      <c r="A31" s="128"/>
+      <c r="B31" s="131"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4704,8 +4719,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="127"/>
-      <c r="B32" s="130"/>
+      <c r="A32" s="129"/>
+      <c r="B32" s="132"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4829,12 +4844,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="122" t="s">
+      <c r="A41" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="123"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="124"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="125"/>
+      <c r="D41" s="126"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4894,7 +4909,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4904,7 +4919,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5014,10 +5029,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5028,8 +5043,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="137"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5038,8 +5053,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="137"/>
-      <c r="B9" s="138"/>
+      <c r="A9" s="154"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5048,8 +5063,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="137"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="154"/>
+      <c r="B10" s="153"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5058,8 +5073,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="137"/>
-      <c r="B11" s="138"/>
+      <c r="A11" s="154"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5068,8 +5083,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="137"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="154"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5078,10 +5093,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="140" t="s">
+      <c r="A13" s="156" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="138" t="s">
+      <c r="B13" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5092,8 +5107,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="140"/>
-      <c r="B14" s="138"/>
+      <c r="A14" s="156"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5102,8 +5117,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="140"/>
-      <c r="B15" s="138"/>
+      <c r="A15" s="156"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5112,10 +5127,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="141" t="s">
+      <c r="A16" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="142" t="s">
+      <c r="B16" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5126,8 +5141,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="141"/>
-      <c r="B17" s="142"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="148"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5136,8 +5151,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="141"/>
-      <c r="B18" s="142"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="148"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5146,8 +5161,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="141"/>
-      <c r="B19" s="142"/>
+      <c r="A19" s="139"/>
+      <c r="B19" s="148"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5156,8 +5171,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="141"/>
-      <c r="B20" s="142"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="148"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5166,8 +5181,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="141"/>
-      <c r="B21" s="142"/>
+      <c r="A21" s="139"/>
+      <c r="B21" s="148"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5176,8 +5191,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="141"/>
-      <c r="B22" s="142"/>
+      <c r="A22" s="139"/>
+      <c r="B22" s="148"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5186,8 +5201,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="141"/>
-      <c r="B23" s="142"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="148"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5196,26 +5211,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="141"/>
-      <c r="B24" s="142"/>
-      <c r="C24" s="141" t="s">
+      <c r="A24" s="139"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="139" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="148" t="s">
+      <c r="D24" s="140" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="141"/>
-      <c r="B25" s="142"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="148"/>
+      <c r="A25" s="139"/>
+      <c r="B25" s="148"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="140"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="137" t="s">
+      <c r="A26" s="154" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="138" t="s">
+      <c r="B26" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5226,8 +5241,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="137"/>
-      <c r="B27" s="138"/>
+      <c r="A27" s="154"/>
+      <c r="B27" s="153"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5254,28 +5269,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="139" t="s">
+      <c r="A30" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="138" t="s">
+      <c r="B30" s="153" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="141" t="s">
+      <c r="C30" s="139" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="151" t="s">
+      <c r="D30" s="143" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="139"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="141"/>
-      <c r="D31" s="151"/>
+      <c r="A31" s="155"/>
+      <c r="B31" s="153"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="143"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="139"/>
-      <c r="B32" s="138"/>
+      <c r="A32" s="155"/>
+      <c r="B32" s="153"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5284,8 +5299,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="139"/>
-      <c r="B33" s="138"/>
+      <c r="A33" s="155"/>
+      <c r="B33" s="153"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5294,8 +5309,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="139"/>
-      <c r="B34" s="138"/>
+      <c r="A34" s="155"/>
+      <c r="B34" s="153"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5304,8 +5319,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="139"/>
-      <c r="B35" s="138"/>
+      <c r="A35" s="155"/>
+      <c r="B35" s="153"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5314,8 +5329,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="139"/>
-      <c r="B36" s="138"/>
+      <c r="A36" s="155"/>
+      <c r="B36" s="153"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5324,26 +5339,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="139"/>
-      <c r="B37" s="138"/>
-      <c r="C37" s="152" t="s">
+      <c r="A37" s="155"/>
+      <c r="B37" s="153"/>
+      <c r="C37" s="144" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="154" t="s">
+      <c r="D37" s="146" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="139"/>
-      <c r="B38" s="138"/>
-      <c r="C38" s="153"/>
-      <c r="D38" s="154"/>
+      <c r="A38" s="155"/>
+      <c r="B38" s="153"/>
+      <c r="C38" s="145"/>
+      <c r="D38" s="146"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="137" t="s">
+      <c r="A39" s="154" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="138" t="s">
+      <c r="B39" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5354,8 +5369,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="137"/>
-      <c r="B40" s="138"/>
+      <c r="A40" s="154"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5382,10 +5397,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="139" t="s">
+      <c r="A43" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="138" t="s">
+      <c r="B43" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5394,8 +5409,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="139"/>
-      <c r="B44" s="138"/>
+      <c r="A44" s="155"/>
+      <c r="B44" s="153"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5404,10 +5419,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="145" t="s">
+      <c r="A45" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="138" t="s">
+      <c r="B45" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5416,8 +5431,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="146"/>
-      <c r="B46" s="138"/>
+      <c r="A46" s="151"/>
+      <c r="B46" s="153"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5426,8 +5441,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="146"/>
-      <c r="B47" s="138"/>
+      <c r="A47" s="151"/>
+      <c r="B47" s="153"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5436,8 +5451,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="147"/>
-      <c r="B48" s="138"/>
+      <c r="A48" s="152"/>
+      <c r="B48" s="153"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5446,10 +5461,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="142" t="s">
+      <c r="A49" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="142" t="s">
+      <c r="B49" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9553,8 +9568,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="142"/>
-      <c r="B50" s="142"/>
+      <c r="A50" s="148"/>
+      <c r="B50" s="148"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13658,8 +13673,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="142"/>
-      <c r="B51" s="142"/>
+      <c r="A51" s="148"/>
+      <c r="B51" s="148"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17763,8 +17778,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="142"/>
-      <c r="B52" s="142"/>
+      <c r="A52" s="148"/>
+      <c r="B52" s="148"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21868,12 +21883,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="142"/>
-      <c r="B53" s="142"/>
-      <c r="C53" s="150" t="s">
+      <c r="A53" s="148"/>
+      <c r="B53" s="148"/>
+      <c r="C53" s="142" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="151" t="s">
+      <c r="D53" s="143" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25973,10 +25988,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="142"/>
-      <c r="B54" s="142"/>
-      <c r="C54" s="150"/>
-      <c r="D54" s="151"/>
+      <c r="A54" s="148"/>
+      <c r="B54" s="148"/>
+      <c r="C54" s="142"/>
+      <c r="D54" s="143"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30094,10 +30109,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="143" t="s">
+      <c r="A57" s="147" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="142" t="s">
+      <c r="B57" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30108,8 +30123,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="143"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="147"/>
+      <c r="B58" s="148"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30118,8 +30133,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="143"/>
-      <c r="B59" s="142"/>
+      <c r="A59" s="147"/>
+      <c r="B59" s="148"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30128,8 +30143,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="143"/>
-      <c r="B60" s="142"/>
+      <c r="A60" s="147"/>
+      <c r="B60" s="148"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30138,8 +30153,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="143"/>
-      <c r="B61" s="142"/>
+      <c r="A61" s="147"/>
+      <c r="B61" s="148"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30148,8 +30163,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="143"/>
-      <c r="B62" s="142"/>
+      <c r="A62" s="147"/>
+      <c r="B62" s="148"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30158,8 +30173,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="143"/>
-      <c r="B63" s="142"/>
+      <c r="A63" s="147"/>
+      <c r="B63" s="148"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30168,16 +30183,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="143"/>
-      <c r="B64" s="142"/>
+      <c r="A64" s="147"/>
+      <c r="B64" s="148"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="143"/>
-      <c r="B65" s="142"/>
+      <c r="A65" s="147"/>
+      <c r="B65" s="148"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30186,16 +30201,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="143"/>
-      <c r="B66" s="142"/>
+      <c r="A66" s="147"/>
+      <c r="B66" s="148"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="143"/>
-      <c r="B67" s="142"/>
+      <c r="A67" s="147"/>
+      <c r="B67" s="148"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30204,8 +30219,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="143"/>
-      <c r="B68" s="142"/>
+      <c r="A68" s="147"/>
+      <c r="B68" s="148"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30214,8 +30229,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="143"/>
-      <c r="B69" s="142"/>
+      <c r="A69" s="147"/>
+      <c r="B69" s="148"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30224,8 +30239,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="143"/>
-      <c r="B70" s="142"/>
+      <c r="A70" s="147"/>
+      <c r="B70" s="148"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30234,8 +30249,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="143"/>
-      <c r="B71" s="142"/>
+      <c r="A71" s="147"/>
+      <c r="B71" s="148"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30244,8 +30259,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="143"/>
-      <c r="B72" s="142"/>
+      <c r="A72" s="147"/>
+      <c r="B72" s="148"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30254,16 +30269,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="143"/>
-      <c r="B73" s="142"/>
+      <c r="A73" s="147"/>
+      <c r="B73" s="148"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="143"/>
-      <c r="B74" s="142"/>
+      <c r="A74" s="147"/>
+      <c r="B74" s="148"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30272,18 +30287,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="143"/>
-      <c r="B75" s="142"/>
-      <c r="C75" s="149"/>
-      <c r="D75" s="144" t="s">
+      <c r="A75" s="147"/>
+      <c r="B75" s="148"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="149" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="143"/>
-      <c r="B76" s="142"/>
-      <c r="C76" s="149"/>
-      <c r="D76" s="144"/>
+      <c r="A76" s="147"/>
+      <c r="B76" s="148"/>
+      <c r="C76" s="141"/>
+      <c r="D76" s="149"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30307,8 +30322,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30317,29 +30332,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30354,6 +30353,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30407,10 +30422,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30421,8 +30436,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="137"/>
-      <c r="B5" s="138"/>
+      <c r="A5" s="154"/>
+      <c r="B5" s="153"/>
       <c r="C5" s="164" t="s">
         <v>190</v>
       </c>
@@ -30431,58 +30446,58 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="137"/>
-      <c r="B6" s="138"/>
+      <c r="A6" s="154"/>
+      <c r="B6" s="153"/>
       <c r="C6" s="164"/>
       <c r="D6" s="163"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="137"/>
-      <c r="B7" s="138"/>
+      <c r="A7" s="154"/>
+      <c r="B7" s="153"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="137"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="137"/>
-      <c r="B9" s="138"/>
+      <c r="A9" s="154"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="140" t="s">
+      <c r="A10" s="156" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="162"/>
+      <c r="C10" s="166"/>
       <c r="D10" s="163" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="140"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="162"/>
+      <c r="A11" s="156"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="163"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="140"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="162"/>
+      <c r="A12" s="156"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="166"/>
       <c r="D12" s="163"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C13" s="165"/>
@@ -30491,62 +30506,62 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="141"/>
-      <c r="B14" s="142"/>
+      <c r="A14" s="139"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="165"/>
       <c r="D14" s="163"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="141"/>
-      <c r="B15" s="142"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="148"/>
       <c r="C15" s="165"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="141"/>
-      <c r="B16" s="142"/>
+      <c r="A16" s="139"/>
+      <c r="B16" s="148"/>
       <c r="C16" s="165"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="141"/>
-      <c r="B17" s="142"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="148"/>
       <c r="C17" s="165"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="141"/>
-      <c r="B18" s="142"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="148"/>
       <c r="C18" s="165"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="141"/>
-      <c r="B19" s="142"/>
+      <c r="A19" s="139"/>
+      <c r="B19" s="148"/>
       <c r="C19" s="165"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="141"/>
-      <c r="B20" s="142"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="148"/>
       <c r="C20" s="165"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="141"/>
-      <c r="B21" s="142"/>
+      <c r="A21" s="139"/>
+      <c r="B21" s="148"/>
       <c r="C21" s="165"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="141"/>
-      <c r="B22" s="142"/>
+      <c r="A22" s="139"/>
+      <c r="B22" s="148"/>
       <c r="C22" s="165"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="141"/>
-      <c r="B23" s="142"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="148"/>
       <c r="C23" s="165"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
@@ -30645,10 +30660,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="166" t="s">
+      <c r="A32" s="157" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="169" t="s">
+      <c r="B32" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30659,26 +30674,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="167"/>
-      <c r="B33" s="170"/>
+      <c r="A33" s="158"/>
+      <c r="B33" s="161"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="167"/>
-      <c r="B34" s="170"/>
+      <c r="A34" s="158"/>
+      <c r="B34" s="161"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="167"/>
-      <c r="B35" s="170"/>
+      <c r="A35" s="158"/>
+      <c r="B35" s="161"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="168"/>
-      <c r="B36" s="171"/>
+      <c r="A36" s="159"/>
+      <c r="B36" s="162"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30707,10 +30722,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="139" t="s">
+      <c r="A39" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="138" t="s">
+      <c r="B39" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30721,8 +30736,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="139"/>
-      <c r="B40" s="138"/>
+      <c r="A40" s="155"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30731,84 +30746,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="137" t="s">
+      <c r="A41" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="138" t="s">
+      <c r="B41" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="162" t="s">
+      <c r="C41" s="166" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="141" t="s">
+      <c r="D41" s="139" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="137"/>
-      <c r="B42" s="138"/>
-      <c r="C42" s="162"/>
-      <c r="D42" s="141"/>
+      <c r="A42" s="154"/>
+      <c r="B42" s="153"/>
+      <c r="C42" s="166"/>
+      <c r="D42" s="139"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="137"/>
-      <c r="B43" s="138"/>
-      <c r="C43" s="162" t="s">
+      <c r="A43" s="154"/>
+      <c r="B43" s="153"/>
+      <c r="C43" s="166" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="144" t="s">
+      <c r="D43" s="149" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="137"/>
-      <c r="B44" s="138"/>
-      <c r="C44" s="162"/>
-      <c r="D44" s="144"/>
+      <c r="A44" s="154"/>
+      <c r="B44" s="153"/>
+      <c r="C44" s="166"/>
+      <c r="D44" s="149"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="143" t="s">
+      <c r="A45" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="142" t="s">
+      <c r="B45" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="158"/>
+      <c r="C45" s="170"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="143"/>
-      <c r="B46" s="142"/>
-      <c r="C46" s="159"/>
-      <c r="D46" s="155" t="s">
+      <c r="A46" s="147"/>
+      <c r="B46" s="148"/>
+      <c r="C46" s="171"/>
+      <c r="D46" s="167" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="143"/>
-      <c r="B47" s="142"/>
-      <c r="C47" s="159"/>
-      <c r="D47" s="156"/>
+      <c r="A47" s="147"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="171"/>
+      <c r="D47" s="168"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="143"/>
-      <c r="B48" s="142"/>
-      <c r="C48" s="160"/>
-      <c r="D48" s="156"/>
+      <c r="A48" s="147"/>
+      <c r="B48" s="148"/>
+      <c r="C48" s="172"/>
+      <c r="D48" s="168"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="143"/>
-      <c r="B49" s="142"/>
-      <c r="C49" s="150"/>
-      <c r="D49" s="156"/>
+      <c r="A49" s="147"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="142"/>
+      <c r="D49" s="168"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="143"/>
-      <c r="B50" s="142"/>
-      <c r="C50" s="150"/>
-      <c r="D50" s="157"/>
+      <c r="A50" s="147"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="142"/>
+      <c r="D50" s="169"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30831,10 +30846,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="142" t="s">
+      <c r="A53" s="148" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="142" t="s">
+      <c r="B53" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30845,8 +30860,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="142"/>
-      <c r="B54" s="142"/>
+      <c r="A54" s="148"/>
+      <c r="B54" s="148"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30855,8 +30870,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="142"/>
-      <c r="B55" s="142"/>
+      <c r="A55" s="148"/>
+      <c r="B55" s="148"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30865,9 +30880,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="142"/>
-      <c r="B56" s="142"/>
-      <c r="C56" s="161" t="s">
+      <c r="A56" s="148"/>
+      <c r="B56" s="148"/>
+      <c r="C56" s="173" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30875,16 +30890,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="142"/>
-      <c r="B57" s="142"/>
-      <c r="C57" s="161"/>
+      <c r="A57" s="148"/>
+      <c r="B57" s="148"/>
+      <c r="C57" s="173"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="142"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="148"/>
+      <c r="B58" s="148"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30893,8 +30908,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="142"/>
-      <c r="B59" s="142"/>
+      <c r="A59" s="148"/>
+      <c r="B59" s="148"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30903,9 +30918,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="142"/>
-      <c r="B60" s="142"/>
-      <c r="C60" s="161" t="s">
+      <c r="A60" s="148"/>
+      <c r="B60" s="148"/>
+      <c r="C60" s="173" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30913,25 +30928,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="142"/>
-      <c r="B61" s="142"/>
-      <c r="C61" s="161"/>
+      <c r="A61" s="148"/>
+      <c r="B61" s="148"/>
+      <c r="C61" s="173"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="142"/>
-      <c r="B62" s="142"/>
-      <c r="C62" s="161"/>
+      <c r="A62" s="148"/>
+      <c r="B62" s="148"/>
+      <c r="C62" s="173"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="142"/>
-      <c r="B63" s="142"/>
-      <c r="C63" s="162" t="s">
+      <c r="A63" s="148"/>
+      <c r="B63" s="148"/>
+      <c r="C63" s="166" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30939,30 +30954,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="142"/>
-      <c r="B64" s="142"/>
-      <c r="C64" s="162"/>
-      <c r="D64" s="144" t="s">
+      <c r="A64" s="148"/>
+      <c r="B64" s="148"/>
+      <c r="C64" s="166"/>
+      <c r="D64" s="149" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="142"/>
-      <c r="B65" s="142"/>
-      <c r="C65" s="162"/>
-      <c r="D65" s="144"/>
+      <c r="A65" s="148"/>
+      <c r="B65" s="148"/>
+      <c r="C65" s="166"/>
+      <c r="D65" s="149"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="142"/>
-      <c r="B66" s="142"/>
-      <c r="C66" s="162"/>
-      <c r="D66" s="144"/>
+      <c r="A66" s="148"/>
+      <c r="B66" s="148"/>
+      <c r="C66" s="166"/>
+      <c r="D66" s="149"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="142"/>
-      <c r="B67" s="142"/>
-      <c r="C67" s="162"/>
-      <c r="D67" s="144"/>
+      <c r="A67" s="148"/>
+      <c r="B67" s="148"/>
+      <c r="C67" s="166"/>
+      <c r="D67" s="149"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31018,23 +31033,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31051,6 +31049,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31059,10 +31074,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31096,10 +31111,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="173" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="100"/>
@@ -31108,8 +31123,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141"/>
-      <c r="B4" s="161"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="173"/>
       <c r="C4" s="113" t="s">
         <v>235</v>
       </c>
@@ -31121,7 +31136,7 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="161"/>
+      <c r="B5" s="173"/>
       <c r="C5" s="113" t="s">
         <v>235</v>
       </c>
@@ -31133,7 +31148,7 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="161"/>
+      <c r="B6" s="173"/>
       <c r="C6" s="113" t="s">
         <v>22</v>
       </c>
@@ -31142,18 +31157,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="182" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="161"/>
+      <c r="B7" s="173"/>
       <c r="C7" s="100"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="186"/>
-      <c r="B8" s="161"/>
+      <c r="A8" s="183"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="100"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
@@ -31163,7 +31178,7 @@
       <c r="A9" t="s">
         <v>290</v>
       </c>
-      <c r="B9" s="161"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="100" t="s">
         <v>30</v>
       </c>
@@ -31173,7 +31188,7 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="161"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="100"/>
       <c r="D10" s="111" t="s">
         <v>259</v>
@@ -31188,10 +31203,10 @@
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="189" t="s">
+      <c r="A12" s="186" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="180" t="s">
+      <c r="B12" s="177" t="s">
         <v>234</v>
       </c>
       <c r="C12" s="100"/>
@@ -31200,24 +31215,24 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="190"/>
-      <c r="B13" s="181"/>
+      <c r="A13" s="187"/>
+      <c r="B13" s="178"/>
       <c r="C13" s="100"/>
       <c r="D13" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="190"/>
-      <c r="B14" s="181"/>
+      <c r="A14" s="187"/>
+      <c r="B14" s="178"/>
       <c r="C14" s="100"/>
       <c r="D14" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="191"/>
-      <c r="B15" s="182"/>
+      <c r="A15" s="188"/>
+      <c r="B15" s="179"/>
       <c r="C15" s="58" t="s">
         <v>300</v>
       </c>
@@ -31226,10 +31241,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="174" t="s">
+      <c r="A16" s="193" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="161" t="s">
+      <c r="B16" s="173" t="s">
         <v>234</v>
       </c>
       <c r="C16" s="58" t="s">
@@ -31240,21 +31255,21 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="175"/>
-      <c r="B17" s="161"/>
+      <c r="A17" s="194"/>
+      <c r="B17" s="173"/>
       <c r="C17" s="58"/>
       <c r="D17" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="161" t="s">
+      <c r="A18" s="173" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="161" t="s">
+      <c r="B18" s="173" t="s">
         <v>234</v>
       </c>
-      <c r="C18" s="192" t="s">
+      <c r="C18" s="190" t="s">
         <v>239</v>
       </c>
       <c r="D18" s="118" t="s">
@@ -31262,17 +31277,17 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="161"/>
-      <c r="B19" s="161"/>
-      <c r="C19" s="192"/>
+      <c r="A19" s="173"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="190"/>
       <c r="D19" s="107" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="161"/>
-      <c r="B20" s="161"/>
-      <c r="C20" s="192" t="s">
+      <c r="A20" s="173"/>
+      <c r="B20" s="173"/>
+      <c r="C20" s="190" t="s">
         <v>240</v>
       </c>
       <c r="D20" s="58" t="s">
@@ -31280,16 +31295,16 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="161"/>
-      <c r="B21" s="161"/>
-      <c r="C21" s="192"/>
+      <c r="A21" s="173"/>
+      <c r="B21" s="173"/>
+      <c r="C21" s="190"/>
       <c r="D21" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="161"/>
-      <c r="B22" s="161"/>
+      <c r="A22" s="173"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="120" t="s">
         <v>307</v>
       </c>
@@ -31298,10 +31313,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="142" t="s">
+      <c r="A23" s="148" t="s">
         <v>296</v>
       </c>
-      <c r="B23" s="161" t="s">
+      <c r="B23" s="173" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
@@ -31312,8 +31327,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="142"/>
-      <c r="B24" s="161"/>
+      <c r="A24" s="148"/>
+      <c r="B24" s="173"/>
       <c r="C24" s="61" t="s">
         <v>281</v>
       </c>
@@ -31330,10 +31345,10 @@
       <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="185" t="s">
+      <c r="A26" s="182" t="s">
         <v>260</v>
       </c>
-      <c r="B26" s="161" t="s">
+      <c r="B26" s="173" t="s">
         <v>234</v>
       </c>
       <c r="C26" s="100"/>
@@ -31342,8 +31357,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="186"/>
-      <c r="B27" s="161"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="173"/>
       <c r="C27" s="100"/>
       <c r="D27" s="58" t="s">
         <v>257</v>
@@ -31364,10 +31379,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="142" t="s">
+      <c r="A29" s="196" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="161" t="s">
+      <c r="B29" s="184" t="s">
         <v>234</v>
       </c>
       <c r="C29" s="58" t="s">
@@ -31378,8 +31393,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="142"/>
-      <c r="B30" s="161"/>
+      <c r="A30" s="197"/>
+      <c r="B30" s="195"/>
       <c r="C30" s="58" t="s">
         <v>270</v>
       </c>
@@ -31388,8 +31403,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="142"/>
-      <c r="B31" s="161"/>
+      <c r="A31" s="197"/>
+      <c r="B31" s="195"/>
       <c r="C31" s="58" t="s">
         <v>269</v>
       </c>
@@ -31398,8 +31413,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="142"/>
-      <c r="B32" s="161"/>
+      <c r="A32" s="197"/>
+      <c r="B32" s="195"/>
       <c r="C32" s="107" t="s">
         <v>277</v>
       </c>
@@ -31408,8 +31423,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="142"/>
-      <c r="B33" s="161"/>
+      <c r="A33" s="197"/>
+      <c r="B33" s="195"/>
       <c r="C33" s="58" t="s">
         <v>282</v>
       </c>
@@ -31418,8 +31433,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="142"/>
-      <c r="B34" s="161"/>
+      <c r="A34" s="197"/>
+      <c r="B34" s="195"/>
       <c r="C34" s="58" t="s">
         <v>283</v>
       </c>
@@ -31428,8 +31443,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="142"/>
-      <c r="B35" s="161"/>
+      <c r="A35" s="197"/>
+      <c r="B35" s="195"/>
       <c r="C35" s="107" t="s">
         <v>288</v>
       </c>
@@ -31438,8 +31453,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="142"/>
-      <c r="B36" s="161"/>
+      <c r="A36" s="197"/>
+      <c r="B36" s="195"/>
       <c r="C36" s="107" t="s">
         <v>302</v>
       </c>
@@ -31448,8 +31463,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="142"/>
-      <c r="B37" s="161"/>
+      <c r="A37" s="197"/>
+      <c r="B37" s="195"/>
       <c r="C37" s="107" t="s">
         <v>289</v>
       </c>
@@ -31458,9 +31473,9 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="142"/>
-      <c r="B38" s="161"/>
-      <c r="C38" s="193" t="s">
+      <c r="A38" s="197"/>
+      <c r="B38" s="195"/>
+      <c r="C38" s="122" t="s">
         <v>244</v>
       </c>
       <c r="D38" s="119" t="s">
@@ -31468,9 +31483,9 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="142"/>
-      <c r="B39" s="161"/>
-      <c r="C39" s="194" t="s">
+      <c r="A39" s="197"/>
+      <c r="B39" s="195"/>
+      <c r="C39" s="123" t="s">
         <v>311</v>
       </c>
       <c r="D39" s="107" t="s">
@@ -31478,22 +31493,18 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B40" s="121" t="s">
-        <v>234</v>
-      </c>
+      <c r="A40" s="198"/>
+      <c r="B40" s="185"/>
       <c r="C40" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="107" t="s">
-        <v>274</v>
+        <v>312</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="58" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B41" s="121" t="s">
         <v>234</v>
@@ -31505,295 +31516,309 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="39" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B42" s="121" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="107" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="44"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="99"/>
-      <c r="B43" s="67"/>
-      <c r="C43" s="100"/>
-      <c r="D43" s="79" t="s">
+    <row r="44" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="99"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="100"/>
+      <c r="D44" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="161" t="s">
+    <row r="45" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="173" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="161" t="s">
+      <c r="B45" s="173" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="113" t="s">
+      <c r="C45" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D45" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="161"/>
-      <c r="B45" s="161"/>
-      <c r="C45" s="113">
-        <v>10.1</v>
-      </c>
-      <c r="D45" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="161"/>
-      <c r="B46" s="161"/>
+      <c r="A46" s="173"/>
+      <c r="B46" s="173"/>
       <c r="C46" s="113">
-        <v>10.199999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="D46" s="58" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="161"/>
-      <c r="B47" s="161"/>
-      <c r="C47" s="114" t="s">
-        <v>293</v>
-      </c>
-      <c r="D47" s="109" t="s">
-        <v>294</v>
+      <c r="A47" s="173"/>
+      <c r="B47" s="173"/>
+      <c r="C47" s="113">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="141" t="s">
-        <v>247</v>
-      </c>
-      <c r="B48" s="161" t="s">
-        <v>234</v>
-      </c>
-      <c r="C48" s="172"/>
-      <c r="D48" s="176" t="s">
-        <v>261</v>
+      <c r="A48" s="173"/>
+      <c r="B48" s="173"/>
+      <c r="C48" s="114" t="s">
+        <v>293</v>
+      </c>
+      <c r="D48" s="109" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="141"/>
-      <c r="B49" s="161"/>
-      <c r="C49" s="173"/>
-      <c r="D49" s="176"/>
+      <c r="A49" s="139" t="s">
+        <v>247</v>
+      </c>
+      <c r="B49" s="173" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="191"/>
+      <c r="D49" s="189" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="105" t="s">
+      <c r="A50" s="139"/>
+      <c r="B50" s="173"/>
+      <c r="C50" s="192"/>
+      <c r="D50" s="189"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="105" t="s">
         <v>262</v>
       </c>
-      <c r="B50" s="106" t="s">
+      <c r="B51" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C50" s="113" t="s">
+      <c r="C51" s="113" t="s">
         <v>250</v>
       </c>
-      <c r="D50" s="107" t="s">
+      <c r="D51" s="107" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="95" t="s">
+    <row r="52" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B51" s="39"/>
-      <c r="C51" s="103"/>
-      <c r="D51" s="98"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B52" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C52" s="115" t="s">
-        <v>265</v>
-      </c>
-      <c r="D52" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="B52" s="39"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="98"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="177" t="s">
-        <v>285</v>
-      </c>
-      <c r="B53" s="180" t="s">
+      <c r="A53" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B53" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="116" t="s">
-        <v>295</v>
+      <c r="C53" s="115" t="s">
+        <v>265</v>
       </c>
       <c r="D53" s="58" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="178"/>
-      <c r="B54" s="181"/>
-      <c r="C54" s="58" t="s">
+      <c r="A54" s="174" t="s">
+        <v>285</v>
+      </c>
+      <c r="B54" s="177" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="116" t="s">
+        <v>295</v>
+      </c>
+      <c r="D54" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="175"/>
+      <c r="B55" s="178"/>
+      <c r="C55" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D54" s="107" t="s">
+      <c r="D55" s="107" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="179"/>
-      <c r="B55" s="182"/>
-      <c r="C55" s="115" t="s">
+    <row r="56" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="176"/>
+      <c r="B56" s="179"/>
+      <c r="C56" s="115" t="s">
         <v>286</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D56" s="58" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="98"/>
-      <c r="C56" s="110"/>
-      <c r="D56" s="98"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="183" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="187" t="s">
-        <v>271</v>
-      </c>
-      <c r="C57" s="115" t="s">
-        <v>265</v>
-      </c>
-      <c r="D57" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="A57" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="98"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="98"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="184"/>
-      <c r="B58" s="188"/>
+      <c r="A58" s="180" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="184" t="s">
+        <v>271</v>
+      </c>
       <c r="C58" s="115" t="s">
         <v>265</v>
       </c>
       <c r="D58" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="181"/>
+      <c r="B59" s="185"/>
+      <c r="C59" s="115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D59" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="97" t="s">
+    <row r="60" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="106" t="s">
+      <c r="B60" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C59" s="102" t="s">
+      <c r="C60" s="102" t="s">
         <v>264</v>
       </c>
-      <c r="D59" s="58" t="s">
+      <c r="D60" s="58" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B60" s="108" t="s">
-        <v>271</v>
-      </c>
-      <c r="C60" s="100"/>
-      <c r="D60" s="61" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="97" t="s">
+      <c r="A61" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B61" s="108" t="s">
+        <v>271</v>
+      </c>
+      <c r="C61" s="100"/>
+      <c r="D61" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="106" t="s">
+      <c r="B62" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C61" s="102" t="s">
+      <c r="C62" s="102" t="s">
         <v>264</v>
       </c>
-      <c r="D61" s="58" t="s">
+      <c r="D62" s="58" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B62" s="98"/>
-      <c r="C62" s="110"/>
-      <c r="D62" s="98"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="58"/>
-      <c r="B63" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C63" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="107" t="s">
-        <v>274</v>
-      </c>
+      <c r="A63" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B63" s="98"/>
+      <c r="C63" s="110"/>
+      <c r="D63" s="98"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="98" t="s">
-        <v>279</v>
-      </c>
-      <c r="B64" s="98"/>
-      <c r="C64" s="110"/>
-      <c r="D64" s="98"/>
+      <c r="A64" s="58"/>
+      <c r="B64" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C64" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="107" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="58"/>
-      <c r="B65" s="106" t="s">
+      <c r="A65" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B65" s="98"/>
+      <c r="C65" s="110"/>
+      <c r="D65" s="98"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="58"/>
+      <c r="B66" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C65" s="100" t="s">
+      <c r="C66" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="D65" s="107" t="s">
+      <c r="D66" s="107" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B29:B40"/>
+    <mergeCell ref="A29:A40"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A49:A50"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B58:B59"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B12:B15"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B29:B39"/>
-    <mergeCell ref="A29:A39"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Updated Validation and Changelog spreadsheets"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="316">
   <si>
     <t>Document</t>
   </si>
@@ -2750,6 +2750,15 @@
   <si>
     <t>code 3012</t>
   </si>
+  <si>
+    <t>REST HTTP Codes</t>
+  </si>
+  <si>
+    <t>4XX's corrected to 200's</t>
+  </si>
+  <si>
+    <t>code 2040</t>
+  </si>
 </sst>
 </file>
 
@@ -3351,7 +3360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3666,10 +3675,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3885,16 +3896,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4300,12 +4308,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="126"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4328,12 +4336,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="126"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="128"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4373,10 +4381,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="127" t="s">
+      <c r="A7" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="130">
+      <c r="B7" s="132">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4390,8 +4398,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="128"/>
-      <c r="B8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4403,8 +4411,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="128"/>
-      <c r="B9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4416,8 +4424,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="128"/>
-      <c r="B10" s="131"/>
+      <c r="A10" s="130"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4429,8 +4437,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="128"/>
-      <c r="B11" s="131"/>
+      <c r="A11" s="130"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4442,8 +4450,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="129"/>
-      <c r="B12" s="132"/>
+      <c r="A12" s="131"/>
+      <c r="B12" s="134"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4455,10 +4463,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="135" t="s">
+      <c r="A13" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="130">
+      <c r="B13" s="132">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4472,8 +4480,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="136"/>
-      <c r="B14" s="132"/>
+      <c r="A14" s="138"/>
+      <c r="B14" s="134"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4519,12 +4527,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="124" t="s">
+      <c r="A17" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="125"/>
-      <c r="C17" s="125"/>
-      <c r="D17" s="126"/>
+      <c r="B17" s="127"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="128"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4564,21 +4572,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="124" t="s">
+      <c r="A20" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="126"/>
+      <c r="B20" s="127"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="128"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="137" t="s">
+      <c r="A21" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="134">
+      <c r="B21" s="136">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4592,8 +4600,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="138"/>
-      <c r="B22" s="132"/>
+      <c r="A22" s="140"/>
+      <c r="B22" s="134"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4616,18 +4624,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="125"/>
-      <c r="C24" s="125"/>
-      <c r="D24" s="126"/>
+      <c r="B24" s="127"/>
+      <c r="C24" s="127"/>
+      <c r="D24" s="128"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="133" t="s">
+      <c r="A25" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="134">
+      <c r="B25" s="136">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4641,8 +4649,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="128"/>
-      <c r="B26" s="131"/>
+      <c r="A26" s="130"/>
+      <c r="B26" s="133"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4654,8 +4662,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="128"/>
-      <c r="B27" s="131"/>
+      <c r="A27" s="130"/>
+      <c r="B27" s="133"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4667,8 +4675,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="128"/>
-      <c r="B28" s="131"/>
+      <c r="A28" s="130"/>
+      <c r="B28" s="133"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4680,8 +4688,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="128"/>
-      <c r="B29" s="131"/>
+      <c r="A29" s="130"/>
+      <c r="B29" s="133"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4693,8 +4701,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="128"/>
-      <c r="B30" s="131"/>
+      <c r="A30" s="130"/>
+      <c r="B30" s="133"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4706,8 +4714,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="128"/>
-      <c r="B31" s="131"/>
+      <c r="A31" s="130"/>
+      <c r="B31" s="133"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4719,8 +4727,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="129"/>
-      <c r="B32" s="132"/>
+      <c r="A32" s="131"/>
+      <c r="B32" s="134"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4844,12 +4852,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="124" t="s">
+      <c r="A41" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="125"/>
-      <c r="C41" s="125"/>
-      <c r="D41" s="126"/>
+      <c r="B41" s="127"/>
+      <c r="C41" s="127"/>
+      <c r="D41" s="128"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -5029,10 +5037,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="154" t="s">
+      <c r="A7" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5043,8 +5051,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="154"/>
-      <c r="B8" s="153"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="155"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5053,8 +5061,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="154"/>
-      <c r="B9" s="153"/>
+      <c r="A9" s="156"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5063,8 +5071,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="154"/>
-      <c r="B10" s="153"/>
+      <c r="A10" s="156"/>
+      <c r="B10" s="155"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5073,8 +5081,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="154"/>
-      <c r="B11" s="153"/>
+      <c r="A11" s="156"/>
+      <c r="B11" s="155"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5083,8 +5091,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="154"/>
-      <c r="B12" s="153"/>
+      <c r="A12" s="156"/>
+      <c r="B12" s="155"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5093,10 +5101,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="156" t="s">
+      <c r="A13" s="158" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="153" t="s">
+      <c r="B13" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5107,8 +5115,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="156"/>
-      <c r="B14" s="153"/>
+      <c r="A14" s="158"/>
+      <c r="B14" s="155"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5117,8 +5125,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="156"/>
-      <c r="B15" s="153"/>
+      <c r="A15" s="158"/>
+      <c r="B15" s="155"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5127,10 +5135,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="139" t="s">
+      <c r="A16" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5141,8 +5149,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="139"/>
-      <c r="B17" s="148"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="150"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5151,8 +5159,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="139"/>
-      <c r="B18" s="148"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="150"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5161,8 +5169,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="139"/>
-      <c r="B19" s="148"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="150"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5171,8 +5179,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="139"/>
-      <c r="B20" s="148"/>
+      <c r="A20" s="141"/>
+      <c r="B20" s="150"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5181,8 +5189,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="139"/>
-      <c r="B21" s="148"/>
+      <c r="A21" s="141"/>
+      <c r="B21" s="150"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5191,8 +5199,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="139"/>
-      <c r="B22" s="148"/>
+      <c r="A22" s="141"/>
+      <c r="B22" s="150"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5201,8 +5209,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="139"/>
-      <c r="B23" s="148"/>
+      <c r="A23" s="141"/>
+      <c r="B23" s="150"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5211,26 +5219,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="139"/>
-      <c r="B24" s="148"/>
-      <c r="C24" s="139" t="s">
+      <c r="A24" s="141"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="141" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="140" t="s">
+      <c r="D24" s="142" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="139"/>
-      <c r="B25" s="148"/>
-      <c r="C25" s="139"/>
-      <c r="D25" s="140"/>
+      <c r="A25" s="141"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="142"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="154" t="s">
+      <c r="A26" s="156" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="153" t="s">
+      <c r="B26" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5241,8 +5249,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="154"/>
-      <c r="B27" s="153"/>
+      <c r="A27" s="156"/>
+      <c r="B27" s="155"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5269,28 +5277,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="155" t="s">
+      <c r="A30" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="153" t="s">
+      <c r="B30" s="155" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="139" t="s">
+      <c r="C30" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="143" t="s">
+      <c r="D30" s="145" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="155"/>
-      <c r="B31" s="153"/>
-      <c r="C31" s="139"/>
-      <c r="D31" s="143"/>
+      <c r="A31" s="157"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="145"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="155"/>
-      <c r="B32" s="153"/>
+      <c r="A32" s="157"/>
+      <c r="B32" s="155"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5299,8 +5307,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="155"/>
-      <c r="B33" s="153"/>
+      <c r="A33" s="157"/>
+      <c r="B33" s="155"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5309,8 +5317,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="155"/>
-      <c r="B34" s="153"/>
+      <c r="A34" s="157"/>
+      <c r="B34" s="155"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5319,8 +5327,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="155"/>
-      <c r="B35" s="153"/>
+      <c r="A35" s="157"/>
+      <c r="B35" s="155"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5329,8 +5337,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="155"/>
-      <c r="B36" s="153"/>
+      <c r="A36" s="157"/>
+      <c r="B36" s="155"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5339,26 +5347,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="155"/>
-      <c r="B37" s="153"/>
-      <c r="C37" s="144" t="s">
+      <c r="A37" s="157"/>
+      <c r="B37" s="155"/>
+      <c r="C37" s="146" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="146" t="s">
+      <c r="D37" s="148" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="155"/>
-      <c r="B38" s="153"/>
-      <c r="C38" s="145"/>
-      <c r="D38" s="146"/>
+      <c r="A38" s="157"/>
+      <c r="B38" s="155"/>
+      <c r="C38" s="147"/>
+      <c r="D38" s="148"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="154" t="s">
+      <c r="A39" s="156" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B39" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5369,8 +5377,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="154"/>
-      <c r="B40" s="153"/>
+      <c r="A40" s="156"/>
+      <c r="B40" s="155"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5397,10 +5405,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="155" t="s">
+      <c r="A43" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="153" t="s">
+      <c r="B43" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5409,8 +5417,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="155"/>
-      <c r="B44" s="153"/>
+      <c r="A44" s="157"/>
+      <c r="B44" s="155"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5419,10 +5427,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="150" t="s">
+      <c r="A45" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="153" t="s">
+      <c r="B45" s="155" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5431,8 +5439,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="151"/>
-      <c r="B46" s="153"/>
+      <c r="A46" s="153"/>
+      <c r="B46" s="155"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5441,8 +5449,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="151"/>
-      <c r="B47" s="153"/>
+      <c r="A47" s="153"/>
+      <c r="B47" s="155"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5451,8 +5459,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="152"/>
-      <c r="B48" s="153"/>
+      <c r="A48" s="154"/>
+      <c r="B48" s="155"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5461,10 +5469,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="148" t="s">
+      <c r="A49" s="150" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="148" t="s">
+      <c r="B49" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9568,8 +9576,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="148"/>
-      <c r="B50" s="148"/>
+      <c r="A50" s="150"/>
+      <c r="B50" s="150"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13673,8 +13681,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="148"/>
-      <c r="B51" s="148"/>
+      <c r="A51" s="150"/>
+      <c r="B51" s="150"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17778,8 +17786,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="148"/>
-      <c r="B52" s="148"/>
+      <c r="A52" s="150"/>
+      <c r="B52" s="150"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21883,12 +21891,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="148"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="142" t="s">
+      <c r="A53" s="150"/>
+      <c r="B53" s="150"/>
+      <c r="C53" s="144" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="143" t="s">
+      <c r="D53" s="145" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25988,10 +25996,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="148"/>
-      <c r="B54" s="148"/>
-      <c r="C54" s="142"/>
-      <c r="D54" s="143"/>
+      <c r="A54" s="150"/>
+      <c r="B54" s="150"/>
+      <c r="C54" s="144"/>
+      <c r="D54" s="145"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30109,10 +30117,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="147" t="s">
+      <c r="A57" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="148" t="s">
+      <c r="B57" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30123,8 +30131,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="147"/>
-      <c r="B58" s="148"/>
+      <c r="A58" s="149"/>
+      <c r="B58" s="150"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30133,8 +30141,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="147"/>
-      <c r="B59" s="148"/>
+      <c r="A59" s="149"/>
+      <c r="B59" s="150"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30143,8 +30151,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="147"/>
-      <c r="B60" s="148"/>
+      <c r="A60" s="149"/>
+      <c r="B60" s="150"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30153,8 +30161,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="147"/>
-      <c r="B61" s="148"/>
+      <c r="A61" s="149"/>
+      <c r="B61" s="150"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30163,8 +30171,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="147"/>
-      <c r="B62" s="148"/>
+      <c r="A62" s="149"/>
+      <c r="B62" s="150"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30173,8 +30181,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="147"/>
-      <c r="B63" s="148"/>
+      <c r="A63" s="149"/>
+      <c r="B63" s="150"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30183,16 +30191,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="147"/>
-      <c r="B64" s="148"/>
+      <c r="A64" s="149"/>
+      <c r="B64" s="150"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="147"/>
-      <c r="B65" s="148"/>
+      <c r="A65" s="149"/>
+      <c r="B65" s="150"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30201,16 +30209,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="147"/>
-      <c r="B66" s="148"/>
+      <c r="A66" s="149"/>
+      <c r="B66" s="150"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="147"/>
-      <c r="B67" s="148"/>
+      <c r="A67" s="149"/>
+      <c r="B67" s="150"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30219,8 +30227,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="147"/>
-      <c r="B68" s="148"/>
+      <c r="A68" s="149"/>
+      <c r="B68" s="150"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30229,8 +30237,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="147"/>
-      <c r="B69" s="148"/>
+      <c r="A69" s="149"/>
+      <c r="B69" s="150"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30239,8 +30247,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="147"/>
-      <c r="B70" s="148"/>
+      <c r="A70" s="149"/>
+      <c r="B70" s="150"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30249,8 +30257,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="147"/>
-      <c r="B71" s="148"/>
+      <c r="A71" s="149"/>
+      <c r="B71" s="150"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30259,8 +30267,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="147"/>
-      <c r="B72" s="148"/>
+      <c r="A72" s="149"/>
+      <c r="B72" s="150"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30269,16 +30277,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="147"/>
-      <c r="B73" s="148"/>
+      <c r="A73" s="149"/>
+      <c r="B73" s="150"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="147"/>
-      <c r="B74" s="148"/>
+      <c r="A74" s="149"/>
+      <c r="B74" s="150"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30287,18 +30295,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="147"/>
-      <c r="B75" s="148"/>
-      <c r="C75" s="141"/>
-      <c r="D75" s="149" t="s">
+      <c r="A75" s="149"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="143"/>
+      <c r="D75" s="151" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="147"/>
-      <c r="B76" s="148"/>
-      <c r="C76" s="141"/>
-      <c r="D76" s="149"/>
+      <c r="A76" s="149"/>
+      <c r="B76" s="150"/>
+      <c r="C76" s="143"/>
+      <c r="D76" s="151"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30422,10 +30430,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="154" t="s">
+      <c r="A4" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="153" t="s">
+      <c r="B4" s="155" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30436,133 +30444,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="154"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="164" t="s">
+      <c r="A5" s="156"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="166" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="163" t="s">
+      <c r="D5" s="165" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="154"/>
-      <c r="B6" s="153"/>
-      <c r="C6" s="164"/>
-      <c r="D6" s="163"/>
+      <c r="A6" s="156"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="165"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="154"/>
-      <c r="B7" s="153"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="155"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="154"/>
-      <c r="B8" s="153"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="155"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="154"/>
-      <c r="B9" s="153"/>
+      <c r="A9" s="156"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="156" t="s">
+      <c r="A10" s="158" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="166"/>
-      <c r="D10" s="163" t="s">
+      <c r="C10" s="168"/>
+      <c r="D10" s="165" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="156"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="166"/>
-      <c r="D11" s="163"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="165"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="156"/>
-      <c r="B12" s="153"/>
-      <c r="C12" s="166"/>
-      <c r="D12" s="163"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="155"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="165"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="139" t="s">
+      <c r="A13" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="150" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="163" t="s">
+      <c r="C13" s="167"/>
+      <c r="D13" s="165" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="139"/>
-      <c r="B14" s="148"/>
-      <c r="C14" s="165"/>
-      <c r="D14" s="163"/>
+      <c r="A14" s="141"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="167"/>
+      <c r="D14" s="165"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="139"/>
-      <c r="B15" s="148"/>
-      <c r="C15" s="165"/>
+      <c r="A15" s="141"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="167"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="139"/>
-      <c r="B16" s="148"/>
-      <c r="C16" s="165"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="167"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="139"/>
-      <c r="B17" s="148"/>
-      <c r="C17" s="165"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="167"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="139"/>
-      <c r="B18" s="148"/>
-      <c r="C18" s="165"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="139"/>
-      <c r="B19" s="148"/>
-      <c r="C19" s="165"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="167"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="139"/>
-      <c r="B20" s="148"/>
-      <c r="C20" s="165"/>
+      <c r="A20" s="141"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="167"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="139"/>
-      <c r="B21" s="148"/>
-      <c r="C21" s="165"/>
+      <c r="A21" s="141"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="167"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="139"/>
-      <c r="B22" s="148"/>
-      <c r="C22" s="165"/>
+      <c r="A22" s="141"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="167"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="139"/>
-      <c r="B23" s="148"/>
-      <c r="C23" s="165"/>
+      <c r="A23" s="141"/>
+      <c r="B23" s="150"/>
+      <c r="C23" s="167"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30660,10 +30668,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="157" t="s">
+      <c r="A32" s="159" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="160" t="s">
+      <c r="B32" s="162" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30674,26 +30682,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="158"/>
-      <c r="B33" s="161"/>
+      <c r="A33" s="160"/>
+      <c r="B33" s="163"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="158"/>
-      <c r="B34" s="161"/>
+      <c r="A34" s="160"/>
+      <c r="B34" s="163"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="158"/>
-      <c r="B35" s="161"/>
+      <c r="A35" s="160"/>
+      <c r="B35" s="163"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="159"/>
-      <c r="B36" s="162"/>
+      <c r="A36" s="161"/>
+      <c r="B36" s="164"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30722,10 +30730,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="155" t="s">
+      <c r="A39" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B39" s="155" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30736,8 +30744,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="155"/>
-      <c r="B40" s="153"/>
+      <c r="A40" s="157"/>
+      <c r="B40" s="155"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30746,84 +30754,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="154" t="s">
+      <c r="A41" s="156" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="153" t="s">
+      <c r="B41" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="166" t="s">
+      <c r="C41" s="168" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="139" t="s">
+      <c r="D41" s="141" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="154"/>
-      <c r="B42" s="153"/>
-      <c r="C42" s="166"/>
-      <c r="D42" s="139"/>
+      <c r="A42" s="156"/>
+      <c r="B42" s="155"/>
+      <c r="C42" s="168"/>
+      <c r="D42" s="141"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="154"/>
-      <c r="B43" s="153"/>
-      <c r="C43" s="166" t="s">
+      <c r="A43" s="156"/>
+      <c r="B43" s="155"/>
+      <c r="C43" s="168" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="149" t="s">
+      <c r="D43" s="151" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="154"/>
-      <c r="B44" s="153"/>
-      <c r="C44" s="166"/>
-      <c r="D44" s="149"/>
+      <c r="A44" s="156"/>
+      <c r="B44" s="155"/>
+      <c r="C44" s="168"/>
+      <c r="D44" s="151"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="147" t="s">
+      <c r="A45" s="149" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="150" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="170"/>
+      <c r="C45" s="172"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="147"/>
-      <c r="B46" s="148"/>
-      <c r="C46" s="171"/>
-      <c r="D46" s="167" t="s">
+      <c r="A46" s="149"/>
+      <c r="B46" s="150"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="169" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="147"/>
-      <c r="B47" s="148"/>
-      <c r="C47" s="171"/>
-      <c r="D47" s="168"/>
+      <c r="A47" s="149"/>
+      <c r="B47" s="150"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="170"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="147"/>
-      <c r="B48" s="148"/>
-      <c r="C48" s="172"/>
-      <c r="D48" s="168"/>
+      <c r="A48" s="149"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="174"/>
+      <c r="D48" s="170"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="147"/>
-      <c r="B49" s="148"/>
-      <c r="C49" s="142"/>
-      <c r="D49" s="168"/>
+      <c r="A49" s="149"/>
+      <c r="B49" s="150"/>
+      <c r="C49" s="144"/>
+      <c r="D49" s="170"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="147"/>
-      <c r="B50" s="148"/>
-      <c r="C50" s="142"/>
-      <c r="D50" s="169"/>
+      <c r="A50" s="149"/>
+      <c r="B50" s="150"/>
+      <c r="C50" s="144"/>
+      <c r="D50" s="171"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30846,10 +30854,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="148" t="s">
+      <c r="A53" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="148" t="s">
+      <c r="B53" s="150" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30860,8 +30868,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="148"/>
-      <c r="B54" s="148"/>
+      <c r="A54" s="150"/>
+      <c r="B54" s="150"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30870,8 +30878,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="148"/>
-      <c r="B55" s="148"/>
+      <c r="A55" s="150"/>
+      <c r="B55" s="150"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30880,9 +30888,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="148"/>
-      <c r="B56" s="148"/>
-      <c r="C56" s="173" t="s">
+      <c r="A56" s="150"/>
+      <c r="B56" s="150"/>
+      <c r="C56" s="175" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30890,16 +30898,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="148"/>
-      <c r="B57" s="148"/>
-      <c r="C57" s="173"/>
+      <c r="A57" s="150"/>
+      <c r="B57" s="150"/>
+      <c r="C57" s="175"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="148"/>
-      <c r="B58" s="148"/>
+      <c r="A58" s="150"/>
+      <c r="B58" s="150"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30908,8 +30916,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="148"/>
-      <c r="B59" s="148"/>
+      <c r="A59" s="150"/>
+      <c r="B59" s="150"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30918,9 +30926,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="148"/>
-      <c r="B60" s="148"/>
-      <c r="C60" s="173" t="s">
+      <c r="A60" s="150"/>
+      <c r="B60" s="150"/>
+      <c r="C60" s="175" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30928,25 +30936,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="148"/>
-      <c r="B61" s="148"/>
-      <c r="C61" s="173"/>
+      <c r="A61" s="150"/>
+      <c r="B61" s="150"/>
+      <c r="C61" s="175"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="148"/>
-      <c r="B62" s="148"/>
-      <c r="C62" s="173"/>
+      <c r="A62" s="150"/>
+      <c r="B62" s="150"/>
+      <c r="C62" s="175"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="148"/>
-      <c r="B63" s="148"/>
-      <c r="C63" s="166" t="s">
+      <c r="A63" s="150"/>
+      <c r="B63" s="150"/>
+      <c r="C63" s="168" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30954,30 +30962,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="148"/>
-      <c r="B64" s="148"/>
-      <c r="C64" s="166"/>
-      <c r="D64" s="149" t="s">
+      <c r="A64" s="150"/>
+      <c r="B64" s="150"/>
+      <c r="C64" s="168"/>
+      <c r="D64" s="151" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="148"/>
-      <c r="B65" s="148"/>
-      <c r="C65" s="166"/>
-      <c r="D65" s="149"/>
+      <c r="A65" s="150"/>
+      <c r="B65" s="150"/>
+      <c r="C65" s="168"/>
+      <c r="D65" s="151"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="148"/>
-      <c r="B66" s="148"/>
-      <c r="C66" s="166"/>
-      <c r="D66" s="149"/>
+      <c r="A66" s="150"/>
+      <c r="B66" s="150"/>
+      <c r="C66" s="168"/>
+      <c r="D66" s="151"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="148"/>
-      <c r="B67" s="148"/>
-      <c r="C67" s="166"/>
-      <c r="D67" s="149"/>
+      <c r="A67" s="150"/>
+      <c r="B67" s="150"/>
+      <c r="C67" s="168"/>
+      <c r="D67" s="151"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31074,10 +31082,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31111,10 +31119,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="173" t="s">
+      <c r="B3" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="100"/>
@@ -31123,8 +31131,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="139"/>
-      <c r="B4" s="173"/>
+      <c r="A4" s="141"/>
+      <c r="B4" s="175"/>
       <c r="C4" s="113" t="s">
         <v>235</v>
       </c>
@@ -31136,7 +31144,7 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="173"/>
+      <c r="B5" s="175"/>
       <c r="C5" s="113" t="s">
         <v>235</v>
       </c>
@@ -31148,7 +31156,7 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="173"/>
+      <c r="B6" s="175"/>
       <c r="C6" s="113" t="s">
         <v>22</v>
       </c>
@@ -31157,18 +31165,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="182" t="s">
+      <c r="A7" s="184" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="173"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="100"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="183"/>
-      <c r="B8" s="173"/>
+      <c r="A8" s="185"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="100"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
@@ -31178,7 +31186,7 @@
       <c r="A9" t="s">
         <v>290</v>
       </c>
-      <c r="B9" s="173"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="100" t="s">
         <v>30</v>
       </c>
@@ -31188,7 +31196,7 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="173"/>
+      <c r="B10" s="175"/>
       <c r="C10" s="100"/>
       <c r="D10" s="111" t="s">
         <v>259</v>
@@ -31203,10 +31211,10 @@
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="186" t="s">
+      <c r="A12" s="188" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C12" s="100"/>
@@ -31215,24 +31223,24 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="187"/>
-      <c r="B13" s="178"/>
+      <c r="A13" s="189"/>
+      <c r="B13" s="180"/>
       <c r="C13" s="100"/>
       <c r="D13" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="187"/>
-      <c r="B14" s="178"/>
+      <c r="A14" s="189"/>
+      <c r="B14" s="180"/>
       <c r="C14" s="100"/>
       <c r="D14" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="188"/>
-      <c r="B15" s="179"/>
+      <c r="A15" s="190"/>
+      <c r="B15" s="181"/>
       <c r="C15" s="58" t="s">
         <v>300</v>
       </c>
@@ -31241,10 +31249,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="193" t="s">
+      <c r="A16" s="195" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="173" t="s">
+      <c r="B16" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C16" s="58" t="s">
@@ -31255,21 +31263,21 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="194"/>
-      <c r="B17" s="173"/>
+      <c r="A17" s="196"/>
+      <c r="B17" s="175"/>
       <c r="C17" s="58"/>
       <c r="D17" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="173" t="s">
+      <c r="A18" s="175" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="173" t="s">
+      <c r="B18" s="175" t="s">
         <v>234</v>
       </c>
-      <c r="C18" s="190" t="s">
+      <c r="C18" s="192" t="s">
         <v>239</v>
       </c>
       <c r="D18" s="118" t="s">
@@ -31277,17 +31285,17 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="173"/>
-      <c r="B19" s="173"/>
-      <c r="C19" s="190"/>
+      <c r="A19" s="175"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="192"/>
       <c r="D19" s="107" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="173"/>
-      <c r="B20" s="173"/>
-      <c r="C20" s="190" t="s">
+      <c r="A20" s="175"/>
+      <c r="B20" s="175"/>
+      <c r="C20" s="192" t="s">
         <v>240</v>
       </c>
       <c r="D20" s="58" t="s">
@@ -31295,16 +31303,16 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="173"/>
-      <c r="B21" s="173"/>
-      <c r="C21" s="190"/>
+      <c r="A21" s="175"/>
+      <c r="B21" s="175"/>
+      <c r="C21" s="192"/>
       <c r="D21" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="173"/>
-      <c r="B22" s="173"/>
+      <c r="A22" s="175"/>
+      <c r="B22" s="175"/>
       <c r="C22" s="120" t="s">
         <v>307</v>
       </c>
@@ -31313,10 +31321,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="148" t="s">
+      <c r="A23" s="150" t="s">
         <v>296</v>
       </c>
-      <c r="B23" s="173" t="s">
+      <c r="B23" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
@@ -31327,8 +31335,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="148"/>
-      <c r="B24" s="173"/>
+      <c r="A24" s="150"/>
+      <c r="B24" s="175"/>
       <c r="C24" s="61" t="s">
         <v>281</v>
       </c>
@@ -31345,10 +31353,10 @@
       <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="182" t="s">
+      <c r="A26" s="184" t="s">
         <v>260</v>
       </c>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C26" s="100"/>
@@ -31357,8 +31365,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="183"/>
-      <c r="B27" s="173"/>
+      <c r="A27" s="185"/>
+      <c r="B27" s="175"/>
       <c r="C27" s="100"/>
       <c r="D27" s="58" t="s">
         <v>257</v>
@@ -31379,13 +31387,13 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="196" t="s">
+      <c r="A29" s="197" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="184" t="s">
+      <c r="B29" s="175" t="s">
         <v>234</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="122" t="s">
         <v>268</v>
       </c>
       <c r="D29" s="58" t="s">
@@ -31393,9 +31401,9 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="197"/>
-      <c r="B30" s="195"/>
-      <c r="C30" s="58" t="s">
+      <c r="A30" s="198"/>
+      <c r="B30" s="175"/>
+      <c r="C30" s="122" t="s">
         <v>270</v>
       </c>
       <c r="D30" s="58" t="s">
@@ -31403,9 +31411,9 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="197"/>
-      <c r="B31" s="195"/>
-      <c r="C31" s="58" t="s">
+      <c r="A31" s="198"/>
+      <c r="B31" s="175"/>
+      <c r="C31" s="122" t="s">
         <v>269</v>
       </c>
       <c r="D31" s="58" t="s">
@@ -31413,9 +31421,9 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="197"/>
-      <c r="B32" s="195"/>
-      <c r="C32" s="107" t="s">
+      <c r="A32" s="198"/>
+      <c r="B32" s="175"/>
+      <c r="C32" s="123" t="s">
         <v>277</v>
       </c>
       <c r="D32" s="107" t="s">
@@ -31423,9 +31431,9 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="197"/>
-      <c r="B33" s="195"/>
-      <c r="C33" s="58" t="s">
+      <c r="A33" s="198"/>
+      <c r="B33" s="175"/>
+      <c r="C33" s="122" t="s">
         <v>282</v>
       </c>
       <c r="D33" s="58" t="s">
@@ -31433,9 +31441,9 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="197"/>
-      <c r="B34" s="195"/>
-      <c r="C34" s="58" t="s">
+      <c r="A34" s="198"/>
+      <c r="B34" s="175"/>
+      <c r="C34" s="122" t="s">
         <v>283</v>
       </c>
       <c r="D34" s="58" t="s">
@@ -31443,9 +31451,9 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="197"/>
-      <c r="B35" s="195"/>
-      <c r="C35" s="107" t="s">
+      <c r="A35" s="198"/>
+      <c r="B35" s="175"/>
+      <c r="C35" s="123" t="s">
         <v>288</v>
       </c>
       <c r="D35" s="107" t="s">
@@ -31453,9 +31461,9 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="197"/>
-      <c r="B36" s="195"/>
-      <c r="C36" s="107" t="s">
+      <c r="A36" s="198"/>
+      <c r="B36" s="175"/>
+      <c r="C36" s="123" t="s">
         <v>302</v>
       </c>
       <c r="D36" s="107" t="s">
@@ -31463,9 +31471,9 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="197"/>
-      <c r="B37" s="195"/>
-      <c r="C37" s="107" t="s">
+      <c r="A37" s="198"/>
+      <c r="B37" s="175"/>
+      <c r="C37" s="123" t="s">
         <v>289</v>
       </c>
       <c r="D37" s="107" t="s">
@@ -31473,9 +31481,9 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="197"/>
-      <c r="B38" s="195"/>
-      <c r="C38" s="122" t="s">
+      <c r="A38" s="198"/>
+      <c r="B38" s="175"/>
+      <c r="C38" s="124" t="s">
         <v>244</v>
       </c>
       <c r="D38" s="119" t="s">
@@ -31483,9 +31491,9 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="197"/>
-      <c r="B39" s="195"/>
-      <c r="C39" s="123" t="s">
+      <c r="A39" s="198"/>
+      <c r="B39" s="175"/>
+      <c r="C39" s="125" t="s">
         <v>311</v>
       </c>
       <c r="D39" s="107" t="s">
@@ -31494,8 +31502,8 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="198"/>
-      <c r="B40" s="185"/>
-      <c r="C40" s="58" t="s">
+      <c r="B40" s="175"/>
+      <c r="C40" s="122" t="s">
         <v>312</v>
       </c>
       <c r="D40" s="58" t="s">
@@ -31503,242 +31511,236 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B41" s="121" t="s">
-        <v>234</v>
-      </c>
-      <c r="C41" s="58" t="s">
-        <v>30</v>
+      <c r="A41" s="198"/>
+      <c r="B41" s="175"/>
+      <c r="C41" s="107" t="s">
+        <v>313</v>
       </c>
       <c r="D41" s="107" t="s">
-        <v>274</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="199"/>
+      <c r="B42" s="175"/>
+      <c r="C42" s="107" t="s">
+        <v>315</v>
+      </c>
+      <c r="D42" s="107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" s="121" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="107" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B42" s="121" t="s">
+      <c r="B44" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C42" s="58" t="s">
+      <c r="C44" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="107" t="s">
+      <c r="D44" s="107" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="39" t="s">
+    <row r="45" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="44"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="44"/>
     </row>
-    <row r="44" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="99"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="100"/>
-      <c r="D44" s="79" t="s">
+    <row r="46" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="99"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="100"/>
+      <c r="D46" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="173" t="s">
+    <row r="47" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="175" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="173" t="s">
+      <c r="B47" s="175" t="s">
         <v>234</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C47" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="D45" s="58" t="s">
+      <c r="D47" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="173"/>
-      <c r="B46" s="173"/>
-      <c r="C46" s="113">
-        <v>10.1</v>
-      </c>
-      <c r="D46" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="173"/>
-      <c r="B47" s="173"/>
-      <c r="C47" s="113">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D47" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="173"/>
-      <c r="B48" s="173"/>
-      <c r="C48" s="114" t="s">
-        <v>293</v>
-      </c>
-      <c r="D48" s="109" t="s">
-        <v>294</v>
+      <c r="A48" s="175"/>
+      <c r="B48" s="175"/>
+      <c r="C48" s="113">
+        <v>10.1</v>
+      </c>
+      <c r="D48" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="139" t="s">
-        <v>247</v>
-      </c>
-      <c r="B49" s="173" t="s">
-        <v>234</v>
-      </c>
-      <c r="C49" s="191"/>
-      <c r="D49" s="189" t="s">
-        <v>261</v>
+      <c r="A49" s="175"/>
+      <c r="B49" s="175"/>
+      <c r="C49" s="113">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="139"/>
-      <c r="B50" s="173"/>
-      <c r="C50" s="192"/>
-      <c r="D50" s="189"/>
+      <c r="A50" s="175"/>
+      <c r="B50" s="175"/>
+      <c r="C50" s="114" t="s">
+        <v>293</v>
+      </c>
+      <c r="D50" s="109" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="105" t="s">
-        <v>262</v>
-      </c>
-      <c r="B51" s="106" t="s">
+      <c r="A51" s="141" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51" s="175" t="s">
         <v>234</v>
       </c>
-      <c r="C51" s="113" t="s">
-        <v>250</v>
-      </c>
-      <c r="D51" s="107" t="s">
-        <v>251</v>
+      <c r="C51" s="193"/>
+      <c r="D51" s="191" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B52" s="39"/>
-      <c r="C52" s="103"/>
-      <c r="D52" s="98"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="141"/>
+      <c r="B52" s="175"/>
+      <c r="C52" s="194"/>
+      <c r="D52" s="191"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="58" t="s">
-        <v>249</v>
+      <c r="A53" s="105" t="s">
+        <v>262</v>
       </c>
       <c r="B53" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="115" t="s">
-        <v>265</v>
-      </c>
-      <c r="D53" s="58" t="s">
-        <v>267</v>
+      <c r="C53" s="113" t="s">
+        <v>250</v>
+      </c>
+      <c r="D53" s="107" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="174" t="s">
-        <v>285</v>
-      </c>
-      <c r="B54" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C54" s="116" t="s">
-        <v>295</v>
-      </c>
-      <c r="D54" s="58" t="s">
-        <v>251</v>
-      </c>
+    <row r="54" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B54" s="39"/>
+      <c r="C54" s="103"/>
+      <c r="D54" s="98"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="175"/>
-      <c r="B55" s="178"/>
-      <c r="C55" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D55" s="107" t="s">
-        <v>306</v>
+      <c r="A55" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B55" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="176"/>
-      <c r="B56" s="179"/>
-      <c r="C56" s="115" t="s">
-        <v>286</v>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="176" t="s">
+        <v>285</v>
+      </c>
+      <c r="B56" s="179" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="116" t="s">
+        <v>295</v>
       </c>
       <c r="D56" s="58" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="98"/>
-      <c r="C57" s="110"/>
-      <c r="D57" s="98"/>
+      <c r="A57" s="177"/>
+      <c r="B57" s="180"/>
+      <c r="C57" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D57" s="107" t="s">
+        <v>306</v>
+      </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="180" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="184" t="s">
-        <v>271</v>
-      </c>
+    <row r="58" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="178"/>
+      <c r="B58" s="181"/>
       <c r="C58" s="115" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="D58" s="58" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="181"/>
-      <c r="B59" s="185"/>
-      <c r="C59" s="115" t="s">
+      <c r="A59" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="98"/>
+      <c r="C59" s="110"/>
+      <c r="D59" s="98"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="182" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="186" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="115" t="s">
         <v>265</v>
       </c>
-      <c r="D59" s="58" t="s">
+      <c r="D60" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="183"/>
+      <c r="B61" s="187"/>
+      <c r="C61" s="115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="97" t="s">
+    <row r="62" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B60" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C60" s="102" t="s">
-        <v>264</v>
-      </c>
-      <c r="D60" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B61" s="108" t="s">
-        <v>271</v>
-      </c>
-      <c r="C61" s="100"/>
-      <c r="D61" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="97" t="s">
-        <v>60</v>
       </c>
       <c r="B62" s="106" t="s">
         <v>271</v>
@@ -31747,32 +31749,38 @@
         <v>264</v>
       </c>
       <c r="D62" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B63" s="108" t="s">
+        <v>271</v>
+      </c>
+      <c r="C63" s="100"/>
+      <c r="D63" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C64" s="102" t="s">
+        <v>264</v>
+      </c>
+      <c r="D64" s="58" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B63" s="98"/>
-      <c r="C63" s="110"/>
-      <c r="D63" s="98"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="58"/>
-      <c r="B64" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C64" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" s="107" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="98" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B65" s="98"/>
       <c r="C65" s="110"/>
@@ -31790,33 +31798,53 @@
         <v>274</v>
       </c>
     </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B67" s="98"/>
+      <c r="C67" s="110"/>
+      <c r="D67" s="98"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="58"/>
+      <c r="B68" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="107" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="27">
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B29:B40"/>
-    <mergeCell ref="A29:A40"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="B29:B42"/>
+    <mergeCell ref="A29:A42"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B47:B50"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A51:A52"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B12:B15"/>
   </mergeCells>

</xml_diff>

<commit_message>
removed compression, added rule 1016
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMOD_Documentation\paye-employers-documentation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owalsh01\IdeaProjects\paye-employers-documentation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
+    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="346">
   <si>
     <t>Document</t>
   </si>
@@ -2875,6 +2875,21 @@
   </si>
   <si>
     <t>code 3008</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>Guide to webservice compression</t>
+  </si>
+  <si>
+    <t>Receiving Compressed Responses</t>
+  </si>
+  <si>
+    <t>Removed compression size limit</t>
+  </si>
+  <si>
+    <t>code 1016</t>
   </si>
 </sst>
 </file>
@@ -3010,7 +3025,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3032,6 +3047,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3452,7 +3473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3744,6 +3765,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3897,12 +3930,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4280,15 +4314,15 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4305,18 +4339,18 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="113" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="115"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="119"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -4333,18 +4367,18 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="113" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="114"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="115"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="119"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -4361,7 +4395,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -4378,11 +4412,11 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="119">
+      <c r="B7" s="123">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4395,9 +4429,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="117"/>
-      <c r="B8" s="120"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="121"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4408,9 +4442,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="117"/>
-      <c r="B9" s="120"/>
+    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="121"/>
+      <c r="B9" s="124"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4421,9 +4455,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="117"/>
-      <c r="B10" s="120"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="121"/>
+      <c r="B10" s="124"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4434,9 +4468,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="117"/>
-      <c r="B11" s="120"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="121"/>
+      <c r="B11" s="124"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4447,9 +4481,9 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="118"/>
-      <c r="B12" s="121"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="122"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4460,11 +4494,11 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="124" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="128" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="119">
+      <c r="B13" s="123">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4477,9 +4511,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="125"/>
-      <c r="B14" s="121"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="129"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4490,7 +4524,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4507,7 +4541,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4524,18 +4558,18 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="113" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="115"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="119"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4552,7 +4586,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4569,22 +4603,22 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="113" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="115"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="119"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="126" t="s">
+    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="123">
+      <c r="B21" s="127">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4597,9 +4631,9 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="127"/>
-      <c r="B22" s="121"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="131"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4607,7 +4641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4621,19 +4655,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="113" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="115"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="119"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="122" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="123">
+      <c r="B25" s="127">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4646,9 +4680,9 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="117"/>
-      <c r="B26" s="120"/>
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="121"/>
+      <c r="B26" s="124"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4659,9 +4693,9 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="117"/>
-      <c r="B27" s="120"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="121"/>
+      <c r="B27" s="124"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4672,9 +4706,9 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="117"/>
-      <c r="B28" s="120"/>
+    <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="121"/>
+      <c r="B28" s="124"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4685,9 +4719,9 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="117"/>
-      <c r="B29" s="120"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="121"/>
+      <c r="B29" s="124"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4698,9 +4732,9 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="117"/>
-      <c r="B30" s="120"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="121"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4711,9 +4745,9 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="117"/>
-      <c r="B31" s="120"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="121"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4724,9 +4758,9 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="118"/>
-      <c r="B32" s="121"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="122"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4737,7 +4771,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4751,7 +4785,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4765,7 +4799,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4779,7 +4813,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4793,7 +4827,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4807,7 +4841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4821,7 +4855,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4835,7 +4869,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4849,15 +4883,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="113" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="114"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="115"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="119"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4871,7 +4905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4885,7 +4919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4899,7 +4933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4960,15 +4994,15 @@
       <selection activeCell="A30" sqref="A30:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4982,7 +5016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -4990,7 +5024,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -5002,7 +5036,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -5014,7 +5048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -5026,7 +5060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
@@ -5034,11 +5068,11 @@
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="143" t="s">
+    <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="142" t="s">
+      <c r="B7" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5048,9 +5082,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="143"/>
-      <c r="B8" s="142"/>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="147"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5058,9 +5092,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="143"/>
-      <c r="B9" s="142"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="147"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5068,9 +5102,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="143"/>
-      <c r="B10" s="142"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="147"/>
+      <c r="B10" s="146"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5078,9 +5112,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="143"/>
-      <c r="B11" s="142"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="147"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5088,9 +5122,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="143"/>
-      <c r="B12" s="142"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="147"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5098,11 +5132,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="145" t="s">
+    <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="149" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5112,9 +5146,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="145"/>
-      <c r="B14" s="142"/>
+    <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="149"/>
+      <c r="B14" s="146"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5122,9 +5156,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="145"/>
-      <c r="B15" s="142"/>
+    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="149"/>
+      <c r="B15" s="146"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5132,11 +5166,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="128" t="s">
+    <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="137" t="s">
+      <c r="B16" s="141" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5146,9 +5180,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="128"/>
-      <c r="B17" s="137"/>
+    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="132"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5156,9 +5190,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="128"/>
-      <c r="B18" s="137"/>
+    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="132"/>
+      <c r="B18" s="141"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5166,9 +5200,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="128"/>
-      <c r="B19" s="137"/>
+    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="132"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5176,9 +5210,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="128"/>
-      <c r="B20" s="137"/>
+    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="132"/>
+      <c r="B20" s="141"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5186,9 +5220,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="128"/>
-      <c r="B21" s="137"/>
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="132"/>
+      <c r="B21" s="141"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5196,9 +5230,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="128"/>
-      <c r="B22" s="137"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="132"/>
+      <c r="B22" s="141"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5206,9 +5240,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="128"/>
-      <c r="B23" s="137"/>
+    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="132"/>
+      <c r="B23" s="141"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5216,27 +5250,27 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="128"/>
-      <c r="B24" s="137"/>
-      <c r="C24" s="128" t="s">
+    <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="132"/>
+      <c r="B24" s="141"/>
+      <c r="C24" s="132" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="129" t="s">
+      <c r="D24" s="133" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="128"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="129"/>
+    <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="132"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="133"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="143" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="147" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="142" t="s">
+      <c r="B26" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5246,15 +5280,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="143"/>
-      <c r="B27" s="142"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="147"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -5266,7 +5300,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -5274,29 +5308,29 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="144" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="142" t="s">
+      <c r="B30" s="146" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="128" t="s">
+      <c r="C30" s="132" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="132" t="s">
+      <c r="D30" s="136" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="144"/>
-      <c r="B31" s="142"/>
-      <c r="C31" s="128"/>
-      <c r="D31" s="132"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="148"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="136"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="144"/>
-      <c r="B32" s="142"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="148"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5304,9 +5338,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="144"/>
-      <c r="B33" s="142"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="148"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5314,9 +5348,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="144"/>
-      <c r="B34" s="142"/>
+    <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="148"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5324,9 +5358,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="144"/>
-      <c r="B35" s="142"/>
+    <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="148"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5334,9 +5368,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="144"/>
-      <c r="B36" s="142"/>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="148"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5344,27 +5378,27 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="144"/>
-      <c r="B37" s="142"/>
-      <c r="C37" s="133" t="s">
+    <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="148"/>
+      <c r="B37" s="146"/>
+      <c r="C37" s="137" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="135" t="s">
+      <c r="D37" s="139" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="144"/>
-      <c r="B38" s="142"/>
-      <c r="C38" s="134"/>
-      <c r="D38" s="135"/>
+    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="148"/>
+      <c r="B38" s="146"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="139"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="143" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="142" t="s">
+      <c r="B39" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5374,15 +5408,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="143"/>
-      <c r="B40" s="142"/>
+    <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="147"/>
+      <c r="B40" s="146"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -5394,7 +5428,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
@@ -5402,11 +5436,11 @@
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="144" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="142" t="s">
+      <c r="B43" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5414,9 +5448,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="144"/>
-      <c r="B44" s="142"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="148"/>
+      <c r="B44" s="146"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5424,11 +5458,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="139" t="s">
+    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="142" t="s">
+      <c r="B45" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5436,9 +5470,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="140"/>
-      <c r="B46" s="142"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="144"/>
+      <c r="B46" s="146"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5446,9 +5480,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="140"/>
-      <c r="B47" s="142"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="144"/>
+      <c r="B47" s="146"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5456,9 +5490,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="141"/>
-      <c r="B48" s="142"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="145"/>
+      <c r="B48" s="146"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5466,11 +5500,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="137" t="s">
+    <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A49" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="137" t="s">
+      <c r="B49" s="141" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9573,9 +9607,9 @@
       <c r="XEY49" s="42"/>
       <c r="XFC49" s="42"/>
     </row>
-    <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="137"/>
-      <c r="B50" s="137"/>
+    <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="141"/>
+      <c r="B50" s="141"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13678,9 +13712,9 @@
       <c r="XEY50" s="42"/>
       <c r="XFC50" s="42"/>
     </row>
-    <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="137"/>
-      <c r="B51" s="137"/>
+    <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A51" s="141"/>
+      <c r="B51" s="141"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17783,9 +17817,9 @@
       <c r="XEY51" s="42"/>
       <c r="XFC51" s="42"/>
     </row>
-    <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="137"/>
-      <c r="B52" s="137"/>
+    <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A52" s="141"/>
+      <c r="B52" s="141"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21888,13 +21922,13 @@
       <c r="XEY52" s="42"/>
       <c r="XFC52" s="42"/>
     </row>
-    <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="137"/>
-      <c r="B53" s="137"/>
-      <c r="C53" s="131" t="s">
+    <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A53" s="141"/>
+      <c r="B53" s="141"/>
+      <c r="C53" s="135" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="132" t="s">
+      <c r="D53" s="136" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25993,11 +26027,11 @@
       <c r="XEY53" s="42"/>
       <c r="XFC53" s="42"/>
     </row>
-    <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="137"/>
-      <c r="C54" s="131"/>
-      <c r="D54" s="132"/>
+    <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="141"/>
+      <c r="B54" s="141"/>
+      <c r="C54" s="135"/>
+      <c r="D54" s="136"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30094,7 +30128,7 @@
       <c r="XEY54" s="42"/>
       <c r="XFC54" s="42"/>
     </row>
-    <row r="55" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
@@ -30102,7 +30136,7 @@
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
     </row>
-    <row r="56" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -30114,11 +30148,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="136" t="s">
+    <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A57" s="140" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="137" t="s">
+      <c r="B57" s="141" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30128,9 +30162,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="136"/>
-      <c r="B58" s="137"/>
+    <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="140"/>
+      <c r="B58" s="141"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30138,9 +30172,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="136"/>
-      <c r="B59" s="137"/>
+    <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A59" s="140"/>
+      <c r="B59" s="141"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30148,9 +30182,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="136"/>
-      <c r="B60" s="137"/>
+    <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="140"/>
+      <c r="B60" s="141"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30158,9 +30192,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="136"/>
-      <c r="B61" s="137"/>
+    <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A61" s="140"/>
+      <c r="B61" s="141"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30168,9 +30202,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="136"/>
-      <c r="B62" s="137"/>
+    <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A62" s="140"/>
+      <c r="B62" s="141"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30178,9 +30212,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="136"/>
-      <c r="B63" s="137"/>
+    <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A63" s="140"/>
+      <c r="B63" s="141"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30188,17 +30222,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="136"/>
-      <c r="B64" s="137"/>
+    <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A64" s="140"/>
+      <c r="B64" s="141"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="136"/>
-      <c r="B65" s="137"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="140"/>
+      <c r="B65" s="141"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30206,17 +30240,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="136"/>
-      <c r="B66" s="137"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="140"/>
+      <c r="B66" s="141"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="136"/>
-      <c r="B67" s="137"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="140"/>
+      <c r="B67" s="141"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30224,9 +30258,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="136"/>
-      <c r="B68" s="137"/>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="140"/>
+      <c r="B68" s="141"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30234,9 +30268,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="136"/>
-      <c r="B69" s="137"/>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="140"/>
+      <c r="B69" s="141"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30244,9 +30278,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="136"/>
-      <c r="B70" s="137"/>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="140"/>
+      <c r="B70" s="141"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30254,9 +30288,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="136"/>
-      <c r="B71" s="137"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="140"/>
+      <c r="B71" s="141"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30264,9 +30298,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="136"/>
-      <c r="B72" s="137"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="140"/>
+      <c r="B72" s="141"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30274,17 +30308,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="136"/>
-      <c r="B73" s="137"/>
+    <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="140"/>
+      <c r="B73" s="141"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="136"/>
-      <c r="B74" s="137"/>
+    <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="140"/>
+      <c r="B74" s="141"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30292,21 +30326,21 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="136"/>
-      <c r="B75" s="137"/>
-      <c r="C75" s="130"/>
-      <c r="D75" s="138" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="140"/>
+      <c r="B75" s="141"/>
+      <c r="C75" s="134"/>
+      <c r="D75" s="142" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="136"/>
-      <c r="B76" s="137"/>
-      <c r="C76" s="130"/>
-      <c r="D76" s="138"/>
+    <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="140"/>
+      <c r="B76" s="141"/>
+      <c r="C76" s="134"/>
+      <c r="D76" s="142"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
@@ -30314,13 +30348,13 @@
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -30389,15 +30423,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" customWidth="1"/>
-    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30411,7 +30445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -30419,7 +30453,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
@@ -30427,11 +30461,11 @@
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="143" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="146" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30441,139 +30475,139 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="143"/>
-      <c r="B5" s="142"/>
-      <c r="C5" s="153" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="147"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="157" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="156" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="143"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="153"/>
-      <c r="D6" s="152"/>
+    <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="147"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="156"/>
     </row>
-    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="143"/>
-      <c r="B7" s="142"/>
+    <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="147"/>
+      <c r="B7" s="146"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="143"/>
-      <c r="B8" s="142"/>
+    <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="147"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="143"/>
-      <c r="B9" s="142"/>
+    <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="147"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="145" t="s">
+    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="149" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="142" t="s">
+      <c r="B10" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="155"/>
-      <c r="D10" s="152" t="s">
+      <c r="C10" s="159"/>
+      <c r="D10" s="156" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="145"/>
-      <c r="B11" s="142"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="152"/>
+    <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="149"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="156"/>
     </row>
-    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="145"/>
-      <c r="B12" s="142"/>
-      <c r="C12" s="155"/>
-      <c r="D12" s="152"/>
+    <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="149"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="156"/>
     </row>
-    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="128" t="s">
+    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="154"/>
-      <c r="D13" s="152" t="s">
+      <c r="C13" s="158"/>
+      <c r="D13" s="156" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="128"/>
-      <c r="B14" s="137"/>
-      <c r="C14" s="154"/>
-      <c r="D14" s="152"/>
+    <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="132"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="158"/>
+      <c r="D14" s="156"/>
     </row>
-    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="128"/>
-      <c r="B15" s="137"/>
-      <c r="C15" s="154"/>
+    <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="132"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="158"/>
       <c r="D15" s="49"/>
     </row>
-    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="128"/>
-      <c r="B16" s="137"/>
-      <c r="C16" s="154"/>
+    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="132"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="158"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="128"/>
-      <c r="B17" s="137"/>
-      <c r="C17" s="154"/>
+    <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="132"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="158"/>
       <c r="D17" s="49"/>
     </row>
-    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="128"/>
-      <c r="B18" s="137"/>
-      <c r="C18" s="154"/>
+    <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="132"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="158"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="128"/>
-      <c r="B19" s="137"/>
-      <c r="C19" s="154"/>
+    <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="132"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="158"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="128"/>
-      <c r="B20" s="137"/>
-      <c r="C20" s="154"/>
+    <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="132"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="158"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="128"/>
-      <c r="B21" s="137"/>
-      <c r="C21" s="154"/>
+    <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="132"/>
+      <c r="B21" s="141"/>
+      <c r="C21" s="158"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="128"/>
-      <c r="B22" s="137"/>
-      <c r="C22" s="154"/>
+    <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="132"/>
+      <c r="B22" s="141"/>
+      <c r="C22" s="158"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="128"/>
-      <c r="B23" s="137"/>
-      <c r="C23" s="154"/>
+    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="132"/>
+      <c r="B23" s="141"/>
+      <c r="C23" s="158"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
@@ -30587,7 +30621,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30601,7 +30635,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30613,7 +30647,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
@@ -30621,7 +30655,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30635,7 +30669,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="85"/>
       <c r="B29" s="84"/>
       <c r="C29" s="70" t="s">
@@ -30645,7 +30679,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30655,7 +30689,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30665,11 +30699,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="146" t="s">
+    <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="150" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="149" t="s">
+      <c r="B32" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30679,27 +30713,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="147"/>
-      <c r="B33" s="150"/>
+    <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="151"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
-    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="147"/>
-      <c r="B34" s="150"/>
+    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="151"/>
+      <c r="B34" s="154"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="147"/>
-      <c r="B35" s="150"/>
+    <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="151"/>
+      <c r="B35" s="154"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
-    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="148"/>
-      <c r="B36" s="151"/>
+    <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="152"/>
+      <c r="B36" s="155"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30707,7 +30741,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>27</v>
       </c>
@@ -30719,7 +30753,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
@@ -30727,11 +30761,11 @@
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="144" t="s">
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="142" t="s">
+      <c r="B39" s="146" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30741,9 +30775,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="144"/>
-      <c r="B40" s="142"/>
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="148"/>
+      <c r="B40" s="146"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30751,87 +30785,87 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="143" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="142" t="s">
+      <c r="B41" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="155" t="s">
+      <c r="C41" s="159" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="128" t="s">
+      <c r="D41" s="132" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="143"/>
-      <c r="B42" s="142"/>
-      <c r="C42" s="155"/>
-      <c r="D42" s="128"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="147"/>
+      <c r="B42" s="146"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="132"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="143"/>
-      <c r="B43" s="142"/>
-      <c r="C43" s="155" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="147"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="159" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="138" t="s">
+      <c r="D43" s="142" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="143"/>
-      <c r="B44" s="142"/>
-      <c r="C44" s="155"/>
-      <c r="D44" s="138"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="147"/>
+      <c r="B44" s="146"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="142"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="136" t="s">
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="137" t="s">
+      <c r="B45" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="159"/>
+      <c r="C45" s="163"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="136"/>
-      <c r="B46" s="137"/>
-      <c r="C46" s="160"/>
-      <c r="D46" s="156" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="140"/>
+      <c r="B46" s="141"/>
+      <c r="C46" s="164"/>
+      <c r="D46" s="160" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="136"/>
-      <c r="B47" s="137"/>
-      <c r="C47" s="160"/>
-      <c r="D47" s="157"/>
+    <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="140"/>
+      <c r="B47" s="141"/>
+      <c r="C47" s="164"/>
+      <c r="D47" s="161"/>
     </row>
-    <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="136"/>
-      <c r="B48" s="137"/>
-      <c r="C48" s="161"/>
-      <c r="D48" s="157"/>
+    <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="140"/>
+      <c r="B48" s="141"/>
+      <c r="C48" s="165"/>
+      <c r="D48" s="161"/>
     </row>
-    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="136"/>
-      <c r="B49" s="137"/>
-      <c r="C49" s="131"/>
-      <c r="D49" s="157"/>
+    <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="140"/>
+      <c r="B49" s="141"/>
+      <c r="C49" s="135"/>
+      <c r="D49" s="161"/>
     </row>
-    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="136"/>
-      <c r="B50" s="137"/>
-      <c r="C50" s="131"/>
-      <c r="D50" s="158"/>
+    <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="140"/>
+      <c r="B50" s="141"/>
+      <c r="C50" s="135"/>
+      <c r="D50" s="162"/>
     </row>
-    <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
@@ -30839,7 +30873,7 @@
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
     </row>
-    <row r="52" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
@@ -30851,11 +30885,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="137" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="141" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="137" t="s">
+      <c r="B53" s="141" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30865,9 +30899,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="137"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="141"/>
+      <c r="B54" s="141"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30875,9 +30909,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="137"/>
-      <c r="B55" s="137"/>
+    <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="141"/>
+      <c r="B55" s="141"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30885,27 +30919,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="137"/>
-      <c r="B56" s="137"/>
-      <c r="C56" s="162" t="s">
+    <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="141"/>
+      <c r="B56" s="141"/>
+      <c r="C56" s="166" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="137"/>
-      <c r="B57" s="137"/>
-      <c r="C57" s="162"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="141"/>
+      <c r="B57" s="141"/>
+      <c r="C57" s="166"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="137"/>
-      <c r="B58" s="137"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="141"/>
+      <c r="B58" s="141"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30913,9 +30947,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="137"/>
-      <c r="B59" s="137"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="141"/>
+      <c r="B59" s="141"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30923,116 +30957,116 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="137"/>
-      <c r="B60" s="137"/>
-      <c r="C60" s="162" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="141"/>
+      <c r="B60" s="141"/>
+      <c r="C60" s="166" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="137"/>
-      <c r="B61" s="137"/>
-      <c r="C61" s="162"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="141"/>
+      <c r="B61" s="141"/>
+      <c r="C61" s="166"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="137"/>
-      <c r="B62" s="137"/>
-      <c r="C62" s="162"/>
+    <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="141"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="166"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="137"/>
-      <c r="B63" s="137"/>
-      <c r="C63" s="155" t="s">
+    <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="141"/>
+      <c r="B63" s="141"/>
+      <c r="C63" s="159" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="137"/>
-      <c r="B64" s="137"/>
-      <c r="C64" s="155"/>
-      <c r="D64" s="138" t="s">
+    <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="141"/>
+      <c r="B64" s="141"/>
+      <c r="C64" s="159"/>
+      <c r="D64" s="142" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="137"/>
-      <c r="B65" s="137"/>
-      <c r="C65" s="155"/>
-      <c r="D65" s="138"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="141"/>
+      <c r="B65" s="141"/>
+      <c r="C65" s="159"/>
+      <c r="D65" s="142"/>
     </row>
-    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="137"/>
-      <c r="B66" s="137"/>
-      <c r="C66" s="155"/>
-      <c r="D66" s="138"/>
+    <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="141"/>
+      <c r="B66" s="141"/>
+      <c r="C66" s="159"/>
+      <c r="D66" s="142"/>
     </row>
-    <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="137"/>
-      <c r="B67" s="137"/>
-      <c r="C67" s="155"/>
-      <c r="D67" s="138"/>
+    <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="141"/>
+      <c r="B67" s="141"/>
+      <c r="C67" s="159"/>
+      <c r="D67" s="142"/>
     </row>
-    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -31080,21 +31114,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -31108,927 +31142,959 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>24</v>
+        <v>341</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="128" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="113" t="s">
+        <v>342</v>
+      </c>
+      <c r="B3" s="114" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="116" t="s">
+        <v>343</v>
+      </c>
+      <c r="D3" s="115" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="44"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="162" t="s">
+      <c r="B5" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="128"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="106" t="s">
+    <row r="6" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="132"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D6" s="102" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="58" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="162"/>
-      <c r="C5" s="106" t="s">
+      <c r="B7" s="166"/>
+      <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="104" t="s">
+      <c r="D7" s="104" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="58" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="162"/>
-      <c r="C6" s="106" t="s">
+      <c r="B8" s="166"/>
+      <c r="C8" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D8" s="104" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="162" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="166" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="79" t="s">
+      <c r="B9" s="166"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="162"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="166"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="162"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="110" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="166"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="110" t="s">
         <v>325</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D11" s="58" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="58" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="58" t="s">
+      <c r="B12" s="166"/>
+      <c r="C12" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="58"/>
+      <c r="D12" s="58"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="104" t="s">
+      <c r="B13" s="166"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="104" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B12" s="162"/>
-      <c r="C12" s="58" t="s">
+      <c r="B14" s="166"/>
+      <c r="C14" s="58" t="s">
         <v>332</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D14" s="100" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+    <row r="15" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="163" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="167" t="s">
         <v>237</v>
       </c>
-      <c r="B14" s="162" t="s">
+      <c r="B16" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="163"/>
-      <c r="B15" s="162"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="163"/>
-      <c r="B16" s="162"/>
       <c r="C16" s="58"/>
       <c r="D16" s="58" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="167"/>
+      <c r="B17" s="166"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="167"/>
+      <c r="B18" s="166"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="163"/>
-      <c r="B17" s="162"/>
-      <c r="C17" s="58" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="167"/>
+      <c r="B19" s="166"/>
+      <c r="C19" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D19" s="58" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="163"/>
-      <c r="B18" s="162"/>
-      <c r="C18" s="58" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="167"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="D18" s="100" t="s">
+      <c r="D20" s="100" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="144" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="162" t="s">
+      <c r="B21" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C21" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D21" s="100" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="144"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="148"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="144"/>
-      <c r="B21" s="162"/>
-      <c r="C21" s="108" t="s">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="148"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="108" t="s">
         <v>329</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D23" s="100" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="128" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="132" t="s">
         <v>222</v>
       </c>
-      <c r="B22" s="162" t="s">
+      <c r="B24" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="165" t="s">
+      <c r="C24" s="168" t="s">
         <v>239</v>
       </c>
-      <c r="D22" s="103" t="s">
+      <c r="D24" s="103" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="128"/>
-      <c r="B23" s="162"/>
-      <c r="C23" s="165"/>
-      <c r="D23" s="100" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="132"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="168"/>
+      <c r="D25" s="100" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="128"/>
-      <c r="B24" s="162"/>
-      <c r="C24" s="165" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="132"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="168" t="s">
         <v>240</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D26" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="128"/>
-      <c r="B25" s="162"/>
-      <c r="C25" s="165"/>
-      <c r="D25" s="61" t="s">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="132"/>
+      <c r="B27" s="166"/>
+      <c r="C27" s="168"/>
+      <c r="D27" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="128"/>
-      <c r="B26" s="162"/>
-      <c r="C26" s="105" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="132"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="105" t="s">
         <v>307</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D28" s="58" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="128"/>
-      <c r="B27" s="162"/>
-      <c r="C27" s="105">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="132"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="105">
         <v>2.1</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D29" s="58" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="128"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="105" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="132"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D30" s="58" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="137" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="141" t="s">
         <v>296</v>
       </c>
-      <c r="B29" s="162" t="s">
+      <c r="B31" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C31" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D31" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="137"/>
-      <c r="B30" s="162"/>
-      <c r="C30" s="61" t="s">
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="141"/>
+      <c r="B32" s="166"/>
+      <c r="C32" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D32" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
+    <row r="33" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="44"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="44"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="128" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="132" t="s">
         <v>260</v>
       </c>
-      <c r="B32" s="162" t="s">
+      <c r="B34" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="79" t="s">
+      <c r="C34" s="58"/>
+      <c r="D34" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="128"/>
-      <c r="B33" s="162"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="132"/>
+      <c r="B35" s="166"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="58" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="58" t="s">
         <v>334</v>
       </c>
-      <c r="B34" s="105" t="s">
+      <c r="B36" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C34" s="79" t="s">
+      <c r="C36" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D36" s="100" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="96" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B35" s="105" t="s">
+      <c r="B37" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C35" s="106" t="s">
+      <c r="C37" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="104" t="s">
+      <c r="D37" s="104" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="137" t="s">
+    <row r="38" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="162" t="s">
+      <c r="B38" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C38" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D36" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="137"/>
-      <c r="B37" s="162"/>
-      <c r="C37" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="D37" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="137"/>
-      <c r="B38" s="162"/>
-      <c r="C38" s="58" t="s">
-        <v>269</v>
       </c>
       <c r="D38" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="137"/>
-      <c r="B39" s="162"/>
-      <c r="C39" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D39" s="100" t="s">
-        <v>102</v>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="141"/>
+      <c r="B39" s="166"/>
+      <c r="C39" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D39" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="137"/>
-      <c r="B40" s="162"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="141"/>
+      <c r="B40" s="166"/>
       <c r="C40" s="58" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="137"/>
-      <c r="B41" s="162"/>
-      <c r="C41" s="58" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="141"/>
+      <c r="B41" s="166"/>
+      <c r="C41" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D41" s="100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="141"/>
+      <c r="B42" s="166"/>
+      <c r="C42" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="141"/>
+      <c r="B43" s="166"/>
+      <c r="C43" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D43" s="58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="137"/>
-      <c r="B42" s="162"/>
-      <c r="C42" s="100" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="141"/>
+      <c r="B44" s="166"/>
+      <c r="C44" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="D42" s="100" t="s">
+      <c r="D44" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="137"/>
-      <c r="B43" s="162"/>
-      <c r="C43" s="100" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="141"/>
+      <c r="B45" s="166"/>
+      <c r="C45" s="100" t="s">
         <v>302</v>
       </c>
-      <c r="D43" s="100" t="s">
+      <c r="D45" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="137"/>
-      <c r="B44" s="162"/>
-      <c r="C44" s="100" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="141"/>
+      <c r="B46" s="166"/>
+      <c r="C46" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="D44" s="100" t="s">
+      <c r="D46" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="137"/>
-      <c r="B45" s="162"/>
-      <c r="C45" s="107" t="s">
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="141"/>
+      <c r="B47" s="166"/>
+      <c r="C47" s="107" t="s">
         <v>244</v>
       </c>
-      <c r="D45" s="104" t="s">
+      <c r="D47" s="104" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="137"/>
-      <c r="B46" s="162"/>
-      <c r="C46" s="108" t="s">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="141"/>
+      <c r="B48" s="166"/>
+      <c r="C48" s="108" t="s">
         <v>311</v>
       </c>
-      <c r="D46" s="100" t="s">
+      <c r="D48" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="137"/>
-      <c r="B47" s="162"/>
-      <c r="C47" s="58" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="141"/>
+      <c r="B49" s="166"/>
+      <c r="C49" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="D47" s="58" t="s">
+      <c r="D49" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="137"/>
-      <c r="B48" s="162"/>
-      <c r="C48" s="100" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="141"/>
+      <c r="B50" s="166"/>
+      <c r="C50" s="100" t="s">
         <v>313</v>
       </c>
-      <c r="D48" s="100" t="s">
+      <c r="D50" s="100" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="137"/>
-      <c r="B49" s="162"/>
-      <c r="C49" s="100" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="141"/>
+      <c r="B51" s="166"/>
+      <c r="C51" s="100" t="s">
         <v>315</v>
       </c>
-      <c r="D49" s="100" t="s">
+      <c r="D51" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="137"/>
-      <c r="B50" s="162"/>
-      <c r="C50" s="100" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="141"/>
+      <c r="B52" s="166"/>
+      <c r="C52" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="D50" s="100" t="s">
+      <c r="D52" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="137"/>
-      <c r="B51" s="162"/>
-      <c r="C51" s="58" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="141"/>
+      <c r="B53" s="166"/>
+      <c r="C53" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D51" s="58" t="s">
+      <c r="D53" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="137"/>
-      <c r="B52" s="162"/>
-      <c r="C52" s="100" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="141"/>
+      <c r="B54" s="166"/>
+      <c r="C54" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="D52" s="100" t="s">
+      <c r="D54" s="100" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="137"/>
-      <c r="B53" s="162"/>
-      <c r="C53" s="100" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="141"/>
+      <c r="B55" s="166"/>
+      <c r="C55" s="100" t="s">
         <v>319</v>
-      </c>
-      <c r="D53" s="100" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="162"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="109" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="137"/>
-      <c r="B55" s="162"/>
-      <c r="C55" s="100" t="s">
-        <v>322</v>
       </c>
       <c r="D55" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="137"/>
-      <c r="B56" s="162"/>
-      <c r="C56" s="100" t="s">
-        <v>268</v>
-      </c>
-      <c r="D56" s="100" t="s">
-        <v>251</v>
+    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="141"/>
+      <c r="B56" s="166"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="109" t="s">
+        <v>321</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="137"/>
-      <c r="B57" s="162"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="141"/>
+      <c r="B57" s="166"/>
       <c r="C57" s="100" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="D57" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="137"/>
-      <c r="B58" s="162"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="141"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="100" t="s">
-        <v>340</v>
+        <v>268</v>
       </c>
       <c r="D58" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="137"/>
-      <c r="B59" s="162"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="141"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="100" t="s">
+        <v>339</v>
+      </c>
+      <c r="D59" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="141"/>
+      <c r="B60" s="166"/>
+      <c r="C60" s="100" t="s">
+        <v>340</v>
+      </c>
+      <c r="D60" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="141"/>
+      <c r="B61" s="166"/>
+      <c r="C61" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="D59" s="100" t="s">
+      <c r="D61" s="100" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="58"/>
-      <c r="B60" s="58"/>
-      <c r="C60" s="100" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="141"/>
+      <c r="B62" s="166"/>
+      <c r="C62" s="170" t="s">
+        <v>345</v>
+      </c>
+      <c r="D62" s="170" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="58"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="100" t="s">
         <v>338</v>
       </c>
-      <c r="D60" s="100" t="s">
+      <c r="D63" s="100" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="58" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="B61" s="106" t="s">
+      <c r="B64" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C61" s="58" t="s">
+      <c r="C64" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="100" t="s">
+      <c r="D64" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="58" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B62" s="106" t="s">
+      <c r="B65" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C62" s="58" t="s">
+      <c r="C65" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="100" t="s">
+      <c r="D65" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="39" t="s">
+    <row r="66" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="44"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="44"/>
     </row>
-    <row r="64" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="99"/>
-      <c r="B64" s="67"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="79" t="s">
+    <row r="67" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="99"/>
+      <c r="B67" s="67"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="162" t="s">
+    <row r="68" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="162" t="s">
+      <c r="B68" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C65" s="106" t="s">
+      <c r="C68" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="D65" s="58" t="s">
+      <c r="D68" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="162"/>
-      <c r="B66" s="162"/>
-      <c r="C66" s="106">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="166"/>
+      <c r="B69" s="166"/>
+      <c r="C69" s="106">
         <v>10.1</v>
       </c>
-      <c r="D66" s="58" t="s">
+      <c r="D69" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="162"/>
-      <c r="B67" s="162"/>
-      <c r="C67" s="106">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="166"/>
+      <c r="B70" s="166"/>
+      <c r="C70" s="106">
         <v>10.199999999999999</v>
       </c>
-      <c r="D67" s="58" t="s">
+      <c r="D70" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="162"/>
-      <c r="B68" s="162"/>
-      <c r="C68" s="111" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="166"/>
+      <c r="B71" s="166"/>
+      <c r="C71" s="111" t="s">
         <v>293</v>
       </c>
-      <c r="D68" s="101" t="s">
+      <c r="D71" s="101" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="128" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="132" t="s">
         <v>247</v>
       </c>
-      <c r="B69" s="162" t="s">
+      <c r="B72" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="162"/>
-      <c r="D69" s="164" t="s">
+      <c r="C72" s="166"/>
+      <c r="D72" s="169" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="128"/>
-      <c r="B70" s="162"/>
-      <c r="C70" s="162"/>
-      <c r="D70" s="164"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="132"/>
+      <c r="B73" s="166"/>
+      <c r="C73" s="166"/>
+      <c r="D73" s="169"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="104" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="B71" s="106" t="s">
+      <c r="B74" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C71" s="106" t="s">
+      <c r="C74" s="106" t="s">
         <v>250</v>
       </c>
-      <c r="D71" s="100" t="s">
+      <c r="D74" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="95" t="s">
+    <row r="75" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B72" s="39"/>
-      <c r="C72" s="98"/>
-      <c r="D72" s="98"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="98"/>
+      <c r="D75" s="98"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="58" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="B73" s="106" t="s">
+      <c r="B76" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C73" s="112" t="s">
+      <c r="C76" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D73" s="58" t="s">
+      <c r="D76" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="128" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="132" t="s">
         <v>285</v>
       </c>
-      <c r="B74" s="162" t="s">
+      <c r="B77" s="166" t="s">
         <v>234</v>
       </c>
-      <c r="C74" s="101" t="s">
+      <c r="C77" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="D74" s="58" t="s">
+      <c r="D77" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="128"/>
-      <c r="B75" s="162"/>
-      <c r="C75" s="58" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="132"/>
+      <c r="B78" s="166"/>
+      <c r="C78" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D75" s="100" t="s">
+      <c r="D78" s="100" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="128"/>
-      <c r="B76" s="162"/>
-      <c r="C76" s="112" t="s">
+    <row r="79" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="132"/>
+      <c r="B79" s="166"/>
+      <c r="C79" s="112" t="s">
         <v>286</v>
       </c>
-      <c r="D76" s="58" t="s">
+      <c r="D79" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="98" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="98"/>
-      <c r="C77" s="98"/>
-      <c r="D77" s="98"/>
+      <c r="B80" s="98"/>
+      <c r="C80" s="98"/>
+      <c r="D80" s="98"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="145" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="149" t="s">
         <v>58</v>
       </c>
-      <c r="B78" s="162" t="s">
+      <c r="B81" s="166" t="s">
         <v>271</v>
       </c>
-      <c r="C78" s="112" t="s">
+      <c r="C81" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D78" s="58" t="s">
+      <c r="D81" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="145"/>
-      <c r="B79" s="162"/>
-      <c r="C79" s="112" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="149"/>
+      <c r="B82" s="166"/>
+      <c r="C82" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D79" s="58" t="s">
+      <c r="D82" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="97" t="s">
+    <row r="83" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B80" s="106" t="s">
+      <c r="B83" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C80" s="61" t="s">
+      <c r="C83" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D80" s="58" t="s">
+      <c r="D83" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="58" t="s">
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="58" t="s">
         <v>291</v>
       </c>
-      <c r="B81" s="106" t="s">
+      <c r="B84" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C81" s="58"/>
-      <c r="D81" s="61" t="s">
+      <c r="C84" s="58"/>
+      <c r="D84" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="97" t="s">
+    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="106" t="s">
+      <c r="B85" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C82" s="61" t="s">
+      <c r="C85" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D82" s="58" t="s">
+      <c r="D85" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="98" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="98" t="s">
         <v>273</v>
       </c>
-      <c r="B83" s="98"/>
-      <c r="C83" s="98"/>
-      <c r="D83" s="98"/>
+      <c r="B86" s="98"/>
+      <c r="C86" s="98"/>
+      <c r="D86" s="98"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="58"/>
-      <c r="B84" s="106" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="58"/>
+      <c r="B87" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C84" s="58" t="s">
+      <c r="C87" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D84" s="100" t="s">
+      <c r="D87" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="98" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="98" t="s">
         <v>279</v>
       </c>
-      <c r="B85" s="98"/>
-      <c r="C85" s="98"/>
-      <c r="D85" s="98"/>
+      <c r="B88" s="98"/>
+      <c r="C88" s="98"/>
+      <c r="D88" s="98"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="58"/>
-      <c r="B86" s="106" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="58"/>
+      <c r="B89" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C86" s="58" t="s">
+      <c r="C89" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D86" s="100" t="s">
+      <c r="D89" s="100" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C69:C70"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A36:A59"/>
-    <mergeCell ref="B36:B59"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A38:A62"/>
+    <mergeCell ref="B38:B62"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B5:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Compression Guide and REST Integration guide updates"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owalsh01\IdeaProjects\paye-employers-documentation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMOD_Documentation\paye-employers-documentation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
+    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,20 @@
     <sheet name="v1.0Milestone 2" sheetId="3" r:id="rId3"/>
     <sheet name="1.0 Release Candidate 2" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$4</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="349">
   <si>
     <t>Document</t>
   </si>
@@ -2890,6 +2893,15 @@
   </si>
   <si>
     <t>code 1016</t>
+  </si>
+  <si>
+    <t>Accepted date formats added</t>
+  </si>
+  <si>
+    <t>Compressing a REST/JSON Request:</t>
+  </si>
+  <si>
+    <t>Note on the HTTP method override added</t>
   </si>
 </sst>
 </file>
@@ -3765,18 +3777,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3822,8 +3832,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3846,66 +3886,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3927,8 +3907,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3936,7 +3943,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4314,15 +4326,15 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4339,7 +4351,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="117" t="s">
         <v>25</v>
       </c>
@@ -4350,7 +4362,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -4367,7 +4379,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="117" t="s">
         <v>24</v>
       </c>
@@ -4378,7 +4390,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -4395,7 +4407,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -4412,7 +4424,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="120" t="s">
         <v>3</v>
       </c>
@@ -4429,7 +4441,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="121"/>
       <c r="B8" s="124"/>
       <c r="C8" s="11" t="s">
@@ -4442,7 +4454,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="121"/>
       <c r="B9" s="124"/>
       <c r="C9" s="11" t="s">
@@ -4455,7 +4467,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="121"/>
       <c r="B10" s="124"/>
       <c r="C10" s="11" t="s">
@@ -4468,7 +4480,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="121"/>
       <c r="B11" s="124"/>
       <c r="C11" s="11" t="s">
@@ -4481,7 +4493,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="122"/>
       <c r="B12" s="125"/>
       <c r="C12" s="11" t="s">
@@ -4494,7 +4506,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="128" t="s">
         <v>74</v>
       </c>
@@ -4511,7 +4523,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="129"/>
       <c r="B14" s="125"/>
       <c r="C14" s="11" t="s">
@@ -4524,7 +4536,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4541,7 +4553,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4558,7 +4570,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="117" t="s">
         <v>28</v>
       </c>
@@ -4569,7 +4581,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4586,7 +4598,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4603,7 +4615,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="117" t="s">
         <v>29</v>
       </c>
@@ -4614,7 +4626,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="130" t="s">
         <v>31</v>
       </c>
@@ -4631,7 +4643,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="131"/>
       <c r="B22" s="125"/>
       <c r="C22" s="27" t="s">
@@ -4641,7 +4653,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4655,7 +4667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="117" t="s">
         <v>40</v>
       </c>
@@ -4663,7 +4675,7 @@
       <c r="C24" s="118"/>
       <c r="D24" s="119"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="126" t="s">
         <v>41</v>
       </c>
@@ -4680,7 +4692,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="121"/>
       <c r="B26" s="124"/>
       <c r="C26" s="11" t="s">
@@ -4693,7 +4705,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="121"/>
       <c r="B27" s="124"/>
       <c r="C27" s="11" t="s">
@@ -4706,7 +4718,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="121"/>
       <c r="B28" s="124"/>
       <c r="C28" s="21" t="s">
@@ -4719,7 +4731,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="121"/>
       <c r="B29" s="124"/>
       <c r="C29" s="11" t="s">
@@ -4732,7 +4744,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="121"/>
       <c r="B30" s="124"/>
       <c r="C30" s="11" t="s">
@@ -4745,7 +4757,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="121"/>
       <c r="B31" s="124"/>
       <c r="C31" s="11" t="s">
@@ -4758,7 +4770,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="122"/>
       <c r="B32" s="125"/>
       <c r="C32" s="11" t="s">
@@ -4771,7 +4783,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4785,7 +4797,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4799,7 +4811,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4813,7 +4825,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4827,7 +4839,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4841,7 +4853,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4855,7 +4867,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4869,7 +4881,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4883,7 +4895,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="117" t="s">
         <v>56</v>
       </c>
@@ -4891,7 +4903,7 @@
       <c r="C41" s="118"/>
       <c r="D41" s="119"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4905,7 +4917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4919,7 +4931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4933,7 +4945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4949,7 +4961,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4959,7 +4971,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4994,15 +5006,15 @@
       <selection activeCell="A30" sqref="A30:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -5016,7 +5028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -5024,7 +5036,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -5036,7 +5048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -5048,7 +5060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -5060,7 +5072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
@@ -5068,11 +5080,11 @@
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="147" t="s">
+    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="146" t="s">
+      <c r="B7" s="133" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5082,9 +5094,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="147"/>
-      <c r="B8" s="146"/>
+    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="132"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5092,9 +5104,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
-      <c r="B9" s="146"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="132"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5102,9 +5114,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="147"/>
-      <c r="B10" s="146"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="132"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5112,9 +5124,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="147"/>
-      <c r="B11" s="146"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="132"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5122,9 +5134,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="147"/>
-      <c r="B12" s="146"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="132"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5132,11 +5144,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="149" t="s">
+    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="146" t="s">
+      <c r="B13" s="133" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5146,9 +5158,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="149"/>
-      <c r="B14" s="146"/>
+    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="135"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5156,9 +5168,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="149"/>
-      <c r="B15" s="146"/>
+    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="135"/>
+      <c r="B15" s="133"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5166,11 +5178,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="132" t="s">
+    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="137" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5180,9 +5192,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="132"/>
-      <c r="B17" s="141"/>
+    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="136"/>
+      <c r="B17" s="137"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5190,9 +5202,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="132"/>
-      <c r="B18" s="141"/>
+    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="136"/>
+      <c r="B18" s="137"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5200,9 +5212,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="132"/>
-      <c r="B19" s="141"/>
+    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="136"/>
+      <c r="B19" s="137"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5210,9 +5222,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="132"/>
-      <c r="B20" s="141"/>
+    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5220,9 +5232,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="132"/>
-      <c r="B21" s="141"/>
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="136"/>
+      <c r="B21" s="137"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5230,9 +5242,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="132"/>
-      <c r="B22" s="141"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="136"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5240,9 +5252,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="132"/>
-      <c r="B23" s="141"/>
+    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="136"/>
+      <c r="B23" s="137"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5250,27 +5262,27 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="132"/>
-      <c r="B24" s="141"/>
-      <c r="C24" s="132" t="s">
+    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="136"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="136" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="133" t="s">
+      <c r="D24" s="143" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="132"/>
-      <c r="B25" s="141"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="133"/>
+    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="136"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="143"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="147" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="132" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="146" t="s">
+      <c r="B26" s="133" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5280,15 +5292,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
-      <c r="B27" s="146"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="132"/>
+      <c r="B27" s="133"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -5300,7 +5312,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -5308,29 +5320,29 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="148" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="146" t="s">
+      <c r="B30" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="132" t="s">
+      <c r="C30" s="136" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="136" t="s">
+      <c r="D30" s="146" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="148"/>
-      <c r="B31" s="146"/>
-      <c r="C31" s="132"/>
-      <c r="D31" s="136"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="134"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="146"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="148"/>
-      <c r="B32" s="146"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="134"/>
+      <c r="B32" s="133"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5338,9 +5350,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="148"/>
-      <c r="B33" s="146"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="134"/>
+      <c r="B33" s="133"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5348,9 +5360,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="148"/>
-      <c r="B34" s="146"/>
+    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="134"/>
+      <c r="B34" s="133"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5358,9 +5370,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="148"/>
-      <c r="B35" s="146"/>
+    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="134"/>
+      <c r="B35" s="133"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5368,9 +5380,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="148"/>
-      <c r="B36" s="146"/>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="134"/>
+      <c r="B36" s="133"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5378,27 +5390,27 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="148"/>
-      <c r="B37" s="146"/>
-      <c r="C37" s="137" t="s">
+    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="134"/>
+      <c r="B37" s="133"/>
+      <c r="C37" s="147" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="139" t="s">
+      <c r="D37" s="149" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="148"/>
-      <c r="B38" s="146"/>
-      <c r="C38" s="138"/>
-      <c r="D38" s="139"/>
+    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="134"/>
+      <c r="B38" s="133"/>
+      <c r="C38" s="148"/>
+      <c r="D38" s="149"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="147" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="146" t="s">
+      <c r="B39" s="133" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5408,15 +5420,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="147"/>
-      <c r="B40" s="146"/>
+    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="132"/>
+      <c r="B40" s="133"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -5428,7 +5440,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
@@ -5436,11 +5448,11 @@
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="148" t="s">
+    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="146" t="s">
+      <c r="B43" s="133" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5448,9 +5460,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="148"/>
-      <c r="B44" s="146"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="134"/>
+      <c r="B44" s="133"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5458,11 +5470,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="143" t="s">
+    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="146" t="s">
+      <c r="B45" s="133" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5470,9 +5482,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="146"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="141"/>
+      <c r="B46" s="133"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5480,9 +5492,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="146"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="141"/>
+      <c r="B47" s="133"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5490,9 +5502,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="145"/>
-      <c r="B48" s="146"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="142"/>
+      <c r="B48" s="133"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5500,11 +5512,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="141" t="s">
+    <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A49" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="141" t="s">
+      <c r="B49" s="137" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9607,9 +9619,9 @@
       <c r="XEY49" s="42"/>
       <c r="XFC49" s="42"/>
     </row>
-    <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="141"/>
-      <c r="B50" s="141"/>
+    <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="137"/>
+      <c r="B50" s="137"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13712,9 +13724,9 @@
       <c r="XEY50" s="42"/>
       <c r="XFC50" s="42"/>
     </row>
-    <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="141"/>
-      <c r="B51" s="141"/>
+    <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A51" s="137"/>
+      <c r="B51" s="137"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17817,9 +17829,9 @@
       <c r="XEY51" s="42"/>
       <c r="XFC51" s="42"/>
     </row>
-    <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="141"/>
-      <c r="B52" s="141"/>
+    <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A52" s="137"/>
+      <c r="B52" s="137"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21922,13 +21934,13 @@
       <c r="XEY52" s="42"/>
       <c r="XFC52" s="42"/>
     </row>
-    <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="141"/>
-      <c r="B53" s="141"/>
-      <c r="C53" s="135" t="s">
+    <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A53" s="137"/>
+      <c r="B53" s="137"/>
+      <c r="C53" s="145" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="136" t="s">
+      <c r="D53" s="146" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26027,11 +26039,11 @@
       <c r="XEY53" s="42"/>
       <c r="XFC53" s="42"/>
     </row>
-    <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="141"/>
-      <c r="B54" s="141"/>
-      <c r="C54" s="135"/>
-      <c r="D54" s="136"/>
+    <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="137"/>
+      <c r="B54" s="137"/>
+      <c r="C54" s="145"/>
+      <c r="D54" s="146"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30128,7 +30140,7 @@
       <c r="XEY54" s="42"/>
       <c r="XFC54" s="42"/>
     </row>
-    <row r="55" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
@@ -30136,7 +30148,7 @@
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
     </row>
-    <row r="56" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -30148,11 +30160,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="140" t="s">
+    <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A57" s="138" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="141" t="s">
+      <c r="B57" s="137" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30162,9 +30174,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="140"/>
-      <c r="B58" s="141"/>
+    <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="138"/>
+      <c r="B58" s="137"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30172,9 +30184,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="140"/>
-      <c r="B59" s="141"/>
+    <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A59" s="138"/>
+      <c r="B59" s="137"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30182,9 +30194,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="140"/>
-      <c r="B60" s="141"/>
+    <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="138"/>
+      <c r="B60" s="137"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30192,9 +30204,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="140"/>
-      <c r="B61" s="141"/>
+    <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A61" s="138"/>
+      <c r="B61" s="137"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30202,9 +30214,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="140"/>
-      <c r="B62" s="141"/>
+    <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A62" s="138"/>
+      <c r="B62" s="137"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30212,9 +30224,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="140"/>
-      <c r="B63" s="141"/>
+    <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A63" s="138"/>
+      <c r="B63" s="137"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30222,17 +30234,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="140"/>
-      <c r="B64" s="141"/>
+    <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+      <c r="A64" s="138"/>
+      <c r="B64" s="137"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="140"/>
-      <c r="B65" s="141"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="138"/>
+      <c r="B65" s="137"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30240,17 +30252,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="140"/>
-      <c r="B66" s="141"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="138"/>
+      <c r="B66" s="137"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="140"/>
-      <c r="B67" s="141"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="138"/>
+      <c r="B67" s="137"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30258,9 +30270,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="140"/>
-      <c r="B68" s="141"/>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="138"/>
+      <c r="B68" s="137"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30268,9 +30280,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="140"/>
-      <c r="B69" s="141"/>
+    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="138"/>
+      <c r="B69" s="137"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30278,9 +30290,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="140"/>
-      <c r="B70" s="141"/>
+    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="138"/>
+      <c r="B70" s="137"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30288,9 +30300,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="140"/>
-      <c r="B71" s="141"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="138"/>
+      <c r="B71" s="137"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30298,9 +30310,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="140"/>
-      <c r="B72" s="141"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="138"/>
+      <c r="B72" s="137"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30308,17 +30320,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="140"/>
-      <c r="B73" s="141"/>
+    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="138"/>
+      <c r="B73" s="137"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="140"/>
-      <c r="B74" s="141"/>
+    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="138"/>
+      <c r="B74" s="137"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30326,21 +30338,21 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="140"/>
-      <c r="B75" s="141"/>
-      <c r="C75" s="134"/>
-      <c r="D75" s="142" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="138"/>
+      <c r="B75" s="137"/>
+      <c r="C75" s="144"/>
+      <c r="D75" s="139" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="140"/>
-      <c r="B76" s="141"/>
-      <c r="C76" s="134"/>
-      <c r="D76" s="142"/>
+    <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="138"/>
+      <c r="B76" s="137"/>
+      <c r="C76" s="144"/>
+      <c r="D76" s="139"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
@@ -30348,13 +30360,13 @@
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -30362,8 +30374,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30372,13 +30384,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30393,22 +30421,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30423,15 +30435,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
-    <col min="4" max="4" width="80.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30445,7 +30457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -30453,7 +30465,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
@@ -30461,11 +30473,11 @@
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="147" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="133" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30475,139 +30487,139 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="147"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="157" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="132"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="159" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="156" t="s">
+      <c r="D5" s="158" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="156"/>
+    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="132"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="159"/>
+      <c r="D6" s="158"/>
     </row>
-    <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="147"/>
-      <c r="B7" s="146"/>
+    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="132"/>
+      <c r="B7" s="133"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="147"/>
-      <c r="B8" s="146"/>
+    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="132"/>
+      <c r="B8" s="133"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
-      <c r="B9" s="146"/>
+    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="132"/>
+      <c r="B9" s="133"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149" t="s">
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="146" t="s">
+      <c r="B10" s="133" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="159"/>
-      <c r="D10" s="156" t="s">
+      <c r="C10" s="157"/>
+      <c r="D10" s="158" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
-      <c r="B11" s="146"/>
-      <c r="C11" s="159"/>
-      <c r="D11" s="156"/>
+    <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="135"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="157"/>
+      <c r="D11" s="158"/>
     </row>
-    <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="146"/>
-      <c r="C12" s="159"/>
-      <c r="D12" s="156"/>
+    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="135"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="157"/>
+      <c r="D12" s="158"/>
     </row>
-    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="132" t="s">
+    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="141" t="s">
+      <c r="B13" s="137" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="156" t="s">
+      <c r="C13" s="160"/>
+      <c r="D13" s="158" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="132"/>
-      <c r="B14" s="141"/>
-      <c r="C14" s="158"/>
-      <c r="D14" s="156"/>
+    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="136"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="160"/>
+      <c r="D14" s="158"/>
     </row>
-    <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="132"/>
-      <c r="B15" s="141"/>
-      <c r="C15" s="158"/>
+    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="136"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="160"/>
       <c r="D15" s="49"/>
     </row>
-    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="132"/>
-      <c r="B16" s="141"/>
-      <c r="C16" s="158"/>
+    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="136"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="160"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="132"/>
-      <c r="B17" s="141"/>
-      <c r="C17" s="158"/>
+    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="136"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="160"/>
       <c r="D17" s="49"/>
     </row>
-    <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="132"/>
-      <c r="B18" s="141"/>
-      <c r="C18" s="158"/>
+    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="136"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="160"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="132"/>
-      <c r="B19" s="141"/>
-      <c r="C19" s="158"/>
+    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="136"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="160"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="132"/>
-      <c r="B20" s="141"/>
-      <c r="C20" s="158"/>
+    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="160"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="132"/>
-      <c r="B21" s="141"/>
-      <c r="C21" s="158"/>
+    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="136"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="160"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="132"/>
-      <c r="B22" s="141"/>
-      <c r="C22" s="158"/>
+    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="136"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="160"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="132"/>
-      <c r="B23" s="141"/>
-      <c r="C23" s="158"/>
+    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="136"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="160"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
@@ -30621,7 +30633,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30635,7 +30647,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30647,7 +30659,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
@@ -30655,7 +30667,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30669,7 +30681,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="85"/>
       <c r="B29" s="84"/>
       <c r="C29" s="70" t="s">
@@ -30679,7 +30691,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30689,7 +30701,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30699,11 +30711,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="150" t="s">
+    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="161" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="164" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30713,27 +30725,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="151"/>
-      <c r="B33" s="154"/>
+    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="162"/>
+      <c r="B33" s="165"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
-    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="151"/>
-      <c r="B34" s="154"/>
+    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="162"/>
+      <c r="B34" s="165"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="151"/>
-      <c r="B35" s="154"/>
+    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="162"/>
+      <c r="B35" s="165"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
-    <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152"/>
-      <c r="B36" s="155"/>
+    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="163"/>
+      <c r="B36" s="166"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30741,7 +30753,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
         <v>27</v>
       </c>
@@ -30753,7 +30765,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
@@ -30761,11 +30773,11 @@
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="148" t="s">
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="146" t="s">
+      <c r="B39" s="133" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30775,9 +30787,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="148"/>
-      <c r="B40" s="146"/>
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="134"/>
+      <c r="B40" s="133"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30785,87 +30797,87 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="147" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="146" t="s">
+      <c r="B41" s="133" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="159" t="s">
+      <c r="C41" s="157" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="132" t="s">
+      <c r="D41" s="136" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="147"/>
-      <c r="B42" s="146"/>
-      <c r="C42" s="159"/>
-      <c r="D42" s="132"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="132"/>
+      <c r="B42" s="133"/>
+      <c r="C42" s="157"/>
+      <c r="D42" s="136"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="147"/>
-      <c r="B43" s="146"/>
-      <c r="C43" s="159" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="132"/>
+      <c r="B43" s="133"/>
+      <c r="C43" s="157" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="142" t="s">
+      <c r="D43" s="139" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="147"/>
-      <c r="B44" s="146"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="142"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="132"/>
+      <c r="B44" s="133"/>
+      <c r="C44" s="157"/>
+      <c r="D44" s="139"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="140" t="s">
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="141" t="s">
+      <c r="B45" s="137" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="163"/>
+      <c r="C45" s="153"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="140"/>
-      <c r="B46" s="141"/>
-      <c r="C46" s="164"/>
-      <c r="D46" s="160" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="138"/>
+      <c r="B46" s="137"/>
+      <c r="C46" s="154"/>
+      <c r="D46" s="150" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="140"/>
-      <c r="B47" s="141"/>
-      <c r="C47" s="164"/>
-      <c r="D47" s="161"/>
+    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="138"/>
+      <c r="B47" s="137"/>
+      <c r="C47" s="154"/>
+      <c r="D47" s="151"/>
     </row>
-    <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="140"/>
-      <c r="B48" s="141"/>
-      <c r="C48" s="165"/>
-      <c r="D48" s="161"/>
+    <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="138"/>
+      <c r="B48" s="137"/>
+      <c r="C48" s="155"/>
+      <c r="D48" s="151"/>
     </row>
-    <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="140"/>
-      <c r="B49" s="141"/>
-      <c r="C49" s="135"/>
-      <c r="D49" s="161"/>
+    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="138"/>
+      <c r="B49" s="137"/>
+      <c r="C49" s="145"/>
+      <c r="D49" s="151"/>
     </row>
-    <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="140"/>
-      <c r="B50" s="141"/>
-      <c r="C50" s="135"/>
-      <c r="D50" s="162"/>
+    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="138"/>
+      <c r="B50" s="137"/>
+      <c r="C50" s="145"/>
+      <c r="D50" s="152"/>
     </row>
-    <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
@@ -30873,7 +30885,7 @@
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
     </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
@@ -30885,11 +30897,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="141" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="141" t="s">
+      <c r="B53" s="137" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30899,9 +30911,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="141"/>
-      <c r="B54" s="141"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="137"/>
+      <c r="B54" s="137"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30909,9 +30921,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="141"/>
-      <c r="B55" s="141"/>
+    <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="137"/>
+      <c r="B55" s="137"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30919,27 +30931,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="141"/>
-      <c r="B56" s="141"/>
-      <c r="C56" s="166" t="s">
+    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="137"/>
+      <c r="B56" s="137"/>
+      <c r="C56" s="156" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="141"/>
-      <c r="B57" s="141"/>
-      <c r="C57" s="166"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="137"/>
+      <c r="B57" s="137"/>
+      <c r="C57" s="156"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="141"/>
-      <c r="B58" s="141"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="137"/>
+      <c r="B58" s="137"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30947,9 +30959,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="141"/>
-      <c r="B59" s="141"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="137"/>
+      <c r="B59" s="137"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30957,122 +30969,139 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="141"/>
-      <c r="B60" s="141"/>
-      <c r="C60" s="166" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="137"/>
+      <c r="B60" s="137"/>
+      <c r="C60" s="156" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="141"/>
-      <c r="B61" s="141"/>
-      <c r="C61" s="166"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="137"/>
+      <c r="B61" s="137"/>
+      <c r="C61" s="156"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="141"/>
-      <c r="B62" s="141"/>
-      <c r="C62" s="166"/>
+    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="137"/>
+      <c r="B62" s="137"/>
+      <c r="C62" s="156"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="141"/>
-      <c r="B63" s="141"/>
-      <c r="C63" s="159" t="s">
+    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="137"/>
+      <c r="B63" s="137"/>
+      <c r="C63" s="157" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="141"/>
-      <c r="B64" s="141"/>
-      <c r="C64" s="159"/>
-      <c r="D64" s="142" t="s">
+    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="137"/>
+      <c r="B64" s="137"/>
+      <c r="C64" s="157"/>
+      <c r="D64" s="139" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="141"/>
-      <c r="B65" s="141"/>
-      <c r="C65" s="159"/>
-      <c r="D65" s="142"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="137"/>
+      <c r="B65" s="137"/>
+      <c r="C65" s="157"/>
+      <c r="D65" s="139"/>
     </row>
-    <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="141"/>
-      <c r="B66" s="141"/>
-      <c r="C66" s="159"/>
-      <c r="D66" s="142"/>
+    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="137"/>
+      <c r="B66" s="137"/>
+      <c r="C66" s="157"/>
+      <c r="D66" s="139"/>
     </row>
-    <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="141"/>
-      <c r="B67" s="141"/>
-      <c r="C67" s="159"/>
-      <c r="D67" s="142"/>
+    <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="137"/>
+      <c r="B67" s="137"/>
+      <c r="C67" s="157"/>
+      <c r="D67" s="139"/>
     </row>
-    <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31089,23 +31118,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31114,21 +31126,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="B6" sqref="B6:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -31142,7 +31154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>341</v>
       </c>
@@ -31150,871 +31162,865 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="113" t="s">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="170" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="170" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="114" t="s">
         <v>343</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="113" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="170"/>
+      <c r="B4" s="170"/>
+      <c r="C4" s="114" t="s">
+        <v>347</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="44"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="44"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="132" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="166" t="s">
+      <c r="B6" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58" t="s">
+      <c r="C6" s="58"/>
+      <c r="D6" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="132"/>
-      <c r="B6" s="166"/>
-      <c r="C6" s="106" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="102" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="166"/>
+    <row r="7" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="136"/>
+      <c r="B7" s="156"/>
       <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="102" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="156"/>
+      <c r="C8" s="106" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="104" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B8" s="166"/>
-      <c r="C8" s="106" t="s">
+      <c r="B9" s="156"/>
+      <c r="C9" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D9" s="104" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="166" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="156" t="s">
         <v>275</v>
       </c>
-      <c r="B9" s="166"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="79" t="s">
+      <c r="B10" s="156"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="166"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="156"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
-      <c r="B11" s="166"/>
-      <c r="C11" s="110" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="156"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="110" t="s">
         <v>325</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D12" s="58" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B12" s="166"/>
-      <c r="C12" s="58" t="s">
+      <c r="B13" s="156"/>
+      <c r="C13" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="58"/>
+      <c r="D13" s="58"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="166"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="104" t="s">
+      <c r="B14" s="156"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="104" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="100" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B14" s="166"/>
-      <c r="C14" s="58" t="s">
+      <c r="B15" s="156"/>
+      <c r="C15" s="58" t="s">
         <v>332</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D15" s="100" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+    <row r="16" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="167" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="169" t="s">
         <v>237</v>
       </c>
-      <c r="B16" s="166" t="s">
+      <c r="B17" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="167"/>
-      <c r="B17" s="166"/>
       <c r="C17" s="58"/>
       <c r="D17" s="58" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="167"/>
-      <c r="B18" s="166"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="169"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="58"/>
       <c r="D18" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="169"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="167"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="58" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="169"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D20" s="58" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="167"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="58" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="169"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D21" s="100" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="148" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="166" t="s">
+      <c r="B22" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C22" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D22" s="100" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="148"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="134"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="148"/>
-      <c r="B23" s="166"/>
-      <c r="C23" s="108" t="s">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="134"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="108" t="s">
         <v>329</v>
       </c>
-      <c r="D23" s="100" t="s">
+      <c r="D24" s="100" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="132" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="156" t="s">
         <v>222</v>
       </c>
-      <c r="B24" s="166" t="s">
+      <c r="B25" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C24" s="168" t="s">
+      <c r="C25" s="167" t="s">
         <v>239</v>
       </c>
-      <c r="D24" s="103" t="s">
+      <c r="D25" s="103" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="132"/>
-      <c r="B25" s="166"/>
-      <c r="C25" s="168"/>
-      <c r="D25" s="100" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="156"/>
+      <c r="B26" s="156"/>
+      <c r="C26" s="167"/>
+      <c r="D26" s="100" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="132"/>
-      <c r="B26" s="166"/>
-      <c r="C26" s="168" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="156"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="167" t="s">
         <v>240</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D27" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="132"/>
-      <c r="B27" s="166"/>
-      <c r="C27" s="168"/>
-      <c r="D27" s="61" t="s">
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="156"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="132"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="105" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="156"/>
+      <c r="B29" s="156"/>
+      <c r="C29" s="105" t="s">
         <v>307</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D29" s="58" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="132"/>
-      <c r="B29" s="166"/>
-      <c r="C29" s="105">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="156"/>
+      <c r="B30" s="156"/>
+      <c r="C30" s="105">
         <v>2.1</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D30" s="58" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="132"/>
-      <c r="B30" s="166"/>
-      <c r="C30" s="105" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="156"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D31" s="58" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="141" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="156"/>
+      <c r="B32" s="156"/>
+      <c r="C32" s="115" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" s="116" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="137" t="s">
         <v>296</v>
       </c>
-      <c r="B31" s="166" t="s">
+      <c r="B33" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C33" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D33" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="141"/>
-      <c r="B32" s="166"/>
-      <c r="C32" s="61" t="s">
+    <row r="34" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="137"/>
+      <c r="B34" s="156"/>
+      <c r="C34" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D34" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+    <row r="35" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="44"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="44"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="132" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="136" t="s">
         <v>260</v>
       </c>
-      <c r="B34" s="166" t="s">
+      <c r="B36" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="79" t="s">
+      <c r="C36" s="58"/>
+      <c r="D36" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="132"/>
-      <c r="B35" s="166"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="136"/>
+      <c r="B37" s="156"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="58" t="s">
         <v>334</v>
       </c>
-      <c r="B36" s="105" t="s">
+      <c r="B38" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="79" t="s">
+      <c r="C38" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D36" s="100" t="s">
+      <c r="D38" s="100" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="96" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B37" s="105" t="s">
+      <c r="B39" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="106" t="s">
+      <c r="C39" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="104" t="s">
+      <c r="D39" s="104" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="141" t="s">
+    <row r="40" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="166" t="s">
+      <c r="B40" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C38" s="58" t="s">
+      <c r="C40" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D38" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="141"/>
-      <c r="B39" s="166"/>
-      <c r="C39" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="D39" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="141"/>
-      <c r="B40" s="166"/>
-      <c r="C40" s="58" t="s">
-        <v>269</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="141"/>
-      <c r="B41" s="166"/>
-      <c r="C41" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D41" s="100" t="s">
-        <v>102</v>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="137"/>
+      <c r="B41" s="156"/>
+      <c r="C41" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="141"/>
-      <c r="B42" s="166"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="137"/>
+      <c r="B42" s="156"/>
       <c r="C42" s="58" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="141"/>
-      <c r="B43" s="166"/>
-      <c r="C43" s="58" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="137"/>
+      <c r="B43" s="156"/>
+      <c r="C43" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D43" s="100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="137"/>
+      <c r="B44" s="156"/>
+      <c r="C44" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="137"/>
+      <c r="B45" s="156"/>
+      <c r="C45" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D45" s="58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="141"/>
-      <c r="B44" s="166"/>
-      <c r="C44" s="100" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="137"/>
+      <c r="B46" s="156"/>
+      <c r="C46" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="D44" s="100" t="s">
+      <c r="D46" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="141"/>
-      <c r="B45" s="166"/>
-      <c r="C45" s="100" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="137"/>
+      <c r="B47" s="156"/>
+      <c r="C47" s="100" t="s">
         <v>302</v>
       </c>
-      <c r="D45" s="100" t="s">
+      <c r="D47" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="141"/>
-      <c r="B46" s="166"/>
-      <c r="C46" s="100" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="137"/>
+      <c r="B48" s="156"/>
+      <c r="C48" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="D46" s="100" t="s">
+      <c r="D48" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="141"/>
-      <c r="B47" s="166"/>
-      <c r="C47" s="107" t="s">
+    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="137"/>
+      <c r="B49" s="156"/>
+      <c r="C49" s="107" t="s">
         <v>244</v>
       </c>
-      <c r="D47" s="104" t="s">
+      <c r="D49" s="104" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="141"/>
-      <c r="B48" s="166"/>
-      <c r="C48" s="108" t="s">
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="137"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="108" t="s">
         <v>311</v>
       </c>
-      <c r="D48" s="100" t="s">
+      <c r="D50" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="141"/>
-      <c r="B49" s="166"/>
-      <c r="C49" s="58" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="137"/>
+      <c r="B51" s="156"/>
+      <c r="C51" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="D49" s="58" t="s">
+      <c r="D51" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="141"/>
-      <c r="B50" s="166"/>
-      <c r="C50" s="100" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="137"/>
+      <c r="B52" s="156"/>
+      <c r="C52" s="100" t="s">
         <v>313</v>
       </c>
-      <c r="D50" s="100" t="s">
+      <c r="D52" s="100" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="141"/>
-      <c r="B51" s="166"/>
-      <c r="C51" s="100" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="137"/>
+      <c r="B53" s="156"/>
+      <c r="C53" s="100" t="s">
         <v>315</v>
       </c>
-      <c r="D51" s="100" t="s">
+      <c r="D53" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="141"/>
-      <c r="B52" s="166"/>
-      <c r="C52" s="100" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="137"/>
+      <c r="B54" s="156"/>
+      <c r="C54" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="D52" s="100" t="s">
+      <c r="D54" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="141"/>
-      <c r="B53" s="166"/>
-      <c r="C53" s="58" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="137"/>
+      <c r="B55" s="156"/>
+      <c r="C55" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D53" s="58" t="s">
+      <c r="D55" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="141"/>
-      <c r="B54" s="166"/>
-      <c r="C54" s="100" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="137"/>
+      <c r="B56" s="156"/>
+      <c r="C56" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="D54" s="100" t="s">
+      <c r="D56" s="100" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="141"/>
-      <c r="B55" s="166"/>
-      <c r="C55" s="100" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="137"/>
+      <c r="B57" s="156"/>
+      <c r="C57" s="100" t="s">
         <v>319</v>
-      </c>
-      <c r="D55" s="100" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="141"/>
-      <c r="B56" s="166"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="109" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="141"/>
-      <c r="B57" s="166"/>
-      <c r="C57" s="100" t="s">
-        <v>322</v>
       </c>
       <c r="D57" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="141"/>
-      <c r="B58" s="166"/>
-      <c r="C58" s="100" t="s">
-        <v>268</v>
-      </c>
-      <c r="D58" s="100" t="s">
-        <v>251</v>
+    <row r="58" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="137"/>
+      <c r="B58" s="156"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="109" t="s">
+        <v>321</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="141"/>
-      <c r="B59" s="166"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="137"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="100" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="D59" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="141"/>
-      <c r="B60" s="166"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="137"/>
+      <c r="B60" s="156"/>
       <c r="C60" s="100" t="s">
-        <v>340</v>
+        <v>268</v>
       </c>
       <c r="D60" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="141"/>
-      <c r="B61" s="166"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="137"/>
+      <c r="B61" s="156"/>
       <c r="C61" s="100" t="s">
+        <v>339</v>
+      </c>
+      <c r="D61" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="137"/>
+      <c r="B62" s="156"/>
+      <c r="C62" s="100" t="s">
+        <v>340</v>
+      </c>
+      <c r="D62" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="137"/>
+      <c r="B63" s="156"/>
+      <c r="C63" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="D61" s="100" t="s">
+      <c r="D63" s="100" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="141"/>
-      <c r="B62" s="166"/>
-      <c r="C62" s="170" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="137"/>
+      <c r="B64" s="156"/>
+      <c r="C64" s="116" t="s">
         <v>345</v>
       </c>
-      <c r="D62" s="170" t="s">
+      <c r="D64" s="116" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="58"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="100" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="58"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="100" t="s">
         <v>338</v>
       </c>
-      <c r="D63" s="100" t="s">
+      <c r="D65" s="100" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="58" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="B64" s="106" t="s">
+      <c r="B66" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C64" s="58" t="s">
+      <c r="C66" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D64" s="100" t="s">
+      <c r="D66" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="58" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B65" s="106" t="s">
+      <c r="B67" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C65" s="58" t="s">
+      <c r="C67" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D65" s="100" t="s">
+      <c r="D67" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="39" t="s">
+    <row r="68" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="44"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="44"/>
     </row>
-    <row r="67" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="99"/>
-      <c r="B67" s="67"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="79" t="s">
+    <row r="69" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="99"/>
+      <c r="B69" s="67"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="166" t="s">
+    <row r="70" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="166" t="s">
+      <c r="B70" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C68" s="106" t="s">
+      <c r="C70" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="D68" s="58" t="s">
+      <c r="D70" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="166"/>
-      <c r="B69" s="166"/>
-      <c r="C69" s="106">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="156"/>
+      <c r="B71" s="156"/>
+      <c r="C71" s="106">
         <v>10.1</v>
       </c>
-      <c r="D69" s="58" t="s">
+      <c r="D71" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="166"/>
-      <c r="B70" s="166"/>
-      <c r="C70" s="106">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="156"/>
+      <c r="B72" s="156"/>
+      <c r="C72" s="106">
         <v>10.199999999999999</v>
       </c>
-      <c r="D70" s="58" t="s">
+      <c r="D72" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="166"/>
-      <c r="B71" s="166"/>
-      <c r="C71" s="111" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="156"/>
+      <c r="B73" s="156"/>
+      <c r="C73" s="111" t="s">
         <v>293</v>
       </c>
-      <c r="D71" s="101" t="s">
+      <c r="D73" s="101" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="132" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="136" t="s">
         <v>247</v>
       </c>
-      <c r="B72" s="166" t="s">
+      <c r="B74" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C72" s="166"/>
-      <c r="D72" s="169" t="s">
+      <c r="C74" s="156"/>
+      <c r="D74" s="168" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="132"/>
-      <c r="B73" s="166"/>
-      <c r="C73" s="166"/>
-      <c r="D73" s="169"/>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="136"/>
+      <c r="B75" s="156"/>
+      <c r="C75" s="156"/>
+      <c r="D75" s="168"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="104" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="104" t="s">
         <v>262</v>
-      </c>
-      <c r="B74" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C74" s="106" t="s">
-        <v>250</v>
-      </c>
-      <c r="D74" s="100" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B75" s="39"/>
-      <c r="C75" s="98"/>
-      <c r="D75" s="98"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="58" t="s">
-        <v>249</v>
       </c>
       <c r="B76" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C76" s="112" t="s">
+      <c r="C76" s="106" t="s">
+        <v>250</v>
+      </c>
+      <c r="D76" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B77" s="39"/>
+      <c r="C77" s="98"/>
+      <c r="D77" s="98"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B78" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D76" s="58" t="s">
+      <c r="D78" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="132" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="136" t="s">
         <v>285</v>
       </c>
-      <c r="B77" s="166" t="s">
+      <c r="B79" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="101" t="s">
+      <c r="C79" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="D77" s="58" t="s">
+      <c r="D79" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="132"/>
-      <c r="B78" s="166"/>
-      <c r="C78" s="58" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="136"/>
+      <c r="B80" s="156"/>
+      <c r="C80" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D78" s="100" t="s">
+      <c r="D80" s="100" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="132"/>
-      <c r="B79" s="166"/>
-      <c r="C79" s="112" t="s">
+    <row r="81" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="136"/>
+      <c r="B81" s="156"/>
+      <c r="C81" s="112" t="s">
         <v>286</v>
       </c>
-      <c r="D79" s="58" t="s">
+      <c r="D81" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="98" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B80" s="98"/>
-      <c r="C80" s="98"/>
-      <c r="D80" s="98"/>
+      <c r="B82" s="98"/>
+      <c r="C82" s="98"/>
+      <c r="D82" s="98"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="149" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="B81" s="166" t="s">
+      <c r="B83" s="156" t="s">
         <v>271</v>
       </c>
-      <c r="C81" s="112" t="s">
+      <c r="C83" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D81" s="58" t="s">
+      <c r="D83" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="149"/>
-      <c r="B82" s="166"/>
-      <c r="C82" s="112" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="135"/>
+      <c r="B84" s="156"/>
+      <c r="C84" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D82" s="58" t="s">
+      <c r="D84" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="97" t="s">
+    <row r="85" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B83" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C83" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D83" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B84" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C84" s="58"/>
-      <c r="D84" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="97" t="s">
-        <v>60</v>
       </c>
       <c r="B85" s="106" t="s">
         <v>271</v>
@@ -32023,38 +32029,44 @@
         <v>264</v>
       </c>
       <c r="D85" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B86" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C86" s="58"/>
+      <c r="D86" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B87" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C87" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D87" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="98" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="98" t="s">
         <v>273</v>
-      </c>
-      <c r="B86" s="98"/>
-      <c r="C86" s="98"/>
-      <c r="D86" s="98"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="58"/>
-      <c r="B87" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C87" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D87" s="100" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="98" t="s">
-        <v>279</v>
       </c>
       <c r="B88" s="98"/>
       <c r="C88" s="98"/>
       <c r="D88" s="98"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="58"/>
       <c r="B89" s="106" t="s">
         <v>234</v>
@@ -32066,35 +32078,57 @@
         <v>274</v>
       </c>
     </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B90" s="98"/>
+      <c r="C90" s="98"/>
+      <c r="D90" s="98"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="58"/>
+      <c r="B91" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C91" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91" s="100" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A38:A62"/>
-    <mergeCell ref="B38:B62"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B5:B14"/>
+  <mergeCells count="29">
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A40:A64"/>
+    <mergeCell ref="B40:B64"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B25:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
soap authentication ppt added
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="353">
   <si>
     <t>Document</t>
   </si>
@@ -2911,6 +2911,9 @@
   </si>
   <si>
     <t>Date time zone specification and requirement for 2-digit values added</t>
+  </si>
+  <si>
+    <t>SOAP Request Authentication</t>
   </si>
 </sst>
 </file>
@@ -3494,7 +3497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3799,6 +3802,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3844,8 +3850,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3868,35 +3904,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3916,37 +3955,13 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3969,15 +3984,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4382,12 +4388,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="120"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4410,12 +4416,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="120"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="121"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4455,10 +4461,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="124">
+      <c r="B7" s="125">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4472,8 +4478,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="125"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4485,8 +4491,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="125"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4498,8 +4504,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="125"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="126"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4511,8 +4517,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="125"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="126"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4524,8 +4530,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="123"/>
-      <c r="B12" s="126"/>
+      <c r="A12" s="124"/>
+      <c r="B12" s="127"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4537,10 +4543,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="124">
+      <c r="B13" s="125">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4554,8 +4560,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="130"/>
-      <c r="B14" s="126"/>
+      <c r="A14" s="131"/>
+      <c r="B14" s="127"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4601,12 +4607,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="120"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="121"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4646,21 +4652,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="120"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="121"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="131" t="s">
+      <c r="A21" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="128">
+      <c r="B21" s="129">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4674,8 +4680,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="132"/>
-      <c r="B22" s="126"/>
+      <c r="A22" s="133"/>
+      <c r="B22" s="127"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4698,18 +4704,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="118" t="s">
+      <c r="A24" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="119"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="120"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="121"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="127" t="s">
+      <c r="A25" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="128">
+      <c r="B25" s="129">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4723,8 +4729,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="122"/>
-      <c r="B26" s="125"/>
+      <c r="A26" s="123"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4736,8 +4742,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="122"/>
-      <c r="B27" s="125"/>
+      <c r="A27" s="123"/>
+      <c r="B27" s="126"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4749,8 +4755,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="122"/>
-      <c r="B28" s="125"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="126"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4762,8 +4768,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="122"/>
-      <c r="B29" s="125"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="126"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4775,8 +4781,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="122"/>
-      <c r="B30" s="125"/>
+      <c r="A30" s="123"/>
+      <c r="B30" s="126"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4788,8 +4794,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="122"/>
-      <c r="B31" s="125"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="126"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4801,8 +4807,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="123"/>
-      <c r="B32" s="126"/>
+      <c r="A32" s="124"/>
+      <c r="B32" s="127"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4926,12 +4932,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="118" t="s">
+      <c r="A41" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="119"/>
-      <c r="C41" s="119"/>
-      <c r="D41" s="120"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="121"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -4991,7 +4997,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5001,7 +5007,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5111,10 +5117,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="148" t="s">
+      <c r="A7" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5125,8 +5131,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="148"/>
-      <c r="B8" s="147"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5135,8 +5141,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="148"/>
-      <c r="B9" s="147"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5145,8 +5151,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="148"/>
-      <c r="B10" s="147"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5155,8 +5161,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="148"/>
-      <c r="B11" s="147"/>
+      <c r="A11" s="134"/>
+      <c r="B11" s="135"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5165,8 +5171,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="148"/>
-      <c r="B12" s="147"/>
+      <c r="A12" s="134"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5175,10 +5181,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="137" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5189,8 +5195,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="150"/>
-      <c r="B14" s="147"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5199,8 +5205,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
-      <c r="B15" s="147"/>
+      <c r="A15" s="137"/>
+      <c r="B15" s="135"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5209,10 +5215,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="133" t="s">
+      <c r="A16" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="142" t="s">
+      <c r="B16" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5223,8 +5229,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="133"/>
-      <c r="B17" s="142"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="139"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5233,8 +5239,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="133"/>
-      <c r="B18" s="142"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="139"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5243,8 +5249,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="133"/>
-      <c r="B19" s="142"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="139"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5253,8 +5259,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="133"/>
-      <c r="B20" s="142"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="139"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5263,8 +5269,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="133"/>
-      <c r="B21" s="142"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="139"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5273,8 +5279,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
-      <c r="B22" s="142"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="139"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5283,8 +5289,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="133"/>
-      <c r="B23" s="142"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="139"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5293,26 +5299,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="133"/>
-      <c r="B24" s="142"/>
-      <c r="C24" s="133" t="s">
+      <c r="A24" s="138"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="138" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="134" t="s">
+      <c r="D24" s="145" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="133"/>
-      <c r="B25" s="142"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="134"/>
+      <c r="A25" s="138"/>
+      <c r="B25" s="139"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="145"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="148" t="s">
+      <c r="A26" s="134" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5323,8 +5329,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="148"/>
-      <c r="B27" s="147"/>
+      <c r="A27" s="134"/>
+      <c r="B27" s="135"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5351,28 +5357,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="149" t="s">
+      <c r="A30" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="147" t="s">
+      <c r="B30" s="135" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="133" t="s">
+      <c r="C30" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="137" t="s">
+      <c r="D30" s="148" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="149"/>
-      <c r="B31" s="147"/>
-      <c r="C31" s="133"/>
-      <c r="D31" s="137"/>
+      <c r="A31" s="136"/>
+      <c r="B31" s="135"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="148"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="149"/>
-      <c r="B32" s="147"/>
+      <c r="A32" s="136"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5381,8 +5387,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="149"/>
-      <c r="B33" s="147"/>
+      <c r="A33" s="136"/>
+      <c r="B33" s="135"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5391,8 +5397,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="149"/>
-      <c r="B34" s="147"/>
+      <c r="A34" s="136"/>
+      <c r="B34" s="135"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5401,8 +5407,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="149"/>
-      <c r="B35" s="147"/>
+      <c r="A35" s="136"/>
+      <c r="B35" s="135"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5411,8 +5417,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="149"/>
-      <c r="B36" s="147"/>
+      <c r="A36" s="136"/>
+      <c r="B36" s="135"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5421,26 +5427,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="149"/>
-      <c r="B37" s="147"/>
-      <c r="C37" s="138" t="s">
+      <c r="A37" s="136"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="149" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="140" t="s">
+      <c r="D37" s="151" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="149"/>
-      <c r="B38" s="147"/>
-      <c r="C38" s="139"/>
-      <c r="D38" s="140"/>
+      <c r="A38" s="136"/>
+      <c r="B38" s="135"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="151"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="148" t="s">
+      <c r="A39" s="134" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="147" t="s">
+      <c r="B39" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5451,8 +5457,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="148"/>
-      <c r="B40" s="147"/>
+      <c r="A40" s="134"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5479,10 +5485,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="149" t="s">
+      <c r="A43" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="147" t="s">
+      <c r="B43" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5491,8 +5497,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="149"/>
-      <c r="B44" s="147"/>
+      <c r="A44" s="136"/>
+      <c r="B44" s="135"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5501,10 +5507,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="144" t="s">
+      <c r="A45" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="147" t="s">
+      <c r="B45" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5513,8 +5519,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="145"/>
-      <c r="B46" s="147"/>
+      <c r="A46" s="143"/>
+      <c r="B46" s="135"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5523,8 +5529,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="145"/>
-      <c r="B47" s="147"/>
+      <c r="A47" s="143"/>
+      <c r="B47" s="135"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5533,8 +5539,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="146"/>
-      <c r="B48" s="147"/>
+      <c r="A48" s="144"/>
+      <c r="B48" s="135"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5543,10 +5549,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="142" t="s">
+      <c r="A49" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="142" t="s">
+      <c r="B49" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9650,8 +9656,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="142"/>
-      <c r="B50" s="142"/>
+      <c r="A50" s="139"/>
+      <c r="B50" s="139"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13755,8 +13761,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="142"/>
-      <c r="B51" s="142"/>
+      <c r="A51" s="139"/>
+      <c r="B51" s="139"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17860,8 +17866,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="142"/>
-      <c r="B52" s="142"/>
+      <c r="A52" s="139"/>
+      <c r="B52" s="139"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21965,12 +21971,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="142"/>
-      <c r="B53" s="142"/>
-      <c r="C53" s="136" t="s">
+      <c r="A53" s="139"/>
+      <c r="B53" s="139"/>
+      <c r="C53" s="147" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="137" t="s">
+      <c r="D53" s="148" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26070,10 +26076,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="142"/>
-      <c r="B54" s="142"/>
-      <c r="C54" s="136"/>
-      <c r="D54" s="137"/>
+      <c r="A54" s="139"/>
+      <c r="B54" s="139"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30191,10 +30197,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="141" t="s">
+      <c r="A57" s="140" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="142" t="s">
+      <c r="B57" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30205,8 +30211,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="141"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="140"/>
+      <c r="B58" s="139"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30215,8 +30221,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="141"/>
-      <c r="B59" s="142"/>
+      <c r="A59" s="140"/>
+      <c r="B59" s="139"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30225,8 +30231,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="141"/>
-      <c r="B60" s="142"/>
+      <c r="A60" s="140"/>
+      <c r="B60" s="139"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30235,8 +30241,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="141"/>
-      <c r="B61" s="142"/>
+      <c r="A61" s="140"/>
+      <c r="B61" s="139"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30245,8 +30251,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="141"/>
-      <c r="B62" s="142"/>
+      <c r="A62" s="140"/>
+      <c r="B62" s="139"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30255,8 +30261,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="141"/>
-      <c r="B63" s="142"/>
+      <c r="A63" s="140"/>
+      <c r="B63" s="139"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30265,16 +30271,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="141"/>
-      <c r="B64" s="142"/>
+      <c r="A64" s="140"/>
+      <c r="B64" s="139"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="141"/>
-      <c r="B65" s="142"/>
+      <c r="A65" s="140"/>
+      <c r="B65" s="139"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30283,16 +30289,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="141"/>
-      <c r="B66" s="142"/>
+      <c r="A66" s="140"/>
+      <c r="B66" s="139"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="141"/>
-      <c r="B67" s="142"/>
+      <c r="A67" s="140"/>
+      <c r="B67" s="139"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30301,8 +30307,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="141"/>
-      <c r="B68" s="142"/>
+      <c r="A68" s="140"/>
+      <c r="B68" s="139"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30311,8 +30317,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="141"/>
-      <c r="B69" s="142"/>
+      <c r="A69" s="140"/>
+      <c r="B69" s="139"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30321,8 +30327,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="141"/>
-      <c r="B70" s="142"/>
+      <c r="A70" s="140"/>
+      <c r="B70" s="139"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30331,8 +30337,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="141"/>
-      <c r="B71" s="142"/>
+      <c r="A71" s="140"/>
+      <c r="B71" s="139"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30341,8 +30347,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="141"/>
-      <c r="B72" s="142"/>
+      <c r="A72" s="140"/>
+      <c r="B72" s="139"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30351,16 +30357,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="141"/>
-      <c r="B73" s="142"/>
+      <c r="A73" s="140"/>
+      <c r="B73" s="139"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="141"/>
-      <c r="B74" s="142"/>
+      <c r="A74" s="140"/>
+      <c r="B74" s="139"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30369,18 +30375,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="141"/>
-      <c r="B75" s="142"/>
-      <c r="C75" s="135"/>
-      <c r="D75" s="143" t="s">
+      <c r="A75" s="140"/>
+      <c r="B75" s="139"/>
+      <c r="C75" s="146"/>
+      <c r="D75" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="141"/>
-      <c r="B76" s="142"/>
-      <c r="C76" s="135"/>
-      <c r="D76" s="143"/>
+      <c r="A76" s="140"/>
+      <c r="B76" s="139"/>
+      <c r="C76" s="146"/>
+      <c r="D76" s="141"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30404,8 +30410,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30414,13 +30420,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30435,22 +30457,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30504,10 +30510,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="147" t="s">
+      <c r="B4" s="135" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30518,133 +30524,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="148"/>
-      <c r="B5" s="147"/>
-      <c r="C5" s="158" t="s">
+      <c r="A5" s="134"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="161" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="157" t="s">
+      <c r="D5" s="160" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="148"/>
-      <c r="B6" s="147"/>
-      <c r="C6" s="158"/>
-      <c r="D6" s="157"/>
+      <c r="A6" s="134"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="148"/>
-      <c r="B7" s="147"/>
+      <c r="A7" s="134"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="148"/>
-      <c r="B8" s="147"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="148"/>
-      <c r="B9" s="147"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="137" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="160"/>
-      <c r="D10" s="157" t="s">
+      <c r="C10" s="159"/>
+      <c r="D10" s="160" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="150"/>
-      <c r="B11" s="147"/>
-      <c r="C11" s="160"/>
-      <c r="D11" s="157"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="135"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
-      <c r="B12" s="147"/>
-      <c r="C12" s="160"/>
-      <c r="D12" s="157"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="135"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="160"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="159"/>
-      <c r="D13" s="157" t="s">
+      <c r="C13" s="162"/>
+      <c r="D13" s="160" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="133"/>
-      <c r="B14" s="142"/>
-      <c r="C14" s="159"/>
-      <c r="D14" s="157"/>
+      <c r="A14" s="138"/>
+      <c r="B14" s="139"/>
+      <c r="C14" s="162"/>
+      <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
-      <c r="B15" s="142"/>
-      <c r="C15" s="159"/>
+      <c r="A15" s="138"/>
+      <c r="B15" s="139"/>
+      <c r="C15" s="162"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="133"/>
-      <c r="B16" s="142"/>
-      <c r="C16" s="159"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="162"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="133"/>
-      <c r="B17" s="142"/>
-      <c r="C17" s="159"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="162"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="133"/>
-      <c r="B18" s="142"/>
-      <c r="C18" s="159"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="133"/>
-      <c r="B19" s="142"/>
-      <c r="C19" s="159"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="162"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="133"/>
-      <c r="B20" s="142"/>
-      <c r="C20" s="159"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="139"/>
+      <c r="C20" s="162"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="133"/>
-      <c r="B21" s="142"/>
-      <c r="C21" s="159"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="162"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
-      <c r="B22" s="142"/>
-      <c r="C22" s="159"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="162"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="133"/>
-      <c r="B23" s="142"/>
-      <c r="C23" s="159"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="162"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30742,10 +30748,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="151" t="s">
+      <c r="A32" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="154" t="s">
+      <c r="B32" s="166" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30756,26 +30762,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="152"/>
-      <c r="B33" s="155"/>
+      <c r="A33" s="164"/>
+      <c r="B33" s="167"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="152"/>
-      <c r="B34" s="155"/>
+      <c r="A34" s="164"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="152"/>
-      <c r="B35" s="155"/>
+      <c r="A35" s="164"/>
+      <c r="B35" s="167"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="153"/>
-      <c r="B36" s="156"/>
+      <c r="A36" s="165"/>
+      <c r="B36" s="168"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30804,10 +30810,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="149" t="s">
+      <c r="A39" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="147" t="s">
+      <c r="B39" s="135" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30818,8 +30824,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="149"/>
-      <c r="B40" s="147"/>
+      <c r="A40" s="136"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30828,84 +30834,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="148" t="s">
+      <c r="A41" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="147" t="s">
+      <c r="B41" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="160" t="s">
+      <c r="C41" s="159" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="133" t="s">
+      <c r="D41" s="138" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="148"/>
-      <c r="B42" s="147"/>
-      <c r="C42" s="160"/>
-      <c r="D42" s="133"/>
+      <c r="A42" s="134"/>
+      <c r="B42" s="135"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="138"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="148"/>
-      <c r="B43" s="147"/>
-      <c r="C43" s="160" t="s">
+      <c r="A43" s="134"/>
+      <c r="B43" s="135"/>
+      <c r="C43" s="159" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="143" t="s">
+      <c r="D43" s="141" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="148"/>
-      <c r="B44" s="147"/>
-      <c r="C44" s="160"/>
-      <c r="D44" s="143"/>
+      <c r="A44" s="134"/>
+      <c r="B44" s="135"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="141"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="141" t="s">
+      <c r="A45" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="142" t="s">
+      <c r="B45" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="164"/>
+      <c r="C45" s="155"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="141"/>
-      <c r="B46" s="142"/>
-      <c r="C46" s="165"/>
-      <c r="D46" s="161" t="s">
+      <c r="A46" s="140"/>
+      <c r="B46" s="139"/>
+      <c r="C46" s="156"/>
+      <c r="D46" s="152" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="141"/>
-      <c r="B47" s="142"/>
-      <c r="C47" s="165"/>
-      <c r="D47" s="162"/>
+      <c r="A47" s="140"/>
+      <c r="B47" s="139"/>
+      <c r="C47" s="156"/>
+      <c r="D47" s="153"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="141"/>
-      <c r="B48" s="142"/>
-      <c r="C48" s="166"/>
-      <c r="D48" s="162"/>
+      <c r="A48" s="140"/>
+      <c r="B48" s="139"/>
+      <c r="C48" s="157"/>
+      <c r="D48" s="153"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="141"/>
-      <c r="B49" s="142"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="162"/>
+      <c r="A49" s="140"/>
+      <c r="B49" s="139"/>
+      <c r="C49" s="147"/>
+      <c r="D49" s="153"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="141"/>
-      <c r="B50" s="142"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="163"/>
+      <c r="A50" s="140"/>
+      <c r="B50" s="139"/>
+      <c r="C50" s="147"/>
+      <c r="D50" s="154"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -30928,10 +30934,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="142" t="s">
+      <c r="A53" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="142" t="s">
+      <c r="B53" s="139" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30942,8 +30948,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="142"/>
-      <c r="B54" s="142"/>
+      <c r="A54" s="139"/>
+      <c r="B54" s="139"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30952,8 +30958,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="142"/>
-      <c r="B55" s="142"/>
+      <c r="A55" s="139"/>
+      <c r="B55" s="139"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30962,9 +30968,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="142"/>
-      <c r="B56" s="142"/>
-      <c r="C56" s="167" t="s">
+      <c r="A56" s="139"/>
+      <c r="B56" s="139"/>
+      <c r="C56" s="158" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30972,16 +30978,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="142"/>
-      <c r="B57" s="142"/>
-      <c r="C57" s="167"/>
+      <c r="A57" s="139"/>
+      <c r="B57" s="139"/>
+      <c r="C57" s="158"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="142"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="139"/>
+      <c r="B58" s="139"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30990,8 +30996,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="142"/>
+      <c r="A59" s="139"/>
+      <c r="B59" s="139"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31000,9 +31006,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="142"/>
-      <c r="B60" s="142"/>
-      <c r="C60" s="167" t="s">
+      <c r="A60" s="139"/>
+      <c r="B60" s="139"/>
+      <c r="C60" s="158" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31010,25 +31016,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="142"/>
-      <c r="B61" s="142"/>
-      <c r="C61" s="167"/>
+      <c r="A61" s="139"/>
+      <c r="B61" s="139"/>
+      <c r="C61" s="158"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="142"/>
-      <c r="B62" s="142"/>
-      <c r="C62" s="167"/>
+      <c r="A62" s="139"/>
+      <c r="B62" s="139"/>
+      <c r="C62" s="158"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="142"/>
-      <c r="B63" s="142"/>
-      <c r="C63" s="160" t="s">
+      <c r="A63" s="139"/>
+      <c r="B63" s="139"/>
+      <c r="C63" s="159" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31036,30 +31042,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="142"/>
-      <c r="B64" s="142"/>
-      <c r="C64" s="160"/>
-      <c r="D64" s="143" t="s">
+      <c r="A64" s="139"/>
+      <c r="B64" s="139"/>
+      <c r="C64" s="159"/>
+      <c r="D64" s="141" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="142"/>
-      <c r="B65" s="142"/>
-      <c r="C65" s="160"/>
-      <c r="D65" s="143"/>
+      <c r="A65" s="139"/>
+      <c r="B65" s="139"/>
+      <c r="C65" s="159"/>
+      <c r="D65" s="141"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="142"/>
-      <c r="B66" s="142"/>
-      <c r="C66" s="160"/>
-      <c r="D66" s="143"/>
+      <c r="A66" s="139"/>
+      <c r="B66" s="139"/>
+      <c r="C66" s="159"/>
+      <c r="D66" s="141"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="142"/>
-      <c r="B67" s="142"/>
-      <c r="C67" s="160"/>
-      <c r="D67" s="143"/>
+      <c r="A67" s="139"/>
+      <c r="B67" s="139"/>
+      <c r="C67" s="159"/>
+      <c r="D67" s="141"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31115,6 +31121,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31131,23 +31154,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31156,10 +31162,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31193,10 +31199,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="172" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="172" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="114" t="s">
@@ -31207,8 +31213,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="168"/>
-      <c r="B4" s="168"/>
+      <c r="A4" s="172"/>
+      <c r="B4" s="172"/>
       <c r="C4" s="114" t="s">
         <v>347</v>
       </c>
@@ -31225,10 +31231,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="167" t="s">
+      <c r="B6" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31237,8 +31243,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133"/>
-      <c r="B7" s="167"/>
+      <c r="A7" s="138"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
@@ -31250,7 +31256,7 @@
       <c r="A8" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="167"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="106" t="s">
         <v>235</v>
       </c>
@@ -31262,7 +31268,7 @@
       <c r="A9" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="167"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="106" t="s">
         <v>22</v>
       </c>
@@ -31271,26 +31277,26 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="167" t="s">
+      <c r="A10" s="158" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="167"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="58"/>
       <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="167"/>
-      <c r="B11" s="167"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="167"/>
-      <c r="B12" s="167"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="110" t="s">
         <v>325</v>
       </c>
@@ -31302,8 +31308,8 @@
       <c r="A13" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="167"/>
-      <c r="C13" s="58" t="s">
+      <c r="B13" s="177"/>
+      <c r="C13" s="118" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="58"/>
@@ -31312,7 +31318,7 @@
       <c r="A14" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="167"/>
+      <c r="B14" s="177"/>
       <c r="C14" s="58"/>
       <c r="D14" s="104" t="s">
         <v>259</v>
@@ -31322,561 +31328,557 @@
       <c r="A15" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B15" s="167"/>
-      <c r="C15" s="58" t="s">
+      <c r="B15" s="177"/>
+      <c r="C15" s="118" t="s">
         <v>332</v>
       </c>
       <c r="D15" s="100" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="100" t="s">
+        <v>352</v>
+      </c>
+      <c r="B16" s="178"/>
+      <c r="C16" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="100"/>
+    </row>
+    <row r="17" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="175" t="s">
-        <v>237</v>
-      </c>
-      <c r="B17" s="167" t="s">
-        <v>234</v>
-      </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58" t="s">
-        <v>258</v>
-      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="175"/>
-      <c r="B18" s="167"/>
+      <c r="A18" s="171" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" s="158" t="s">
+        <v>234</v>
+      </c>
       <c r="C18" s="58"/>
       <c r="D18" s="58" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="175"/>
-      <c r="B19" s="167"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="158"/>
       <c r="C19" s="58"/>
       <c r="D19" s="58" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="175"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="58" t="s">
-        <v>300</v>
-      </c>
+      <c r="A20" s="171"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="58" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="175"/>
-      <c r="B21" s="167"/>
+      <c r="A21" s="171"/>
+      <c r="B21" s="158"/>
       <c r="C21" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="D21" s="100" t="s">
-        <v>327</v>
+        <v>300</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="149" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="167" t="s">
-        <v>234</v>
-      </c>
+      <c r="A22" s="171"/>
+      <c r="B22" s="158"/>
       <c r="C22" s="58" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="D22" s="100" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="149"/>
-      <c r="B23" s="167"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58" t="s">
+      <c r="A23" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="158" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="100" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="136"/>
+      <c r="B24" s="158"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="149"/>
-      <c r="B24" s="167"/>
-      <c r="C24" s="108" t="s">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="136"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="108" t="s">
         <v>329</v>
       </c>
-      <c r="D24" s="100" t="s">
+      <c r="D25" s="100" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="167" t="s">
-        <v>222</v>
-      </c>
-      <c r="B25" s="167" t="s">
-        <v>234</v>
-      </c>
-      <c r="C25" s="176" t="s">
-        <v>239</v>
-      </c>
-      <c r="D25" s="103" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="167"/>
-      <c r="B26" s="167"/>
-      <c r="C26" s="176"/>
-      <c r="D26" s="100" t="s">
-        <v>278</v>
+      <c r="A26" s="158" t="s">
+        <v>222</v>
+      </c>
+      <c r="B26" s="158" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="169" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="103" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="167"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="176" t="s">
+      <c r="A27" s="158"/>
+      <c r="B27" s="158"/>
+      <c r="C27" s="169"/>
+      <c r="D27" s="100" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="158"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="169" t="s">
         <v>240</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D28" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="167"/>
-      <c r="B28" s="167"/>
-      <c r="C28" s="176"/>
-      <c r="D28" s="61" t="s">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="158"/>
+      <c r="B29" s="158"/>
+      <c r="C29" s="169"/>
+      <c r="D29" s="61" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="167"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="105" t="s">
-        <v>307</v>
-      </c>
-      <c r="D29" s="58" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="167"/>
-      <c r="B30" s="167"/>
-      <c r="C30" s="105">
-        <v>2.1</v>
+      <c r="A30" s="158"/>
+      <c r="B30" s="158"/>
+      <c r="C30" s="105" t="s">
+        <v>307</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="167"/>
-      <c r="B31" s="167"/>
-      <c r="C31" s="105" t="s">
-        <v>239</v>
+      <c r="A31" s="158"/>
+      <c r="B31" s="158"/>
+      <c r="C31" s="105">
+        <v>2.1</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="167"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="117" t="s">
+      <c r="A32" s="158"/>
+      <c r="B32" s="158"/>
+      <c r="C32" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="D32" s="116" t="s">
-        <v>346</v>
+      <c r="D32" s="58" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="167"/>
-      <c r="B33" s="167"/>
-      <c r="C33" s="115" t="s">
+      <c r="A33" s="158"/>
+      <c r="B33" s="158"/>
+      <c r="C33" s="117" t="s">
         <v>239</v>
       </c>
-      <c r="D33" s="100" t="s">
+      <c r="D33" s="116" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="158"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="115" t="s">
+        <v>239</v>
+      </c>
+      <c r="D34" s="100" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="142" t="s">
+    <row r="35" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="139" t="s">
         <v>296</v>
       </c>
-      <c r="B34" s="167" t="s">
+      <c r="B35" s="158" t="s">
         <v>234</v>
       </c>
-      <c r="C34" s="58" t="s">
+      <c r="C35" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D35" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="142"/>
-      <c r="B35" s="167"/>
-      <c r="C35" s="61" t="s">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="139"/>
+      <c r="B36" s="158"/>
+      <c r="C36" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D36" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="142"/>
-      <c r="B36" s="167"/>
-      <c r="C36" s="58" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="139"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="58" t="s">
         <v>350</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D37" s="58" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="44"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="133" t="s">
-        <v>260</v>
-      </c>
-      <c r="B38" s="167" t="s">
-        <v>234</v>
-      </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="79" t="s">
-        <v>261</v>
-      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="133"/>
-      <c r="B39" s="167"/>
+      <c r="A39" s="138" t="s">
+        <v>260</v>
+      </c>
+      <c r="B39" s="158" t="s">
+        <v>234</v>
+      </c>
       <c r="C39" s="58"/>
-      <c r="D39" s="58" t="s">
-        <v>257</v>
+      <c r="D39" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="B40" s="105" t="s">
-        <v>234</v>
-      </c>
-      <c r="C40" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="D40" s="100" t="s">
-        <v>336</v>
+      <c r="A40" s="138"/>
+      <c r="B40" s="158"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="96" t="s">
-        <v>243</v>
+      <c r="A41" s="58" t="s">
+        <v>334</v>
       </c>
       <c r="B41" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C41" s="106" t="s">
+      <c r="C41" s="79" t="s">
+        <v>335</v>
+      </c>
+      <c r="D41" s="100" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B42" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="104" t="s">
+      <c r="D42" s="104" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="169" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="173" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="172" t="s">
+      <c r="B43" s="176" t="s">
         <v>234</v>
       </c>
-      <c r="C42" s="58" t="s">
+      <c r="C43" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D42" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="170"/>
-      <c r="B43" s="173"/>
-      <c r="C43" s="58" t="s">
-        <v>270</v>
       </c>
       <c r="D43" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="170"/>
-      <c r="B44" s="173"/>
+      <c r="A44" s="174"/>
+      <c r="B44" s="177"/>
       <c r="C44" s="58" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D44" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="170"/>
-      <c r="B45" s="173"/>
-      <c r="C45" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D45" s="100" t="s">
-        <v>102</v>
+      <c r="A45" s="174"/>
+      <c r="B45" s="177"/>
+      <c r="C45" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="170"/>
-      <c r="B46" s="173"/>
-      <c r="C46" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="D46" s="58" t="s">
-        <v>251</v>
+      <c r="A46" s="174"/>
+      <c r="B46" s="177"/>
+      <c r="C46" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" s="100" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="170"/>
-      <c r="B47" s="173"/>
+      <c r="A47" s="174"/>
+      <c r="B47" s="177"/>
       <c r="C47" s="58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D47" s="58" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="170"/>
-      <c r="B48" s="173"/>
-      <c r="C48" s="100" t="s">
-        <v>288</v>
-      </c>
-      <c r="D48" s="100" t="s">
-        <v>251</v>
+      <c r="A48" s="174"/>
+      <c r="B48" s="177"/>
+      <c r="C48" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D48" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="170"/>
-      <c r="B49" s="173"/>
+      <c r="A49" s="174"/>
+      <c r="B49" s="177"/>
       <c r="C49" s="100" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D49" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="170"/>
-      <c r="B50" s="173"/>
+      <c r="A50" s="174"/>
+      <c r="B50" s="177"/>
       <c r="C50" s="100" t="s">
+        <v>302</v>
+      </c>
+      <c r="D50" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="174"/>
+      <c r="B51" s="177"/>
+      <c r="C51" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="D50" s="100" t="s">
+      <c r="D51" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="170"/>
-      <c r="B51" s="173"/>
-      <c r="C51" s="107" t="s">
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="174"/>
+      <c r="B52" s="177"/>
+      <c r="C52" s="107" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="104" t="s">
+      <c r="D52" s="104" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="170"/>
-      <c r="B52" s="173"/>
-      <c r="C52" s="108" t="s">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="174"/>
+      <c r="B53" s="177"/>
+      <c r="C53" s="108" t="s">
         <v>311</v>
       </c>
-      <c r="D52" s="100" t="s">
+      <c r="D53" s="100" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="170"/>
-      <c r="B53" s="173"/>
-      <c r="C53" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="D53" s="58" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="170"/>
-      <c r="B54" s="173"/>
-      <c r="C54" s="100" t="s">
-        <v>313</v>
-      </c>
-      <c r="D54" s="100" t="s">
-        <v>314</v>
+      <c r="A54" s="174"/>
+      <c r="B54" s="177"/>
+      <c r="C54" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D54" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="170"/>
-      <c r="B55" s="173"/>
+      <c r="A55" s="174"/>
+      <c r="B55" s="177"/>
       <c r="C55" s="100" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D55" s="100" t="s">
-        <v>102</v>
+        <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="170"/>
-      <c r="B56" s="173"/>
+      <c r="A56" s="174"/>
+      <c r="B56" s="177"/>
       <c r="C56" s="100" t="s">
-        <v>268</v>
+        <v>315</v>
       </c>
       <c r="D56" s="100" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="170"/>
-      <c r="B57" s="173"/>
-      <c r="C57" s="58" t="s">
-        <v>318</v>
-      </c>
-      <c r="D57" s="58" t="s">
+      <c r="A57" s="174"/>
+      <c r="B57" s="177"/>
+      <c r="C57" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="D57" s="100" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="170"/>
-      <c r="B58" s="173"/>
-      <c r="C58" s="100" t="s">
-        <v>283</v>
-      </c>
-      <c r="D58" s="100" t="s">
-        <v>320</v>
+      <c r="A58" s="174"/>
+      <c r="B58" s="177"/>
+      <c r="C58" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D58" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="170"/>
-      <c r="B59" s="173"/>
+      <c r="A59" s="174"/>
+      <c r="B59" s="177"/>
       <c r="C59" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="D59" s="100" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="174"/>
+      <c r="B60" s="177"/>
+      <c r="C60" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="D59" s="100" t="s">
+      <c r="D60" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="170"/>
-      <c r="B60" s="173"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="109" t="s">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="174"/>
+      <c r="B61" s="177"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="109" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="170"/>
-      <c r="B61" s="173"/>
-      <c r="C61" s="100" t="s">
-        <v>322</v>
-      </c>
-      <c r="D61" s="100" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="170"/>
-      <c r="B62" s="173"/>
+      <c r="A62" s="174"/>
+      <c r="B62" s="177"/>
       <c r="C62" s="100" t="s">
-        <v>268</v>
+        <v>322</v>
       </c>
       <c r="D62" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="170"/>
-      <c r="B63" s="173"/>
+      <c r="A63" s="174"/>
+      <c r="B63" s="177"/>
       <c r="C63" s="100" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="D63" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="170"/>
-      <c r="B64" s="173"/>
+      <c r="A64" s="174"/>
+      <c r="B64" s="177"/>
       <c r="C64" s="100" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D64" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="170"/>
-      <c r="B65" s="173"/>
+      <c r="A65" s="174"/>
+      <c r="B65" s="177"/>
       <c r="C65" s="100" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="D65" s="100" t="s">
-        <v>323</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="170"/>
-      <c r="B66" s="173"/>
-      <c r="C66" s="116" t="s">
-        <v>345</v>
-      </c>
-      <c r="D66" s="116" t="s">
-        <v>251</v>
+      <c r="A66" s="174"/>
+      <c r="B66" s="177"/>
+      <c r="C66" s="100" t="s">
+        <v>324</v>
+      </c>
+      <c r="D66" s="100" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="171"/>
-      <c r="B67" s="174"/>
-      <c r="C67" s="100" t="s">
-        <v>338</v>
-      </c>
-      <c r="D67" s="100" t="s">
-        <v>337</v>
+      <c r="A67" s="174"/>
+      <c r="B67" s="177"/>
+      <c r="C67" s="116" t="s">
+        <v>345</v>
+      </c>
+      <c r="D67" s="116" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B68" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C68" s="58" t="s">
-        <v>30</v>
+      <c r="A68" s="175"/>
+      <c r="B68" s="178"/>
+      <c r="C68" s="100" t="s">
+        <v>338</v>
       </c>
       <c r="D68" s="100" t="s">
-        <v>274</v>
+        <v>337</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="58" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B69" s="106" t="s">
         <v>234</v>
@@ -31888,297 +31890,311 @@
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="39" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C70" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="100" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="44"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="44"/>
     </row>
-    <row r="71" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="99"/>
-      <c r="B71" s="67"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="79" t="s">
+    <row r="72" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="99"/>
+      <c r="B72" s="67"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="167" t="s">
+    <row r="73" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="158" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="167" t="s">
+      <c r="B73" s="158" t="s">
         <v>234</v>
       </c>
-      <c r="C72" s="106" t="s">
+      <c r="C73" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="D72" s="58" t="s">
+      <c r="D73" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="167"/>
-      <c r="B73" s="167"/>
-      <c r="C73" s="106">
-        <v>10.1</v>
-      </c>
-      <c r="D73" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="167"/>
-      <c r="B74" s="167"/>
+      <c r="A74" s="158"/>
+      <c r="B74" s="158"/>
       <c r="C74" s="106">
-        <v>10.199999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="D74" s="58" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="167"/>
-      <c r="B75" s="167"/>
-      <c r="C75" s="111" t="s">
-        <v>293</v>
-      </c>
-      <c r="D75" s="101" t="s">
-        <v>294</v>
+      <c r="A75" s="158"/>
+      <c r="B75" s="158"/>
+      <c r="C75" s="106">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D75" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="133" t="s">
-        <v>247</v>
-      </c>
-      <c r="B76" s="167" t="s">
-        <v>234</v>
-      </c>
-      <c r="C76" s="167"/>
-      <c r="D76" s="177" t="s">
-        <v>261</v>
+      <c r="A76" s="158"/>
+      <c r="B76" s="158"/>
+      <c r="C76" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="D76" s="101" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="133"/>
-      <c r="B77" s="167"/>
-      <c r="C77" s="167"/>
-      <c r="D77" s="177"/>
+      <c r="A77" s="138" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" s="158" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="158"/>
+      <c r="D77" s="170" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="104" t="s">
+      <c r="A78" s="138"/>
+      <c r="B78" s="158"/>
+      <c r="C78" s="158"/>
+      <c r="D78" s="170"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="B78" s="106" t="s">
+      <c r="B79" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C78" s="106" t="s">
+      <c r="C79" s="106" t="s">
         <v>250</v>
       </c>
-      <c r="D78" s="100" t="s">
+      <c r="D79" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="95" t="s">
+    <row r="80" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B79" s="39"/>
-      <c r="C79" s="98"/>
-      <c r="D79" s="98"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B80" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C80" s="112" t="s">
-        <v>265</v>
-      </c>
-      <c r="D80" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="B80" s="39"/>
+      <c r="C80" s="98"/>
+      <c r="D80" s="98"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="133" t="s">
-        <v>285</v>
-      </c>
-      <c r="B81" s="167" t="s">
+      <c r="A81" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B81" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C81" s="101" t="s">
-        <v>295</v>
+      <c r="C81" s="112" t="s">
+        <v>265</v>
       </c>
       <c r="D81" s="58" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="133"/>
-      <c r="B82" s="167"/>
-      <c r="C82" s="58" t="s">
+      <c r="A82" s="138" t="s">
+        <v>285</v>
+      </c>
+      <c r="B82" s="158" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" s="101" t="s">
+        <v>295</v>
+      </c>
+      <c r="D82" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="138"/>
+      <c r="B83" s="158"/>
+      <c r="C83" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D82" s="100" t="s">
+      <c r="D83" s="100" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="133"/>
-      <c r="B83" s="167"/>
-      <c r="C83" s="112" t="s">
+    <row r="84" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="138"/>
+      <c r="B84" s="158"/>
+      <c r="C84" s="112" t="s">
         <v>286</v>
       </c>
-      <c r="D83" s="58" t="s">
+      <c r="D84" s="58" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B84" s="98"/>
-      <c r="C84" s="98"/>
-      <c r="D84" s="98"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="150" t="s">
-        <v>58</v>
-      </c>
-      <c r="B85" s="167" t="s">
-        <v>271</v>
-      </c>
-      <c r="C85" s="112" t="s">
-        <v>265</v>
-      </c>
-      <c r="D85" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="A85" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B85" s="98"/>
+      <c r="C85" s="98"/>
+      <c r="D85" s="98"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="150"/>
-      <c r="B86" s="167"/>
+      <c r="A86" s="137" t="s">
+        <v>58</v>
+      </c>
+      <c r="B86" s="158" t="s">
+        <v>271</v>
+      </c>
       <c r="C86" s="112" t="s">
         <v>265</v>
       </c>
       <c r="D86" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="137"/>
+      <c r="B87" s="158"/>
+      <c r="C87" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D87" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="97" t="s">
+    <row r="88" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B87" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C87" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D87" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="58" t="s">
-        <v>291</v>
       </c>
       <c r="B88" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C88" s="58"/>
-      <c r="D88" s="61" t="s">
-        <v>292</v>
+      <c r="C88" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D88" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="97" t="s">
-        <v>60</v>
+      <c r="A89" s="58" t="s">
+        <v>291</v>
       </c>
       <c r="B89" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C89" s="61" t="s">
+      <c r="C89" s="58"/>
+      <c r="D89" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C90" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D89" s="58" t="s">
+      <c r="D90" s="58" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B90" s="98"/>
-      <c r="C90" s="98"/>
-      <c r="D90" s="98"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="58"/>
-      <c r="B91" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C91" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D91" s="100" t="s">
-        <v>274</v>
-      </c>
+      <c r="A91" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B91" s="98"/>
+      <c r="C91" s="98"/>
+      <c r="D91" s="98"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="98" t="s">
-        <v>279</v>
-      </c>
-      <c r="B92" s="98"/>
-      <c r="C92" s="98"/>
-      <c r="D92" s="98"/>
+      <c r="A92" s="58"/>
+      <c r="B92" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C92" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" s="100" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="58"/>
-      <c r="B93" s="106" t="s">
+      <c r="A93" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B93" s="98"/>
+      <c r="C93" s="98"/>
+      <c r="D93" s="98"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="58"/>
+      <c r="B94" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C93" s="58" t="s">
+      <c r="C94" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D93" s="100" t="s">
+      <c r="D94" s="100" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A25:A33"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A67"/>
-    <mergeCell ref="B42:B67"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A43:A68"/>
+    <mergeCell ref="B43:B68"/>
+    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A26:A34"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="B35:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
validation rules changed to async and 4002 added to payroll
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -20,17 +20,17 @@
   <definedNames>
     <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="357">
   <si>
     <t>Document</t>
   </si>
@@ -2914,6 +2914,18 @@
   </si>
   <si>
     <t>Accepted Date specification updated</t>
+  </si>
+  <si>
+    <t>code 4002</t>
+  </si>
+  <si>
+    <t>Added to Payroll Submission</t>
+  </si>
+  <si>
+    <t>Corrected to Async</t>
+  </si>
+  <si>
+    <t>code 4002, 4003, 4004, 1010</t>
   </si>
 </sst>
 </file>
@@ -3497,7 +3509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3850,8 +3862,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3874,35 +3916,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3922,37 +3967,13 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3976,14 +3997,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4997,7 +5013,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5007,7 +5023,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5117,10 +5133,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149" t="s">
+      <c r="A7" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5131,8 +5147,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5141,8 +5157,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5151,8 +5167,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="149"/>
-      <c r="B10" s="148"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5161,8 +5177,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
-      <c r="B11" s="148"/>
+      <c r="A11" s="134"/>
+      <c r="B11" s="135"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5171,8 +5187,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="148"/>
+      <c r="A12" s="134"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5181,10 +5197,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="137" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5195,8 +5211,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="151"/>
-      <c r="B14" s="148"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5205,8 +5221,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="151"/>
-      <c r="B15" s="148"/>
+      <c r="A15" s="137"/>
+      <c r="B15" s="135"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5215,10 +5231,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5229,8 +5245,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="134"/>
-      <c r="B17" s="143"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="139"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5239,8 +5255,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134"/>
-      <c r="B18" s="143"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="139"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5249,8 +5265,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="143"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="139"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5259,8 +5275,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="134"/>
-      <c r="B20" s="143"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="139"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5269,8 +5285,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="143"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="139"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5279,8 +5295,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="134"/>
-      <c r="B22" s="143"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="139"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5289,8 +5305,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
-      <c r="B23" s="143"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="139"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5299,26 +5315,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="134"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="134" t="s">
+      <c r="A24" s="138"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="138" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="135" t="s">
+      <c r="D24" s="145" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="134"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="135"/>
+      <c r="A25" s="138"/>
+      <c r="B25" s="139"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="145"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="149" t="s">
+      <c r="A26" s="134" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5329,8 +5345,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="149"/>
-      <c r="B27" s="148"/>
+      <c r="A27" s="134"/>
+      <c r="B27" s="135"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5357,28 +5373,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="150" t="s">
+      <c r="A30" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="135" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="134" t="s">
+      <c r="C30" s="138" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="138" t="s">
+      <c r="D30" s="148" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="150"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="138"/>
+      <c r="A31" s="136"/>
+      <c r="B31" s="135"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="148"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="150"/>
-      <c r="B32" s="148"/>
+      <c r="A32" s="136"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5387,8 +5403,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="150"/>
-      <c r="B33" s="148"/>
+      <c r="A33" s="136"/>
+      <c r="B33" s="135"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5397,8 +5413,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="150"/>
-      <c r="B34" s="148"/>
+      <c r="A34" s="136"/>
+      <c r="B34" s="135"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5407,8 +5423,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="150"/>
-      <c r="B35" s="148"/>
+      <c r="A35" s="136"/>
+      <c r="B35" s="135"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5417,8 +5433,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150"/>
-      <c r="B36" s="148"/>
+      <c r="A36" s="136"/>
+      <c r="B36" s="135"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5427,26 +5443,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="150"/>
-      <c r="B37" s="148"/>
-      <c r="C37" s="139" t="s">
+      <c r="A37" s="136"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="149" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="141" t="s">
+      <c r="D37" s="151" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="150"/>
-      <c r="B38" s="148"/>
-      <c r="C38" s="140"/>
-      <c r="D38" s="141"/>
+      <c r="A38" s="136"/>
+      <c r="B38" s="135"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="151"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="149" t="s">
+      <c r="A39" s="134" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5457,8 +5473,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="149"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="134"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5485,10 +5501,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="150" t="s">
+      <c r="A43" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="148" t="s">
+      <c r="B43" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5497,8 +5513,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="150"/>
-      <c r="B44" s="148"/>
+      <c r="A44" s="136"/>
+      <c r="B44" s="135"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5507,10 +5523,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="145" t="s">
+      <c r="A45" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="135" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5519,8 +5535,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="146"/>
-      <c r="B46" s="148"/>
+      <c r="A46" s="143"/>
+      <c r="B46" s="135"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5529,8 +5545,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="146"/>
-      <c r="B47" s="148"/>
+      <c r="A47" s="143"/>
+      <c r="B47" s="135"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5539,8 +5555,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="147"/>
-      <c r="B48" s="148"/>
+      <c r="A48" s="144"/>
+      <c r="B48" s="135"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5549,10 +5565,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="143" t="s">
+      <c r="A49" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="143" t="s">
+      <c r="B49" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9656,8 +9672,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="143"/>
-      <c r="B50" s="143"/>
+      <c r="A50" s="139"/>
+      <c r="B50" s="139"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13761,8 +13777,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="143"/>
-      <c r="B51" s="143"/>
+      <c r="A51" s="139"/>
+      <c r="B51" s="139"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17866,8 +17882,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="143"/>
-      <c r="B52" s="143"/>
+      <c r="A52" s="139"/>
+      <c r="B52" s="139"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21971,12 +21987,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="143"/>
-      <c r="B53" s="143"/>
-      <c r="C53" s="137" t="s">
+      <c r="A53" s="139"/>
+      <c r="B53" s="139"/>
+      <c r="C53" s="147" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="138" t="s">
+      <c r="D53" s="148" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26076,10 +26092,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="137"/>
-      <c r="D54" s="138"/>
+      <c r="A54" s="139"/>
+      <c r="B54" s="139"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30197,10 +30213,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="142" t="s">
+      <c r="A57" s="140" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="143" t="s">
+      <c r="B57" s="139" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30211,8 +30227,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="142"/>
-      <c r="B58" s="143"/>
+      <c r="A58" s="140"/>
+      <c r="B58" s="139"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30221,8 +30237,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="143"/>
+      <c r="A59" s="140"/>
+      <c r="B59" s="139"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30231,8 +30247,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="142"/>
-      <c r="B60" s="143"/>
+      <c r="A60" s="140"/>
+      <c r="B60" s="139"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30241,8 +30257,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="142"/>
-      <c r="B61" s="143"/>
+      <c r="A61" s="140"/>
+      <c r="B61" s="139"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30251,8 +30267,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="142"/>
-      <c r="B62" s="143"/>
+      <c r="A62" s="140"/>
+      <c r="B62" s="139"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30261,8 +30277,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="142"/>
-      <c r="B63" s="143"/>
+      <c r="A63" s="140"/>
+      <c r="B63" s="139"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30271,16 +30287,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="142"/>
-      <c r="B64" s="143"/>
+      <c r="A64" s="140"/>
+      <c r="B64" s="139"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="142"/>
-      <c r="B65" s="143"/>
+      <c r="A65" s="140"/>
+      <c r="B65" s="139"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30289,16 +30305,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="142"/>
-      <c r="B66" s="143"/>
+      <c r="A66" s="140"/>
+      <c r="B66" s="139"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="142"/>
-      <c r="B67" s="143"/>
+      <c r="A67" s="140"/>
+      <c r="B67" s="139"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30307,8 +30323,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="142"/>
-      <c r="B68" s="143"/>
+      <c r="A68" s="140"/>
+      <c r="B68" s="139"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30317,8 +30333,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="142"/>
-      <c r="B69" s="143"/>
+      <c r="A69" s="140"/>
+      <c r="B69" s="139"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30327,8 +30343,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="142"/>
-      <c r="B70" s="143"/>
+      <c r="A70" s="140"/>
+      <c r="B70" s="139"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30337,8 +30353,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="142"/>
-      <c r="B71" s="143"/>
+      <c r="A71" s="140"/>
+      <c r="B71" s="139"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30347,8 +30363,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="142"/>
-      <c r="B72" s="143"/>
+      <c r="A72" s="140"/>
+      <c r="B72" s="139"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30357,16 +30373,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="142"/>
-      <c r="B73" s="143"/>
+      <c r="A73" s="140"/>
+      <c r="B73" s="139"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="142"/>
-      <c r="B74" s="143"/>
+      <c r="A74" s="140"/>
+      <c r="B74" s="139"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30375,18 +30391,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="142"/>
-      <c r="B75" s="143"/>
-      <c r="C75" s="136"/>
-      <c r="D75" s="144" t="s">
+      <c r="A75" s="140"/>
+      <c r="B75" s="139"/>
+      <c r="C75" s="146"/>
+      <c r="D75" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="142"/>
-      <c r="B76" s="143"/>
-      <c r="C76" s="136"/>
-      <c r="D76" s="144"/>
+      <c r="A76" s="140"/>
+      <c r="B76" s="139"/>
+      <c r="C76" s="146"/>
+      <c r="D76" s="141"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30410,8 +30426,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30420,13 +30436,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30441,22 +30473,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30510,10 +30526,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="135" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30524,133 +30540,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="149"/>
-      <c r="B5" s="148"/>
-      <c r="C5" s="159" t="s">
+      <c r="A5" s="134"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="161" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="158" t="s">
+      <c r="D5" s="160" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149"/>
-      <c r="B6" s="148"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="158"/>
+      <c r="A6" s="134"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149"/>
-      <c r="B7" s="148"/>
+      <c r="A7" s="134"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="137" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="161"/>
-      <c r="D10" s="158" t="s">
+      <c r="C10" s="159"/>
+      <c r="D10" s="160" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="161"/>
-      <c r="D11" s="158"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="135"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
-      <c r="B12" s="148"/>
-      <c r="C12" s="161"/>
-      <c r="D12" s="158"/>
+      <c r="A12" s="137"/>
+      <c r="B12" s="135"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="160"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="143" t="s">
+      <c r="B13" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="160"/>
-      <c r="D13" s="158" t="s">
+      <c r="C13" s="162"/>
+      <c r="D13" s="160" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="134"/>
-      <c r="B14" s="143"/>
-      <c r="C14" s="160"/>
-      <c r="D14" s="158"/>
+      <c r="A14" s="138"/>
+      <c r="B14" s="139"/>
+      <c r="C14" s="162"/>
+      <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="134"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="160"/>
+      <c r="A15" s="138"/>
+      <c r="B15" s="139"/>
+      <c r="C15" s="162"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="134"/>
-      <c r="B16" s="143"/>
-      <c r="C16" s="160"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="162"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="134"/>
-      <c r="B17" s="143"/>
-      <c r="C17" s="160"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="162"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134"/>
-      <c r="B18" s="143"/>
-      <c r="C18" s="160"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="143"/>
-      <c r="C19" s="160"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="162"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="134"/>
-      <c r="B20" s="143"/>
-      <c r="C20" s="160"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="139"/>
+      <c r="C20" s="162"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="160"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="162"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="134"/>
-      <c r="B22" s="143"/>
-      <c r="C22" s="160"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="162"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="160"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="162"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30748,10 +30764,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="152" t="s">
+      <c r="A32" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="155" t="s">
+      <c r="B32" s="166" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30762,26 +30778,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="153"/>
-      <c r="B33" s="156"/>
+      <c r="A33" s="164"/>
+      <c r="B33" s="167"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="153"/>
-      <c r="B34" s="156"/>
+      <c r="A34" s="164"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="153"/>
-      <c r="B35" s="156"/>
+      <c r="A35" s="164"/>
+      <c r="B35" s="167"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="154"/>
-      <c r="B36" s="157"/>
+      <c r="A36" s="165"/>
+      <c r="B36" s="168"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30810,10 +30826,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150" t="s">
+      <c r="A39" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="135" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30824,8 +30840,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="150"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="136"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30834,84 +30850,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="149" t="s">
+      <c r="A41" s="134" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="135" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="161" t="s">
+      <c r="C41" s="159" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="134" t="s">
+      <c r="D41" s="138" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="149"/>
-      <c r="B42" s="148"/>
-      <c r="C42" s="161"/>
-      <c r="D42" s="134"/>
+      <c r="A42" s="134"/>
+      <c r="B42" s="135"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="138"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="149"/>
-      <c r="B43" s="148"/>
-      <c r="C43" s="161" t="s">
+      <c r="A43" s="134"/>
+      <c r="B43" s="135"/>
+      <c r="C43" s="159" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="144" t="s">
+      <c r="D43" s="141" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="149"/>
-      <c r="B44" s="148"/>
-      <c r="C44" s="161"/>
-      <c r="D44" s="144"/>
+      <c r="A44" s="134"/>
+      <c r="B44" s="135"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="141"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="142" t="s">
+      <c r="A45" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="143" t="s">
+      <c r="B45" s="139" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="165"/>
+      <c r="C45" s="155"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="142"/>
-      <c r="B46" s="143"/>
-      <c r="C46" s="166"/>
-      <c r="D46" s="162" t="s">
+      <c r="A46" s="140"/>
+      <c r="B46" s="139"/>
+      <c r="C46" s="156"/>
+      <c r="D46" s="152" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="142"/>
-      <c r="B47" s="143"/>
-      <c r="C47" s="166"/>
-      <c r="D47" s="163"/>
+      <c r="A47" s="140"/>
+      <c r="B47" s="139"/>
+      <c r="C47" s="156"/>
+      <c r="D47" s="153"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="142"/>
-      <c r="B48" s="143"/>
-      <c r="C48" s="167"/>
-      <c r="D48" s="163"/>
+      <c r="A48" s="140"/>
+      <c r="B48" s="139"/>
+      <c r="C48" s="157"/>
+      <c r="D48" s="153"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="142"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="137"/>
-      <c r="D49" s="163"/>
+      <c r="A49" s="140"/>
+      <c r="B49" s="139"/>
+      <c r="C49" s="147"/>
+      <c r="D49" s="153"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="142"/>
-      <c r="B50" s="143"/>
-      <c r="C50" s="137"/>
-      <c r="D50" s="164"/>
+      <c r="A50" s="140"/>
+      <c r="B50" s="139"/>
+      <c r="C50" s="147"/>
+      <c r="D50" s="154"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -30934,10 +30950,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="143" t="s">
+      <c r="A53" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="143" t="s">
+      <c r="B53" s="139" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30948,8 +30964,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
+      <c r="A54" s="139"/>
+      <c r="B54" s="139"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30958,8 +30974,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="143"/>
-      <c r="B55" s="143"/>
+      <c r="A55" s="139"/>
+      <c r="B55" s="139"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30968,9 +30984,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="143"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="168" t="s">
+      <c r="A56" s="139"/>
+      <c r="B56" s="139"/>
+      <c r="C56" s="158" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30978,16 +30994,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="143"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="168"/>
+      <c r="A57" s="139"/>
+      <c r="B57" s="139"/>
+      <c r="C57" s="158"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="143"/>
-      <c r="B58" s="143"/>
+      <c r="A58" s="139"/>
+      <c r="B58" s="139"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30996,8 +31012,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="143"/>
-      <c r="B59" s="143"/>
+      <c r="A59" s="139"/>
+      <c r="B59" s="139"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31006,9 +31022,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="143"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="168" t="s">
+      <c r="A60" s="139"/>
+      <c r="B60" s="139"/>
+      <c r="C60" s="158" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31016,25 +31032,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="143"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="168"/>
+      <c r="A61" s="139"/>
+      <c r="B61" s="139"/>
+      <c r="C61" s="158"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="143"/>
-      <c r="B62" s="143"/>
-      <c r="C62" s="168"/>
+      <c r="A62" s="139"/>
+      <c r="B62" s="139"/>
+      <c r="C62" s="158"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="143"/>
-      <c r="B63" s="143"/>
-      <c r="C63" s="161" t="s">
+      <c r="A63" s="139"/>
+      <c r="B63" s="139"/>
+      <c r="C63" s="159" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31042,30 +31058,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="143"/>
-      <c r="B64" s="143"/>
-      <c r="C64" s="161"/>
-      <c r="D64" s="144" t="s">
+      <c r="A64" s="139"/>
+      <c r="B64" s="139"/>
+      <c r="C64" s="159"/>
+      <c r="D64" s="141" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="143"/>
-      <c r="B65" s="143"/>
-      <c r="C65" s="161"/>
-      <c r="D65" s="144"/>
+      <c r="A65" s="139"/>
+      <c r="B65" s="139"/>
+      <c r="C65" s="159"/>
+      <c r="D65" s="141"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="143"/>
-      <c r="B66" s="143"/>
-      <c r="C66" s="161"/>
-      <c r="D66" s="144"/>
+      <c r="A66" s="139"/>
+      <c r="B66" s="139"/>
+      <c r="C66" s="159"/>
+      <c r="D66" s="141"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="143"/>
-      <c r="B67" s="143"/>
-      <c r="C67" s="161"/>
-      <c r="D67" s="144"/>
+      <c r="A67" s="139"/>
+      <c r="B67" s="139"/>
+      <c r="C67" s="159"/>
+      <c r="D67" s="141"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31121,6 +31137,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31137,23 +31170,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31162,10 +31178,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31199,10 +31215,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="172" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="172" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="114" t="s">
@@ -31213,8 +31229,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="169"/>
-      <c r="B4" s="169"/>
+      <c r="A4" s="172"/>
+      <c r="B4" s="172"/>
       <c r="C4" s="114" t="s">
         <v>347</v>
       </c>
@@ -31231,10 +31247,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="134" t="s">
+      <c r="A6" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="173" t="s">
+      <c r="B6" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31243,8 +31259,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="134"/>
-      <c r="B7" s="174"/>
+      <c r="A7" s="138"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
@@ -31256,7 +31272,7 @@
       <c r="A8" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="106" t="s">
         <v>235</v>
       </c>
@@ -31268,7 +31284,7 @@
       <c r="A9" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="106" t="s">
         <v>22</v>
       </c>
@@ -31277,26 +31293,26 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="168" t="s">
+      <c r="A10" s="158" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="58"/>
       <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="168"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="168"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="110" t="s">
         <v>325</v>
       </c>
@@ -31308,7 +31324,7 @@
       <c r="A13" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="174"/>
+      <c r="B13" s="177"/>
       <c r="C13" s="118" t="s">
         <v>30</v>
       </c>
@@ -31318,7 +31334,7 @@
       <c r="A14" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="174"/>
+      <c r="B14" s="177"/>
       <c r="C14" s="58"/>
       <c r="D14" s="104" t="s">
         <v>259</v>
@@ -31328,7 +31344,7 @@
       <c r="A15" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B15" s="174"/>
+      <c r="B15" s="177"/>
       <c r="C15" s="118" t="s">
         <v>332</v>
       </c>
@@ -31340,7 +31356,7 @@
       <c r="A16" s="100" t="s">
         <v>351</v>
       </c>
-      <c r="B16" s="175"/>
+      <c r="B16" s="178"/>
       <c r="C16" s="118" t="s">
         <v>30</v>
       </c>
@@ -31355,10 +31371,10 @@
       <c r="D17" s="39"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="176" t="s">
+      <c r="A18" s="171" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="168" t="s">
+      <c r="B18" s="158" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="58"/>
@@ -31367,24 +31383,24 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="176"/>
-      <c r="B19" s="168"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="158"/>
       <c r="C19" s="58"/>
       <c r="D19" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="176"/>
-      <c r="B20" s="168"/>
+      <c r="A20" s="171"/>
+      <c r="B20" s="158"/>
       <c r="C20" s="58"/>
       <c r="D20" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="176"/>
-      <c r="B21" s="168"/>
+      <c r="A21" s="171"/>
+      <c r="B21" s="158"/>
       <c r="C21" s="58" t="s">
         <v>300</v>
       </c>
@@ -31393,8 +31409,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="176"/>
-      <c r="B22" s="168"/>
+      <c r="A22" s="171"/>
+      <c r="B22" s="158"/>
       <c r="C22" s="58" t="s">
         <v>328</v>
       </c>
@@ -31403,10 +31419,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="150" t="s">
+      <c r="A23" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="168" t="s">
+      <c r="B23" s="158" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
@@ -31417,16 +31433,16 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
-      <c r="B24" s="168"/>
+      <c r="A24" s="136"/>
+      <c r="B24" s="158"/>
       <c r="C24" s="58"/>
       <c r="D24" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
-      <c r="B25" s="168"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="158"/>
       <c r="C25" s="108" t="s">
         <v>329</v>
       </c>
@@ -31435,13 +31451,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="168" t="s">
+      <c r="A26" s="158" t="s">
         <v>222</v>
       </c>
-      <c r="B26" s="168" t="s">
+      <c r="B26" s="158" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="177" t="s">
+      <c r="C26" s="169" t="s">
         <v>239</v>
       </c>
       <c r="D26" s="103" t="s">
@@ -31449,17 +31465,17 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="168"/>
-      <c r="B27" s="168"/>
-      <c r="C27" s="177"/>
+      <c r="A27" s="158"/>
+      <c r="B27" s="158"/>
+      <c r="C27" s="169"/>
       <c r="D27" s="100" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="168"/>
-      <c r="B28" s="168"/>
-      <c r="C28" s="177" t="s">
+      <c r="A28" s="158"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="169" t="s">
         <v>240</v>
       </c>
       <c r="D28" s="58" t="s">
@@ -31467,16 +31483,16 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="168"/>
-      <c r="B29" s="168"/>
-      <c r="C29" s="177"/>
+      <c r="A29" s="158"/>
+      <c r="B29" s="158"/>
+      <c r="C29" s="169"/>
       <c r="D29" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="168"/>
-      <c r="B30" s="168"/>
+      <c r="A30" s="158"/>
+      <c r="B30" s="158"/>
       <c r="C30" s="105" t="s">
         <v>307</v>
       </c>
@@ -31485,8 +31501,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="168"/>
-      <c r="B31" s="168"/>
+      <c r="A31" s="158"/>
+      <c r="B31" s="158"/>
       <c r="C31" s="105">
         <v>2.1</v>
       </c>
@@ -31495,8 +31511,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="168"/>
-      <c r="B32" s="168"/>
+      <c r="A32" s="158"/>
+      <c r="B32" s="158"/>
       <c r="C32" s="105" t="s">
         <v>239</v>
       </c>
@@ -31505,8 +31521,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="168"/>
-      <c r="B33" s="168"/>
+      <c r="A33" s="158"/>
+      <c r="B33" s="158"/>
       <c r="C33" s="117" t="s">
         <v>239</v>
       </c>
@@ -31515,8 +31531,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="168"/>
-      <c r="B34" s="168"/>
+      <c r="A34" s="158"/>
+      <c r="B34" s="158"/>
       <c r="C34" s="115" t="s">
         <v>239</v>
       </c>
@@ -31525,10 +31541,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="143" t="s">
+      <c r="A35" s="139" t="s">
         <v>296</v>
       </c>
-      <c r="B35" s="168" t="s">
+      <c r="B35" s="158" t="s">
         <v>234</v>
       </c>
       <c r="C35" s="58" t="s">
@@ -31539,8 +31555,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="143"/>
-      <c r="B36" s="168"/>
+      <c r="A36" s="139"/>
+      <c r="B36" s="158"/>
       <c r="C36" s="61" t="s">
         <v>281</v>
       </c>
@@ -31549,8 +31565,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="143"/>
-      <c r="B37" s="168"/>
+      <c r="A37" s="139"/>
+      <c r="B37" s="158"/>
       <c r="C37" s="58" t="s">
         <v>350</v>
       </c>
@@ -31567,10 +31583,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="134" t="s">
+      <c r="A39" s="138" t="s">
         <v>260</v>
       </c>
-      <c r="B39" s="168" t="s">
+      <c r="B39" s="158" t="s">
         <v>234</v>
       </c>
       <c r="C39" s="58"/>
@@ -31579,8 +31595,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="134"/>
-      <c r="B40" s="168"/>
+      <c r="A40" s="138"/>
+      <c r="B40" s="158"/>
       <c r="C40" s="58"/>
       <c r="D40" s="58" t="s">
         <v>257</v>
@@ -31615,10 +31631,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="170" t="s">
+      <c r="A43" s="173" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="173" t="s">
+      <c r="B43" s="176" t="s">
         <v>234</v>
       </c>
       <c r="C43" s="58" t="s">
@@ -31629,8 +31645,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="171"/>
-      <c r="B44" s="174"/>
+      <c r="A44" s="174"/>
+      <c r="B44" s="177"/>
       <c r="C44" s="58" t="s">
         <v>270</v>
       </c>
@@ -31639,8 +31655,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="171"/>
-      <c r="B45" s="174"/>
+      <c r="A45" s="174"/>
+      <c r="B45" s="177"/>
       <c r="C45" s="58" t="s">
         <v>269</v>
       </c>
@@ -31649,8 +31665,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="171"/>
-      <c r="B46" s="174"/>
+      <c r="A46" s="174"/>
+      <c r="B46" s="177"/>
       <c r="C46" s="100" t="s">
         <v>277</v>
       </c>
@@ -31659,8 +31675,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="171"/>
-      <c r="B47" s="174"/>
+      <c r="A47" s="174"/>
+      <c r="B47" s="177"/>
       <c r="C47" s="58" t="s">
         <v>282</v>
       </c>
@@ -31669,8 +31685,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="171"/>
-      <c r="B48" s="174"/>
+      <c r="A48" s="174"/>
+      <c r="B48" s="177"/>
       <c r="C48" s="58" t="s">
         <v>283</v>
       </c>
@@ -31679,8 +31695,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="171"/>
-      <c r="B49" s="174"/>
+      <c r="A49" s="174"/>
+      <c r="B49" s="177"/>
       <c r="C49" s="100" t="s">
         <v>288</v>
       </c>
@@ -31689,8 +31705,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="171"/>
-      <c r="B50" s="174"/>
+      <c r="A50" s="174"/>
+      <c r="B50" s="177"/>
       <c r="C50" s="100" t="s">
         <v>302</v>
       </c>
@@ -31699,8 +31715,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="171"/>
-      <c r="B51" s="174"/>
+      <c r="A51" s="174"/>
+      <c r="B51" s="177"/>
       <c r="C51" s="100" t="s">
         <v>289</v>
       </c>
@@ -31709,8 +31725,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="171"/>
-      <c r="B52" s="174"/>
+      <c r="A52" s="174"/>
+      <c r="B52" s="177"/>
       <c r="C52" s="107" t="s">
         <v>244</v>
       </c>
@@ -31719,8 +31735,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="171"/>
-      <c r="B53" s="174"/>
+      <c r="A53" s="174"/>
+      <c r="B53" s="177"/>
       <c r="C53" s="108" t="s">
         <v>311</v>
       </c>
@@ -31729,8 +31745,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="171"/>
-      <c r="B54" s="174"/>
+      <c r="A54" s="174"/>
+      <c r="B54" s="177"/>
       <c r="C54" s="58" t="s">
         <v>312</v>
       </c>
@@ -31739,8 +31755,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="171"/>
-      <c r="B55" s="174"/>
+      <c r="A55" s="174"/>
+      <c r="B55" s="177"/>
       <c r="C55" s="100" t="s">
         <v>313</v>
       </c>
@@ -31749,8 +31765,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="171"/>
-      <c r="B56" s="174"/>
+      <c r="A56" s="174"/>
+      <c r="B56" s="177"/>
       <c r="C56" s="100" t="s">
         <v>315</v>
       </c>
@@ -31759,8 +31775,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="171"/>
-      <c r="B57" s="174"/>
+      <c r="A57" s="174"/>
+      <c r="B57" s="177"/>
       <c r="C57" s="100" t="s">
         <v>268</v>
       </c>
@@ -31769,8 +31785,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="171"/>
-      <c r="B58" s="174"/>
+      <c r="A58" s="174"/>
+      <c r="B58" s="177"/>
       <c r="C58" s="58" t="s">
         <v>318</v>
       </c>
@@ -31779,8 +31795,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="171"/>
-      <c r="B59" s="174"/>
+      <c r="A59" s="174"/>
+      <c r="B59" s="177"/>
       <c r="C59" s="100" t="s">
         <v>283</v>
       </c>
@@ -31789,8 +31805,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="171"/>
-      <c r="B60" s="174"/>
+      <c r="A60" s="174"/>
+      <c r="B60" s="177"/>
       <c r="C60" s="100" t="s">
         <v>319</v>
       </c>
@@ -31799,16 +31815,16 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="171"/>
-      <c r="B61" s="174"/>
+      <c r="A61" s="174"/>
+      <c r="B61" s="177"/>
       <c r="C61" s="58"/>
       <c r="D61" s="109" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="171"/>
-      <c r="B62" s="174"/>
+      <c r="A62" s="174"/>
+      <c r="B62" s="177"/>
       <c r="C62" s="100" t="s">
         <v>322</v>
       </c>
@@ -31817,8 +31833,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="171"/>
-      <c r="B63" s="174"/>
+      <c r="A63" s="174"/>
+      <c r="B63" s="177"/>
       <c r="C63" s="100" t="s">
         <v>268</v>
       </c>
@@ -31827,8 +31843,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="171"/>
-      <c r="B64" s="174"/>
+      <c r="A64" s="174"/>
+      <c r="B64" s="177"/>
       <c r="C64" s="100" t="s">
         <v>339</v>
       </c>
@@ -31837,8 +31853,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="171"/>
-      <c r="B65" s="174"/>
+      <c r="A65" s="174"/>
+      <c r="B65" s="177"/>
       <c r="C65" s="100" t="s">
         <v>340</v>
       </c>
@@ -31847,8 +31863,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="171"/>
-      <c r="B66" s="174"/>
+      <c r="A66" s="174"/>
+      <c r="B66" s="177"/>
       <c r="C66" s="100" t="s">
         <v>324</v>
       </c>
@@ -31857,8 +31873,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="171"/>
-      <c r="B67" s="174"/>
+      <c r="A67" s="174"/>
+      <c r="B67" s="177"/>
       <c r="C67" s="116" t="s">
         <v>345</v>
       </c>
@@ -31867,8 +31883,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="172"/>
-      <c r="B68" s="175"/>
+      <c r="A68" s="174"/>
+      <c r="B68" s="177"/>
       <c r="C68" s="100" t="s">
         <v>338</v>
       </c>
@@ -31877,242 +31893,236 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="58" t="s">
+      <c r="A69" s="174"/>
+      <c r="B69" s="177"/>
+      <c r="C69" s="100" t="s">
+        <v>353</v>
+      </c>
+      <c r="D69" s="100" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="175"/>
+      <c r="B70" s="178"/>
+      <c r="C70" s="180" t="s">
+        <v>356</v>
+      </c>
+      <c r="D70" s="179" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="B69" s="106" t="s">
+      <c r="B71" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="58" t="s">
+      <c r="C71" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="100" t="s">
+      <c r="D71" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="58" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B70" s="106" t="s">
+      <c r="B72" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C70" s="58" t="s">
+      <c r="C72" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D70" s="100" t="s">
+      <c r="D72" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="39" t="s">
+    <row r="73" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="44"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="44"/>
     </row>
-    <row r="72" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="99"/>
-      <c r="B72" s="67"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="79" t="s">
+    <row r="74" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="99"/>
+      <c r="B74" s="67"/>
+      <c r="C74" s="58"/>
+      <c r="D74" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="168" t="s">
+    <row r="75" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="158" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="168" t="s">
+      <c r="B75" s="158" t="s">
         <v>234</v>
       </c>
-      <c r="C73" s="106" t="s">
+      <c r="C75" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="D73" s="58" t="s">
+      <c r="D75" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="168"/>
-      <c r="B74" s="168"/>
-      <c r="C74" s="106">
-        <v>10.1</v>
-      </c>
-      <c r="D74" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="168"/>
-      <c r="B75" s="168"/>
-      <c r="C75" s="106">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D75" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="168"/>
-      <c r="B76" s="168"/>
-      <c r="C76" s="111" t="s">
-        <v>293</v>
-      </c>
-      <c r="D76" s="101" t="s">
-        <v>294</v>
+      <c r="A76" s="158"/>
+      <c r="B76" s="158"/>
+      <c r="C76" s="106">
+        <v>10.1</v>
+      </c>
+      <c r="D76" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="134" t="s">
-        <v>247</v>
-      </c>
-      <c r="B77" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C77" s="168"/>
-      <c r="D77" s="178" t="s">
-        <v>261</v>
+      <c r="A77" s="158"/>
+      <c r="B77" s="158"/>
+      <c r="C77" s="106">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D77" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="134"/>
-      <c r="B78" s="168"/>
-      <c r="C78" s="168"/>
-      <c r="D78" s="178"/>
+      <c r="A78" s="158"/>
+      <c r="B78" s="158"/>
+      <c r="C78" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="D78" s="101" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="B79" s="106" t="s">
+      <c r="A79" s="138" t="s">
+        <v>247</v>
+      </c>
+      <c r="B79" s="158" t="s">
         <v>234</v>
       </c>
-      <c r="C79" s="106" t="s">
-        <v>250</v>
-      </c>
-      <c r="D79" s="100" t="s">
-        <v>251</v>
+      <c r="C79" s="158"/>
+      <c r="D79" s="170" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="98"/>
-      <c r="D80" s="98"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="138"/>
+      <c r="B80" s="158"/>
+      <c r="C80" s="158"/>
+      <c r="D80" s="170"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="58" t="s">
-        <v>249</v>
+      <c r="A81" s="104" t="s">
+        <v>262</v>
       </c>
       <c r="B81" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C81" s="112" t="s">
-        <v>265</v>
-      </c>
-      <c r="D81" s="58" t="s">
-        <v>267</v>
+      <c r="C81" s="106" t="s">
+        <v>250</v>
+      </c>
+      <c r="D81" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="134" t="s">
-        <v>285</v>
-      </c>
-      <c r="B82" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C82" s="101" t="s">
-        <v>295</v>
-      </c>
-      <c r="D82" s="58" t="s">
-        <v>251</v>
-      </c>
+    <row r="82" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B82" s="39"/>
+      <c r="C82" s="98"/>
+      <c r="D82" s="98"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="134"/>
-      <c r="B83" s="168"/>
-      <c r="C83" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D83" s="100" t="s">
-        <v>306</v>
+      <c r="A83" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D83" s="58" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="134"/>
-      <c r="B84" s="168"/>
-      <c r="C84" s="112" t="s">
-        <v>286</v>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="138" t="s">
+        <v>285</v>
+      </c>
+      <c r="B84" s="158" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="101" t="s">
+        <v>295</v>
       </c>
       <c r="D84" s="58" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B85" s="98"/>
-      <c r="C85" s="98"/>
-      <c r="D85" s="98"/>
+      <c r="A85" s="138"/>
+      <c r="B85" s="158"/>
+      <c r="C85" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D85" s="100" t="s">
+        <v>306</v>
+      </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="151" t="s">
-        <v>58</v>
-      </c>
-      <c r="B86" s="168" t="s">
-        <v>271</v>
-      </c>
+    <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="138"/>
+      <c r="B86" s="158"/>
       <c r="C86" s="112" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="D86" s="58" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="151"/>
-      <c r="B87" s="168"/>
-      <c r="C87" s="112" t="s">
+      <c r="A87" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B87" s="98"/>
+      <c r="C87" s="98"/>
+      <c r="D87" s="98"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="137" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88" s="158" t="s">
+        <v>271</v>
+      </c>
+      <c r="C88" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D87" s="58" t="s">
+      <c r="D88" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="137"/>
+      <c r="B89" s="158"/>
+      <c r="C89" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D89" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="97" t="s">
+    <row r="90" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B88" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C88" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D88" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B89" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C89" s="58"/>
-      <c r="D89" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="97" t="s">
-        <v>60</v>
       </c>
       <c r="B90" s="106" t="s">
         <v>271</v>
@@ -32121,32 +32131,38 @@
         <v>264</v>
       </c>
       <c r="D90" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B91" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C91" s="58"/>
+      <c r="D91" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B92" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C92" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D92" s="58" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="58"/>
-      <c r="B92" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C92" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D92" s="100" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="98" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B93" s="98"/>
       <c r="C93" s="98"/>
@@ -32164,37 +32180,57 @@
         <v>274</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B95" s="98"/>
+      <c r="C95" s="98"/>
+      <c r="D95" s="98"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="58"/>
+      <c r="B96" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C96" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D96" s="100" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A43:A70"/>
+    <mergeCell ref="B43:B70"/>
+    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A79:A80"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B88:B89"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A75:A78"/>
     <mergeCell ref="A26:A34"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A43:A68"/>
-    <mergeCell ref="B43:B68"/>
-    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="B35:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
verification rule 3015 added
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="358">
   <si>
     <t>Document</t>
   </si>
@@ -2926,6 +2926,9 @@
   </si>
   <si>
     <t>code 4002, 4003, 4004, 1010</t>
+  </si>
+  <si>
+    <t>code 3015</t>
   </si>
 </sst>
 </file>
@@ -3817,6 +3820,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3862,38 +3869,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3916,6 +3893,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3935,45 +3972,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3997,9 +3995,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4404,12 +4407,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="123"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4432,12 +4435,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="121"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="123"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4477,10 +4480,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="125">
+      <c r="B7" s="127">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4494,8 +4497,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="126"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="128"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4507,8 +4510,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="123"/>
-      <c r="B9" s="126"/>
+      <c r="A9" s="125"/>
+      <c r="B9" s="128"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4520,8 +4523,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="123"/>
-      <c r="B10" s="126"/>
+      <c r="A10" s="125"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4533,8 +4536,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="123"/>
-      <c r="B11" s="126"/>
+      <c r="A11" s="125"/>
+      <c r="B11" s="128"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4546,8 +4549,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="124"/>
-      <c r="B12" s="127"/>
+      <c r="A12" s="126"/>
+      <c r="B12" s="129"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4559,10 +4562,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="130" t="s">
+      <c r="A13" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="125">
+      <c r="B13" s="127">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4576,8 +4579,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="131"/>
-      <c r="B14" s="127"/>
+      <c r="A14" s="133"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4623,12 +4626,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="119" t="s">
+      <c r="A17" s="121" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="121"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="123"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4668,21 +4671,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="119" t="s">
+      <c r="A20" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="121"/>
+      <c r="B20" s="122"/>
+      <c r="C20" s="122"/>
+      <c r="D20" s="123"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="132" t="s">
+      <c r="A21" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="129">
+      <c r="B21" s="131">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4696,8 +4699,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
-      <c r="B22" s="127"/>
+      <c r="A22" s="135"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4720,18 +4723,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
+      <c r="A24" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="120"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="121"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="123"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="128" t="s">
+      <c r="A25" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="129">
+      <c r="B25" s="131">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4745,8 +4748,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="123"/>
-      <c r="B26" s="126"/>
+      <c r="A26" s="125"/>
+      <c r="B26" s="128"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4758,8 +4761,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
-      <c r="B27" s="126"/>
+      <c r="A27" s="125"/>
+      <c r="B27" s="128"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4771,8 +4774,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="123"/>
-      <c r="B28" s="126"/>
+      <c r="A28" s="125"/>
+      <c r="B28" s="128"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4784,8 +4787,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="123"/>
-      <c r="B29" s="126"/>
+      <c r="A29" s="125"/>
+      <c r="B29" s="128"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4797,8 +4800,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="123"/>
-      <c r="B30" s="126"/>
+      <c r="A30" s="125"/>
+      <c r="B30" s="128"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4810,8 +4813,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="123"/>
-      <c r="B31" s="126"/>
+      <c r="A31" s="125"/>
+      <c r="B31" s="128"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4823,8 +4826,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="124"/>
-      <c r="B32" s="127"/>
+      <c r="A32" s="126"/>
+      <c r="B32" s="129"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4948,12 +4951,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="119" t="s">
+      <c r="A41" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="120"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="121"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="123"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5013,7 +5016,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5023,7 +5026,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5133,10 +5136,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="134" t="s">
+      <c r="A7" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="135" t="s">
+      <c r="B7" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5147,8 +5150,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="134"/>
-      <c r="B8" s="135"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="150"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5157,8 +5160,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="134"/>
-      <c r="B9" s="135"/>
+      <c r="A9" s="151"/>
+      <c r="B9" s="150"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5167,8 +5170,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="134"/>
-      <c r="B10" s="135"/>
+      <c r="A10" s="151"/>
+      <c r="B10" s="150"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5177,8 +5180,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="134"/>
-      <c r="B11" s="135"/>
+      <c r="A11" s="151"/>
+      <c r="B11" s="150"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5187,8 +5190,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="134"/>
-      <c r="B12" s="135"/>
+      <c r="A12" s="151"/>
+      <c r="B12" s="150"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5197,10 +5200,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="153" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="135" t="s">
+      <c r="B13" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5211,8 +5214,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="135"/>
+      <c r="A14" s="153"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5221,8 +5224,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="135"/>
+      <c r="A15" s="153"/>
+      <c r="B15" s="150"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5231,10 +5234,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="138" t="s">
+      <c r="A16" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="145" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5245,8 +5248,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="138"/>
-      <c r="B17" s="139"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="145"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5255,8 +5258,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
-      <c r="B18" s="139"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="145"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5265,8 +5268,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="139"/>
+      <c r="A19" s="136"/>
+      <c r="B19" s="145"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5275,8 +5278,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
-      <c r="B20" s="139"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="145"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5285,8 +5288,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="138"/>
-      <c r="B21" s="139"/>
+      <c r="A21" s="136"/>
+      <c r="B21" s="145"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5295,8 +5298,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="138"/>
-      <c r="B22" s="139"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="145"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5305,8 +5308,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="138"/>
-      <c r="B23" s="139"/>
+      <c r="A23" s="136"/>
+      <c r="B23" s="145"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5315,26 +5318,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="138"/>
-      <c r="B24" s="139"/>
-      <c r="C24" s="138" t="s">
+      <c r="A24" s="136"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="136" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="145" t="s">
+      <c r="D24" s="137" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="138"/>
-      <c r="B25" s="139"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="145"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="145"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="137"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="134" t="s">
+      <c r="A26" s="151" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="135" t="s">
+      <c r="B26" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5345,8 +5348,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="134"/>
-      <c r="B27" s="135"/>
+      <c r="A27" s="151"/>
+      <c r="B27" s="150"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5373,28 +5376,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="136" t="s">
+      <c r="A30" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="135" t="s">
+      <c r="B30" s="150" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="138" t="s">
+      <c r="C30" s="136" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="148" t="s">
+      <c r="D30" s="140" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="136"/>
-      <c r="B31" s="135"/>
-      <c r="C31" s="138"/>
-      <c r="D31" s="148"/>
+      <c r="A31" s="152"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="140"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="136"/>
-      <c r="B32" s="135"/>
+      <c r="A32" s="152"/>
+      <c r="B32" s="150"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5403,8 +5406,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="136"/>
-      <c r="B33" s="135"/>
+      <c r="A33" s="152"/>
+      <c r="B33" s="150"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5413,8 +5416,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="136"/>
-      <c r="B34" s="135"/>
+      <c r="A34" s="152"/>
+      <c r="B34" s="150"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5423,8 +5426,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="136"/>
-      <c r="B35" s="135"/>
+      <c r="A35" s="152"/>
+      <c r="B35" s="150"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5433,8 +5436,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="136"/>
-      <c r="B36" s="135"/>
+      <c r="A36" s="152"/>
+      <c r="B36" s="150"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5443,26 +5446,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="136"/>
-      <c r="B37" s="135"/>
-      <c r="C37" s="149" t="s">
+      <c r="A37" s="152"/>
+      <c r="B37" s="150"/>
+      <c r="C37" s="141" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="151" t="s">
+      <c r="D37" s="143" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="136"/>
-      <c r="B38" s="135"/>
-      <c r="C38" s="150"/>
-      <c r="D38" s="151"/>
+      <c r="A38" s="152"/>
+      <c r="B38" s="150"/>
+      <c r="C38" s="142"/>
+      <c r="D38" s="143"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="134" t="s">
+      <c r="A39" s="151" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="135" t="s">
+      <c r="B39" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5473,8 +5476,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="134"/>
-      <c r="B40" s="135"/>
+      <c r="A40" s="151"/>
+      <c r="B40" s="150"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5501,10 +5504,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="136" t="s">
+      <c r="A43" s="152" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="135" t="s">
+      <c r="B43" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5513,8 +5516,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="136"/>
-      <c r="B44" s="135"/>
+      <c r="A44" s="152"/>
+      <c r="B44" s="150"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5523,10 +5526,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="142" t="s">
+      <c r="A45" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="135" t="s">
+      <c r="B45" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5535,8 +5538,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="143"/>
-      <c r="B46" s="135"/>
+      <c r="A46" s="148"/>
+      <c r="B46" s="150"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5545,8 +5548,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="143"/>
-      <c r="B47" s="135"/>
+      <c r="A47" s="148"/>
+      <c r="B47" s="150"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5555,8 +5558,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="135"/>
+      <c r="A48" s="149"/>
+      <c r="B48" s="150"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5565,10 +5568,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="139" t="s">
+      <c r="A49" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="139" t="s">
+      <c r="B49" s="145" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9672,8 +9675,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="139"/>
-      <c r="B50" s="139"/>
+      <c r="A50" s="145"/>
+      <c r="B50" s="145"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13777,8 +13780,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="139"/>
-      <c r="B51" s="139"/>
+      <c r="A51" s="145"/>
+      <c r="B51" s="145"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17882,8 +17885,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="139"/>
-      <c r="B52" s="139"/>
+      <c r="A52" s="145"/>
+      <c r="B52" s="145"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21987,12 +21990,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="139"/>
-      <c r="B53" s="139"/>
-      <c r="C53" s="147" t="s">
+      <c r="A53" s="145"/>
+      <c r="B53" s="145"/>
+      <c r="C53" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="148" t="s">
+      <c r="D53" s="140" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26092,10 +26095,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="139"/>
-      <c r="B54" s="139"/>
-      <c r="C54" s="147"/>
-      <c r="D54" s="148"/>
+      <c r="A54" s="145"/>
+      <c r="B54" s="145"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="140"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30213,10 +30216,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="140" t="s">
+      <c r="A57" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="139" t="s">
+      <c r="B57" s="145" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30227,8 +30230,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="140"/>
-      <c r="B58" s="139"/>
+      <c r="A58" s="144"/>
+      <c r="B58" s="145"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30237,8 +30240,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="140"/>
-      <c r="B59" s="139"/>
+      <c r="A59" s="144"/>
+      <c r="B59" s="145"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30247,8 +30250,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="140"/>
-      <c r="B60" s="139"/>
+      <c r="A60" s="144"/>
+      <c r="B60" s="145"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30257,8 +30260,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="140"/>
-      <c r="B61" s="139"/>
+      <c r="A61" s="144"/>
+      <c r="B61" s="145"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30267,8 +30270,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="140"/>
-      <c r="B62" s="139"/>
+      <c r="A62" s="144"/>
+      <c r="B62" s="145"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30277,8 +30280,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="140"/>
-      <c r="B63" s="139"/>
+      <c r="A63" s="144"/>
+      <c r="B63" s="145"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30287,16 +30290,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="140"/>
-      <c r="B64" s="139"/>
+      <c r="A64" s="144"/>
+      <c r="B64" s="145"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="140"/>
-      <c r="B65" s="139"/>
+      <c r="A65" s="144"/>
+      <c r="B65" s="145"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30305,16 +30308,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="140"/>
-      <c r="B66" s="139"/>
+      <c r="A66" s="144"/>
+      <c r="B66" s="145"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="140"/>
-      <c r="B67" s="139"/>
+      <c r="A67" s="144"/>
+      <c r="B67" s="145"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30323,8 +30326,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="140"/>
-      <c r="B68" s="139"/>
+      <c r="A68" s="144"/>
+      <c r="B68" s="145"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30333,8 +30336,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="140"/>
-      <c r="B69" s="139"/>
+      <c r="A69" s="144"/>
+      <c r="B69" s="145"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30343,8 +30346,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="140"/>
-      <c r="B70" s="139"/>
+      <c r="A70" s="144"/>
+      <c r="B70" s="145"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30353,8 +30356,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="140"/>
-      <c r="B71" s="139"/>
+      <c r="A71" s="144"/>
+      <c r="B71" s="145"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30363,8 +30366,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="140"/>
-      <c r="B72" s="139"/>
+      <c r="A72" s="144"/>
+      <c r="B72" s="145"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30373,16 +30376,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="140"/>
-      <c r="B73" s="139"/>
+      <c r="A73" s="144"/>
+      <c r="B73" s="145"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="140"/>
-      <c r="B74" s="139"/>
+      <c r="A74" s="144"/>
+      <c r="B74" s="145"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30391,18 +30394,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="140"/>
-      <c r="B75" s="139"/>
-      <c r="C75" s="146"/>
-      <c r="D75" s="141" t="s">
+      <c r="A75" s="144"/>
+      <c r="B75" s="145"/>
+      <c r="C75" s="138"/>
+      <c r="D75" s="146" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="140"/>
-      <c r="B76" s="139"/>
-      <c r="C76" s="146"/>
-      <c r="D76" s="141"/>
+      <c r="A76" s="144"/>
+      <c r="B76" s="145"/>
+      <c r="C76" s="138"/>
+      <c r="D76" s="146"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30426,8 +30429,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30436,29 +30439,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30473,6 +30460,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30526,10 +30529,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="134" t="s">
+      <c r="A4" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="150" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30540,8 +30543,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="134"/>
-      <c r="B5" s="135"/>
+      <c r="A5" s="151"/>
+      <c r="B5" s="150"/>
       <c r="C5" s="161" t="s">
         <v>190</v>
       </c>
@@ -30550,58 +30553,58 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="134"/>
-      <c r="B6" s="135"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="150"/>
       <c r="C6" s="161"/>
       <c r="D6" s="160"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="134"/>
-      <c r="B7" s="135"/>
+      <c r="A7" s="151"/>
+      <c r="B7" s="150"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="134"/>
-      <c r="B8" s="135"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="150"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="134"/>
-      <c r="B9" s="135"/>
+      <c r="A9" s="151"/>
+      <c r="B9" s="150"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="137" t="s">
+      <c r="A10" s="153" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="135" t="s">
+      <c r="B10" s="150" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="159"/>
+      <c r="C10" s="163"/>
       <c r="D10" s="160" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="135"/>
-      <c r="C11" s="159"/>
+      <c r="A11" s="153"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="163"/>
       <c r="D11" s="160"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="135"/>
-      <c r="C12" s="159"/>
+      <c r="A12" s="153"/>
+      <c r="B12" s="150"/>
+      <c r="C12" s="163"/>
       <c r="D12" s="160"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="145" t="s">
         <v>185</v>
       </c>
       <c r="C13" s="162"/>
@@ -30610,62 +30613,62 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="138"/>
-      <c r="B14" s="139"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="145"/>
       <c r="C14" s="162"/>
       <c r="D14" s="160"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="138"/>
-      <c r="B15" s="139"/>
+      <c r="A15" s="136"/>
+      <c r="B15" s="145"/>
       <c r="C15" s="162"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="138"/>
-      <c r="B16" s="139"/>
+      <c r="A16" s="136"/>
+      <c r="B16" s="145"/>
       <c r="C16" s="162"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="138"/>
-      <c r="B17" s="139"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="145"/>
       <c r="C17" s="162"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
-      <c r="B18" s="139"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="145"/>
       <c r="C18" s="162"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
-      <c r="B19" s="139"/>
+      <c r="A19" s="136"/>
+      <c r="B19" s="145"/>
       <c r="C19" s="162"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
-      <c r="B20" s="139"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="145"/>
       <c r="C20" s="162"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="138"/>
-      <c r="B21" s="139"/>
+      <c r="A21" s="136"/>
+      <c r="B21" s="145"/>
       <c r="C21" s="162"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="138"/>
-      <c r="B22" s="139"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="145"/>
       <c r="C22" s="162"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="138"/>
-      <c r="B23" s="139"/>
+      <c r="A23" s="136"/>
+      <c r="B23" s="145"/>
       <c r="C23" s="162"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
@@ -30764,10 +30767,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="163" t="s">
+      <c r="A32" s="154" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="166" t="s">
+      <c r="B32" s="157" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30778,26 +30781,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="164"/>
-      <c r="B33" s="167"/>
+      <c r="A33" s="155"/>
+      <c r="B33" s="158"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="164"/>
-      <c r="B34" s="167"/>
+      <c r="A34" s="155"/>
+      <c r="B34" s="158"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="164"/>
-      <c r="B35" s="167"/>
+      <c r="A35" s="155"/>
+      <c r="B35" s="158"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="165"/>
-      <c r="B36" s="168"/>
+      <c r="A36" s="156"/>
+      <c r="B36" s="159"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30826,10 +30829,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="136" t="s">
+      <c r="A39" s="152" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="135" t="s">
+      <c r="B39" s="150" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30840,8 +30843,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="136"/>
-      <c r="B40" s="135"/>
+      <c r="A40" s="152"/>
+      <c r="B40" s="150"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30850,84 +30853,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="134" t="s">
+      <c r="A41" s="151" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="135" t="s">
+      <c r="B41" s="150" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="159" t="s">
+      <c r="C41" s="163" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="138" t="s">
+      <c r="D41" s="136" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="134"/>
-      <c r="B42" s="135"/>
-      <c r="C42" s="159"/>
-      <c r="D42" s="138"/>
+      <c r="A42" s="151"/>
+      <c r="B42" s="150"/>
+      <c r="C42" s="163"/>
+      <c r="D42" s="136"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="134"/>
-      <c r="B43" s="135"/>
-      <c r="C43" s="159" t="s">
+      <c r="A43" s="151"/>
+      <c r="B43" s="150"/>
+      <c r="C43" s="163" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="141" t="s">
+      <c r="D43" s="146" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="134"/>
-      <c r="B44" s="135"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="141"/>
+      <c r="A44" s="151"/>
+      <c r="B44" s="150"/>
+      <c r="C44" s="163"/>
+      <c r="D44" s="146"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="140" t="s">
+      <c r="A45" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="139" t="s">
+      <c r="B45" s="145" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="155"/>
+      <c r="C45" s="167"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="140"/>
-      <c r="B46" s="139"/>
-      <c r="C46" s="156"/>
-      <c r="D46" s="152" t="s">
+      <c r="A46" s="144"/>
+      <c r="B46" s="145"/>
+      <c r="C46" s="168"/>
+      <c r="D46" s="164" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="140"/>
-      <c r="B47" s="139"/>
-      <c r="C47" s="156"/>
-      <c r="D47" s="153"/>
+      <c r="A47" s="144"/>
+      <c r="B47" s="145"/>
+      <c r="C47" s="168"/>
+      <c r="D47" s="165"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="140"/>
-      <c r="B48" s="139"/>
-      <c r="C48" s="157"/>
-      <c r="D48" s="153"/>
+      <c r="A48" s="144"/>
+      <c r="B48" s="145"/>
+      <c r="C48" s="169"/>
+      <c r="D48" s="165"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="140"/>
-      <c r="B49" s="139"/>
-      <c r="C49" s="147"/>
-      <c r="D49" s="153"/>
+      <c r="A49" s="144"/>
+      <c r="B49" s="145"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="165"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="140"/>
-      <c r="B50" s="139"/>
-      <c r="C50" s="147"/>
-      <c r="D50" s="154"/>
+      <c r="A50" s="144"/>
+      <c r="B50" s="145"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="166"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -30950,10 +30953,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="139" t="s">
+      <c r="A53" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="139" t="s">
+      <c r="B53" s="145" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30964,8 +30967,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="139"/>
-      <c r="B54" s="139"/>
+      <c r="A54" s="145"/>
+      <c r="B54" s="145"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30974,8 +30977,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="139"/>
-      <c r="B55" s="139"/>
+      <c r="A55" s="145"/>
+      <c r="B55" s="145"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30984,9 +30987,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="139"/>
-      <c r="B56" s="139"/>
-      <c r="C56" s="158" t="s">
+      <c r="A56" s="145"/>
+      <c r="B56" s="145"/>
+      <c r="C56" s="170" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30994,16 +30997,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="139"/>
-      <c r="B57" s="139"/>
-      <c r="C57" s="158"/>
+      <c r="A57" s="145"/>
+      <c r="B57" s="145"/>
+      <c r="C57" s="170"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="139"/>
-      <c r="B58" s="139"/>
+      <c r="A58" s="145"/>
+      <c r="B58" s="145"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31012,8 +31015,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="139"/>
-      <c r="B59" s="139"/>
+      <c r="A59" s="145"/>
+      <c r="B59" s="145"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31022,9 +31025,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="139"/>
-      <c r="B60" s="139"/>
-      <c r="C60" s="158" t="s">
+      <c r="A60" s="145"/>
+      <c r="B60" s="145"/>
+      <c r="C60" s="170" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31032,25 +31035,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="139"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="158"/>
+      <c r="A61" s="145"/>
+      <c r="B61" s="145"/>
+      <c r="C61" s="170"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="139"/>
-      <c r="B62" s="139"/>
-      <c r="C62" s="158"/>
+      <c r="A62" s="145"/>
+      <c r="B62" s="145"/>
+      <c r="C62" s="170"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="139"/>
-      <c r="B63" s="139"/>
-      <c r="C63" s="159" t="s">
+      <c r="A63" s="145"/>
+      <c r="B63" s="145"/>
+      <c r="C63" s="163" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31058,30 +31061,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="139"/>
-      <c r="B64" s="139"/>
-      <c r="C64" s="159"/>
-      <c r="D64" s="141" t="s">
+      <c r="A64" s="145"/>
+      <c r="B64" s="145"/>
+      <c r="C64" s="163"/>
+      <c r="D64" s="146" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="139"/>
-      <c r="B65" s="139"/>
-      <c r="C65" s="159"/>
-      <c r="D65" s="141"/>
+      <c r="A65" s="145"/>
+      <c r="B65" s="145"/>
+      <c r="C65" s="163"/>
+      <c r="D65" s="146"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="139"/>
-      <c r="B66" s="139"/>
-      <c r="C66" s="159"/>
-      <c r="D66" s="141"/>
+      <c r="A66" s="145"/>
+      <c r="B66" s="145"/>
+      <c r="C66" s="163"/>
+      <c r="D66" s="146"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="139"/>
-      <c r="B67" s="139"/>
-      <c r="C67" s="159"/>
-      <c r="D67" s="141"/>
+      <c r="A67" s="145"/>
+      <c r="B67" s="145"/>
+      <c r="C67" s="163"/>
+      <c r="D67" s="146"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31137,23 +31140,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31170,6 +31156,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31178,10 +31181,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31215,10 +31218,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="172" t="s">
+      <c r="A3" s="171" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="172" t="s">
+      <c r="B3" s="171" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="114" t="s">
@@ -31229,8 +31232,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="172"/>
-      <c r="B4" s="172"/>
+      <c r="A4" s="171"/>
+      <c r="B4" s="171"/>
       <c r="C4" s="114" t="s">
         <v>347</v>
       </c>
@@ -31247,10 +31250,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="138" t="s">
+      <c r="A6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31259,8 +31262,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="138"/>
-      <c r="B7" s="177"/>
+      <c r="A7" s="136"/>
+      <c r="B7" s="176"/>
       <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
@@ -31272,7 +31275,7 @@
       <c r="A8" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="176"/>
       <c r="C8" s="106" t="s">
         <v>235</v>
       </c>
@@ -31284,7 +31287,7 @@
       <c r="A9" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="176"/>
       <c r="C9" s="106" t="s">
         <v>22</v>
       </c>
@@ -31293,26 +31296,26 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="170" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="58"/>
       <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="158"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="110" t="s">
         <v>325</v>
       </c>
@@ -31324,7 +31327,7 @@
       <c r="A13" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="177"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="118" t="s">
         <v>30</v>
       </c>
@@ -31334,7 +31337,7 @@
       <c r="A14" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="177"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="58"/>
       <c r="D14" s="104" t="s">
         <v>259</v>
@@ -31344,7 +31347,7 @@
       <c r="A15" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B15" s="177"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="118" t="s">
         <v>332</v>
       </c>
@@ -31356,7 +31359,7 @@
       <c r="A16" s="100" t="s">
         <v>351</v>
       </c>
-      <c r="B16" s="178"/>
+      <c r="B16" s="177"/>
       <c r="C16" s="118" t="s">
         <v>30</v>
       </c>
@@ -31371,10 +31374,10 @@
       <c r="D17" s="39"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="171" t="s">
+      <c r="A18" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="170" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="58"/>
@@ -31383,24 +31386,24 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="171"/>
-      <c r="B19" s="158"/>
+      <c r="A19" s="178"/>
+      <c r="B19" s="170"/>
       <c r="C19" s="58"/>
       <c r="D19" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="171"/>
-      <c r="B20" s="158"/>
+      <c r="A20" s="178"/>
+      <c r="B20" s="170"/>
       <c r="C20" s="58"/>
       <c r="D20" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="171"/>
-      <c r="B21" s="158"/>
+      <c r="A21" s="178"/>
+      <c r="B21" s="170"/>
       <c r="C21" s="58" t="s">
         <v>300</v>
       </c>
@@ -31409,8 +31412,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="171"/>
-      <c r="B22" s="158"/>
+      <c r="A22" s="178"/>
+      <c r="B22" s="170"/>
       <c r="C22" s="58" t="s">
         <v>328</v>
       </c>
@@ -31419,10 +31422,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="136" t="s">
+      <c r="A23" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="158" t="s">
+      <c r="B23" s="170" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
@@ -31433,16 +31436,16 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="136"/>
-      <c r="B24" s="158"/>
+      <c r="A24" s="152"/>
+      <c r="B24" s="170"/>
       <c r="C24" s="58"/>
       <c r="D24" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="136"/>
-      <c r="B25" s="158"/>
+      <c r="A25" s="152"/>
+      <c r="B25" s="170"/>
       <c r="C25" s="108" t="s">
         <v>329</v>
       </c>
@@ -31451,13 +31454,13 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="158" t="s">
+      <c r="A26" s="170" t="s">
         <v>222</v>
       </c>
-      <c r="B26" s="158" t="s">
+      <c r="B26" s="170" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="169" t="s">
+      <c r="C26" s="179" t="s">
         <v>239</v>
       </c>
       <c r="D26" s="103" t="s">
@@ -31465,17 +31468,17 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="158"/>
-      <c r="B27" s="158"/>
-      <c r="C27" s="169"/>
+      <c r="A27" s="170"/>
+      <c r="B27" s="170"/>
+      <c r="C27" s="179"/>
       <c r="D27" s="100" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="158"/>
-      <c r="B28" s="158"/>
-      <c r="C28" s="169" t="s">
+      <c r="A28" s="170"/>
+      <c r="B28" s="170"/>
+      <c r="C28" s="179" t="s">
         <v>240</v>
       </c>
       <c r="D28" s="58" t="s">
@@ -31483,16 +31486,16 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="158"/>
-      <c r="B29" s="158"/>
-      <c r="C29" s="169"/>
+      <c r="A29" s="170"/>
+      <c r="B29" s="170"/>
+      <c r="C29" s="179"/>
       <c r="D29" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="158"/>
-      <c r="B30" s="158"/>
+      <c r="A30" s="170"/>
+      <c r="B30" s="170"/>
       <c r="C30" s="105" t="s">
         <v>307</v>
       </c>
@@ -31501,8 +31504,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="158"/>
-      <c r="B31" s="158"/>
+      <c r="A31" s="170"/>
+      <c r="B31" s="170"/>
       <c r="C31" s="105">
         <v>2.1</v>
       </c>
@@ -31511,8 +31514,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="158"/>
-      <c r="B32" s="158"/>
+      <c r="A32" s="170"/>
+      <c r="B32" s="170"/>
       <c r="C32" s="105" t="s">
         <v>239</v>
       </c>
@@ -31521,8 +31524,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="158"/>
-      <c r="B33" s="158"/>
+      <c r="A33" s="170"/>
+      <c r="B33" s="170"/>
       <c r="C33" s="117" t="s">
         <v>239</v>
       </c>
@@ -31531,8 +31534,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="158"/>
-      <c r="B34" s="158"/>
+      <c r="A34" s="170"/>
+      <c r="B34" s="170"/>
       <c r="C34" s="115" t="s">
         <v>239</v>
       </c>
@@ -31541,10 +31544,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="139" t="s">
+      <c r="A35" s="145" t="s">
         <v>296</v>
       </c>
-      <c r="B35" s="158" t="s">
+      <c r="B35" s="170" t="s">
         <v>234</v>
       </c>
       <c r="C35" s="58" t="s">
@@ -31555,8 +31558,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="139"/>
-      <c r="B36" s="158"/>
+      <c r="A36" s="145"/>
+      <c r="B36" s="170"/>
       <c r="C36" s="61" t="s">
         <v>281</v>
       </c>
@@ -31565,8 +31568,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="139"/>
-      <c r="B37" s="158"/>
+      <c r="A37" s="145"/>
+      <c r="B37" s="170"/>
       <c r="C37" s="58" t="s">
         <v>350</v>
       </c>
@@ -31583,10 +31586,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="138" t="s">
+      <c r="A39" s="136" t="s">
         <v>260</v>
       </c>
-      <c r="B39" s="158" t="s">
+      <c r="B39" s="170" t="s">
         <v>234</v>
       </c>
       <c r="C39" s="58"/>
@@ -31595,8 +31598,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="138"/>
-      <c r="B40" s="158"/>
+      <c r="A40" s="136"/>
+      <c r="B40" s="170"/>
       <c r="C40" s="58"/>
       <c r="D40" s="58" t="s">
         <v>257</v>
@@ -31631,10 +31634,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="173" t="s">
+      <c r="A43" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="176" t="s">
+      <c r="B43" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C43" s="58" t="s">
@@ -31645,8 +31648,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="174"/>
-      <c r="B44" s="177"/>
+      <c r="A44" s="173"/>
+      <c r="B44" s="176"/>
       <c r="C44" s="58" t="s">
         <v>270</v>
       </c>
@@ -31655,8 +31658,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="174"/>
-      <c r="B45" s="177"/>
+      <c r="A45" s="173"/>
+      <c r="B45" s="176"/>
       <c r="C45" s="58" t="s">
         <v>269</v>
       </c>
@@ -31665,8 +31668,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="174"/>
-      <c r="B46" s="177"/>
+      <c r="A46" s="173"/>
+      <c r="B46" s="176"/>
       <c r="C46" s="100" t="s">
         <v>277</v>
       </c>
@@ -31675,8 +31678,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="174"/>
-      <c r="B47" s="177"/>
+      <c r="A47" s="173"/>
+      <c r="B47" s="176"/>
       <c r="C47" s="58" t="s">
         <v>282</v>
       </c>
@@ -31685,8 +31688,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="174"/>
-      <c r="B48" s="177"/>
+      <c r="A48" s="173"/>
+      <c r="B48" s="176"/>
       <c r="C48" s="58" t="s">
         <v>283</v>
       </c>
@@ -31695,8 +31698,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="174"/>
-      <c r="B49" s="177"/>
+      <c r="A49" s="173"/>
+      <c r="B49" s="176"/>
       <c r="C49" s="100" t="s">
         <v>288</v>
       </c>
@@ -31705,8 +31708,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="174"/>
-      <c r="B50" s="177"/>
+      <c r="A50" s="173"/>
+      <c r="B50" s="176"/>
       <c r="C50" s="100" t="s">
         <v>302</v>
       </c>
@@ -31715,8 +31718,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="174"/>
-      <c r="B51" s="177"/>
+      <c r="A51" s="173"/>
+      <c r="B51" s="176"/>
       <c r="C51" s="100" t="s">
         <v>289</v>
       </c>
@@ -31725,8 +31728,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="174"/>
-      <c r="B52" s="177"/>
+      <c r="A52" s="173"/>
+      <c r="B52" s="176"/>
       <c r="C52" s="107" t="s">
         <v>244</v>
       </c>
@@ -31735,8 +31738,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="174"/>
-      <c r="B53" s="177"/>
+      <c r="A53" s="173"/>
+      <c r="B53" s="176"/>
       <c r="C53" s="108" t="s">
         <v>311</v>
       </c>
@@ -31745,8 +31748,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="174"/>
-      <c r="B54" s="177"/>
+      <c r="A54" s="173"/>
+      <c r="B54" s="176"/>
       <c r="C54" s="58" t="s">
         <v>312</v>
       </c>
@@ -31755,8 +31758,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="174"/>
-      <c r="B55" s="177"/>
+      <c r="A55" s="173"/>
+      <c r="B55" s="176"/>
       <c r="C55" s="100" t="s">
         <v>313</v>
       </c>
@@ -31765,8 +31768,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="174"/>
-      <c r="B56" s="177"/>
+      <c r="A56" s="173"/>
+      <c r="B56" s="176"/>
       <c r="C56" s="100" t="s">
         <v>315</v>
       </c>
@@ -31775,8 +31778,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="174"/>
-      <c r="B57" s="177"/>
+      <c r="A57" s="173"/>
+      <c r="B57" s="176"/>
       <c r="C57" s="100" t="s">
         <v>268</v>
       </c>
@@ -31785,8 +31788,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="174"/>
-      <c r="B58" s="177"/>
+      <c r="A58" s="173"/>
+      <c r="B58" s="176"/>
       <c r="C58" s="58" t="s">
         <v>318</v>
       </c>
@@ -31795,8 +31798,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="174"/>
-      <c r="B59" s="177"/>
+      <c r="A59" s="173"/>
+      <c r="B59" s="176"/>
       <c r="C59" s="100" t="s">
         <v>283</v>
       </c>
@@ -31805,8 +31808,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="174"/>
-      <c r="B60" s="177"/>
+      <c r="A60" s="173"/>
+      <c r="B60" s="176"/>
       <c r="C60" s="100" t="s">
         <v>319</v>
       </c>
@@ -31815,16 +31818,16 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="174"/>
-      <c r="B61" s="177"/>
+      <c r="A61" s="173"/>
+      <c r="B61" s="176"/>
       <c r="C61" s="58"/>
       <c r="D61" s="109" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="174"/>
-      <c r="B62" s="177"/>
+      <c r="A62" s="173"/>
+      <c r="B62" s="176"/>
       <c r="C62" s="100" t="s">
         <v>322</v>
       </c>
@@ -31833,8 +31836,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="174"/>
-      <c r="B63" s="177"/>
+      <c r="A63" s="173"/>
+      <c r="B63" s="176"/>
       <c r="C63" s="100" t="s">
         <v>268</v>
       </c>
@@ -31843,8 +31846,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="174"/>
-      <c r="B64" s="177"/>
+      <c r="A64" s="173"/>
+      <c r="B64" s="176"/>
       <c r="C64" s="100" t="s">
         <v>339</v>
       </c>
@@ -31853,8 +31856,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="174"/>
-      <c r="B65" s="177"/>
+      <c r="A65" s="173"/>
+      <c r="B65" s="176"/>
       <c r="C65" s="100" t="s">
         <v>340</v>
       </c>
@@ -31863,8 +31866,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="174"/>
-      <c r="B66" s="177"/>
+      <c r="A66" s="173"/>
+      <c r="B66" s="176"/>
       <c r="C66" s="100" t="s">
         <v>324</v>
       </c>
@@ -31873,8 +31876,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="174"/>
-      <c r="B67" s="177"/>
+      <c r="A67" s="173"/>
+      <c r="B67" s="176"/>
       <c r="C67" s="116" t="s">
         <v>345</v>
       </c>
@@ -31883,8 +31886,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="174"/>
-      <c r="B68" s="177"/>
+      <c r="A68" s="173"/>
+      <c r="B68" s="176"/>
       <c r="C68" s="100" t="s">
         <v>338</v>
       </c>
@@ -31893,8 +31896,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="174"/>
-      <c r="B69" s="177"/>
+      <c r="A69" s="173"/>
+      <c r="B69" s="176"/>
       <c r="C69" s="100" t="s">
         <v>353</v>
       </c>
@@ -31903,32 +31906,28 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="175"/>
-      <c r="B70" s="178"/>
-      <c r="C70" s="180" t="s">
+      <c r="A70" s="173"/>
+      <c r="B70" s="176"/>
+      <c r="C70" s="120" t="s">
         <v>356</v>
       </c>
-      <c r="D70" s="179" t="s">
+      <c r="D70" s="119" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B71" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C71" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="100" t="s">
-        <v>274</v>
+      <c r="A71" s="174"/>
+      <c r="B71" s="177"/>
+      <c r="C71" s="116" t="s">
+        <v>357</v>
+      </c>
+      <c r="D71" s="116" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="58" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B72" s="106" t="s">
         <v>234</v>
@@ -31940,297 +31939,311 @@
         <v>274</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="39" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B73" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="100" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="44"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="44"/>
     </row>
-    <row r="74" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="99"/>
-      <c r="B74" s="67"/>
-      <c r="C74" s="58"/>
-      <c r="D74" s="79" t="s">
+    <row r="75" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="99"/>
+      <c r="B75" s="67"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="158" t="s">
+    <row r="76" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="170" t="s">
         <v>84</v>
       </c>
-      <c r="B75" s="158" t="s">
+      <c r="B76" s="170" t="s">
         <v>234</v>
       </c>
-      <c r="C75" s="106" t="s">
+      <c r="C76" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="D75" s="58" t="s">
+      <c r="D76" s="58" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="158"/>
-      <c r="B76" s="158"/>
-      <c r="C76" s="106">
-        <v>10.1</v>
-      </c>
-      <c r="D76" s="58" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="158"/>
-      <c r="B77" s="158"/>
+      <c r="A77" s="170"/>
+      <c r="B77" s="170"/>
       <c r="C77" s="106">
-        <v>10.199999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="D77" s="58" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="158"/>
-      <c r="B78" s="158"/>
-      <c r="C78" s="111" t="s">
-        <v>293</v>
-      </c>
-      <c r="D78" s="101" t="s">
-        <v>294</v>
+      <c r="A78" s="170"/>
+      <c r="B78" s="170"/>
+      <c r="C78" s="106">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D78" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="138" t="s">
-        <v>247</v>
-      </c>
-      <c r="B79" s="158" t="s">
-        <v>234</v>
-      </c>
-      <c r="C79" s="158"/>
-      <c r="D79" s="170" t="s">
-        <v>261</v>
+      <c r="A79" s="170"/>
+      <c r="B79" s="170"/>
+      <c r="C79" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="D79" s="101" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="138"/>
-      <c r="B80" s="158"/>
-      <c r="C80" s="158"/>
-      <c r="D80" s="170"/>
+      <c r="A80" s="136" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" s="170" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" s="170"/>
+      <c r="D80" s="180" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="104" t="s">
+      <c r="A81" s="136"/>
+      <c r="B81" s="170"/>
+      <c r="C81" s="170"/>
+      <c r="D81" s="180"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="B81" s="106" t="s">
+      <c r="B82" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C81" s="106" t="s">
+      <c r="C82" s="106" t="s">
         <v>250</v>
       </c>
-      <c r="D81" s="100" t="s">
+      <c r="D82" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="95" t="s">
+    <row r="83" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B82" s="39"/>
-      <c r="C82" s="98"/>
-      <c r="D82" s="98"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B83" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C83" s="112" t="s">
-        <v>265</v>
-      </c>
-      <c r="D83" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="B83" s="39"/>
+      <c r="C83" s="98"/>
+      <c r="D83" s="98"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="138" t="s">
-        <v>285</v>
-      </c>
-      <c r="B84" s="158" t="s">
+      <c r="A84" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C84" s="101" t="s">
-        <v>295</v>
+      <c r="C84" s="112" t="s">
+        <v>265</v>
       </c>
       <c r="D84" s="58" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="138"/>
-      <c r="B85" s="158"/>
-      <c r="C85" s="58" t="s">
+      <c r="A85" s="136" t="s">
+        <v>285</v>
+      </c>
+      <c r="B85" s="170" t="s">
+        <v>234</v>
+      </c>
+      <c r="C85" s="101" t="s">
+        <v>295</v>
+      </c>
+      <c r="D85" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="136"/>
+      <c r="B86" s="170"/>
+      <c r="C86" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D85" s="100" t="s">
+      <c r="D86" s="100" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="138"/>
-      <c r="B86" s="158"/>
-      <c r="C86" s="112" t="s">
+    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="136"/>
+      <c r="B87" s="170"/>
+      <c r="C87" s="112" t="s">
         <v>286</v>
       </c>
-      <c r="D86" s="58" t="s">
+      <c r="D87" s="58" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B87" s="98"/>
-      <c r="C87" s="98"/>
-      <c r="D87" s="98"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="137" t="s">
-        <v>58</v>
-      </c>
-      <c r="B88" s="158" t="s">
-        <v>271</v>
-      </c>
-      <c r="C88" s="112" t="s">
-        <v>265</v>
-      </c>
-      <c r="D88" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="A88" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B88" s="98"/>
+      <c r="C88" s="98"/>
+      <c r="D88" s="98"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="137"/>
-      <c r="B89" s="158"/>
+      <c r="A89" s="153" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="170" t="s">
+        <v>271</v>
+      </c>
       <c r="C89" s="112" t="s">
         <v>265</v>
       </c>
       <c r="D89" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="153"/>
+      <c r="B90" s="170"/>
+      <c r="C90" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="97" t="s">
+    <row r="91" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B90" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C90" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D90" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="58" t="s">
-        <v>291</v>
       </c>
       <c r="B91" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C91" s="58"/>
-      <c r="D91" s="61" t="s">
-        <v>292</v>
+      <c r="C91" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D91" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="97" t="s">
-        <v>60</v>
+      <c r="A92" s="58" t="s">
+        <v>291</v>
       </c>
       <c r="B92" s="106" t="s">
         <v>271</v>
       </c>
-      <c r="C92" s="61" t="s">
+      <c r="C92" s="58"/>
+      <c r="D92" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C93" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D92" s="58" t="s">
+      <c r="D93" s="58" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B93" s="98"/>
-      <c r="C93" s="98"/>
-      <c r="D93" s="98"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="58"/>
-      <c r="B94" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C94" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D94" s="100" t="s">
-        <v>274</v>
-      </c>
+      <c r="A94" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B94" s="98"/>
+      <c r="C94" s="98"/>
+      <c r="D94" s="98"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="98" t="s">
-        <v>279</v>
-      </c>
-      <c r="B95" s="98"/>
-      <c r="C95" s="98"/>
-      <c r="D95" s="98"/>
+      <c r="A95" s="58"/>
+      <c r="B95" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C95" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D95" s="100" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="58"/>
-      <c r="B96" s="106" t="s">
+      <c r="A96" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B96" s="98"/>
+      <c r="C96" s="98"/>
+      <c r="D96" s="98"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="58"/>
+      <c r="B97" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C96" s="58" t="s">
+      <c r="C97" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D96" s="100" t="s">
+      <c r="D97" s="100" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A43:A70"/>
-    <mergeCell ref="B43:B70"/>
-    <mergeCell ref="B6:B16"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A80:A81"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B89:B90"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A76:A79"/>
     <mergeCell ref="A26:A34"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A43:A71"/>
+    <mergeCell ref="B43:B71"/>
+    <mergeCell ref="B6:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
edits to schema files
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="364">
   <si>
     <t>Document</t>
   </si>
@@ -2929,6 +2929,24 @@
   </si>
   <si>
     <t>code 3015</t>
+  </si>
+  <si>
+    <t>code 2012, 2013</t>
+  </si>
+  <si>
+    <t>Payroll Submission</t>
+  </si>
+  <si>
+    <t>line item ID specified to be within same payroll run</t>
+  </si>
+  <si>
+    <t>newRPN request</t>
+  </si>
+  <si>
+    <t>removed typo from schema location namespace in example</t>
+  </si>
+  <si>
+    <t>removed typo from PRSIExempt tag in example</t>
   </si>
 </sst>
 </file>
@@ -3512,7 +3530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3824,6 +3842,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3869,8 +3896,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3893,35 +3950,38 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3941,37 +4001,13 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3994,15 +4030,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4407,12 +4434,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4435,12 +4462,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="123"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="126"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4480,10 +4507,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="127">
+      <c r="B7" s="130">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4497,8 +4524,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="125"/>
-      <c r="B8" s="128"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4510,8 +4537,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
-      <c r="B9" s="128"/>
+      <c r="A9" s="128"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4523,8 +4550,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
-      <c r="B10" s="128"/>
+      <c r="A10" s="128"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4536,8 +4563,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
-      <c r="B11" s="128"/>
+      <c r="A11" s="128"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4549,8 +4576,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="126"/>
-      <c r="B12" s="129"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="132"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4562,10 +4589,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="135" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="127">
+      <c r="B13" s="130">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4579,8 +4606,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="133"/>
-      <c r="B14" s="129"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4626,12 +4653,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="121" t="s">
+      <c r="A17" s="124" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="122"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="123"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="126"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4671,21 +4698,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="122"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="123"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="126"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="134" t="s">
+      <c r="A21" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="131">
+      <c r="B21" s="134">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4699,8 +4726,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="135"/>
-      <c r="B22" s="129"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4723,18 +4750,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="122"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="123"/>
+      <c r="B24" s="125"/>
+      <c r="C24" s="125"/>
+      <c r="D24" s="126"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="130" t="s">
+      <c r="A25" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="131">
+      <c r="B25" s="134">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4748,8 +4775,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="125"/>
-      <c r="B26" s="128"/>
+      <c r="A26" s="128"/>
+      <c r="B26" s="131"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4761,8 +4788,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="125"/>
-      <c r="B27" s="128"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="131"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4774,8 +4801,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="128"/>
+      <c r="A28" s="128"/>
+      <c r="B28" s="131"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4787,8 +4814,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="125"/>
-      <c r="B29" s="128"/>
+      <c r="A29" s="128"/>
+      <c r="B29" s="131"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4800,8 +4827,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="125"/>
-      <c r="B30" s="128"/>
+      <c r="A30" s="128"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4813,8 +4840,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
-      <c r="B31" s="128"/>
+      <c r="A31" s="128"/>
+      <c r="B31" s="131"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4826,8 +4853,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="126"/>
-      <c r="B32" s="129"/>
+      <c r="A32" s="129"/>
+      <c r="B32" s="132"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4951,12 +4978,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="122"/>
-      <c r="C41" s="122"/>
-      <c r="D41" s="123"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="125"/>
+      <c r="D41" s="126"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5016,7 +5043,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5026,7 +5053,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5136,10 +5163,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="140" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5150,8 +5177,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="151"/>
-      <c r="B8" s="150"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="140"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5160,8 +5187,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="151"/>
-      <c r="B9" s="150"/>
+      <c r="A9" s="139"/>
+      <c r="B9" s="140"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5170,8 +5197,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="151"/>
-      <c r="B10" s="150"/>
+      <c r="A10" s="139"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5180,8 +5207,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
-      <c r="B11" s="150"/>
+      <c r="A11" s="139"/>
+      <c r="B11" s="140"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5190,8 +5217,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
-      <c r="B12" s="150"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5200,10 +5227,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="153" t="s">
+      <c r="A13" s="142" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="150" t="s">
+      <c r="B13" s="140" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5214,8 +5241,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153"/>
-      <c r="B14" s="150"/>
+      <c r="A14" s="142"/>
+      <c r="B14" s="140"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5224,8 +5251,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="153"/>
-      <c r="B15" s="150"/>
+      <c r="A15" s="142"/>
+      <c r="B15" s="140"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5234,10 +5261,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="136" t="s">
+      <c r="A16" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="145" t="s">
+      <c r="B16" s="144" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5248,8 +5275,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="136"/>
-      <c r="B17" s="145"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="144"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5258,8 +5285,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="136"/>
-      <c r="B18" s="145"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="144"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5268,8 +5295,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="136"/>
-      <c r="B19" s="145"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="144"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5278,8 +5305,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="136"/>
-      <c r="B20" s="145"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="144"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5288,8 +5315,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="136"/>
-      <c r="B21" s="145"/>
+      <c r="A21" s="143"/>
+      <c r="B21" s="144"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5298,8 +5325,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="136"/>
-      <c r="B22" s="145"/>
+      <c r="A22" s="143"/>
+      <c r="B22" s="144"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5308,8 +5335,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="136"/>
-      <c r="B23" s="145"/>
+      <c r="A23" s="143"/>
+      <c r="B23" s="144"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5318,26 +5345,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="136"/>
-      <c r="B24" s="145"/>
-      <c r="C24" s="136" t="s">
+      <c r="A24" s="143"/>
+      <c r="B24" s="144"/>
+      <c r="C24" s="143" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="137" t="s">
+      <c r="D24" s="150" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="136"/>
-      <c r="B25" s="145"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="137"/>
+      <c r="A25" s="143"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="150"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="151" t="s">
+      <c r="A26" s="139" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="150" t="s">
+      <c r="B26" s="140" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5348,8 +5375,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="151"/>
-      <c r="B27" s="150"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="140"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5376,28 +5403,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="152" t="s">
+      <c r="A30" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="150" t="s">
+      <c r="B30" s="140" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="136" t="s">
+      <c r="C30" s="143" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="140" t="s">
+      <c r="D30" s="153" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="152"/>
-      <c r="B31" s="150"/>
-      <c r="C31" s="136"/>
-      <c r="D31" s="140"/>
+      <c r="A31" s="141"/>
+      <c r="B31" s="140"/>
+      <c r="C31" s="143"/>
+      <c r="D31" s="153"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="152"/>
-      <c r="B32" s="150"/>
+      <c r="A32" s="141"/>
+      <c r="B32" s="140"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5406,8 +5433,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="152"/>
-      <c r="B33" s="150"/>
+      <c r="A33" s="141"/>
+      <c r="B33" s="140"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5416,8 +5443,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="152"/>
-      <c r="B34" s="150"/>
+      <c r="A34" s="141"/>
+      <c r="B34" s="140"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5426,8 +5453,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="152"/>
-      <c r="B35" s="150"/>
+      <c r="A35" s="141"/>
+      <c r="B35" s="140"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5436,8 +5463,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152"/>
-      <c r="B36" s="150"/>
+      <c r="A36" s="141"/>
+      <c r="B36" s="140"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5446,26 +5473,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="152"/>
-      <c r="B37" s="150"/>
-      <c r="C37" s="141" t="s">
+      <c r="A37" s="141"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="154" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="143" t="s">
+      <c r="D37" s="156" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="152"/>
-      <c r="B38" s="150"/>
-      <c r="C38" s="142"/>
-      <c r="D38" s="143"/>
+      <c r="A38" s="141"/>
+      <c r="B38" s="140"/>
+      <c r="C38" s="155"/>
+      <c r="D38" s="156"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="151" t="s">
+      <c r="A39" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="150" t="s">
+      <c r="B39" s="140" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5476,8 +5503,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="151"/>
-      <c r="B40" s="150"/>
+      <c r="A40" s="139"/>
+      <c r="B40" s="140"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5504,10 +5531,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="152" t="s">
+      <c r="A43" s="141" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="150" t="s">
+      <c r="B43" s="140" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5516,8 +5543,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="152"/>
-      <c r="B44" s="150"/>
+      <c r="A44" s="141"/>
+      <c r="B44" s="140"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5529,7 +5556,7 @@
       <c r="A45" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="150" t="s">
+      <c r="B45" s="140" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5539,7 +5566,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="148"/>
-      <c r="B46" s="150"/>
+      <c r="B46" s="140"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5549,7 +5576,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="148"/>
-      <c r="B47" s="150"/>
+      <c r="B47" s="140"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5559,7 +5586,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="149"/>
-      <c r="B48" s="150"/>
+      <c r="B48" s="140"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5568,10 +5595,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="145" t="s">
+      <c r="A49" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="145" t="s">
+      <c r="B49" s="144" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9675,8 +9702,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="145"/>
-      <c r="B50" s="145"/>
+      <c r="A50" s="144"/>
+      <c r="B50" s="144"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13780,8 +13807,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="145"/>
-      <c r="B51" s="145"/>
+      <c r="A51" s="144"/>
+      <c r="B51" s="144"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17885,8 +17912,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="145"/>
-      <c r="B52" s="145"/>
+      <c r="A52" s="144"/>
+      <c r="B52" s="144"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21990,12 +22017,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="145"/>
-      <c r="B53" s="145"/>
-      <c r="C53" s="139" t="s">
+      <c r="A53" s="144"/>
+      <c r="B53" s="144"/>
+      <c r="C53" s="152" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="140" t="s">
+      <c r="D53" s="153" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26095,10 +26122,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="145"/>
-      <c r="B54" s="145"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="140"/>
+      <c r="A54" s="144"/>
+      <c r="B54" s="144"/>
+      <c r="C54" s="152"/>
+      <c r="D54" s="153"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30216,10 +30243,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="144" t="s">
+      <c r="A57" s="145" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="145" t="s">
+      <c r="B57" s="144" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30230,8 +30257,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="144"/>
-      <c r="B58" s="145"/>
+      <c r="A58" s="145"/>
+      <c r="B58" s="144"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30240,8 +30267,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="144"/>
-      <c r="B59" s="145"/>
+      <c r="A59" s="145"/>
+      <c r="B59" s="144"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30250,8 +30277,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="144"/>
-      <c r="B60" s="145"/>
+      <c r="A60" s="145"/>
+      <c r="B60" s="144"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30260,8 +30287,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="144"/>
-      <c r="B61" s="145"/>
+      <c r="A61" s="145"/>
+      <c r="B61" s="144"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30270,8 +30297,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="144"/>
-      <c r="B62" s="145"/>
+      <c r="A62" s="145"/>
+      <c r="B62" s="144"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30280,8 +30307,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="144"/>
-      <c r="B63" s="145"/>
+      <c r="A63" s="145"/>
+      <c r="B63" s="144"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30290,16 +30317,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="144"/>
-      <c r="B64" s="145"/>
+      <c r="A64" s="145"/>
+      <c r="B64" s="144"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="144"/>
-      <c r="B65" s="145"/>
+      <c r="A65" s="145"/>
+      <c r="B65" s="144"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30308,16 +30335,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="144"/>
-      <c r="B66" s="145"/>
+      <c r="A66" s="145"/>
+      <c r="B66" s="144"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="144"/>
-      <c r="B67" s="145"/>
+      <c r="A67" s="145"/>
+      <c r="B67" s="144"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30326,8 +30353,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="144"/>
-      <c r="B68" s="145"/>
+      <c r="A68" s="145"/>
+      <c r="B68" s="144"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30336,8 +30363,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="144"/>
-      <c r="B69" s="145"/>
+      <c r="A69" s="145"/>
+      <c r="B69" s="144"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30346,8 +30373,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="144"/>
-      <c r="B70" s="145"/>
+      <c r="A70" s="145"/>
+      <c r="B70" s="144"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30356,8 +30383,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="144"/>
-      <c r="B71" s="145"/>
+      <c r="A71" s="145"/>
+      <c r="B71" s="144"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30366,8 +30393,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="144"/>
-      <c r="B72" s="145"/>
+      <c r="A72" s="145"/>
+      <c r="B72" s="144"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30376,16 +30403,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="144"/>
-      <c r="B73" s="145"/>
+      <c r="A73" s="145"/>
+      <c r="B73" s="144"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="144"/>
-      <c r="B74" s="145"/>
+      <c r="A74" s="145"/>
+      <c r="B74" s="144"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30394,17 +30421,17 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="144"/>
-      <c r="B75" s="145"/>
-      <c r="C75" s="138"/>
+      <c r="A75" s="145"/>
+      <c r="B75" s="144"/>
+      <c r="C75" s="151"/>
       <c r="D75" s="146" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="144"/>
-      <c r="B76" s="145"/>
-      <c r="C76" s="138"/>
+      <c r="A76" s="145"/>
+      <c r="B76" s="144"/>
+      <c r="C76" s="151"/>
       <c r="D76" s="146"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -30429,8 +30456,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30439,13 +30466,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30460,22 +30503,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30529,10 +30556,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="150" t="s">
+      <c r="B4" s="140" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30543,133 +30570,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="151"/>
-      <c r="B5" s="150"/>
-      <c r="C5" s="161" t="s">
+      <c r="A5" s="139"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="166" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="160" t="s">
+      <c r="D5" s="165" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="151"/>
-      <c r="B6" s="150"/>
-      <c r="C6" s="161"/>
-      <c r="D6" s="160"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="165"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="151"/>
-      <c r="B7" s="150"/>
+      <c r="A7" s="139"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="151"/>
-      <c r="B8" s="150"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="140"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="151"/>
-      <c r="B9" s="150"/>
+      <c r="A9" s="139"/>
+      <c r="B9" s="140"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="153" t="s">
+      <c r="A10" s="142" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="163"/>
-      <c r="D10" s="160" t="s">
+      <c r="C10" s="164"/>
+      <c r="D10" s="165" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="153"/>
-      <c r="B11" s="150"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="160"/>
+      <c r="A11" s="142"/>
+      <c r="B11" s="140"/>
+      <c r="C11" s="164"/>
+      <c r="D11" s="165"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="153"/>
-      <c r="B12" s="150"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="160"/>
+      <c r="A12" s="142"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="165"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="145" t="s">
+      <c r="B13" s="144" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="162"/>
-      <c r="D13" s="160" t="s">
+      <c r="C13" s="167"/>
+      <c r="D13" s="165" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="136"/>
-      <c r="B14" s="145"/>
-      <c r="C14" s="162"/>
-      <c r="D14" s="160"/>
+      <c r="A14" s="143"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="167"/>
+      <c r="D14" s="165"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="136"/>
-      <c r="B15" s="145"/>
-      <c r="C15" s="162"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="167"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="136"/>
-      <c r="B16" s="145"/>
-      <c r="C16" s="162"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="167"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="136"/>
-      <c r="B17" s="145"/>
-      <c r="C17" s="162"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="167"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="136"/>
-      <c r="B18" s="145"/>
-      <c r="C18" s="162"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="144"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="136"/>
-      <c r="B19" s="145"/>
-      <c r="C19" s="162"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="144"/>
+      <c r="C19" s="167"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="136"/>
-      <c r="B20" s="145"/>
-      <c r="C20" s="162"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="144"/>
+      <c r="C20" s="167"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="136"/>
-      <c r="B21" s="145"/>
-      <c r="C21" s="162"/>
+      <c r="A21" s="143"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="167"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="136"/>
-      <c r="B22" s="145"/>
-      <c r="C22" s="162"/>
+      <c r="A22" s="143"/>
+      <c r="B22" s="144"/>
+      <c r="C22" s="167"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="136"/>
-      <c r="B23" s="145"/>
-      <c r="C23" s="162"/>
+      <c r="A23" s="143"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="167"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30767,10 +30794,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="154" t="s">
+      <c r="A32" s="168" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="157" t="s">
+      <c r="B32" s="171" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30781,26 +30808,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="155"/>
-      <c r="B33" s="158"/>
+      <c r="A33" s="169"/>
+      <c r="B33" s="172"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="155"/>
-      <c r="B34" s="158"/>
+      <c r="A34" s="169"/>
+      <c r="B34" s="172"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="155"/>
-      <c r="B35" s="158"/>
+      <c r="A35" s="169"/>
+      <c r="B35" s="172"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="156"/>
-      <c r="B36" s="159"/>
+      <c r="A36" s="170"/>
+      <c r="B36" s="173"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30829,10 +30856,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="152" t="s">
+      <c r="A39" s="141" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="150" t="s">
+      <c r="B39" s="140" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30843,8 +30870,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="152"/>
-      <c r="B40" s="150"/>
+      <c r="A40" s="141"/>
+      <c r="B40" s="140"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30853,29 +30880,29 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="151" t="s">
+      <c r="A41" s="139" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="150" t="s">
+      <c r="B41" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="163" t="s">
+      <c r="C41" s="164" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="136" t="s">
+      <c r="D41" s="143" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="151"/>
-      <c r="B42" s="150"/>
-      <c r="C42" s="163"/>
-      <c r="D42" s="136"/>
+      <c r="A42" s="139"/>
+      <c r="B42" s="140"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="143"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="151"/>
-      <c r="B43" s="150"/>
-      <c r="C43" s="163" t="s">
+      <c r="A43" s="139"/>
+      <c r="B43" s="140"/>
+      <c r="C43" s="164" t="s">
         <v>190</v>
       </c>
       <c r="D43" s="146" t="s">
@@ -30883,54 +30910,54 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="151"/>
-      <c r="B44" s="150"/>
-      <c r="C44" s="163"/>
+      <c r="A44" s="139"/>
+      <c r="B44" s="140"/>
+      <c r="C44" s="164"/>
       <c r="D44" s="146"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="144" t="s">
+      <c r="A45" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="145" t="s">
+      <c r="B45" s="144" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="167"/>
+      <c r="C45" s="160"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="144"/>
-      <c r="B46" s="145"/>
-      <c r="C46" s="168"/>
-      <c r="D46" s="164" t="s">
+      <c r="A46" s="145"/>
+      <c r="B46" s="144"/>
+      <c r="C46" s="161"/>
+      <c r="D46" s="157" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="144"/>
-      <c r="B47" s="145"/>
-      <c r="C47" s="168"/>
-      <c r="D47" s="165"/>
+      <c r="A47" s="145"/>
+      <c r="B47" s="144"/>
+      <c r="C47" s="161"/>
+      <c r="D47" s="158"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="144"/>
-      <c r="B48" s="145"/>
-      <c r="C48" s="169"/>
-      <c r="D48" s="165"/>
+      <c r="A48" s="145"/>
+      <c r="B48" s="144"/>
+      <c r="C48" s="162"/>
+      <c r="D48" s="158"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="144"/>
-      <c r="B49" s="145"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="165"/>
+      <c r="A49" s="145"/>
+      <c r="B49" s="144"/>
+      <c r="C49" s="152"/>
+      <c r="D49" s="158"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="144"/>
-      <c r="B50" s="145"/>
-      <c r="C50" s="139"/>
-      <c r="D50" s="166"/>
+      <c r="A50" s="145"/>
+      <c r="B50" s="144"/>
+      <c r="C50" s="152"/>
+      <c r="D50" s="159"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -30953,10 +30980,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="145" t="s">
+      <c r="A53" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="145" t="s">
+      <c r="B53" s="144" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30967,8 +30994,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="145"/>
-      <c r="B54" s="145"/>
+      <c r="A54" s="144"/>
+      <c r="B54" s="144"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30977,8 +31004,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="145"/>
-      <c r="B55" s="145"/>
+      <c r="A55" s="144"/>
+      <c r="B55" s="144"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30987,9 +31014,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="145"/>
-      <c r="B56" s="145"/>
-      <c r="C56" s="170" t="s">
+      <c r="A56" s="144"/>
+      <c r="B56" s="144"/>
+      <c r="C56" s="163" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30997,16 +31024,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="145"/>
-      <c r="B57" s="145"/>
-      <c r="C57" s="170"/>
+      <c r="A57" s="144"/>
+      <c r="B57" s="144"/>
+      <c r="C57" s="163"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="145"/>
-      <c r="B58" s="145"/>
+      <c r="A58" s="144"/>
+      <c r="B58" s="144"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31015,8 +31042,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="145"/>
-      <c r="B59" s="145"/>
+      <c r="A59" s="144"/>
+      <c r="B59" s="144"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31025,9 +31052,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="145"/>
-      <c r="B60" s="145"/>
-      <c r="C60" s="170" t="s">
+      <c r="A60" s="144"/>
+      <c r="B60" s="144"/>
+      <c r="C60" s="163" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31035,25 +31062,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="145"/>
-      <c r="B61" s="145"/>
-      <c r="C61" s="170"/>
+      <c r="A61" s="144"/>
+      <c r="B61" s="144"/>
+      <c r="C61" s="163"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="145"/>
-      <c r="B62" s="145"/>
-      <c r="C62" s="170"/>
+      <c r="A62" s="144"/>
+      <c r="B62" s="144"/>
+      <c r="C62" s="163"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="145"/>
-      <c r="B63" s="145"/>
-      <c r="C63" s="163" t="s">
+      <c r="A63" s="144"/>
+      <c r="B63" s="144"/>
+      <c r="C63" s="164" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31061,29 +31088,29 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="145"/>
-      <c r="B64" s="145"/>
-      <c r="C64" s="163"/>
+      <c r="A64" s="144"/>
+      <c r="B64" s="144"/>
+      <c r="C64" s="164"/>
       <c r="D64" s="146" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="145"/>
-      <c r="B65" s="145"/>
-      <c r="C65" s="163"/>
+      <c r="A65" s="144"/>
+      <c r="B65" s="144"/>
+      <c r="C65" s="164"/>
       <c r="D65" s="146"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="145"/>
-      <c r="B66" s="145"/>
-      <c r="C66" s="163"/>
+      <c r="A66" s="144"/>
+      <c r="B66" s="144"/>
+      <c r="C66" s="164"/>
       <c r="D66" s="146"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="145"/>
-      <c r="B67" s="145"/>
-      <c r="C67" s="163"/>
+      <c r="A67" s="144"/>
+      <c r="B67" s="144"/>
+      <c r="C67" s="164"/>
       <c r="D67" s="146"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -31140,6 +31167,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31156,23 +31200,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31181,10 +31208,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31218,10 +31245,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="177" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="177" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="114" t="s">
@@ -31232,8 +31259,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="171"/>
-      <c r="B4" s="171"/>
+      <c r="A4" s="177"/>
+      <c r="B4" s="177"/>
       <c r="C4" s="114" t="s">
         <v>347</v>
       </c>
@@ -31250,10 +31277,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="175" t="s">
+      <c r="B6" s="163" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31262,8 +31289,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="136"/>
-      <c r="B7" s="176"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="163"/>
       <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
@@ -31275,7 +31302,9 @@
       <c r="A8" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="176"/>
+      <c r="B8" s="123" t="s">
+        <v>234</v>
+      </c>
       <c r="C8" s="106" t="s">
         <v>235</v>
       </c>
@@ -31287,7 +31316,9 @@
       <c r="A9" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="176"/>
+      <c r="B9" s="123" t="s">
+        <v>234</v>
+      </c>
       <c r="C9" s="106" t="s">
         <v>22</v>
       </c>
@@ -31296,26 +31327,28 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="170" t="s">
+      <c r="A10" s="163" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="176"/>
+      <c r="B10" s="163" t="s">
+        <v>234</v>
+      </c>
       <c r="C10" s="58"/>
       <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="170"/>
-      <c r="B11" s="176"/>
+      <c r="A11" s="163"/>
+      <c r="B11" s="163"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="170"/>
-      <c r="B12" s="176"/>
+      <c r="A12" s="163"/>
+      <c r="B12" s="163"/>
       <c r="C12" s="110" t="s">
         <v>325</v>
       </c>
@@ -31327,794 +31360,796 @@
       <c r="A13" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="176"/>
+      <c r="B13" s="123" t="s">
+        <v>234</v>
+      </c>
       <c r="C13" s="118" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="58"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="168" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="176"/>
+      <c r="B14" s="181" t="s">
+        <v>234</v>
+      </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="122" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="100" t="s">
-        <v>331</v>
-      </c>
-      <c r="B15" s="176"/>
-      <c r="C15" s="118" t="s">
-        <v>332</v>
-      </c>
-      <c r="D15" s="100" t="s">
-        <v>333</v>
+      <c r="A15" s="169"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="121" t="s">
+        <v>361</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="100" t="s">
-        <v>351</v>
-      </c>
-      <c r="B16" s="177"/>
-      <c r="C16" s="118" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="100"/>
+      <c r="A16" s="169"/>
+      <c r="B16" s="182"/>
+      <c r="C16" s="121" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>363</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="170"/>
+      <c r="B17" s="183"/>
+      <c r="C17" s="121" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" s="100" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="178" t="s">
-        <v>237</v>
-      </c>
-      <c r="B18" s="170" t="s">
+      <c r="A18" s="100" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58" t="s">
-        <v>258</v>
+      <c r="C18" s="118" t="s">
+        <v>332</v>
+      </c>
+      <c r="D18" s="100" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="178"/>
-      <c r="B19" s="170"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58" t="s">
-        <v>252</v>
-      </c>
+      <c r="A19" s="100" t="s">
+        <v>351</v>
+      </c>
+      <c r="B19" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="100"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="178"/>
-      <c r="B20" s="170"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58" t="s">
-        <v>254</v>
-      </c>
+    <row r="20" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="178"/>
-      <c r="B21" s="170"/>
-      <c r="C21" s="58" t="s">
-        <v>300</v>
-      </c>
+      <c r="A21" s="176" t="s">
+        <v>237</v>
+      </c>
+      <c r="B21" s="163" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="58"/>
       <c r="D21" s="58" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="178"/>
-      <c r="B22" s="170"/>
-      <c r="C22" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="D22" s="100" t="s">
-        <v>327</v>
+      <c r="A22" s="176"/>
+      <c r="B22" s="163"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="152" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>303</v>
-      </c>
-      <c r="D23" s="100" t="s">
-        <v>304</v>
+      <c r="A23" s="176"/>
+      <c r="B23" s="163"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
-      <c r="B24" s="170"/>
-      <c r="C24" s="58"/>
+      <c r="A24" s="176"/>
+      <c r="B24" s="163"/>
+      <c r="C24" s="58" t="s">
+        <v>300</v>
+      </c>
       <c r="D24" s="58" t="s">
-        <v>238</v>
+        <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="152"/>
-      <c r="B25" s="170"/>
-      <c r="C25" s="108" t="s">
-        <v>329</v>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="176"/>
+      <c r="B25" s="163"/>
+      <c r="C25" s="58" t="s">
+        <v>328</v>
       </c>
       <c r="D25" s="100" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="170" t="s">
-        <v>222</v>
-      </c>
-      <c r="B26" s="170" t="s">
+      <c r="A26" s="141" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="179" t="s">
-        <v>239</v>
-      </c>
-      <c r="D26" s="103" t="s">
-        <v>241</v>
+      <c r="C26" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D26" s="100" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="170"/>
-      <c r="B27" s="170"/>
-      <c r="C27" s="179"/>
-      <c r="D27" s="100" t="s">
-        <v>278</v>
+      <c r="A27" s="141"/>
+      <c r="B27" s="163"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58" t="s">
+        <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="170"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="179" t="s">
-        <v>240</v>
-      </c>
-      <c r="D28" s="58" t="s">
-        <v>299</v>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="141"/>
+      <c r="B28" s="163"/>
+      <c r="C28" s="108" t="s">
+        <v>329</v>
+      </c>
+      <c r="D28" s="100" t="s">
+        <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="170"/>
-      <c r="B29" s="170"/>
-      <c r="C29" s="179"/>
-      <c r="D29" s="61" t="s">
-        <v>242</v>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="141"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="108" t="s">
+        <v>359</v>
+      </c>
+      <c r="D29" s="100" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="170"/>
-      <c r="B30" s="170"/>
-      <c r="C30" s="105" t="s">
-        <v>307</v>
-      </c>
-      <c r="D30" s="58" t="s">
-        <v>308</v>
+      <c r="A30" s="163" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="163" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="174" t="s">
+        <v>239</v>
+      </c>
+      <c r="D30" s="103" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="170"/>
-      <c r="B31" s="170"/>
-      <c r="C31" s="105">
-        <v>2.1</v>
-      </c>
-      <c r="D31" s="58" t="s">
-        <v>316</v>
+      <c r="A31" s="163"/>
+      <c r="B31" s="163"/>
+      <c r="C31" s="174"/>
+      <c r="D31" s="100" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="170"/>
-      <c r="B32" s="170"/>
-      <c r="C32" s="105" t="s">
-        <v>239</v>
+      <c r="A32" s="163"/>
+      <c r="B32" s="163"/>
+      <c r="C32" s="174" t="s">
+        <v>240</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="170"/>
-      <c r="B33" s="170"/>
-      <c r="C33" s="117" t="s">
-        <v>239</v>
-      </c>
-      <c r="D33" s="116" t="s">
-        <v>346</v>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="163"/>
+      <c r="B33" s="163"/>
+      <c r="C33" s="174"/>
+      <c r="D33" s="61" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="170"/>
-      <c r="B34" s="170"/>
-      <c r="C34" s="115" t="s">
+      <c r="A34" s="163"/>
+      <c r="B34" s="163"/>
+      <c r="C34" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="163"/>
+      <c r="B35" s="163"/>
+      <c r="C35" s="105">
+        <v>2.1</v>
+      </c>
+      <c r="D35" s="58" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="163"/>
+      <c r="B36" s="163"/>
+      <c r="C36" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="D34" s="100" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="145" t="s">
-        <v>296</v>
-      </c>
-      <c r="B35" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="C35" s="58" t="s">
-        <v>297</v>
-      </c>
-      <c r="D35" s="58" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="145"/>
-      <c r="B36" s="170"/>
-      <c r="C36" s="61" t="s">
-        <v>281</v>
-      </c>
       <c r="D36" s="58" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="145"/>
-      <c r="B37" s="170"/>
-      <c r="C37" s="58" t="s">
-        <v>350</v>
-      </c>
-      <c r="D37" s="58" t="s">
-        <v>349</v>
+      <c r="A37" s="163"/>
+      <c r="B37" s="163"/>
+      <c r="C37" s="117" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" s="116" t="s">
+        <v>346</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="44"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="163"/>
+      <c r="B38" s="163"/>
+      <c r="C38" s="115" t="s">
+        <v>239</v>
+      </c>
+      <c r="D38" s="100" t="s">
+        <v>352</v>
+      </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="136" t="s">
-        <v>260</v>
-      </c>
-      <c r="B39" s="170" t="s">
+    <row r="39" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="144" t="s">
+        <v>296</v>
+      </c>
+      <c r="B39" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="79" t="s">
-        <v>261</v>
+      <c r="C39" s="58" t="s">
+        <v>297</v>
+      </c>
+      <c r="D39" s="58" t="s">
+        <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="136"/>
-      <c r="B40" s="170"/>
-      <c r="C40" s="58"/>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="144"/>
+      <c r="B40" s="163"/>
+      <c r="C40" s="61" t="s">
+        <v>281</v>
+      </c>
       <c r="D40" s="58" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="B41" s="105" t="s">
+      <c r="A41" s="144"/>
+      <c r="B41" s="163"/>
+      <c r="C41" s="58" t="s">
+        <v>350</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="44"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="143" t="s">
+        <v>260</v>
+      </c>
+      <c r="B43" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C41" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="D41" s="100" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="B42" s="105" t="s">
-        <v>234</v>
-      </c>
-      <c r="C42" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="104" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="172" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="175" t="s">
-        <v>234</v>
-      </c>
-      <c r="C43" s="58" t="s">
-        <v>268</v>
-      </c>
-      <c r="D43" s="58" t="s">
-        <v>251</v>
+      <c r="C43" s="58"/>
+      <c r="D43" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="173"/>
-      <c r="B44" s="176"/>
-      <c r="C44" s="58" t="s">
-        <v>270</v>
-      </c>
+      <c r="A44" s="143"/>
+      <c r="B44" s="163"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="58" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="173"/>
-      <c r="B45" s="176"/>
-      <c r="C45" s="58" t="s">
-        <v>269</v>
-      </c>
-      <c r="D45" s="58" t="s">
-        <v>251</v>
+      <c r="A45" s="58" t="s">
+        <v>334</v>
+      </c>
+      <c r="B45" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="79" t="s">
+        <v>335</v>
+      </c>
+      <c r="D45" s="100" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="173"/>
-      <c r="B46" s="176"/>
-      <c r="C46" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D46" s="100" t="s">
-        <v>102</v>
+      <c r="A46" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="C46" s="106" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="104" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="173"/>
-      <c r="B47" s="176"/>
+    <row r="47" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="178" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="181" t="s">
+        <v>234</v>
+      </c>
       <c r="C47" s="58" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="D47" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="173"/>
-      <c r="B48" s="176"/>
+      <c r="A48" s="179"/>
+      <c r="B48" s="182"/>
       <c r="C48" s="58" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D48" s="58" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="173"/>
-      <c r="B49" s="176"/>
-      <c r="C49" s="100" t="s">
-        <v>288</v>
-      </c>
-      <c r="D49" s="100" t="s">
+      <c r="A49" s="179"/>
+      <c r="B49" s="182"/>
+      <c r="C49" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D49" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="173"/>
-      <c r="B50" s="176"/>
+      <c r="A50" s="179"/>
+      <c r="B50" s="182"/>
       <c r="C50" s="100" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
       <c r="D50" s="100" t="s">
-        <v>251</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="173"/>
-      <c r="B51" s="176"/>
-      <c r="C51" s="100" t="s">
-        <v>289</v>
-      </c>
-      <c r="D51" s="100" t="s">
-        <v>102</v>
+      <c r="A51" s="179"/>
+      <c r="B51" s="182"/>
+      <c r="C51" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D51" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="173"/>
-      <c r="B52" s="176"/>
-      <c r="C52" s="107" t="s">
-        <v>244</v>
-      </c>
-      <c r="D52" s="104" t="s">
-        <v>245</v>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="179"/>
+      <c r="B52" s="182"/>
+      <c r="C52" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D52" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="173"/>
-      <c r="B53" s="176"/>
-      <c r="C53" s="108" t="s">
-        <v>311</v>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="179"/>
+      <c r="B53" s="182"/>
+      <c r="C53" s="100" t="s">
+        <v>288</v>
       </c>
       <c r="D53" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="173"/>
-      <c r="B54" s="176"/>
-      <c r="C54" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="D54" s="58" t="s">
-        <v>100</v>
+      <c r="A54" s="179"/>
+      <c r="B54" s="182"/>
+      <c r="C54" s="100" t="s">
+        <v>302</v>
+      </c>
+      <c r="D54" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="173"/>
-      <c r="B55" s="176"/>
+      <c r="A55" s="179"/>
+      <c r="B55" s="182"/>
       <c r="C55" s="100" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="D55" s="100" t="s">
-        <v>314</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="173"/>
-      <c r="B56" s="176"/>
-      <c r="C56" s="100" t="s">
-        <v>315</v>
-      </c>
-      <c r="D56" s="100" t="s">
-        <v>102</v>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="179"/>
+      <c r="B56" s="182"/>
+      <c r="C56" s="107" t="s">
+        <v>244</v>
+      </c>
+      <c r="D56" s="104" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="173"/>
-      <c r="B57" s="176"/>
-      <c r="C57" s="100" t="s">
-        <v>268</v>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="179"/>
+      <c r="B57" s="182"/>
+      <c r="C57" s="108" t="s">
+        <v>311</v>
       </c>
       <c r="D57" s="100" t="s">
-        <v>102</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="173"/>
-      <c r="B58" s="176"/>
+      <c r="A58" s="179"/>
+      <c r="B58" s="182"/>
       <c r="C58" s="58" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D58" s="58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="173"/>
-      <c r="B59" s="176"/>
+      <c r="A59" s="179"/>
+      <c r="B59" s="182"/>
       <c r="C59" s="100" t="s">
-        <v>283</v>
+        <v>313</v>
       </c>
       <c r="D59" s="100" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="173"/>
-      <c r="B60" s="176"/>
+      <c r="A60" s="179"/>
+      <c r="B60" s="182"/>
       <c r="C60" s="100" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D60" s="100" t="s">
-        <v>251</v>
+        <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="173"/>
-      <c r="B61" s="176"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="109" t="s">
-        <v>321</v>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="179"/>
+      <c r="B61" s="182"/>
+      <c r="C61" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="D61" s="100" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="173"/>
-      <c r="B62" s="176"/>
-      <c r="C62" s="100" t="s">
-        <v>322</v>
-      </c>
-      <c r="D62" s="100" t="s">
-        <v>251</v>
+      <c r="A62" s="179"/>
+      <c r="B62" s="182"/>
+      <c r="C62" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D62" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="173"/>
-      <c r="B63" s="176"/>
+      <c r="A63" s="179"/>
+      <c r="B63" s="182"/>
       <c r="C63" s="100" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="D63" s="100" t="s">
-        <v>251</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="173"/>
-      <c r="B64" s="176"/>
+      <c r="A64" s="179"/>
+      <c r="B64" s="182"/>
       <c r="C64" s="100" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="D64" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="173"/>
-      <c r="B65" s="176"/>
-      <c r="C65" s="100" t="s">
-        <v>340</v>
-      </c>
-      <c r="D65" s="100" t="s">
-        <v>251</v>
+    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="179"/>
+      <c r="B65" s="182"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="109" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="173"/>
-      <c r="B66" s="176"/>
+      <c r="A66" s="179"/>
+      <c r="B66" s="182"/>
       <c r="C66" s="100" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D66" s="100" t="s">
-        <v>323</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="173"/>
-      <c r="B67" s="176"/>
-      <c r="C67" s="116" t="s">
-        <v>345</v>
-      </c>
-      <c r="D67" s="116" t="s">
+      <c r="A67" s="179"/>
+      <c r="B67" s="182"/>
+      <c r="C67" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="173"/>
-      <c r="B68" s="176"/>
+      <c r="A68" s="179"/>
+      <c r="B68" s="182"/>
       <c r="C68" s="100" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D68" s="100" t="s">
-        <v>337</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="173"/>
-      <c r="B69" s="176"/>
+      <c r="A69" s="179"/>
+      <c r="B69" s="182"/>
       <c r="C69" s="100" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="D69" s="100" t="s">
-        <v>354</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="173"/>
-      <c r="B70" s="176"/>
-      <c r="C70" s="120" t="s">
-        <v>356</v>
-      </c>
-      <c r="D70" s="119" t="s">
-        <v>355</v>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="179"/>
+      <c r="B70" s="182"/>
+      <c r="C70" s="100" t="s">
+        <v>324</v>
+      </c>
+      <c r="D70" s="100" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="174"/>
-      <c r="B71" s="177"/>
+      <c r="A71" s="179"/>
+      <c r="B71" s="182"/>
       <c r="C71" s="116" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="D71" s="116" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B72" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C72" s="58" t="s">
-        <v>30</v>
+      <c r="A72" s="179"/>
+      <c r="B72" s="182"/>
+      <c r="C72" s="100" t="s">
+        <v>338</v>
       </c>
       <c r="D72" s="100" t="s">
-        <v>274</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="58" t="s">
-        <v>310</v>
-      </c>
-      <c r="B73" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" s="58" t="s">
-        <v>30</v>
+      <c r="A73" s="179"/>
+      <c r="B73" s="182"/>
+      <c r="C73" s="100" t="s">
+        <v>353</v>
       </c>
       <c r="D73" s="100" t="s">
-        <v>274</v>
+        <v>354</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="44"/>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="179"/>
+      <c r="B74" s="182"/>
+      <c r="C74" s="120" t="s">
+        <v>356</v>
+      </c>
+      <c r="D74" s="119" t="s">
+        <v>355</v>
+      </c>
     </row>
-    <row r="75" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="99"/>
-      <c r="B75" s="67"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="79" t="s">
-        <v>261</v>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="179"/>
+      <c r="B75" s="182"/>
+      <c r="C75" s="100" t="s">
+        <v>357</v>
+      </c>
+      <c r="D75" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="170" t="s">
-        <v>84</v>
-      </c>
-      <c r="B76" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="C76" s="106" t="s">
-        <v>246</v>
-      </c>
-      <c r="D76" s="58" t="s">
-        <v>253</v>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="180"/>
+      <c r="B76" s="183"/>
+      <c r="C76" s="100" t="s">
+        <v>358</v>
+      </c>
+      <c r="D76" s="100" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="170"/>
-      <c r="B77" s="170"/>
-      <c r="C77" s="106">
-        <v>10.1</v>
-      </c>
-      <c r="D77" s="58" t="s">
-        <v>272</v>
+      <c r="A77" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="B77" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" s="100" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="170"/>
-      <c r="B78" s="170"/>
-      <c r="C78" s="106">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D78" s="58" t="s">
-        <v>272</v>
+      <c r="A78" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B78" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" s="100" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="170"/>
-      <c r="B79" s="170"/>
-      <c r="C79" s="111" t="s">
-        <v>293</v>
-      </c>
-      <c r="D79" s="101" t="s">
-        <v>294</v>
-      </c>
+    <row r="79" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="44"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="136" t="s">
-        <v>247</v>
-      </c>
-      <c r="B80" s="170" t="s">
+    <row r="80" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="99"/>
+      <c r="B80" s="67"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="163" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="163" t="s">
         <v>234</v>
       </c>
-      <c r="C80" s="170"/>
-      <c r="D80" s="180" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="136"/>
-      <c r="B81" s="170"/>
-      <c r="C81" s="170"/>
-      <c r="D81" s="180"/>
+      <c r="C81" s="106" t="s">
+        <v>246</v>
+      </c>
+      <c r="D81" s="58" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="104" t="s">
-        <v>262